<commit_message>
icd list update (#42)
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/gbd.ICD.Map.xlsx
+++ b/myCBD/myInfo/gbd.ICD.Map.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\0.CBD\myCBD\myInfo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="10935"/>
   </bookViews>
@@ -13,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$A$1:$AA$220</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,7 +35,7 @@
     <author>Dauphine, David (CDPH-CHSI)</author>
   </authors>
   <commentList>
-    <comment ref="Q1" authorId="0">
+    <comment ref="Q1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -54,7 +59,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C57" authorId="1">
+    <comment ref="C57" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -78,7 +83,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S126" authorId="2">
+    <comment ref="S126" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -107,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2832" uniqueCount="1391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2833" uniqueCount="1392">
   <si>
     <t>I. Communicable, maternal, perinatal and nutritional conditions</t>
   </si>
@@ -4516,11 +4521,14 @@
   <si>
     <t>Cancer/Malignant neoplasms</t>
   </si>
+  <si>
+    <t>Test</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###0.;###0."/>
   </numFmts>
@@ -5290,7 +5298,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5325,7 +5333,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5534,13 +5542,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA227"/>
+  <dimension ref="A1:AB227"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="V217" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="1" topLeftCell="Z2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A202" sqref="A202"/>
+      <selection pane="bottomRight" activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5575,7 +5583,7 @@
     <col min="28" max="16384" width="8.85546875" style="55"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="55" t="s">
         <v>1162</v>
       </c>
@@ -5655,8 +5663,11 @@
       <c r="AA1" s="10" t="s">
         <v>930</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB1" s="55" t="s">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" s="55" t="str">
         <f>Y2</f>
         <v>All CAUSES</v>
@@ -5705,7 +5716,7 @@
       </c>
       <c r="AA2" s="10"/>
     </row>
-    <row r="3" spans="1:27" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="55" t="str">
         <f t="shared" ref="A3:A66" si="0">IF(I3&lt;&gt;"",CONCATENATE("  ",D3,". ",IF(E3="",E3,IF(F3="",CONCATENATE("  ",E3,". "),CONCATENATE("  ",E3,".  ",F3,". "))),W3),"")</f>
         <v xml:space="preserve">  A. Communicable, maternal, perinatal and nutritional conditions</v>
@@ -5762,7 +5773,7 @@
       </c>
       <c r="AA3" s="2"/>
     </row>
-    <row r="4" spans="1:27" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="55" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  A.   99. Other Infectious Diseases</v>
@@ -5807,7 +5818,7 @@
       <c r="Z4" s="15"/>
       <c r="AA4" s="2"/>
     </row>
-    <row r="5" spans="1:27" ht="102" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" ht="102" x14ac:dyDescent="0.2">
       <c r="A5" s="55" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -5861,7 +5872,7 @@
       </c>
       <c r="AA5" s="2"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" s="55" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  A.   01. Tuberculosis</v>
@@ -5927,7 +5938,7 @@
       </c>
       <c r="AA6" s="2"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" s="55" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  A.   02. HIV/ and other Sexually transmitted diseases (STDs)</v>
@@ -5972,7 +5983,7 @@
       <c r="Z7" s="15"/>
       <c r="AA7" s="2"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" s="55" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  A.   02.  a. Sexually transmitted diseases (STDs) excluding HIV</v>
@@ -6039,7 +6050,7 @@
       </c>
       <c r="AA8" s="2"/>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" s="55" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6104,7 +6115,7 @@
       </c>
       <c r="AA9" s="2"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" s="55" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6169,7 +6180,7 @@
       </c>
       <c r="AA10" s="2"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" s="55" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6234,7 +6245,7 @@
       </c>
       <c r="AA11" s="2"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" s="55" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6297,7 +6308,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="55" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6362,7 +6373,7 @@
       </c>
       <c r="AA13" s="2"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" s="55" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  A.   02.  b. HIV/AIDS</v>
@@ -6429,7 +6440,7 @@
       </c>
       <c r="AA14" s="2"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" s="55" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6490,7 +6501,7 @@
       </c>
       <c r="AA15" s="2"/>
     </row>
-    <row r="16" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="55" t="str">
         <f t="shared" si="0"/>
         <v/>

</xml_diff>

<commit_message>
ICD 10 sheet cleaning
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/gbd.ICD.Map.xlsx
+++ b/myCBD/myInfo/gbd.ICD.Map.xlsx
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2835" uniqueCount="1394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2832" uniqueCount="1391">
   <si>
     <t>I. Communicable, maternal, perinatal and nutritional conditions</t>
   </si>
@@ -4520,15 +4520,6 @@
   </si>
   <si>
     <t>Cancer/Malignant neoplasms</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>more test</t>
-  </si>
-  <si>
-    <t>uno mas</t>
   </si>
 </sst>
 </file>
@@ -5548,13 +5539,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD227"/>
+  <dimension ref="A1:AA227"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="8" ySplit="1" topLeftCell="AA2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC2" sqref="AC2"/>
+      <selection pane="bottomRight" activeCell="AB1" sqref="AB1:AD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5589,7 +5580,7 @@
     <col min="28" max="16384" width="8.85546875" style="55"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="55" t="s">
         <v>1162</v>
       </c>
@@ -5669,17 +5660,8 @@
       <c r="AA1" s="10" t="s">
         <v>930</v>
       </c>
-      <c r="AB1" s="55" t="s">
-        <v>1391</v>
-      </c>
-      <c r="AC1" s="55" t="s">
-        <v>1392</v>
-      </c>
-      <c r="AD1" s="55" t="s">
-        <v>1393</v>
-      </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" s="55" t="str">
         <f>Y2</f>
         <v>All CAUSES</v>
@@ -5728,7 +5710,7 @@
       </c>
       <c r="AA2" s="10"/>
     </row>
-    <row r="3" spans="1:30" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="55" t="str">
         <f t="shared" ref="A3:A66" si="0">IF(I3&lt;&gt;"",CONCATENATE("  ",D3,". ",IF(E3="",E3,IF(F3="",CONCATENATE("  ",E3,". "),CONCATENATE("  ",E3,".  ",F3,". "))),W3),"")</f>
         <v xml:space="preserve">  A. Communicable, maternal, perinatal and nutritional conditions</v>
@@ -5785,7 +5767,7 @@
       </c>
       <c r="AA3" s="2"/>
     </row>
-    <row r="4" spans="1:30" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="55" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  A.   99. Other Infectious Diseases</v>
@@ -5830,7 +5812,7 @@
       <c r="Z4" s="15"/>
       <c r="AA4" s="2"/>
     </row>
-    <row r="5" spans="1:30" ht="102" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="102" x14ac:dyDescent="0.2">
       <c r="A5" s="55" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -5884,7 +5866,7 @@
       </c>
       <c r="AA5" s="2"/>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" s="55" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  A.   01. Tuberculosis</v>
@@ -5950,7 +5932,7 @@
       </c>
       <c r="AA6" s="2"/>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" s="55" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  A.   02. HIV/ and other Sexually transmitted diseases (STDs)</v>
@@ -5995,7 +5977,7 @@
       <c r="Z7" s="15"/>
       <c r="AA7" s="2"/>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" s="55" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  A.   02.  a. Sexually transmitted diseases (STDs) excluding HIV</v>
@@ -6062,7 +6044,7 @@
       </c>
       <c r="AA8" s="2"/>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" s="55" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6127,7 +6109,7 @@
       </c>
       <c r="AA9" s="2"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" s="55" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6192,7 +6174,7 @@
       </c>
       <c r="AA10" s="2"/>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" s="55" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6257,7 +6239,7 @@
       </c>
       <c r="AA11" s="2"/>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" s="55" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6320,7 +6302,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="13" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="55" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6385,7 +6367,7 @@
       </c>
       <c r="AA13" s="2"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" s="55" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">  A.   02.  b. HIV/AIDS</v>
@@ -6452,7 +6434,7 @@
       </c>
       <c r="AA14" s="2"/>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15" s="55" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6513,7 +6495,7 @@
       </c>
       <c r="AA15" s="2"/>
     </row>
-    <row r="16" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="55" t="str">
         <f t="shared" si="0"/>
         <v/>

</xml_diff>

<commit_message>
preparing for local installation
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/gbd.ICD.Map.xlsx
+++ b/myCBD/myInfo/gbd.ICD.Map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="10935"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="10935"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -4628,7 +4628,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -4931,9 +4931,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" textRotation="90"/>
     </xf>
@@ -4942,6 +4939,12 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="29">
@@ -5278,10 +5281,10 @@
   <dimension ref="A1:AA227"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="I218" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="1" topLeftCell="P147" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E220" sqref="E220"/>
+      <selection pane="bottomRight" activeCell="A148" sqref="A148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5342,7 +5345,7 @@
       <c r="I1" s="84" t="s">
         <v>1124</v>
       </c>
-      <c r="J1" s="107" t="s">
+      <c r="J1" s="106" t="s">
         <v>1169</v>
       </c>
       <c r="K1" s="9" t="s">
@@ -14521,13 +14524,13 @@
       <c r="L148" s="65" t="s">
         <v>1164</v>
       </c>
-      <c r="M148" s="108"/>
+      <c r="M148" s="107"/>
       <c r="N148" s="92"/>
       <c r="O148" s="9"/>
-      <c r="P148" s="9" t="s">
+      <c r="P148" s="109" t="s">
         <v>1209</v>
       </c>
-      <c r="Q148" s="106" t="s">
+      <c r="Q148" s="110" t="s">
         <v>1277</v>
       </c>
       <c r="R148" s="9" t="s">
@@ -19111,7 +19114,7 @@
       <c r="C221" s="75" t="s">
         <v>1307</v>
       </c>
-      <c r="D221" s="109" t="s">
+      <c r="D221" s="108" t="s">
         <v>1145</v>
       </c>
       <c r="E221" s="100" t="s">

</xml_diff>

<commit_message>
new data supression and error message cleaning
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/gbd.ICD.Map.xlsx
+++ b/myCBD/myInfo/gbd.ICD.Map.xlsx
@@ -4163,9 +4163,6 @@
     <t>Added I271 from other cardiovascular diseases per IHME. Move M725-M726 per IHME ("skin_cellulitis"), to other infectious diseases per CCB.</t>
   </si>
   <si>
-    <t>Added R95 as it's own new row, was missing before for some reason</t>
-  </si>
-  <si>
     <t>[Note: A02 (botulism) and A05 (salmonella unspecified) mapped differently in IHME, but left here as is]
 IHME labels as skin_cellulitis; no such category in CCB; this seems like best location</t>
   </si>
@@ -4287,6 +4284,9 @@
       </rPr>
       <t>Congestive heart failure</t>
     </r>
+  </si>
+  <si>
+    <t>Added R95 as it's own new row, was missing before for some reason; included with neonatal conditions (A09); had been its own condition (D12)</t>
   </si>
 </sst>
 </file>
@@ -5177,8 +5177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q148" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="R164" sqref="R164"/>
+    <sheetView tabSelected="1" topLeftCell="A220" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I224" sqref="I224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -5234,7 +5234,7 @@
         <v>1124</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>1271</v>
@@ -8049,7 +8049,7 @@
         <v>880</v>
       </c>
       <c r="V51" s="5" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="52" spans="1:22" ht="16.5" x14ac:dyDescent="0.25">
@@ -9359,7 +9359,7 @@
       </c>
       <c r="O74" s="59"/>
       <c r="P74" s="60" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="Q74" s="59" t="s">
         <v>557</v>
@@ -12401,7 +12401,7 @@
         <v>1272</v>
       </c>
       <c r="M126" s="59" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="N126" s="66" t="s">
         <v>1273</v>
@@ -13640,7 +13640,7 @@
         <v>D06</v>
       </c>
       <c r="I148" s="57" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="J148" s="18" t="s">
         <v>1164</v>
@@ -13649,7 +13649,7 @@
         <v>1205</v>
       </c>
       <c r="L148" s="58" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="M148" s="59" t="s">
         <v>454</v>
@@ -14496,16 +14496,16 @@
         <v>C05</v>
       </c>
       <c r="I163" s="5" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="J163" s="5" t="s">
         <v>1217</v>
       </c>
       <c r="K163" s="5" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="L163" s="49" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="M163" s="59"/>
       <c r="N163" s="68"/>
@@ -14513,7 +14513,7 @@
       <c r="P163" s="59"/>
       <c r="Q163" s="59"/>
       <c r="R163" s="5" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="S163" s="50"/>
       <c r="T163" s="5"/>
@@ -14547,16 +14547,16 @@
         <v>C99</v>
       </c>
       <c r="I164" s="5" t="s">
+        <v>1339</v>
+      </c>
+      <c r="J164" s="5" t="s">
         <v>1340</v>
       </c>
-      <c r="J164" s="5" t="s">
+      <c r="K164" s="5" t="s">
         <v>1341</v>
       </c>
-      <c r="K164" s="5" t="s">
+      <c r="L164" s="19" t="s">
         <v>1342</v>
-      </c>
-      <c r="L164" s="19" t="s">
-        <v>1343</v>
       </c>
       <c r="M164" s="59" t="s">
         <v>469</v>
@@ -14572,7 +14572,7 @@
         <v>1102</v>
       </c>
       <c r="R164" s="79" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="S164" s="52" t="s">
         <v>99</v>
@@ -15348,7 +15348,7 @@
       </c>
       <c r="V177" s="2"/>
     </row>
-    <row r="178" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:22" ht="51" x14ac:dyDescent="0.25">
       <c r="A178" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -17090,7 +17090,7 @@
       </c>
       <c r="O208" s="66"/>
       <c r="P208" s="60" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="Q208" s="59" t="s">
         <v>654</v>
@@ -17975,27 +17975,24 @@
         <v>1230</v>
       </c>
     </row>
-    <row r="224" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:22" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A224" s="44" t="str">
         <f t="shared" si="18"/>
-        <v>.....D.12. - Sudden infant death syndrome</v>
+        <v/>
       </c>
       <c r="D224" s="56" t="s">
-        <v>1144</v>
+        <v>1140</v>
       </c>
       <c r="E224" s="55" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="G224" s="42" t="str">
         <f t="shared" si="21"/>
-        <v>cD12</v>
-      </c>
-      <c r="H224" s="40" t="str">
-        <f>CONCATENATE(D224,E224,F224)</f>
-        <v>D12</v>
-      </c>
+        <v>cA09</v>
+      </c>
+      <c r="H224" s="40"/>
       <c r="I224" s="16" t="s">
-        <v>1324</v>
+        <v>1344</v>
       </c>
       <c r="J224" s="48" t="s">
         <v>1228</v>
@@ -18027,7 +18024,7 @@
         <v>Z02</v>
       </c>
       <c r="R225" s="48" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="226" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
@@ -18067,7 +18064,7 @@
         <v>Z</v>
       </c>
       <c r="R227" s="48" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="228" spans="1:18" x14ac:dyDescent="0.25">
@@ -18328,24 +18325,24 @@
   <sheetData>
     <row r="11" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="75" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="D11" s="76" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="E11" s="76" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="12" spans="3:5" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="77" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D12" s="78" t="s">
         <v>1335</v>
       </c>
-      <c r="D12" s="78" t="s">
+      <c r="E12" s="78" t="s">
         <v>1336</v>
-      </c>
-      <c r="E12" s="78" t="s">
-        <v>1337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new links; ICD10 work
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/gbd.ICD.Map.xlsx
+++ b/myCBD/myInfo/gbd.ICD.Map.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\0.CBD\myCBD\myInfo\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="10935"/>
   </bookViews>
@@ -36,7 +31,7 @@
     <author>Dauphine, David (CDPH-CHSI)</author>
   </authors>
   <commentList>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -60,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C57" authorId="1" shapeId="0">
+    <comment ref="C57" authorId="1">
       <text>
         <r>
           <rPr>
@@ -84,7 +79,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P126" authorId="2" shapeId="0">
+    <comment ref="P126" authorId="2">
       <text>
         <r>
           <rPr>
@@ -4345,7 +4340,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###0.;###0."/>
   </numFmts>
@@ -4661,7 +4656,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -4905,6 +4900,12 @@
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -4993,7 +4994,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5028,7 +5029,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5239,7 +5240,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L94" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F109" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="M111" sqref="M111"/>
     </sheetView>
   </sheetViews>
@@ -11774,13 +11775,13 @@
       <c r="J111" s="5" t="s">
         <v>1163</v>
       </c>
-      <c r="K111" s="5" t="s">
+      <c r="K111" s="83" t="s">
         <v>1260</v>
       </c>
       <c r="L111" s="49" t="s">
         <v>1349</v>
       </c>
-      <c r="M111" s="49" t="s">
+      <c r="M111" s="84" t="s">
         <v>1352</v>
       </c>
       <c r="N111" s="49" t="s">

</xml_diff>

<commit_message>
notes about abnormal glucose ICD-10-CM code.
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/gbd.ICD.Map.xlsx
+++ b/myCBD/myInfo/gbd.ICD.Map.xlsx
@@ -4312,13 +4312,13 @@
     <t>regExICD10_CM</t>
   </si>
   <si>
-    <t>E08-E13</t>
-  </si>
-  <si>
     <t>E0[8-9]|E1[0-3]</t>
   </si>
   <si>
     <t>ICD-10-CM from CDC ICD-10-CM 2016 definitions (https://www.cdc.gov/nchs/icd/icd10cm.htm)</t>
+  </si>
+  <si>
+    <t>E08-E13, R730 abnormal glucose excludes diabetes, so shouldn't include here? R739 is hyperglycemia, unspecified--include?</t>
   </si>
 </sst>
 </file>
@@ -5218,8 +5218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="X112" sqref="X112"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L160" sqref="L160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -11760,10 +11760,10 @@
         <v>1348</v>
       </c>
       <c r="M111" s="49" t="s">
+        <v>1353</v>
+      </c>
+      <c r="N111" s="49" t="s">
         <v>1351</v>
-      </c>
-      <c r="N111" s="49" t="s">
-        <v>1352</v>
       </c>
       <c r="O111" s="59" t="s">
         <v>975</v>
@@ -11791,7 +11791,7 @@
         <v>66</v>
       </c>
       <c r="X111" s="2" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="112" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added ICD-10-CM codes (match ICD-10 codes) for mental disorders and cardiovascular disease.
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/gbd.ICD.Map.xlsx
+++ b/myCBD/myInfo/gbd.ICD.Map.xlsx
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2783" uniqueCount="1354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2807" uniqueCount="1363">
   <si>
     <t>I. Communicable, maternal, perinatal and nutritional conditions</t>
   </si>
@@ -4319,6 +4319,33 @@
   </si>
   <si>
     <t>E08-E13, R730 abnormal glucose excludes diabetes, so shouldn't include here? R739 is hyperglycemia, unspecified--include?</t>
+  </si>
+  <si>
+    <t>F2[0-9]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I30-I33, I38, I40, I42, I43? </t>
+  </si>
+  <si>
+    <t>I3[0-3,8]|I4[0,2-3]</t>
+  </si>
+  <si>
+    <t>I0[1-9]</t>
+  </si>
+  <si>
+    <t>G4[5-6]|I6[0-9]</t>
+  </si>
+  <si>
+    <t>Why is I00 included if it refers to rheumatic fever without heart involvement?</t>
+  </si>
+  <si>
+    <t>I26, I27.0, 127.2-127.9, I28, I34-I37, I44-I49, I51, I70-I83.9, I85, I86-I99</t>
+  </si>
+  <si>
+    <t>I26|I27[0, 2-9]|I28|I3[4-7]|I4[4-9]|I51|I7|I8[0-4,6-9]|I85|I8[6-9]|I9[0-9]</t>
+  </si>
+  <si>
+    <t>Include I43 ICD-10-CM? I43 is cardiomyopathy in diseases classified elsewhere</t>
   </si>
 </sst>
 </file>
@@ -5218,8 +5245,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L160" sqref="L160"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="W149" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="X162" sqref="X162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -12352,8 +12382,12 @@
       <c r="L122" s="19" t="s">
         <v>797</v>
       </c>
-      <c r="M122" s="19"/>
-      <c r="N122" s="19"/>
+      <c r="M122" s="19" t="s">
+        <v>980</v>
+      </c>
+      <c r="N122" s="19" t="s">
+        <v>797</v>
+      </c>
       <c r="O122" s="59" t="s">
         <v>980</v>
       </c>
@@ -12408,8 +12442,12 @@
       <c r="L123" s="19" t="s">
         <v>798</v>
       </c>
-      <c r="M123" s="19"/>
-      <c r="N123" s="19"/>
+      <c r="M123" s="19" t="s">
+        <v>981</v>
+      </c>
+      <c r="N123" s="19" t="s">
+        <v>798</v>
+      </c>
       <c r="O123" s="59" t="s">
         <v>981</v>
       </c>
@@ -12464,8 +12502,12 @@
       <c r="L124" s="49" t="s">
         <v>799</v>
       </c>
-      <c r="M124" s="49"/>
-      <c r="N124" s="49"/>
+      <c r="M124" s="49" t="s">
+        <v>442</v>
+      </c>
+      <c r="N124" s="49" t="s">
+        <v>799</v>
+      </c>
       <c r="O124" s="59" t="s">
         <v>442</v>
       </c>
@@ -12518,10 +12560,14 @@
         <v>443</v>
       </c>
       <c r="L125" s="49" t="s">
-        <v>754</v>
-      </c>
-      <c r="M125" s="49"/>
-      <c r="N125" s="49"/>
+        <v>1354</v>
+      </c>
+      <c r="M125" s="49" t="s">
+        <v>443</v>
+      </c>
+      <c r="N125" s="49" t="s">
+        <v>1354</v>
+      </c>
       <c r="O125" s="59" t="s">
         <v>443</v>
       </c>
@@ -14451,8 +14497,12 @@
       <c r="L158" s="49" t="s">
         <v>826</v>
       </c>
-      <c r="M158" s="49"/>
-      <c r="N158" s="49"/>
+      <c r="M158" s="49" t="s">
+        <v>464</v>
+      </c>
+      <c r="N158" s="49" t="s">
+        <v>1357</v>
+      </c>
       <c r="O158" s="59" t="s">
         <v>464</v>
       </c>
@@ -14514,8 +14564,12 @@
       <c r="L159" s="49" t="s">
         <v>827</v>
       </c>
-      <c r="M159" s="49"/>
-      <c r="N159" s="49"/>
+      <c r="M159" s="49" t="s">
+        <v>465</v>
+      </c>
+      <c r="N159" s="49" t="s">
+        <v>827</v>
+      </c>
       <c r="O159" s="59" t="s">
         <v>465</v>
       </c>
@@ -14577,8 +14631,12 @@
       <c r="L160" s="49" t="s">
         <v>828</v>
       </c>
-      <c r="M160" s="49"/>
-      <c r="N160" s="49"/>
+      <c r="M160" s="49" t="s">
+        <v>466</v>
+      </c>
+      <c r="N160" s="49" t="s">
+        <v>828</v>
+      </c>
       <c r="O160" s="59" t="s">
         <v>466</v>
       </c>
@@ -14644,8 +14702,12 @@
       <c r="L161" s="49" t="s">
         <v>1233</v>
       </c>
-      <c r="M161" s="49"/>
-      <c r="N161" s="49"/>
+      <c r="M161" s="49" t="s">
+        <v>1232</v>
+      </c>
+      <c r="N161" s="49" t="s">
+        <v>1358</v>
+      </c>
       <c r="O161" s="59" t="s">
         <v>467</v>
       </c>
@@ -14707,8 +14769,12 @@
       <c r="L162" s="49" t="s">
         <v>830</v>
       </c>
-      <c r="M162" s="49"/>
-      <c r="N162" s="49"/>
+      <c r="M162" s="49" t="s">
+        <v>1355</v>
+      </c>
+      <c r="N162" s="49" t="s">
+        <v>1356</v>
+      </c>
       <c r="O162" s="59" t="s">
         <v>468</v>
       </c>
@@ -14734,7 +14800,9 @@
       <c r="W162" s="51" t="s">
         <v>98</v>
       </c>
-      <c r="X162" s="2"/>
+      <c r="X162" s="81" t="s">
+        <v>1362</v>
+      </c>
     </row>
     <row r="163" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A163" s="44" t="str">
@@ -14770,8 +14838,12 @@
       <c r="L163" s="49" t="s">
         <v>1331</v>
       </c>
-      <c r="M163" s="49"/>
-      <c r="N163" s="49"/>
+      <c r="M163" s="49" t="s">
+        <v>1331</v>
+      </c>
+      <c r="N163" s="49" t="s">
+        <v>1331</v>
+      </c>
       <c r="O163" s="59"/>
       <c r="P163" s="68"/>
       <c r="Q163" s="69"/>
@@ -14823,8 +14895,12 @@
       <c r="L164" s="19" t="s">
         <v>1341</v>
       </c>
-      <c r="M164" s="19"/>
-      <c r="N164" s="19"/>
+      <c r="M164" s="19" t="s">
+        <v>1360</v>
+      </c>
+      <c r="N164" s="19" t="s">
+        <v>1361</v>
+      </c>
       <c r="O164" s="59" t="s">
         <v>469</v>
       </c>
@@ -14850,7 +14926,9 @@
       <c r="W164" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="X164" s="2"/>
+      <c r="X164" s="81" t="s">
+        <v>1359</v>
+      </c>
     </row>
     <row r="165" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A165" s="44" t="str">

</xml_diff>

<commit_message>
Kidney disease a, b, c.
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/gbd.ICD.Map.xlsx
+++ b/myCBD/myInfo/gbd.ICD.Map.xlsx
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2807" uniqueCount="1363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2810" uniqueCount="1363">
   <si>
     <t>I. Communicable, maternal, perinatal and nutritional conditions</t>
   </si>
@@ -5246,10 +5246,10 @@
   <dimension ref="A1:X228"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B175" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="I183" sqref="I183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -15920,10 +15920,12 @@
       <c r="E181" s="26" t="s">
         <v>1157</v>
       </c>
-      <c r="F181" s="6"/>
+      <c r="F181" s="6" t="s">
+        <v>1126</v>
+      </c>
       <c r="G181" s="40" t="str">
         <f t="shared" ref="G181:G189" si="17">CONCATENATE("c",D181,E181,F181)</f>
-        <v>cD10</v>
+        <v>cD10a</v>
       </c>
       <c r="H181" s="40"/>
       <c r="I181" s="5"/>
@@ -15980,10 +15982,12 @@
       <c r="E182" s="26" t="s">
         <v>1157</v>
       </c>
-      <c r="F182" s="6"/>
+      <c r="F182" s="6" t="s">
+        <v>1127</v>
+      </c>
       <c r="G182" s="40" t="str">
         <f t="shared" si="17"/>
-        <v>cD10</v>
+        <v>cD10b</v>
       </c>
       <c r="H182" s="40"/>
       <c r="I182" s="5"/>
@@ -16040,10 +16044,12 @@
       <c r="E183" s="26" t="s">
         <v>1157</v>
       </c>
-      <c r="F183" s="6"/>
+      <c r="F183" s="6" t="s">
+        <v>1130</v>
+      </c>
       <c r="G183" s="40" t="str">
         <f t="shared" si="17"/>
-        <v>cD10</v>
+        <v>cD10c</v>
       </c>
       <c r="H183" s="40"/>
       <c r="I183" s="5"/>

</xml_diff>

<commit_message>
Fixed typos in Mental Health Disorders label/name
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/gbd.ICD.Map.xlsx
+++ b/myCBD/myInfo/gbd.ICD.Map.xlsx
@@ -3547,9 +3547,6 @@
     <t>OTHER</t>
   </si>
   <si>
-    <t>E.1. Mental Health disoders (non-subsance use)</t>
-  </si>
-  <si>
     <t>E.2. Substance use</t>
   </si>
   <si>
@@ -3650,9 +3647,6 @@
   </si>
   <si>
     <t>Other Chronic</t>
-  </si>
-  <si>
-    <t>Mental Health disoders (non-subsance use)</t>
   </si>
   <si>
     <t>Substance use (Mental Health)</t>
@@ -4346,6 +4340,12 @@
   </si>
   <si>
     <t>Include I43 ICD-10-CM? I43 is cardiomyopathy in diseases classified elsewhere</t>
+  </si>
+  <si>
+    <t>E.1. Mental Health disorders (non-substance use)</t>
+  </si>
+  <si>
+    <t>Mental Health disorders (non-substance use)</t>
   </si>
 </sst>
 </file>
@@ -5246,10 +5246,10 @@
   <dimension ref="A1:X228"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B175" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B109" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I183" sqref="I183"/>
+      <selection pane="bottomRight" activeCell="C118" sqref="C118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -5281,7 +5281,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>761</v>
@@ -5290,7 +5290,7 @@
         <v>763</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="E1" s="24" t="s">
         <v>1121</v>
@@ -5305,10 +5305,10 @@
         <v>1124</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>384</v>
@@ -5317,19 +5317,19 @@
         <v>759</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="O1" s="59" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="P1" s="59" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="Q1" s="59" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="R1" s="61" t="s">
         <v>509</v>
@@ -5344,10 +5344,10 @@
         <v>762</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="W1" s="45" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
       <c r="X1" s="6" t="s">
         <v>930</v>
@@ -5411,7 +5411,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E3" s="26"/>
       <c r="F3" s="6"/>
@@ -5463,7 +5463,7 @@
         <v>1129</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E4" s="26">
         <v>99</v>
@@ -5558,10 +5558,10 @@
         <v>2</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="40" t="str">
@@ -5617,10 +5617,10 @@
         <v>1125</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="40"/>
@@ -5640,11 +5640,11 @@
       <c r="R7" s="59"/>
       <c r="S7" s="59"/>
       <c r="T7" s="2" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="U7" s="20"/>
       <c r="V7" s="2" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="W7" s="45"/>
       <c r="X7" s="2"/>
@@ -5658,13 +5658,13 @@
         <v>4</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>1126</v>
@@ -5725,10 +5725,10 @@
         <v>4</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>1126</v>
@@ -5785,10 +5785,10 @@
         <v>5</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>1126</v>
@@ -5845,10 +5845,10 @@
         <v>6</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>1126</v>
@@ -5905,10 +5905,10 @@
         <v>7</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>1126</v>
@@ -5963,10 +5963,10 @@
         <v>8</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>1126</v>
@@ -6020,13 +6020,13 @@
         <v>10</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>1127</v>
@@ -6085,10 +6085,10 @@
         <v>686</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>1127</v>
@@ -6141,10 +6141,10 @@
         <v>687</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>1127</v>
@@ -6201,7 +6201,7 @@
         <v>10</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E17" s="26">
         <v>99</v>
@@ -6311,7 +6311,7 @@
         <v>12</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E19" s="26">
         <v>99</v>
@@ -6369,7 +6369,7 @@
         <v>13</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E20" s="26">
         <v>99</v>
@@ -6427,7 +6427,7 @@
         <v>14</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E21" s="26">
         <v>99</v>
@@ -6485,7 +6485,7 @@
         <v>15</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E22" s="26">
         <v>99</v>
@@ -6543,10 +6543,10 @@
         <v>16</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="40" t="str">
@@ -6604,10 +6604,10 @@
         <v>17</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="40" t="str">
@@ -6665,10 +6665,10 @@
         <v>688</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="40"/>
@@ -6719,10 +6719,10 @@
         <v>689</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="40" t="str">
@@ -6773,10 +6773,10 @@
         <v>690</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>1126</v>
@@ -6827,7 +6827,7 @@
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="34" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="D28" s="27"/>
       <c r="E28" s="26"/>
@@ -6860,10 +6860,10 @@
         <v>691</v>
       </c>
       <c r="D29" s="27" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>1127</v>
@@ -6919,10 +6919,10 @@
         <v>692</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E30" s="26" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="40" t="str">
@@ -7024,7 +7024,7 @@
         <v>18</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E32" s="26">
         <v>99</v>
@@ -7082,7 +7082,7 @@
         <v>19</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E33" s="26">
         <v>99</v>
@@ -7140,7 +7140,7 @@
         <v>20</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E34" s="26">
         <v>99</v>
@@ -7198,7 +7198,7 @@
         <v>21</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E35" s="26">
         <v>99</v>
@@ -7256,7 +7256,7 @@
         <v>22</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E36" s="26">
         <v>99</v>
@@ -7314,7 +7314,7 @@
         <v>23</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E37" s="26">
         <v>99</v>
@@ -7368,7 +7368,7 @@
         <v>24</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E38" s="26">
         <v>99</v>
@@ -7422,7 +7422,7 @@
         <v>694</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E39" s="26">
         <v>99</v>
@@ -7480,7 +7480,7 @@
         <v>695</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E40" s="26">
         <v>99</v>
@@ -7538,7 +7538,7 @@
         <v>889</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E41" s="26">
         <v>99</v>
@@ -7592,7 +7592,7 @@
         <v>890</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E42" s="26">
         <v>99</v>
@@ -7650,7 +7650,7 @@
         <v>891</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E43" s="26">
         <v>99</v>
@@ -7704,7 +7704,7 @@
         <v>893</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E44" s="26">
         <v>99</v>
@@ -7762,7 +7762,7 @@
         <v>894</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E45" s="26">
         <v>99</v>
@@ -7875,7 +7875,7 @@
         <v>25</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E47" s="26">
         <v>99</v>
@@ -7933,7 +7933,7 @@
         <v>26</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E48" s="26">
         <v>99</v>
@@ -7987,7 +7987,7 @@
         <v>27</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E49" s="26">
         <v>99</v>
@@ -8041,7 +8041,7 @@
         <v>696</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E50" s="26">
         <v>99</v>
@@ -8095,7 +8095,7 @@
         <v>880</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E51" s="26">
         <v>99</v>
@@ -8107,16 +8107,16 @@
       </c>
       <c r="H51" s="40"/>
       <c r="I51" s="5" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="L51" s="19" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="M51" s="19"/>
       <c r="N51" s="19"/>
@@ -8146,7 +8146,7 @@
         <v>880</v>
       </c>
       <c r="X51" s="5" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="52" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
@@ -8161,10 +8161,10 @@
         <v>28</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E52" s="26" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="F52" s="6"/>
       <c r="G52" s="40"/>
@@ -8221,10 +8221,10 @@
         <v>29</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E53" s="26" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="F53" s="6"/>
       <c r="G53" s="40" t="str">
@@ -8238,7 +8238,7 @@
         <v>404</v>
       </c>
       <c r="L53" s="80" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="M53" s="80"/>
       <c r="N53" s="80"/>
@@ -8281,10 +8281,10 @@
         <v>30</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E54" s="26" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="F54" s="6"/>
       <c r="G54" s="40" t="str">
@@ -8339,10 +8339,10 @@
         <v>31</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E55" s="26" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="F55" s="6"/>
       <c r="G55" s="40" t="str">
@@ -8397,10 +8397,10 @@
         <v>32</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E56" s="26" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F56" s="6"/>
       <c r="G56" s="40" t="s">
@@ -8459,10 +8459,10 @@
         <v>33</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E57" s="26" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F57" s="6"/>
       <c r="G57" s="40" t="str">
@@ -8517,10 +8517,10 @@
         <v>34</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E58" s="26" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F58" s="6"/>
       <c r="G58" s="40" t="str">
@@ -8575,10 +8575,10 @@
         <v>35</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E59" s="26" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F59" s="6"/>
       <c r="G59" s="40" t="str">
@@ -8633,10 +8633,10 @@
         <v>36</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E60" s="26" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F60" s="6"/>
       <c r="G60" s="40" t="str">
@@ -8691,10 +8691,10 @@
         <v>37</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E61" s="26" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F61" s="6"/>
       <c r="G61" s="40" t="str">
@@ -8749,10 +8749,10 @@
         <v>38</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E62" s="26" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F62" s="6"/>
       <c r="G62" s="40" t="str">
@@ -8807,10 +8807,10 @@
         <v>39</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E63" s="26" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="F63" s="6"/>
       <c r="G63" s="40" t="s">
@@ -8869,10 +8869,10 @@
         <v>40</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E64" s="26" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="F64" s="6"/>
       <c r="G64" s="40" t="str">
@@ -8927,10 +8927,10 @@
         <v>41</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E65" s="26" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="F65" s="6"/>
       <c r="G65" s="40" t="str">
@@ -8985,10 +8985,10 @@
         <v>42</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E66" s="26" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="F66" s="6"/>
       <c r="G66" s="40" t="str">
@@ -9043,10 +9043,10 @@
         <v>43</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E67" s="26" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="F67" s="6"/>
       <c r="G67" s="40" t="str">
@@ -9055,16 +9055,16 @@
       </c>
       <c r="H67" s="40"/>
       <c r="I67" s="5" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="J67" s="5" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K67" s="5" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="L67" s="19" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
       <c r="M67" s="19"/>
       <c r="N67" s="19"/>
@@ -9107,7 +9107,7 @@
         <v>44</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E68" s="26"/>
       <c r="F68" s="6"/>
@@ -9162,7 +9162,7 @@
         <v>45</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E69" s="26">
         <v>99</v>
@@ -9179,7 +9179,7 @@
         <v>420</v>
       </c>
       <c r="L69" s="16" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="O69" s="59" t="s">
         <v>420</v>
@@ -9220,7 +9220,7 @@
         <v>46</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E70" s="26">
         <v>99</v>
@@ -9278,7 +9278,7 @@
         <v>47</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E71" s="26">
         <v>99</v>
@@ -9332,7 +9332,7 @@
         <v>48</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E72" s="26">
         <v>99</v>
@@ -9390,7 +9390,7 @@
         <v>697</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E73" s="26">
         <v>99</v>
@@ -9470,7 +9470,7 @@
       </c>
       <c r="Q74" s="59"/>
       <c r="R74" s="60" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="S74" s="59" t="s">
         <v>557</v>
@@ -9496,10 +9496,10 @@
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="35" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="D75" s="25" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E75" s="26"/>
       <c r="F75" s="6"/>
@@ -9520,10 +9520,10 @@
       <c r="R75" s="59"/>
       <c r="S75" s="59"/>
       <c r="T75" s="20" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="V75" s="45" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="X75" s="2"/>
     </row>
@@ -9539,7 +9539,7 @@
         <v>51</v>
       </c>
       <c r="D76" s="25" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E76" s="26"/>
       <c r="F76" s="6"/>
@@ -9572,7 +9572,7 @@
         <v>558</v>
       </c>
       <c r="T76" s="2" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="U76" s="20" t="s">
         <v>51</v>
@@ -9597,10 +9597,10 @@
         <v>52</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E77" s="26" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="F77" s="6"/>
       <c r="G77" s="40" t="str">
@@ -9614,10 +9614,10 @@
       <c r="I77" s="5"/>
       <c r="J77" s="5"/>
       <c r="K77" s="5" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="L77" s="49" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="M77" s="49"/>
       <c r="N77" s="49"/>
@@ -9656,10 +9656,10 @@
         <v>698</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E78" s="26" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="F78" s="6"/>
       <c r="G78" s="40" t="str">
@@ -9668,16 +9668,16 @@
       </c>
       <c r="H78" s="40"/>
       <c r="I78" s="18" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="J78" s="17" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K78" s="5" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="L78" s="19" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="M78" s="19"/>
       <c r="N78" s="19"/>
@@ -9720,10 +9720,10 @@
         <v>699</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E79" s="26" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="F79" s="6"/>
       <c r="G79" s="40" t="str">
@@ -9732,16 +9732,16 @@
       </c>
       <c r="H79" s="40"/>
       <c r="I79" s="19" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="J79" s="17" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K79" s="5" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
       <c r="L79" s="49" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="M79" s="49"/>
       <c r="N79" s="49"/>
@@ -9784,10 +9784,10 @@
         <v>700</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E80" s="26" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="F80" s="6"/>
       <c r="G80" s="40" t="str">
@@ -9844,10 +9844,10 @@
         <v>53</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E81" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F81" s="6"/>
       <c r="G81" s="40" t="str">
@@ -9859,16 +9859,16 @@
         <v>B02</v>
       </c>
       <c r="I81" s="18" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="J81" s="17" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K81" s="5" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="L81" s="49" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="M81" s="49"/>
       <c r="N81" s="49"/>
@@ -9911,10 +9911,10 @@
         <v>54</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E82" s="26" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F82" s="6"/>
       <c r="G82" s="40" t="str">
@@ -9926,16 +9926,16 @@
         <v>B03</v>
       </c>
       <c r="I82" s="18" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="J82" s="17" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K82" s="5" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="L82" s="49" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="M82" s="49"/>
       <c r="N82" s="49"/>
@@ -9980,10 +9980,10 @@
         <v>55</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E83" s="26" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="F83" s="6"/>
       <c r="G83" s="40" t="str">
@@ -9995,16 +9995,16 @@
         <v>B04</v>
       </c>
       <c r="I83" s="16" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="J83" s="17" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K83" s="5" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="L83" s="49" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="M83" s="49"/>
       <c r="N83" s="49"/>
@@ -10047,10 +10047,10 @@
         <v>56</v>
       </c>
       <c r="D84" s="27" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E84" s="26" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="F84" s="6"/>
       <c r="G84" s="40" t="str">
@@ -10062,16 +10062,16 @@
         <v>B05</v>
       </c>
       <c r="I84" s="18" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="J84" s="17" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K84" s="5" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="L84" s="49" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="M84" s="49"/>
       <c r="N84" s="49"/>
@@ -10114,10 +10114,10 @@
         <v>57</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E85" s="26" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="F85" s="6"/>
       <c r="G85" s="40" t="str">
@@ -10129,16 +10129,16 @@
         <v>B06</v>
       </c>
       <c r="I85" s="18" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="J85" s="17" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K85" s="5" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="L85" s="49" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="M85" s="49"/>
       <c r="N85" s="49"/>
@@ -10181,10 +10181,10 @@
         <v>58</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E86" s="26" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="F86" s="6"/>
       <c r="G86" s="40" t="str">
@@ -10196,16 +10196,16 @@
         <v>B07</v>
       </c>
       <c r="I86" s="18" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
       <c r="J86" s="17" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K86" s="5" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="L86" s="49" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="M86" s="49"/>
       <c r="N86" s="49"/>
@@ -10248,10 +10248,10 @@
         <v>59</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E87" s="26" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F87" s="6"/>
       <c r="G87" s="40" t="s">
@@ -10262,7 +10262,7 @@
         <v>B08</v>
       </c>
       <c r="J87" s="17" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K87" s="5" t="s">
         <v>952</v>
@@ -10307,10 +10307,10 @@
         <v>701</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E88" s="26" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F88" s="6"/>
       <c r="G88" s="40" t="str">
@@ -10319,16 +10319,16 @@
       </c>
       <c r="H88" s="40"/>
       <c r="I88" s="18" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
       <c r="J88" s="17" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K88" s="5" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="L88" s="49" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="M88" s="49"/>
       <c r="N88" s="49"/>
@@ -10371,10 +10371,10 @@
         <v>702</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E89" s="26" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F89" s="6"/>
       <c r="G89" s="40" t="str">
@@ -10383,16 +10383,16 @@
       </c>
       <c r="H89" s="40"/>
       <c r="I89" s="18" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
       <c r="J89" s="17" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K89" s="5" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="L89" s="49" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="M89" s="49"/>
       <c r="N89" s="49"/>
@@ -10435,10 +10435,10 @@
         <v>60</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E90" s="26" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="F90" s="6"/>
       <c r="G90" s="40" t="str">
@@ -10450,16 +10450,16 @@
         <v>B09</v>
       </c>
       <c r="I90" s="16" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="J90" s="17" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K90" s="5" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="L90" s="49" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="M90" s="49"/>
       <c r="N90" s="49"/>
@@ -10497,10 +10497,10 @@
       </c>
       <c r="B91" s="2"/>
       <c r="C91" s="37" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E91" s="26">
         <v>10</v>
@@ -10512,7 +10512,7 @@
         <v>B10</v>
       </c>
       <c r="J91" s="17" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K91" s="5"/>
       <c r="L91" s="49"/>
@@ -10524,11 +10524,11 @@
       <c r="R91" s="59"/>
       <c r="S91" s="59"/>
       <c r="T91" s="5" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="U91" s="20"/>
       <c r="V91" s="5" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="W91" s="45"/>
       <c r="X91" s="2"/>
@@ -10545,10 +10545,10 @@
         <v>61</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E92" s="26" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="F92" s="6"/>
       <c r="G92" s="40" t="str">
@@ -10557,16 +10557,16 @@
       </c>
       <c r="H92" s="40"/>
       <c r="I92" s="5" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
       <c r="J92" s="17" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K92" s="5" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="L92" s="49" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="M92" s="49"/>
       <c r="N92" s="49"/>
@@ -10609,7 +10609,7 @@
         <v>62</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E93" s="26">
         <v>10</v>
@@ -10621,16 +10621,16 @@
       </c>
       <c r="H93" s="40"/>
       <c r="I93" s="5" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="J93" s="17" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K93" s="5" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L93" s="49" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="M93" s="49"/>
       <c r="N93" s="49"/>
@@ -10673,7 +10673,7 @@
         <v>63</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E94" s="26">
         <v>11</v>
@@ -10688,16 +10688,16 @@
         <v>B11</v>
       </c>
       <c r="I94" s="5" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="J94" s="17" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K94" s="5" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
       <c r="L94" s="49" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="M94" s="49"/>
       <c r="N94" s="49"/>
@@ -10740,10 +10740,10 @@
         <v>64</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E95" s="26" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="F95" s="6"/>
       <c r="G95" s="40" t="str">
@@ -10755,16 +10755,16 @@
         <v>B12</v>
       </c>
       <c r="I95" s="19" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="J95" s="17" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K95" s="5" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="L95" s="49" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="M95" s="49"/>
       <c r="N95" s="49"/>
@@ -10807,7 +10807,7 @@
         <v>703</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E96" s="26">
         <v>99</v>
@@ -10819,16 +10819,16 @@
       </c>
       <c r="H96" s="40"/>
       <c r="I96" s="19" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
       <c r="J96" s="17" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K96" s="5" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="L96" s="49" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="M96" s="49"/>
       <c r="N96" s="49"/>
@@ -10871,7 +10871,7 @@
         <v>704</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E97" s="26">
         <v>13</v>
@@ -10886,16 +10886,16 @@
         <v>B13</v>
       </c>
       <c r="I97" s="19" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
       <c r="J97" s="17" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K97" s="5" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="L97" s="49" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="M97" s="49"/>
       <c r="N97" s="49"/>
@@ -10938,7 +10938,7 @@
         <v>705</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E98" s="26">
         <v>14</v>
@@ -10953,16 +10953,16 @@
         <v>B14</v>
       </c>
       <c r="I98" s="5" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
       <c r="J98" s="17" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K98" s="5" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="L98" s="49" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="M98" s="49"/>
       <c r="N98" s="49"/>
@@ -11005,7 +11005,7 @@
         <v>706</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E99" s="26">
         <v>15</v>
@@ -11020,16 +11020,16 @@
         <v>B15</v>
       </c>
       <c r="I99" s="16" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
       <c r="J99" s="17" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K99" s="5" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
       <c r="L99" s="19" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="M99" s="19"/>
       <c r="N99" s="19"/>
@@ -11072,7 +11072,7 @@
         <v>707</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E100" s="26">
         <v>99</v>
@@ -11084,16 +11084,16 @@
       </c>
       <c r="H100" s="40"/>
       <c r="I100" s="19" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
       <c r="J100" s="17" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K100" s="5" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
       <c r="L100" s="49" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="M100" s="49"/>
       <c r="N100" s="49"/>
@@ -11136,7 +11136,7 @@
         <v>708</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E101" s="26">
         <v>99</v>
@@ -11148,16 +11148,16 @@
       </c>
       <c r="H101" s="40"/>
       <c r="I101" s="19" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
       <c r="J101" s="17" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K101" s="5" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="L101" s="49" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="M101" s="49"/>
       <c r="N101" s="49"/>
@@ -11200,7 +11200,7 @@
         <v>709</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E102" s="26">
         <v>99</v>
@@ -11212,16 +11212,16 @@
       </c>
       <c r="H102" s="40"/>
       <c r="I102" s="19" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
       <c r="J102" s="17" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K102" s="5" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="L102" s="49" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="M102" s="49"/>
       <c r="N102" s="49"/>
@@ -11264,7 +11264,7 @@
         <v>710</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E103" s="26">
         <v>99</v>
@@ -11324,7 +11324,7 @@
         <v>711</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E104" s="26">
         <v>16</v>
@@ -11384,7 +11384,7 @@
         <v>712</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E105" s="26">
         <v>16</v>
@@ -11449,7 +11449,7 @@
         <v>713</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E106" s="26">
         <v>16</v>
@@ -11514,7 +11514,7 @@
         <v>714</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E107" s="26">
         <v>16</v>
@@ -11579,7 +11579,7 @@
         <v>715</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E108" s="26">
         <v>17</v>
@@ -11642,7 +11642,7 @@
         <v>716</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E109" s="26">
         <v>99</v>
@@ -11657,16 +11657,16 @@
         <v>B99</v>
       </c>
       <c r="I109" s="5" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
       <c r="J109" s="5" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K109" s="5" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="L109" s="49" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="M109" s="49"/>
       <c r="N109" s="49"/>
@@ -11705,7 +11705,7 @@
         <v>65</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E110" s="26">
         <v>99</v>
@@ -11717,10 +11717,10 @@
       </c>
       <c r="H110" s="40"/>
       <c r="K110" s="5" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="L110" s="5" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="M110" s="5"/>
       <c r="N110" s="5"/>
@@ -11763,10 +11763,10 @@
         <v>66</v>
       </c>
       <c r="D111" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E111" s="26" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="F111" s="6"/>
       <c r="G111" s="40" t="str">
@@ -11778,22 +11778,22 @@
         <v>D01</v>
       </c>
       <c r="I111" s="5" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="J111" s="5" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K111" s="5" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="L111" s="49" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="M111" s="49" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="N111" s="49" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="O111" s="59" t="s">
         <v>975</v>
@@ -11821,7 +11821,7 @@
         <v>66</v>
       </c>
       <c r="X111" s="2" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="112" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
@@ -11836,10 +11836,10 @@
         <v>67</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E112" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F112" s="6"/>
       <c r="G112" s="40" t="s">
@@ -11852,18 +11852,18 @@
       <c r="I112" s="5"/>
       <c r="J112" s="5"/>
       <c r="K112" s="5" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="L112" s="19" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
       <c r="M112" s="19"/>
       <c r="N112" s="19"/>
       <c r="O112" s="59" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="P112" s="66" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
       <c r="Q112" s="69"/>
       <c r="R112" s="59" t="s">
@@ -11898,10 +11898,10 @@
         <v>717</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E113" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F113" s="6"/>
       <c r="G113" s="40" t="str">
@@ -11958,10 +11958,10 @@
         <v>718</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E114" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F114" s="6"/>
       <c r="G114" s="40" t="str">
@@ -12018,10 +12018,10 @@
         <v>719</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E115" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F115" s="6"/>
       <c r="G115" s="40" t="str">
@@ -12078,10 +12078,10 @@
         <v>720</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E116" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F116" s="6"/>
       <c r="G116" s="40" t="str">
@@ -12187,18 +12187,18 @@
     </row>
     <row r="118" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A118" s="44" t="str">
-        <f t="shared" si="4"/>
-        <v>.....D.03. - Mental Health disoders (non-subsance use)</v>
+        <f>IF(H118&lt;&gt;"",IF(F118&lt;&gt;"",CONCATENATE("..........",D118,".",E118,".",F118,". - ",T118),IF(E118&lt;&gt;"",CONCATENATE(".....",D118,".",E118,". - ",T118),CONCATENATE(D118,". - ",T118))),"")</f>
+        <v>.....D.03. - Mental Health disorders (non-substance use)</v>
       </c>
       <c r="B118" s="2"/>
       <c r="C118" s="32" t="s">
-        <v>1132</v>
+        <v>1361</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E118" s="26" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F118" s="6"/>
       <c r="G118" s="40" t="s">
@@ -12220,11 +12220,11 @@
       <c r="R118" s="59"/>
       <c r="S118" s="59"/>
       <c r="T118" s="2" t="s">
-        <v>1160</v>
+        <v>1362</v>
       </c>
       <c r="U118" s="20"/>
       <c r="V118" s="2" t="s">
-        <v>1160</v>
+        <v>1362</v>
       </c>
       <c r="W118" s="45"/>
       <c r="X118" s="2"/>
@@ -12236,13 +12236,13 @@
       </c>
       <c r="B119" s="2"/>
       <c r="C119" s="32" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E119" s="26" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="F119" s="6"/>
       <c r="G119" s="40"/>
@@ -12262,11 +12262,11 @@
       <c r="R119" s="59"/>
       <c r="S119" s="59"/>
       <c r="T119" s="2" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="U119" s="20"/>
       <c r="V119" s="2" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="W119" s="45"/>
       <c r="X119" s="2"/>
@@ -12363,10 +12363,10 @@
         <v>723</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E122" s="26" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F122" s="6"/>
       <c r="G122" s="40" t="str">
@@ -12423,10 +12423,10 @@
         <v>724</v>
       </c>
       <c r="D123" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E123" s="26" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F123" s="6"/>
       <c r="G123" s="40" t="str">
@@ -12483,10 +12483,10 @@
         <v>725</v>
       </c>
       <c r="D124" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E124" s="26" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F124" s="6"/>
       <c r="G124" s="40" t="str">
@@ -12543,10 +12543,10 @@
         <v>69</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E125" s="26" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F125" s="6"/>
       <c r="G125" s="40" t="str">
@@ -12560,13 +12560,13 @@
         <v>443</v>
       </c>
       <c r="L125" s="49" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
       <c r="M125" s="49" t="s">
         <v>443</v>
       </c>
       <c r="N125" s="49" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
       <c r="O125" s="59" t="s">
         <v>443</v>
@@ -12607,10 +12607,10 @@
         <v>70</v>
       </c>
       <c r="D126" s="27" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E126" s="26" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="F126" s="6" t="s">
         <v>1126</v>
@@ -12624,24 +12624,24 @@
         <v>D04a</v>
       </c>
       <c r="I126" s="5" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="J126" s="5" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="K126" s="5" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="L126" s="19" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="M126" s="19"/>
       <c r="N126" s="19"/>
       <c r="O126" s="59" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
       <c r="P126" s="66" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="Q126" s="69"/>
       <c r="R126" s="59" t="s">
@@ -12729,10 +12729,10 @@
         <v>668</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E128" s="26" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="F128" s="6" t="s">
         <v>1127</v>
@@ -12794,10 +12794,10 @@
         <v>669</v>
       </c>
       <c r="D129" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E129" s="26" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="F129" s="28" t="s">
         <v>1130</v>
@@ -12859,13 +12859,13 @@
         <v>726</v>
       </c>
       <c r="D130" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E130" s="26" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="F130" s="28" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="G130" s="40" t="str">
         <f t="shared" si="10"/>
@@ -12924,10 +12924,10 @@
         <v>727</v>
       </c>
       <c r="D131" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E131" s="26" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="F131" s="6"/>
       <c r="G131" s="40" t="str">
@@ -12979,10 +12979,10 @@
         <v>728</v>
       </c>
       <c r="D132" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E132" s="26" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="F132" s="6"/>
       <c r="G132" s="40" t="str">
@@ -12991,16 +12991,16 @@
       </c>
       <c r="H132" s="40"/>
       <c r="I132" s="5" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="J132" s="5" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K132" s="5" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="L132" s="19" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="M132" s="19"/>
       <c r="N132" s="19"/>
@@ -13030,7 +13030,7 @@
         <v>728</v>
       </c>
       <c r="X132" s="2" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="133" spans="1:24" x14ac:dyDescent="0.25">
@@ -13045,10 +13045,10 @@
         <v>72</v>
       </c>
       <c r="D133" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E133" s="26" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F133" s="6"/>
       <c r="G133" s="40" t="str">
@@ -13101,10 +13101,10 @@
         <v>73</v>
       </c>
       <c r="D134" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E134" s="26" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F134" s="6"/>
       <c r="G134" s="40" t="str">
@@ -13161,10 +13161,10 @@
         <v>729</v>
       </c>
       <c r="D135" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E135" s="26" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F135" s="6"/>
       <c r="G135" s="40" t="str">
@@ -13266,10 +13266,10 @@
         <v>730</v>
       </c>
       <c r="D137" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E137" s="26" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F137" s="6"/>
       <c r="G137" s="40" t="str">
@@ -13322,10 +13322,10 @@
         <v>731</v>
       </c>
       <c r="D138" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E138" s="26" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F138" s="6"/>
       <c r="G138" s="40" t="str">
@@ -13378,10 +13378,10 @@
         <v>75</v>
       </c>
       <c r="D139" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E139" s="26" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F139" s="6"/>
       <c r="G139" s="40" t="str">
@@ -13434,10 +13434,10 @@
         <v>76</v>
       </c>
       <c r="D140" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E140" s="26" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F140" s="6"/>
       <c r="G140" s="40" t="str">
@@ -13549,10 +13549,10 @@
         <v>732</v>
       </c>
       <c r="D142" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E142" s="26" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="F142" s="6"/>
       <c r="G142" s="40" t="str">
@@ -13612,10 +13612,10 @@
         <v>79</v>
       </c>
       <c r="D143" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E143" s="26" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="F143" s="6"/>
       <c r="G143" s="40" t="str">
@@ -13672,10 +13672,10 @@
         <v>80</v>
       </c>
       <c r="D144" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E144" s="26" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="F144" s="6"/>
       <c r="G144" s="40" t="str">
@@ -13732,10 +13732,10 @@
         <v>81</v>
       </c>
       <c r="D145" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E145" s="26" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="F145" s="6"/>
       <c r="G145" s="40" t="str">
@@ -13792,10 +13792,10 @@
         <v>82</v>
       </c>
       <c r="D146" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E146" s="26" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="F146" s="6"/>
       <c r="G146" s="40" t="str">
@@ -13848,10 +13848,10 @@
         <v>83</v>
       </c>
       <c r="D147" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E147" s="26" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="F147" s="6"/>
       <c r="G147" s="40" t="str">
@@ -13904,10 +13904,10 @@
         <v>84</v>
       </c>
       <c r="D148" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E148" s="26" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="F148" s="6"/>
       <c r="G148" s="40" t="str">
@@ -13919,16 +13919,16 @@
         <v>D06</v>
       </c>
       <c r="I148" s="57" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="J148" s="18" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K148" s="5" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="L148" s="58" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="M148" s="58"/>
       <c r="N148" s="58"/>
@@ -14026,7 +14026,7 @@
         <v>86</v>
       </c>
       <c r="D150" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E150" s="26">
         <v>99</v>
@@ -14082,7 +14082,7 @@
         <v>87</v>
       </c>
       <c r="D151" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E151" s="26">
         <v>99</v>
@@ -14138,7 +14138,7 @@
         <v>733</v>
       </c>
       <c r="D152" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E152" s="26">
         <v>99</v>
@@ -14194,7 +14194,7 @@
         <v>89</v>
       </c>
       <c r="D153" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E153" s="26">
         <v>99</v>
@@ -14250,7 +14250,7 @@
         <v>90</v>
       </c>
       <c r="D154" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E154" s="26">
         <v>99</v>
@@ -14267,7 +14267,7 @@
         <v>460</v>
       </c>
       <c r="L154" s="49" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="M154" s="49"/>
       <c r="N154" s="49"/>
@@ -14306,7 +14306,7 @@
         <v>91</v>
       </c>
       <c r="D155" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E155" s="26">
         <v>99</v>
@@ -14362,7 +14362,7 @@
         <v>92</v>
       </c>
       <c r="D156" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E156" s="26">
         <v>99</v>
@@ -14420,7 +14420,7 @@
         <v>93</v>
       </c>
       <c r="D157" s="25" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E157" s="26"/>
       <c r="F157" s="6"/>
@@ -14478,7 +14478,7 @@
         <v>94</v>
       </c>
       <c r="D158" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E158" s="26">
         <v>99</v>
@@ -14501,7 +14501,7 @@
         <v>464</v>
       </c>
       <c r="N158" s="49" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="O158" s="59" t="s">
         <v>464</v>
@@ -14542,10 +14542,10 @@
         <v>95</v>
       </c>
       <c r="D159" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E159" s="26" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="F159" s="6"/>
       <c r="G159" s="40" t="str">
@@ -14609,10 +14609,10 @@
         <v>96</v>
       </c>
       <c r="D160" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E160" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F160" s="6"/>
       <c r="G160" s="40" t="str">
@@ -14676,10 +14676,10 @@
         <v>97</v>
       </c>
       <c r="D161" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E161" s="26" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F161" s="6"/>
       <c r="G161" s="40" t="str">
@@ -14691,22 +14691,22 @@
         <v>C03</v>
       </c>
       <c r="I161" s="5" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="J161" s="5" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K161" s="5" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="L161" s="49" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="M161" s="49" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="N161" s="49" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="O161" s="59" t="s">
         <v>467</v>
@@ -14747,10 +14747,10 @@
         <v>98</v>
       </c>
       <c r="D162" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E162" s="26" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="F162" s="6"/>
       <c r="G162" s="40" t="str">
@@ -14770,10 +14770,10 @@
         <v>830</v>
       </c>
       <c r="M162" s="49" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
       <c r="N162" s="49" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="O162" s="59" t="s">
         <v>468</v>
@@ -14801,7 +14801,7 @@
         <v>98</v>
       </c>
       <c r="X162" s="81" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="163" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
@@ -14812,10 +14812,10 @@
       <c r="B163" s="2"/>
       <c r="C163" s="36"/>
       <c r="D163" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E163" s="26" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="F163" s="6"/>
       <c r="G163" s="40" t="str">
@@ -14827,22 +14827,22 @@
         <v>C05</v>
       </c>
       <c r="I163" s="5" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="J163" s="5" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="K163" s="5" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="L163" s="49" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="M163" s="49" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="N163" s="49" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="O163" s="59"/>
       <c r="P163" s="68"/>
@@ -14850,7 +14850,7 @@
       <c r="R163" s="59"/>
       <c r="S163" s="59"/>
       <c r="T163" s="5" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
       <c r="U163" s="50"/>
       <c r="V163" s="5"/>
@@ -14869,7 +14869,7 @@
         <v>99</v>
       </c>
       <c r="D164" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E164" s="26">
         <v>99</v>
@@ -14884,22 +14884,22 @@
         <v>C99</v>
       </c>
       <c r="I164" s="5" t="s">
+        <v>1336</v>
+      </c>
+      <c r="J164" s="5" t="s">
+        <v>1337</v>
+      </c>
+      <c r="K164" s="5" t="s">
         <v>1338</v>
       </c>
-      <c r="J164" s="5" t="s">
+      <c r="L164" s="19" t="s">
         <v>1339</v>
       </c>
-      <c r="K164" s="5" t="s">
-        <v>1340</v>
-      </c>
-      <c r="L164" s="19" t="s">
-        <v>1341</v>
-      </c>
       <c r="M164" s="19" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
       <c r="N164" s="19" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
       <c r="O164" s="59" t="s">
         <v>469</v>
@@ -14915,7 +14915,7 @@
         <v>1102</v>
       </c>
       <c r="T164" s="79" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="U164" s="52" t="s">
         <v>99</v>
@@ -14927,7 +14927,7 @@
         <v>99</v>
       </c>
       <c r="X164" s="81" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="165" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
@@ -14999,10 +14999,10 @@
         <v>101</v>
       </c>
       <c r="D166" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E166" s="26" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="F166" s="6"/>
       <c r="G166" s="40" t="str">
@@ -15062,10 +15062,10 @@
         <v>102</v>
       </c>
       <c r="D167" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E167" s="26" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F167" s="6"/>
       <c r="G167" s="40" t="str">
@@ -15119,13 +15119,13 @@
         <v>157</v>
       </c>
       <c r="C168" s="31" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="D168" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E168" s="26" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F168" s="6"/>
       <c r="G168" s="40" t="str">
@@ -15185,10 +15185,10 @@
         <v>104</v>
       </c>
       <c r="D169" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E169" s="26" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="F169" s="6"/>
       <c r="G169" s="40" t="s">
@@ -15222,10 +15222,10 @@
         <v>682</v>
       </c>
       <c r="T169" s="81" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="U169" s="20" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="V169" s="2" t="s">
         <v>281</v>
@@ -15247,10 +15247,10 @@
         <v>105</v>
       </c>
       <c r="D170" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E170" s="26" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="F170" s="6"/>
       <c r="G170" s="40" t="str">
@@ -15307,10 +15307,10 @@
         <v>106</v>
       </c>
       <c r="D171" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E171" s="26" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="F171" s="6"/>
       <c r="G171" s="40" t="str">
@@ -15322,16 +15322,16 @@
         <v>D11</v>
       </c>
       <c r="I171" s="16" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="J171" s="5" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K171" s="5" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="L171" s="49" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
       <c r="M171" s="49"/>
       <c r="N171" s="49"/>
@@ -15374,10 +15374,10 @@
         <v>107</v>
       </c>
       <c r="D172" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E172" s="26" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="F172" s="6"/>
       <c r="G172" s="40" t="str">
@@ -15434,10 +15434,10 @@
         <v>734</v>
       </c>
       <c r="D173" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E173" s="26" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="F173" s="6"/>
       <c r="G173" s="40" t="str">
@@ -15494,10 +15494,10 @@
         <v>735</v>
       </c>
       <c r="D174" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E174" s="26" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="F174" s="6"/>
       <c r="G174" s="40" t="str">
@@ -15554,10 +15554,10 @@
         <v>667</v>
       </c>
       <c r="D175" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E175" s="26" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="F175" s="6"/>
       <c r="G175" s="40" t="str">
@@ -15614,10 +15614,10 @@
         <v>736</v>
       </c>
       <c r="D176" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E176" s="26" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="F176" s="6"/>
       <c r="G176" s="40" t="str">
@@ -15674,10 +15674,10 @@
         <v>737</v>
       </c>
       <c r="D177" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E177" s="26" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="F177" s="6"/>
       <c r="G177" s="40" t="str">
@@ -15734,10 +15734,10 @@
         <v>738</v>
       </c>
       <c r="D178" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E178" s="26" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="F178" s="6"/>
       <c r="G178" s="40" t="str">
@@ -15746,16 +15746,16 @@
       </c>
       <c r="H178" s="40"/>
       <c r="I178" s="5" t="s">
+        <v>1206</v>
+      </c>
+      <c r="J178" s="5" t="s">
+        <v>1162</v>
+      </c>
+      <c r="K178" s="5" t="s">
+        <v>1207</v>
+      </c>
+      <c r="L178" s="49" t="s">
         <v>1208</v>
-      </c>
-      <c r="J178" s="5" t="s">
-        <v>1164</v>
-      </c>
-      <c r="K178" s="5" t="s">
-        <v>1209</v>
-      </c>
-      <c r="L178" s="49" t="s">
-        <v>1210</v>
       </c>
       <c r="M178" s="49"/>
       <c r="N178" s="49"/>
@@ -15853,10 +15853,10 @@
         <v>109</v>
       </c>
       <c r="D180" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E180" s="26" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="F180" s="6"/>
       <c r="G180" s="40" t="s">
@@ -15915,10 +15915,10 @@
         <v>739</v>
       </c>
       <c r="D181" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E181" s="26" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="F181" s="6" t="s">
         <v>1126</v>
@@ -15977,10 +15977,10 @@
         <v>740</v>
       </c>
       <c r="D182" s="27" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E182" s="26" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="F182" s="6" t="s">
         <v>1127</v>
@@ -16039,10 +16039,10 @@
         <v>741</v>
       </c>
       <c r="D183" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E183" s="26" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="F183" s="6" t="s">
         <v>1130</v>
@@ -16101,7 +16101,7 @@
         <v>742</v>
       </c>
       <c r="D184" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E184" s="26">
         <v>99</v>
@@ -16157,7 +16157,7 @@
         <v>110</v>
       </c>
       <c r="D185" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E185" s="26">
         <v>99</v>
@@ -16217,7 +16217,7 @@
         <v>743</v>
       </c>
       <c r="D186" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E186" s="26">
         <v>99</v>
@@ -16277,7 +16277,7 @@
         <v>112</v>
       </c>
       <c r="D187" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E187" s="26">
         <v>99</v>
@@ -16337,7 +16337,7 @@
         <v>113</v>
       </c>
       <c r="D188" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E188" s="26">
         <v>99</v>
@@ -16397,7 +16397,7 @@
         <v>114</v>
       </c>
       <c r="D189" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E189" s="26">
         <v>99</v>
@@ -16514,7 +16514,7 @@
         <v>116</v>
       </c>
       <c r="D191" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E191" s="26">
         <v>99</v>
@@ -16574,7 +16574,7 @@
         <v>117</v>
       </c>
       <c r="D192" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E192" s="26">
         <v>99</v>
@@ -16630,7 +16630,7 @@
         <v>118</v>
       </c>
       <c r="D193" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E193" s="26">
         <v>99</v>
@@ -16686,7 +16686,7 @@
         <v>119</v>
       </c>
       <c r="D194" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E194" s="26">
         <v>99</v>
@@ -16742,7 +16742,7 @@
         <v>120</v>
       </c>
       <c r="D195" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E195" s="26">
         <v>99</v>
@@ -16754,16 +16754,16 @@
       </c>
       <c r="H195" s="40"/>
       <c r="I195" s="5" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
       <c r="J195" s="5" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="K195" s="5" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="L195" s="49" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="M195" s="49"/>
       <c r="N195" s="49"/>
@@ -16806,10 +16806,10 @@
         <v>121</v>
       </c>
       <c r="D196" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E196" s="26" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="F196" s="6"/>
       <c r="G196" s="40" t="s">
@@ -16868,10 +16868,10 @@
         <v>122</v>
       </c>
       <c r="D197" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E197" s="26" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="F197" s="6"/>
       <c r="G197" s="40" t="str">
@@ -16928,10 +16928,10 @@
         <v>123</v>
       </c>
       <c r="D198" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E198" s="26" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="F198" s="6"/>
       <c r="G198" s="40" t="str">
@@ -16988,10 +16988,10 @@
         <v>124</v>
       </c>
       <c r="D199" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E199" s="26" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="F199" s="6"/>
       <c r="G199" s="40" t="str">
@@ -17048,10 +17048,10 @@
         <v>125</v>
       </c>
       <c r="D200" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E200" s="26" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="F200" s="6"/>
       <c r="G200" s="40" t="str">
@@ -17108,10 +17108,10 @@
         <v>126</v>
       </c>
       <c r="D201" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E201" s="26" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="F201" s="6"/>
       <c r="G201" s="40" t="str">
@@ -17168,10 +17168,10 @@
         <v>127</v>
       </c>
       <c r="D202" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E202" s="26" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="F202" s="6"/>
       <c r="G202" s="40" t="str">
@@ -17281,7 +17281,7 @@
         <v>129</v>
       </c>
       <c r="D204" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E204" s="26">
         <v>99</v>
@@ -17337,7 +17337,7 @@
         <v>130</v>
       </c>
       <c r="D205" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E205" s="26">
         <v>99</v>
@@ -17393,7 +17393,7 @@
         <v>131</v>
       </c>
       <c r="D206" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E206" s="26">
         <v>99</v>
@@ -17449,7 +17449,7 @@
         <v>744</v>
       </c>
       <c r="D207" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E207" s="26">
         <v>99</v>
@@ -17505,7 +17505,7 @@
         <v>132</v>
       </c>
       <c r="D208" s="25" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="E208" s="26"/>
       <c r="F208" s="6"/>
@@ -17532,7 +17532,7 @@
       </c>
       <c r="Q208" s="66"/>
       <c r="R208" s="60" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
       <c r="S208" s="59" t="s">
         <v>654</v>
@@ -17563,10 +17563,10 @@
         <v>133</v>
       </c>
       <c r="D209" s="6" t="s">
+        <v>1144</v>
+      </c>
+      <c r="E209" s="26" t="s">
         <v>1145</v>
-      </c>
-      <c r="E209" s="26" t="s">
-        <v>1146</v>
       </c>
       <c r="F209" s="6"/>
       <c r="G209" s="40"/>
@@ -17623,10 +17623,10 @@
         <v>134</v>
       </c>
       <c r="D210" s="6" t="s">
+        <v>1144</v>
+      </c>
+      <c r="E210" s="26" t="s">
         <v>1145</v>
-      </c>
-      <c r="E210" s="26" t="s">
-        <v>1146</v>
       </c>
       <c r="F210" s="6" t="s">
         <v>1126</v>
@@ -17640,16 +17640,16 @@
         <v>E01a</v>
       </c>
       <c r="I210" s="5" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="J210" s="5" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K210" s="5" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="L210" s="19" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="M210" s="19"/>
       <c r="N210" s="19"/>
@@ -17692,10 +17692,10 @@
         <v>135</v>
       </c>
       <c r="D211" s="6" t="s">
+        <v>1144</v>
+      </c>
+      <c r="E211" s="26" t="s">
         <v>1145</v>
-      </c>
-      <c r="E211" s="26" t="s">
-        <v>1146</v>
       </c>
       <c r="F211" s="6" t="s">
         <v>1128</v>
@@ -17754,10 +17754,10 @@
         <v>136</v>
       </c>
       <c r="D212" s="6" t="s">
+        <v>1144</v>
+      </c>
+      <c r="E212" s="26" t="s">
         <v>1145</v>
-      </c>
-      <c r="E212" s="26" t="s">
-        <v>1146</v>
       </c>
       <c r="F212" s="6" t="s">
         <v>1127</v>
@@ -17819,10 +17819,10 @@
         <v>137</v>
       </c>
       <c r="D213" s="6" t="s">
+        <v>1144</v>
+      </c>
+      <c r="E213" s="26" t="s">
         <v>1145</v>
-      </c>
-      <c r="E213" s="26" t="s">
-        <v>1146</v>
       </c>
       <c r="F213" s="6" t="s">
         <v>1128</v>
@@ -17879,10 +17879,10 @@
         <v>745</v>
       </c>
       <c r="D214" s="6" t="s">
+        <v>1144</v>
+      </c>
+      <c r="E214" s="26" t="s">
         <v>1145</v>
-      </c>
-      <c r="E214" s="26" t="s">
-        <v>1146</v>
       </c>
       <c r="F214" s="6" t="s">
         <v>1128</v>
@@ -17941,10 +17941,10 @@
         <v>746</v>
       </c>
       <c r="D215" s="6" t="s">
+        <v>1144</v>
+      </c>
+      <c r="E215" s="26" t="s">
         <v>1145</v>
-      </c>
-      <c r="E215" s="26" t="s">
-        <v>1146</v>
       </c>
       <c r="F215" s="6" t="s">
         <v>1128</v>
@@ -18003,10 +18003,10 @@
         <v>747</v>
       </c>
       <c r="D216" s="6" t="s">
+        <v>1144</v>
+      </c>
+      <c r="E216" s="26" t="s">
         <v>1145</v>
-      </c>
-      <c r="E216" s="26" t="s">
-        <v>1146</v>
       </c>
       <c r="F216" s="6" t="s">
         <v>1128</v>
@@ -18017,16 +18017,16 @@
       </c>
       <c r="H216" s="40"/>
       <c r="I216" s="5" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="J216" s="5" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="K216" s="5" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="L216" s="49" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="M216" s="49"/>
       <c r="N216" s="49"/>
@@ -18065,10 +18065,10 @@
         <v>748</v>
       </c>
       <c r="D217" s="6" t="s">
+        <v>1144</v>
+      </c>
+      <c r="E217" s="26" t="s">
         <v>1145</v>
-      </c>
-      <c r="E217" s="26" t="s">
-        <v>1146</v>
       </c>
       <c r="F217" s="6" t="s">
         <v>1128</v>
@@ -18082,16 +18082,16 @@
         <v>E01x</v>
       </c>
       <c r="I217" s="5" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="J217" s="5" t="s">
+        <v>1263</v>
+      </c>
+      <c r="K217" s="5" t="s">
+        <v>1264</v>
+      </c>
+      <c r="L217" s="49" t="s">
         <v>1265</v>
-      </c>
-      <c r="K217" s="5" t="s">
-        <v>1266</v>
-      </c>
-      <c r="L217" s="49" t="s">
-        <v>1267</v>
       </c>
       <c r="M217" s="49"/>
       <c r="N217" s="49"/>
@@ -18121,7 +18121,7 @@
         <v>887</v>
       </c>
       <c r="X217" s="22" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="218" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
@@ -18189,10 +18189,10 @@
         <v>140</v>
       </c>
       <c r="D219" s="6" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="E219" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F219" s="6"/>
       <c r="G219" s="40" t="str">
@@ -18204,16 +18204,16 @@
         <v>E02</v>
       </c>
       <c r="I219" s="5" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="J219" s="5" t="s">
+        <v>1215</v>
+      </c>
+      <c r="K219" s="5" t="s">
+        <v>1216</v>
+      </c>
+      <c r="L219" s="49" t="s">
         <v>1217</v>
-      </c>
-      <c r="K219" s="5" t="s">
-        <v>1218</v>
-      </c>
-      <c r="L219" s="49" t="s">
-        <v>1219</v>
       </c>
       <c r="M219" s="49"/>
       <c r="N219" s="49"/>
@@ -18231,7 +18231,7 @@
         <v>999</v>
       </c>
       <c r="T219" s="5" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="U219" s="20" t="s">
         <v>140</v>
@@ -18256,10 +18256,10 @@
         <v>141</v>
       </c>
       <c r="D220" s="6" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="E220" s="26" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F220" s="6"/>
       <c r="G220" s="40" t="str">
@@ -18271,16 +18271,16 @@
         <v>E03</v>
       </c>
       <c r="I220" s="5" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="J220" s="5" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="K220" s="5" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="L220" s="19" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="M220" s="19"/>
       <c r="N220" s="19"/>
@@ -18298,7 +18298,7 @@
         <v>998</v>
       </c>
       <c r="T220" s="5" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
       <c r="U220" s="20" t="s">
         <v>141</v>
@@ -18323,10 +18323,10 @@
         <v>142</v>
       </c>
       <c r="D221" s="6" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="E221" s="26" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="F221" s="6"/>
       <c r="G221" s="40" t="str">
@@ -18335,16 +18335,16 @@
       </c>
       <c r="H221" s="40"/>
       <c r="I221" s="5" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
       <c r="J221" s="5" t="s">
+        <v>1243</v>
+      </c>
+      <c r="K221" s="5" t="s">
+        <v>1246</v>
+      </c>
+      <c r="L221" s="49" t="s">
         <v>1245</v>
-      </c>
-      <c r="K221" s="5" t="s">
-        <v>1248</v>
-      </c>
-      <c r="L221" s="49" t="s">
-        <v>1247</v>
       </c>
       <c r="M221" s="49"/>
       <c r="N221" s="49"/>
@@ -18370,21 +18370,21 @@
         <v>142</v>
       </c>
       <c r="X221" s="22" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="222" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B222" s="82" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="C222" s="16" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="D222" s="54" t="s">
+        <v>1144</v>
+      </c>
+      <c r="E222" s="55" t="s">
         <v>1145</v>
-      </c>
-      <c r="E222" s="55" t="s">
-        <v>1146</v>
       </c>
       <c r="G222" s="40" t="str">
         <f t="shared" si="21"/>
@@ -18392,19 +18392,19 @@
       </c>
       <c r="H222" s="40"/>
       <c r="I222" s="48" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="J222" s="48" t="s">
+        <v>1279</v>
+      </c>
+      <c r="K222" s="16" t="s">
+        <v>1280</v>
+      </c>
+      <c r="L222" s="16" t="s">
         <v>1281</v>
       </c>
-      <c r="K222" s="16" t="s">
-        <v>1282</v>
-      </c>
-      <c r="L222" s="16" t="s">
-        <v>1283</v>
-      </c>
       <c r="T222" s="48" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="223" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
@@ -18413,10 +18413,10 @@
         <v>.....Z.01. - Symptoms, signs and ill-defined conditions, not elsewhere classified</v>
       </c>
       <c r="D223" s="56" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="E223" s="55" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G223" s="40" t="str">
         <f t="shared" si="21"/>
@@ -18427,19 +18427,19 @@
         <v>Z01</v>
       </c>
       <c r="I223" s="48" t="s">
+        <v>1225</v>
+      </c>
+      <c r="J223" s="48" t="s">
+        <v>1226</v>
+      </c>
+      <c r="K223" s="16" t="s">
         <v>1227</v>
       </c>
-      <c r="J223" s="48" t="s">
+      <c r="L223" s="16" t="s">
+        <v>1261</v>
+      </c>
+      <c r="T223" s="48" t="s">
         <v>1228</v>
-      </c>
-      <c r="K223" s="16" t="s">
-        <v>1229</v>
-      </c>
-      <c r="L223" s="16" t="s">
-        <v>1263</v>
-      </c>
-      <c r="T223" s="48" t="s">
-        <v>1230</v>
       </c>
     </row>
     <row r="224" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
@@ -18448,10 +18448,10 @@
         <v/>
       </c>
       <c r="D224" s="56" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E224" s="55" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="G224" s="42" t="str">
         <f t="shared" si="21"/>
@@ -18459,19 +18459,19 @@
       </c>
       <c r="H224" s="40"/>
       <c r="I224" s="16" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="J224" s="48" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="K224" s="16" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="L224" s="16" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="T224" s="48" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="225" spans="1:20" x14ac:dyDescent="0.25">
@@ -18480,10 +18480,10 @@
         <v>.....Z.02. - Unknown/Missing Value</v>
       </c>
       <c r="D225" s="56" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="E225" s="55" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G225" s="43"/>
       <c r="H225" s="40" t="str">
@@ -18491,7 +18491,7 @@
         <v>Z02</v>
       </c>
       <c r="T225" s="48" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="226" spans="1:20" ht="38.25" x14ac:dyDescent="0.25">
@@ -18500,10 +18500,10 @@
         <v>.....Z.03. - Code does not map</v>
       </c>
       <c r="D226" s="56" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="E226" s="55" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="G226" s="43"/>
       <c r="H226" s="40" t="str">
@@ -18511,10 +18511,10 @@
         <v>Z03</v>
       </c>
       <c r="I226" s="16" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="T226" s="48" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="227" spans="1:20" x14ac:dyDescent="0.25">
@@ -18523,7 +18523,7 @@
         <v>Z. - Unknown/Missing Value</v>
       </c>
       <c r="D227" s="56" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="G227" s="43"/>
       <c r="H227" s="40" t="str">
@@ -18531,7 +18531,7 @@
         <v>Z</v>
       </c>
       <c r="T227" s="48" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="228" spans="1:20" x14ac:dyDescent="0.25">
@@ -18540,10 +18540,10 @@
         <v>.....D.99. - Other Chronic Conditions</v>
       </c>
       <c r="D228" s="56" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E228" s="55" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="G228" s="43"/>
       <c r="H228" s="40" t="str">
@@ -18551,7 +18551,7 @@
         <v>D99</v>
       </c>
       <c r="T228" s="48" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
     </row>
   </sheetData>
@@ -18792,24 +18792,24 @@
   <sheetData>
     <row r="11" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="75" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="D11" s="76" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="E11" s="76" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="12" spans="3:5" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="77" t="s">
+        <v>1331</v>
+      </c>
+      <c r="D12" s="78" t="s">
+        <v>1332</v>
+      </c>
+      <c r="E12" s="78" t="s">
         <v>1333</v>
-      </c>
-      <c r="D12" s="78" t="s">
-        <v>1334</v>
-      </c>
-      <c r="E12" s="78" t="s">
-        <v>1335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added D10 to kidney disease labels.
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/gbd.ICD.Map.xlsx
+++ b/myCBD/myInfo/gbd.ICD.Map.xlsx
@@ -5246,10 +5246,10 @@
   <dimension ref="A1:X228"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B109" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B175" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C118" sqref="C118"/>
+      <selection pane="bottomRight" activeCell="H183" sqref="H183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -15906,7 +15906,7 @@
     <row r="181" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A181" s="44" t="str">
         <f t="shared" si="11"/>
-        <v/>
+        <v>..........D.10.a. - Acute glomerulonephritis</v>
       </c>
       <c r="B181" s="2">
         <v>170</v>
@@ -15927,7 +15927,10 @@
         <f t="shared" ref="G181:G189" si="17">CONCATENATE("c",D181,E181,F181)</f>
         <v>cD10a</v>
       </c>
-      <c r="H181" s="40"/>
+      <c r="H181" s="40" t="str">
+        <f>CONCATENATE(D181,E181,F181)</f>
+        <v>D10a</v>
+      </c>
       <c r="I181" s="5"/>
       <c r="J181" s="5"/>
       <c r="K181" s="5" t="s">
@@ -15968,7 +15971,7 @@
     <row r="182" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A182" s="44" t="str">
         <f t="shared" si="11"/>
-        <v/>
+        <v>..........D.10.b. - Chronic kidney diesease due to diabetes</v>
       </c>
       <c r="B182" s="2">
         <v>171</v>
@@ -15989,7 +15992,10 @@
         <f t="shared" si="17"/>
         <v>cD10b</v>
       </c>
-      <c r="H182" s="40"/>
+      <c r="H182" s="40" t="str">
+        <f>CONCATENATE(D182,E182,F182)</f>
+        <v>D10b</v>
+      </c>
       <c r="I182" s="5"/>
       <c r="J182" s="5"/>
       <c r="K182" s="5" t="s">
@@ -16030,7 +16036,7 @@
     <row r="183" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A183" s="44" t="str">
         <f t="shared" si="11"/>
-        <v/>
+        <v>..........D.10.c. - Other chronic kidney disease</v>
       </c>
       <c r="B183" s="2">
         <v>172</v>
@@ -16051,7 +16057,10 @@
         <f t="shared" si="17"/>
         <v>cD10c</v>
       </c>
-      <c r="H183" s="40"/>
+      <c r="H183" s="40" t="str">
+        <f>CONCATENATE(D183,E183,F183)</f>
+        <v>D10c</v>
+      </c>
       <c r="I183" s="5"/>
       <c r="J183" s="5"/>
       <c r="K183" s="5" t="s">

</xml_diff>

<commit_message>
multiple fixes: navigation, ICD labels, IHME, SDOH
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/gbd.ICD.Map.xlsx
+++ b/myCBD/myInfo/gbd.ICD.Map.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\0.CBD\myCBD\myInfo\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="10935"/>
   </bookViews>
@@ -19,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$A$1:$X$221</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -36,7 +31,7 @@
     <author>Dauphine, David (CDPH-CHSI)</author>
   </authors>
   <commentList>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -60,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C57" authorId="1" shapeId="0">
+    <comment ref="C57" authorId="1">
       <text>
         <r>
           <rPr>
@@ -84,7 +79,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P126" authorId="2" shapeId="0">
+    <comment ref="P126" authorId="2">
       <text>
         <r>
           <rPr>
@@ -113,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2810" uniqueCount="1363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2810" uniqueCount="1366">
   <si>
     <t>I. Communicable, maternal, perinatal and nutritional conditions</t>
   </si>
@@ -4347,11 +4342,20 @@
   <si>
     <t>Mental Health disorders (non-substance use)</t>
   </si>
+  <si>
+    <t>Asthma and other respiratory diseases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mental Health disorders </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Substance use </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###0.;###0."/>
   </numFmts>
@@ -4999,7 +5003,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5034,7 +5038,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5246,10 +5250,10 @@
   <dimension ref="A1:X228"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B175" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B113" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H183" sqref="H183"/>
+      <selection pane="bottomRight" activeCell="A118" sqref="A118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -12188,7 +12192,7 @@
     <row r="118" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A118" s="44" t="str">
         <f>IF(H118&lt;&gt;"",IF(F118&lt;&gt;"",CONCATENATE("..........",D118,".",E118,".",F118,". - ",T118),IF(E118&lt;&gt;"",CONCATENATE(".....",D118,".",E118,". - ",T118),CONCATENATE(D118,". - ",T118))),"")</f>
-        <v>.....D.03. - Mental Health disorders (non-substance use)</v>
+        <v xml:space="preserve">.....D.03. - Mental Health disorders </v>
       </c>
       <c r="B118" s="2"/>
       <c r="C118" s="32" t="s">
@@ -12220,7 +12224,7 @@
       <c r="R118" s="59"/>
       <c r="S118" s="59"/>
       <c r="T118" s="2" t="s">
-        <v>1362</v>
+        <v>1364</v>
       </c>
       <c r="U118" s="20"/>
       <c r="V118" s="2" t="s">
@@ -12232,7 +12236,7 @@
     <row r="119" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A119" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>.....D.04. - Substance use (Mental Health)</v>
+        <v xml:space="preserve">.....D.04. - Substance use </v>
       </c>
       <c r="B119" s="2"/>
       <c r="C119" s="32" t="s">
@@ -12262,7 +12266,7 @@
       <c r="R119" s="59"/>
       <c r="S119" s="59"/>
       <c r="T119" s="2" t="s">
-        <v>1159</v>
+        <v>1365</v>
       </c>
       <c r="U119" s="20"/>
       <c r="V119" s="2" t="s">
@@ -15113,7 +15117,7 @@
     <row r="168" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A168" s="44" t="str">
         <f t="shared" si="11"/>
-        <v>.....D.08. - Other respiratory diseases</v>
+        <v>.....D.08. - Asthma and other respiratory diseases</v>
       </c>
       <c r="B168" s="2">
         <v>157</v>
@@ -15160,7 +15164,7 @@
         <v>1055</v>
       </c>
       <c r="T168" s="5" t="s">
-        <v>280</v>
+        <v>1363</v>
       </c>
       <c r="U168" s="20" t="s">
         <v>103</v>

</xml_diff>

<commit_message>
substantial cleaning/updating for CCLHO
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/gbd.ICD.Map.xlsx
+++ b/myCBD/myInfo/gbd.ICD.Map.xlsx
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2810" uniqueCount="1366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2810" uniqueCount="1368">
   <si>
     <t>I. Communicable, maternal, perinatal and nutritional conditions</t>
   </si>
@@ -3552,30 +3552,6 @@
   </si>
   <si>
     <t>IV. Other Chronic</t>
-  </si>
-  <si>
-    <r>
-      <t>3.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Asthma/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Other respiratory diseases</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve"> hepatitis B (acute and liver cancer)</t>
@@ -4343,13 +4319,43 @@
     <t>Mental Health disorders (non-substance use)</t>
   </si>
   <si>
-    <t>Asthma and other respiratory diseases</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mental Health disorders </t>
   </si>
   <si>
     <t xml:space="preserve">Substance use </t>
+  </si>
+  <si>
+    <r>
+      <t>3.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Other respiratory diseases</t>
+    </r>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>68</t>
   </si>
 </sst>
 </file>
@@ -4671,7 +4677,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -4914,6 +4920,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="29">
@@ -5250,10 +5259,10 @@
   <dimension ref="A1:X228"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B113" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B172" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A118" sqref="A118"/>
+      <selection pane="bottomRight" activeCell="E196" sqref="E196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -5285,7 +5294,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>761</v>
@@ -5294,7 +5303,7 @@
         <v>763</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E1" s="24" t="s">
         <v>1121</v>
@@ -5309,10 +5318,10 @@
         <v>1124</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>384</v>
@@ -5321,19 +5330,19 @@
         <v>759</v>
       </c>
       <c r="M1" s="5" t="s">
+        <v>1346</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>1347</v>
       </c>
-      <c r="N1" s="5" t="s">
-        <v>1348</v>
-      </c>
       <c r="O1" s="59" t="s">
+        <v>1162</v>
+      </c>
+      <c r="P1" s="59" t="s">
         <v>1163</v>
       </c>
-      <c r="P1" s="59" t="s">
-        <v>1164</v>
-      </c>
       <c r="Q1" s="59" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="R1" s="61" t="s">
         <v>509</v>
@@ -5348,10 +5357,10 @@
         <v>762</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="W1" s="45" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="X1" s="6" t="s">
         <v>930</v>
@@ -5415,7 +5424,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E3" s="26"/>
       <c r="F3" s="6"/>
@@ -5467,7 +5476,7 @@
         <v>1129</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E4" s="26">
         <v>99</v>
@@ -5562,10 +5571,10 @@
         <v>2</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="40" t="str">
@@ -5621,10 +5630,10 @@
         <v>1125</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="40"/>
@@ -5644,11 +5653,11 @@
       <c r="R7" s="59"/>
       <c r="S7" s="59"/>
       <c r="T7" s="2" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="U7" s="20"/>
       <c r="V7" s="2" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="W7" s="45"/>
       <c r="X7" s="2"/>
@@ -5665,10 +5674,10 @@
         <v>1133</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>1126</v>
@@ -5729,10 +5738,10 @@
         <v>4</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>1126</v>
@@ -5789,10 +5798,10 @@
         <v>5</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>1126</v>
@@ -5849,10 +5858,10 @@
         <v>6</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>1126</v>
@@ -5909,10 +5918,10 @@
         <v>7</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>1126</v>
@@ -5967,10 +5976,10 @@
         <v>8</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>1126</v>
@@ -6027,10 +6036,10 @@
         <v>1134</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>1127</v>
@@ -6089,10 +6098,10 @@
         <v>686</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>1127</v>
@@ -6145,10 +6154,10 @@
         <v>687</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>1127</v>
@@ -6205,7 +6214,7 @@
         <v>10</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E17" s="26">
         <v>99</v>
@@ -6315,7 +6324,7 @@
         <v>12</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E19" s="26">
         <v>99</v>
@@ -6373,7 +6382,7 @@
         <v>13</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E20" s="26">
         <v>99</v>
@@ -6431,7 +6440,7 @@
         <v>14</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E21" s="26">
         <v>99</v>
@@ -6489,7 +6498,7 @@
         <v>15</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E22" s="26">
         <v>99</v>
@@ -6547,10 +6556,10 @@
         <v>16</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="40" t="str">
@@ -6608,10 +6617,10 @@
         <v>17</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="40" t="str">
@@ -6669,10 +6678,10 @@
         <v>688</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="40"/>
@@ -6723,10 +6732,10 @@
         <v>689</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="40" t="str">
@@ -6777,10 +6786,10 @@
         <v>690</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>1126</v>
@@ -6831,7 +6840,7 @@
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="34" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="D28" s="27"/>
       <c r="E28" s="26"/>
@@ -6864,10 +6873,10 @@
         <v>691</v>
       </c>
       <c r="D29" s="27" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>1127</v>
@@ -6923,10 +6932,10 @@
         <v>692</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E30" s="26" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="40" t="str">
@@ -7028,7 +7037,7 @@
         <v>18</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E32" s="26">
         <v>99</v>
@@ -7086,7 +7095,7 @@
         <v>19</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E33" s="26">
         <v>99</v>
@@ -7144,7 +7153,7 @@
         <v>20</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E34" s="26">
         <v>99</v>
@@ -7202,7 +7211,7 @@
         <v>21</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E35" s="26">
         <v>99</v>
@@ -7260,7 +7269,7 @@
         <v>22</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E36" s="26">
         <v>99</v>
@@ -7318,7 +7327,7 @@
         <v>23</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E37" s="26">
         <v>99</v>
@@ -7372,7 +7381,7 @@
         <v>24</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E38" s="26">
         <v>99</v>
@@ -7426,7 +7435,7 @@
         <v>694</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E39" s="26">
         <v>99</v>
@@ -7484,7 +7493,7 @@
         <v>695</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E40" s="26">
         <v>99</v>
@@ -7542,7 +7551,7 @@
         <v>889</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E41" s="26">
         <v>99</v>
@@ -7596,7 +7605,7 @@
         <v>890</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E42" s="26">
         <v>99</v>
@@ -7654,7 +7663,7 @@
         <v>891</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E43" s="26">
         <v>99</v>
@@ -7708,7 +7717,7 @@
         <v>893</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E44" s="26">
         <v>99</v>
@@ -7766,7 +7775,7 @@
         <v>894</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E45" s="26">
         <v>99</v>
@@ -7879,7 +7888,7 @@
         <v>25</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E47" s="26">
         <v>99</v>
@@ -7937,7 +7946,7 @@
         <v>26</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E48" s="26">
         <v>99</v>
@@ -7991,7 +8000,7 @@
         <v>27</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E49" s="26">
         <v>99</v>
@@ -8045,7 +8054,7 @@
         <v>696</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E50" s="26">
         <v>99</v>
@@ -8099,7 +8108,7 @@
         <v>880</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E51" s="26">
         <v>99</v>
@@ -8111,16 +8120,16 @@
       </c>
       <c r="H51" s="40"/>
       <c r="I51" s="5" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="K51" s="5" t="s">
+        <v>1233</v>
+      </c>
+      <c r="L51" s="19" t="s">
         <v>1234</v>
-      </c>
-      <c r="L51" s="19" t="s">
-        <v>1235</v>
       </c>
       <c r="M51" s="19"/>
       <c r="N51" s="19"/>
@@ -8150,7 +8159,7 @@
         <v>880</v>
       </c>
       <c r="X51" s="5" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="52" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
@@ -8165,10 +8174,10 @@
         <v>28</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E52" s="26" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="F52" s="6"/>
       <c r="G52" s="40"/>
@@ -8225,10 +8234,10 @@
         <v>29</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E53" s="26" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="F53" s="6"/>
       <c r="G53" s="40" t="str">
@@ -8242,7 +8251,7 @@
         <v>404</v>
       </c>
       <c r="L53" s="80" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="M53" s="80"/>
       <c r="N53" s="80"/>
@@ -8285,10 +8294,10 @@
         <v>30</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E54" s="26" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="F54" s="6"/>
       <c r="G54" s="40" t="str">
@@ -8343,10 +8352,10 @@
         <v>31</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E55" s="26" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="F55" s="6"/>
       <c r="G55" s="40" t="str">
@@ -8401,10 +8410,10 @@
         <v>32</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E56" s="26" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="F56" s="6"/>
       <c r="G56" s="40" t="s">
@@ -8463,10 +8472,10 @@
         <v>33</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E57" s="26" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="F57" s="6"/>
       <c r="G57" s="40" t="str">
@@ -8521,10 +8530,10 @@
         <v>34</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E58" s="26" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="F58" s="6"/>
       <c r="G58" s="40" t="str">
@@ -8579,10 +8588,10 @@
         <v>35</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E59" s="26" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="F59" s="6"/>
       <c r="G59" s="40" t="str">
@@ -8637,10 +8646,10 @@
         <v>36</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E60" s="26" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="F60" s="6"/>
       <c r="G60" s="40" t="str">
@@ -8695,10 +8704,10 @@
         <v>37</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E61" s="26" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="F61" s="6"/>
       <c r="G61" s="40" t="str">
@@ -8753,10 +8762,10 @@
         <v>38</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E62" s="26" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="F62" s="6"/>
       <c r="G62" s="40" t="str">
@@ -8811,10 +8820,10 @@
         <v>39</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E63" s="26" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F63" s="6"/>
       <c r="G63" s="40" t="s">
@@ -8873,10 +8882,10 @@
         <v>40</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E64" s="26" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F64" s="6"/>
       <c r="G64" s="40" t="str">
@@ -8931,10 +8940,10 @@
         <v>41</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E65" s="26" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F65" s="6"/>
       <c r="G65" s="40" t="str">
@@ -8989,10 +8998,10 @@
         <v>42</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E66" s="26" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F66" s="6"/>
       <c r="G66" s="40" t="str">
@@ -9047,10 +9056,10 @@
         <v>43</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E67" s="26" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F67" s="6"/>
       <c r="G67" s="40" t="str">
@@ -9059,16 +9068,16 @@
       </c>
       <c r="H67" s="40"/>
       <c r="I67" s="5" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="J67" s="5" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K67" s="5" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="L67" s="19" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="M67" s="19"/>
       <c r="N67" s="19"/>
@@ -9111,7 +9120,7 @@
         <v>44</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E68" s="26"/>
       <c r="F68" s="6"/>
@@ -9166,7 +9175,7 @@
         <v>45</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E69" s="26">
         <v>99</v>
@@ -9183,7 +9192,7 @@
         <v>420</v>
       </c>
       <c r="L69" s="16" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="O69" s="59" t="s">
         <v>420</v>
@@ -9224,7 +9233,7 @@
         <v>46</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E70" s="26">
         <v>99</v>
@@ -9282,7 +9291,7 @@
         <v>47</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E71" s="26">
         <v>99</v>
@@ -9336,7 +9345,7 @@
         <v>48</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E72" s="26">
         <v>99</v>
@@ -9394,7 +9403,7 @@
         <v>697</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E73" s="26">
         <v>99</v>
@@ -9474,7 +9483,7 @@
       </c>
       <c r="Q74" s="59"/>
       <c r="R74" s="60" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="S74" s="59" t="s">
         <v>557</v>
@@ -9503,7 +9512,7 @@
         <v>1135</v>
       </c>
       <c r="D75" s="25" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E75" s="26"/>
       <c r="F75" s="6"/>
@@ -9524,10 +9533,10 @@
       <c r="R75" s="59"/>
       <c r="S75" s="59"/>
       <c r="T75" s="20" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="V75" s="45" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="X75" s="2"/>
     </row>
@@ -9543,7 +9552,7 @@
         <v>51</v>
       </c>
       <c r="D76" s="25" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E76" s="26"/>
       <c r="F76" s="6"/>
@@ -9576,7 +9585,7 @@
         <v>558</v>
       </c>
       <c r="T76" s="2" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="U76" s="20" t="s">
         <v>51</v>
@@ -9601,10 +9610,10 @@
         <v>52</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E77" s="26" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="F77" s="6"/>
       <c r="G77" s="40" t="str">
@@ -9618,10 +9627,10 @@
       <c r="I77" s="5"/>
       <c r="J77" s="5"/>
       <c r="K77" s="5" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="L77" s="49" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="M77" s="49"/>
       <c r="N77" s="49"/>
@@ -9660,10 +9669,10 @@
         <v>698</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E78" s="26" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="F78" s="6"/>
       <c r="G78" s="40" t="str">
@@ -9672,16 +9681,16 @@
       </c>
       <c r="H78" s="40"/>
       <c r="I78" s="18" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="J78" s="17" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K78" s="5" t="s">
+        <v>1274</v>
+      </c>
+      <c r="L78" s="19" t="s">
         <v>1275</v>
-      </c>
-      <c r="L78" s="19" t="s">
-        <v>1276</v>
       </c>
       <c r="M78" s="19"/>
       <c r="N78" s="19"/>
@@ -9724,10 +9733,10 @@
         <v>699</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E79" s="26" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="F79" s="6"/>
       <c r="G79" s="40" t="str">
@@ -9736,16 +9745,16 @@
       </c>
       <c r="H79" s="40"/>
       <c r="I79" s="19" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="J79" s="17" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K79" s="5" t="s">
+        <v>1168</v>
+      </c>
+      <c r="L79" s="49" t="s">
         <v>1169</v>
-      </c>
-      <c r="L79" s="49" t="s">
-        <v>1170</v>
       </c>
       <c r="M79" s="49"/>
       <c r="N79" s="49"/>
@@ -9788,10 +9797,10 @@
         <v>700</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E80" s="26" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="F80" s="6"/>
       <c r="G80" s="40" t="str">
@@ -9848,10 +9857,10 @@
         <v>53</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E81" s="26" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="F81" s="6"/>
       <c r="G81" s="40" t="str">
@@ -9863,16 +9872,16 @@
         <v>B02</v>
       </c>
       <c r="I81" s="18" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="J81" s="17" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K81" s="5" t="s">
+        <v>1170</v>
+      </c>
+      <c r="L81" s="49" t="s">
         <v>1171</v>
-      </c>
-      <c r="L81" s="49" t="s">
-        <v>1172</v>
       </c>
       <c r="M81" s="49"/>
       <c r="N81" s="49"/>
@@ -9915,10 +9924,10 @@
         <v>54</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E82" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F82" s="6"/>
       <c r="G82" s="40" t="str">
@@ -9930,16 +9939,16 @@
         <v>B03</v>
       </c>
       <c r="I82" s="18" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="J82" s="17" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K82" s="5" t="s">
+        <v>1172</v>
+      </c>
+      <c r="L82" s="49" t="s">
         <v>1173</v>
-      </c>
-      <c r="L82" s="49" t="s">
-        <v>1174</v>
       </c>
       <c r="M82" s="49"/>
       <c r="N82" s="49"/>
@@ -9984,10 +9993,10 @@
         <v>55</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E83" s="26" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F83" s="6"/>
       <c r="G83" s="40" t="str">
@@ -9999,16 +10008,16 @@
         <v>B04</v>
       </c>
       <c r="I83" s="16" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="J83" s="17" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K83" s="5" t="s">
+        <v>1247</v>
+      </c>
+      <c r="L83" s="49" t="s">
         <v>1248</v>
-      </c>
-      <c r="L83" s="49" t="s">
-        <v>1249</v>
       </c>
       <c r="M83" s="49"/>
       <c r="N83" s="49"/>
@@ -10051,10 +10060,10 @@
         <v>56</v>
       </c>
       <c r="D84" s="27" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E84" s="26" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="F84" s="6"/>
       <c r="G84" s="40" t="str">
@@ -10066,16 +10075,16 @@
         <v>B05</v>
       </c>
       <c r="I84" s="18" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="J84" s="17" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K84" s="5" t="s">
+        <v>1174</v>
+      </c>
+      <c r="L84" s="49" t="s">
         <v>1175</v>
-      </c>
-      <c r="L84" s="49" t="s">
-        <v>1176</v>
       </c>
       <c r="M84" s="49"/>
       <c r="N84" s="49"/>
@@ -10118,10 +10127,10 @@
         <v>57</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E85" s="26" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="F85" s="6"/>
       <c r="G85" s="40" t="str">
@@ -10133,16 +10142,16 @@
         <v>B06</v>
       </c>
       <c r="I85" s="18" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="J85" s="17" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K85" s="5" t="s">
+        <v>1176</v>
+      </c>
+      <c r="L85" s="49" t="s">
         <v>1177</v>
-      </c>
-      <c r="L85" s="49" t="s">
-        <v>1178</v>
       </c>
       <c r="M85" s="49"/>
       <c r="N85" s="49"/>
@@ -10185,10 +10194,10 @@
         <v>58</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E86" s="26" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="F86" s="6"/>
       <c r="G86" s="40" t="str">
@@ -10200,16 +10209,16 @@
         <v>B07</v>
       </c>
       <c r="I86" s="18" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="J86" s="17" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K86" s="5" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="L86" s="49" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="M86" s="49"/>
       <c r="N86" s="49"/>
@@ -10252,10 +10261,10 @@
         <v>59</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E87" s="26" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="F87" s="6"/>
       <c r="G87" s="40" t="s">
@@ -10266,7 +10275,7 @@
         <v>B08</v>
       </c>
       <c r="J87" s="17" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K87" s="5" t="s">
         <v>952</v>
@@ -10311,10 +10320,10 @@
         <v>701</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E88" s="26" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="F88" s="6"/>
       <c r="G88" s="40" t="str">
@@ -10323,16 +10332,16 @@
       </c>
       <c r="H88" s="40"/>
       <c r="I88" s="18" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="J88" s="17" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K88" s="5" t="s">
+        <v>1251</v>
+      </c>
+      <c r="L88" s="49" t="s">
         <v>1252</v>
-      </c>
-      <c r="L88" s="49" t="s">
-        <v>1253</v>
       </c>
       <c r="M88" s="49"/>
       <c r="N88" s="49"/>
@@ -10375,10 +10384,10 @@
         <v>702</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E89" s="26" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="F89" s="6"/>
       <c r="G89" s="40" t="str">
@@ -10387,16 +10396,16 @@
       </c>
       <c r="H89" s="40"/>
       <c r="I89" s="18" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="J89" s="17" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K89" s="5" t="s">
+        <v>1253</v>
+      </c>
+      <c r="L89" s="49" t="s">
         <v>1254</v>
-      </c>
-      <c r="L89" s="49" t="s">
-        <v>1255</v>
       </c>
       <c r="M89" s="49"/>
       <c r="N89" s="49"/>
@@ -10439,10 +10448,10 @@
         <v>60</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E90" s="26" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F90" s="6"/>
       <c r="G90" s="40" t="str">
@@ -10454,16 +10463,16 @@
         <v>B09</v>
       </c>
       <c r="I90" s="16" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J90" s="17" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K90" s="5" t="s">
+        <v>1180</v>
+      </c>
+      <c r="L90" s="49" t="s">
         <v>1181</v>
-      </c>
-      <c r="L90" s="49" t="s">
-        <v>1182</v>
       </c>
       <c r="M90" s="49"/>
       <c r="N90" s="49"/>
@@ -10501,10 +10510,10 @@
       </c>
       <c r="B91" s="2"/>
       <c r="C91" s="37" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E91" s="26">
         <v>10</v>
@@ -10516,7 +10525,7 @@
         <v>B10</v>
       </c>
       <c r="J91" s="17" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K91" s="5"/>
       <c r="L91" s="49"/>
@@ -10528,11 +10537,11 @@
       <c r="R91" s="59"/>
       <c r="S91" s="59"/>
       <c r="T91" s="5" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="U91" s="20"/>
       <c r="V91" s="5" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="W91" s="45"/>
       <c r="X91" s="2"/>
@@ -10549,10 +10558,10 @@
         <v>61</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E92" s="26" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="F92" s="6"/>
       <c r="G92" s="40" t="str">
@@ -10561,16 +10570,16 @@
       </c>
       <c r="H92" s="40"/>
       <c r="I92" s="5" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="J92" s="17" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K92" s="5" t="s">
+        <v>1182</v>
+      </c>
+      <c r="L92" s="49" t="s">
         <v>1183</v>
-      </c>
-      <c r="L92" s="49" t="s">
-        <v>1184</v>
       </c>
       <c r="M92" s="49"/>
       <c r="N92" s="49"/>
@@ -10613,7 +10622,7 @@
         <v>62</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E93" s="26">
         <v>10</v>
@@ -10625,16 +10634,16 @@
       </c>
       <c r="H93" s="40"/>
       <c r="I93" s="5" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="J93" s="17" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K93" s="5" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="L93" s="49" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="M93" s="49"/>
       <c r="N93" s="49"/>
@@ -10677,7 +10686,7 @@
         <v>63</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E94" s="26">
         <v>11</v>
@@ -10692,16 +10701,16 @@
         <v>B11</v>
       </c>
       <c r="I94" s="5" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="J94" s="17" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K94" s="5" t="s">
+        <v>1208</v>
+      </c>
+      <c r="L94" s="49" t="s">
         <v>1209</v>
-      </c>
-      <c r="L94" s="49" t="s">
-        <v>1210</v>
       </c>
       <c r="M94" s="49"/>
       <c r="N94" s="49"/>
@@ -10744,10 +10753,10 @@
         <v>64</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E95" s="26" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="F95" s="6"/>
       <c r="G95" s="40" t="str">
@@ -10759,16 +10768,16 @@
         <v>B12</v>
       </c>
       <c r="I95" s="19" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="J95" s="17" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K95" s="5" t="s">
+        <v>1184</v>
+      </c>
+      <c r="L95" s="49" t="s">
         <v>1185</v>
-      </c>
-      <c r="L95" s="49" t="s">
-        <v>1186</v>
       </c>
       <c r="M95" s="49"/>
       <c r="N95" s="49"/>
@@ -10811,7 +10820,7 @@
         <v>703</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E96" s="26">
         <v>99</v>
@@ -10823,16 +10832,16 @@
       </c>
       <c r="H96" s="40"/>
       <c r="I96" s="19" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="J96" s="17" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K96" s="5" t="s">
+        <v>1186</v>
+      </c>
+      <c r="L96" s="49" t="s">
         <v>1187</v>
-      </c>
-      <c r="L96" s="49" t="s">
-        <v>1188</v>
       </c>
       <c r="M96" s="49"/>
       <c r="N96" s="49"/>
@@ -10875,7 +10884,7 @@
         <v>704</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E97" s="26">
         <v>13</v>
@@ -10890,16 +10899,16 @@
         <v>B13</v>
       </c>
       <c r="I97" s="19" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="J97" s="17" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K97" s="5" t="s">
+        <v>1210</v>
+      </c>
+      <c r="L97" s="49" t="s">
         <v>1211</v>
-      </c>
-      <c r="L97" s="49" t="s">
-        <v>1212</v>
       </c>
       <c r="M97" s="49"/>
       <c r="N97" s="49"/>
@@ -10942,7 +10951,7 @@
         <v>705</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E98" s="26">
         <v>14</v>
@@ -10957,16 +10966,16 @@
         <v>B14</v>
       </c>
       <c r="I98" s="5" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="J98" s="17" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K98" s="5" t="s">
+        <v>1256</v>
+      </c>
+      <c r="L98" s="49" t="s">
         <v>1257</v>
-      </c>
-      <c r="L98" s="49" t="s">
-        <v>1258</v>
       </c>
       <c r="M98" s="49"/>
       <c r="N98" s="49"/>
@@ -11009,7 +11018,7 @@
         <v>706</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E99" s="26">
         <v>15</v>
@@ -11024,16 +11033,16 @@
         <v>B15</v>
       </c>
       <c r="I99" s="16" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="J99" s="17" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K99" s="5" t="s">
+        <v>1188</v>
+      </c>
+      <c r="L99" s="19" t="s">
         <v>1189</v>
-      </c>
-      <c r="L99" s="19" t="s">
-        <v>1190</v>
       </c>
       <c r="M99" s="19"/>
       <c r="N99" s="19"/>
@@ -11076,7 +11085,7 @@
         <v>707</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E100" s="26">
         <v>99</v>
@@ -11088,16 +11097,16 @@
       </c>
       <c r="H100" s="40"/>
       <c r="I100" s="19" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="J100" s="17" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K100" s="5" t="s">
+        <v>1190</v>
+      </c>
+      <c r="L100" s="49" t="s">
         <v>1191</v>
-      </c>
-      <c r="L100" s="49" t="s">
-        <v>1192</v>
       </c>
       <c r="M100" s="49"/>
       <c r="N100" s="49"/>
@@ -11140,7 +11149,7 @@
         <v>708</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E101" s="26">
         <v>99</v>
@@ -11152,16 +11161,16 @@
       </c>
       <c r="H101" s="40"/>
       <c r="I101" s="19" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="J101" s="17" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K101" s="5" t="s">
+        <v>1192</v>
+      </c>
+      <c r="L101" s="49" t="s">
         <v>1193</v>
-      </c>
-      <c r="L101" s="49" t="s">
-        <v>1194</v>
       </c>
       <c r="M101" s="49"/>
       <c r="N101" s="49"/>
@@ -11204,7 +11213,7 @@
         <v>709</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E102" s="26">
         <v>99</v>
@@ -11216,16 +11225,16 @@
       </c>
       <c r="H102" s="40"/>
       <c r="I102" s="19" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="J102" s="17" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K102" s="5" t="s">
+        <v>1194</v>
+      </c>
+      <c r="L102" s="49" t="s">
         <v>1195</v>
-      </c>
-      <c r="L102" s="49" t="s">
-        <v>1196</v>
       </c>
       <c r="M102" s="49"/>
       <c r="N102" s="49"/>
@@ -11268,7 +11277,7 @@
         <v>710</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E103" s="26">
         <v>99</v>
@@ -11328,7 +11337,7 @@
         <v>711</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E104" s="26">
         <v>16</v>
@@ -11388,7 +11397,7 @@
         <v>712</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E105" s="26">
         <v>16</v>
@@ -11453,7 +11462,7 @@
         <v>713</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E106" s="26">
         <v>16</v>
@@ -11518,7 +11527,7 @@
         <v>714</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E107" s="26">
         <v>16</v>
@@ -11583,7 +11592,7 @@
         <v>715</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E108" s="26">
         <v>17</v>
@@ -11646,7 +11655,7 @@
         <v>716</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E109" s="26">
         <v>99</v>
@@ -11661,16 +11670,16 @@
         <v>B99</v>
       </c>
       <c r="I109" s="5" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="J109" s="5" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K109" s="5" t="s">
+        <v>1212</v>
+      </c>
+      <c r="L109" s="49" t="s">
         <v>1213</v>
-      </c>
-      <c r="L109" s="49" t="s">
-        <v>1214</v>
       </c>
       <c r="M109" s="49"/>
       <c r="N109" s="49"/>
@@ -11709,7 +11718,7 @@
         <v>65</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E110" s="26">
         <v>99</v>
@@ -11721,10 +11730,10 @@
       </c>
       <c r="H110" s="40"/>
       <c r="K110" s="5" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="L110" s="5" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="M110" s="5"/>
       <c r="N110" s="5"/>
@@ -11767,10 +11776,10 @@
         <v>66</v>
       </c>
       <c r="D111" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E111" s="26" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="F111" s="6"/>
       <c r="G111" s="40" t="str">
@@ -11782,22 +11791,22 @@
         <v>D01</v>
       </c>
       <c r="I111" s="5" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="J111" s="5" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K111" s="5" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="L111" s="49" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="M111" s="49" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="N111" s="49" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="O111" s="59" t="s">
         <v>975</v>
@@ -11825,7 +11834,7 @@
         <v>66</v>
       </c>
       <c r="X111" s="2" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="112" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
@@ -11840,10 +11849,10 @@
         <v>67</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E112" s="26" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="F112" s="6"/>
       <c r="G112" s="40" t="s">
@@ -11856,18 +11865,18 @@
       <c r="I112" s="5"/>
       <c r="J112" s="5"/>
       <c r="K112" s="5" t="s">
+        <v>1316</v>
+      </c>
+      <c r="L112" s="19" t="s">
         <v>1317</v>
-      </c>
-      <c r="L112" s="19" t="s">
-        <v>1318</v>
       </c>
       <c r="M112" s="19"/>
       <c r="N112" s="19"/>
       <c r="O112" s="59" t="s">
+        <v>1316</v>
+      </c>
+      <c r="P112" s="66" t="s">
         <v>1317</v>
-      </c>
-      <c r="P112" s="66" t="s">
-        <v>1318</v>
       </c>
       <c r="Q112" s="69"/>
       <c r="R112" s="59" t="s">
@@ -11902,10 +11911,10 @@
         <v>717</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E113" s="26" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="F113" s="6"/>
       <c r="G113" s="40" t="str">
@@ -11962,10 +11971,10 @@
         <v>718</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E114" s="26" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="F114" s="6"/>
       <c r="G114" s="40" t="str">
@@ -12022,10 +12031,10 @@
         <v>719</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E115" s="26" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="F115" s="6"/>
       <c r="G115" s="40" t="str">
@@ -12082,10 +12091,10 @@
         <v>720</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E116" s="26" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="F116" s="6"/>
       <c r="G116" s="40" t="str">
@@ -12196,13 +12205,13 @@
       </c>
       <c r="B118" s="2"/>
       <c r="C118" s="32" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E118" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F118" s="6"/>
       <c r="G118" s="40" t="s">
@@ -12224,11 +12233,11 @@
       <c r="R118" s="59"/>
       <c r="S118" s="59"/>
       <c r="T118" s="2" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
       <c r="U118" s="20"/>
       <c r="V118" s="2" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="W118" s="45"/>
       <c r="X118" s="2"/>
@@ -12243,10 +12252,10 @@
         <v>1132</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E119" s="26" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F119" s="6"/>
       <c r="G119" s="40"/>
@@ -12266,11 +12275,11 @@
       <c r="R119" s="59"/>
       <c r="S119" s="59"/>
       <c r="T119" s="2" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
       <c r="U119" s="20"/>
       <c r="V119" s="2" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="W119" s="45"/>
       <c r="X119" s="2"/>
@@ -12367,10 +12376,10 @@
         <v>723</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E122" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F122" s="6"/>
       <c r="G122" s="40" t="str">
@@ -12427,10 +12436,10 @@
         <v>724</v>
       </c>
       <c r="D123" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E123" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F123" s="6"/>
       <c r="G123" s="40" t="str">
@@ -12487,10 +12496,10 @@
         <v>725</v>
       </c>
       <c r="D124" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E124" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F124" s="6"/>
       <c r="G124" s="40" t="str">
@@ -12547,10 +12556,10 @@
         <v>69</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E125" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F125" s="6"/>
       <c r="G125" s="40" t="str">
@@ -12564,13 +12573,13 @@
         <v>443</v>
       </c>
       <c r="L125" s="49" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="M125" s="49" t="s">
         <v>443</v>
       </c>
       <c r="N125" s="49" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="O125" s="59" t="s">
         <v>443</v>
@@ -12611,10 +12620,10 @@
         <v>70</v>
       </c>
       <c r="D126" s="27" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E126" s="26" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F126" s="6" t="s">
         <v>1126</v>
@@ -12628,24 +12637,24 @@
         <v>D04a</v>
       </c>
       <c r="I126" s="5" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="J126" s="5" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="K126" s="5" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="L126" s="19" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="M126" s="19"/>
       <c r="N126" s="19"/>
       <c r="O126" s="59" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="P126" s="66" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="Q126" s="69"/>
       <c r="R126" s="59" t="s">
@@ -12733,10 +12742,10 @@
         <v>668</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E128" s="26" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F128" s="6" t="s">
         <v>1127</v>
@@ -12798,10 +12807,10 @@
         <v>669</v>
       </c>
       <c r="D129" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E129" s="26" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F129" s="28" t="s">
         <v>1130</v>
@@ -12863,13 +12872,13 @@
         <v>726</v>
       </c>
       <c r="D130" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E130" s="26" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F130" s="28" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="G130" s="40" t="str">
         <f t="shared" si="10"/>
@@ -12928,10 +12937,10 @@
         <v>727</v>
       </c>
       <c r="D131" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E131" s="26" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F131" s="6"/>
       <c r="G131" s="40" t="str">
@@ -12983,10 +12992,10 @@
         <v>728</v>
       </c>
       <c r="D132" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E132" s="26" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F132" s="6"/>
       <c r="G132" s="40" t="str">
@@ -12995,16 +13004,16 @@
       </c>
       <c r="H132" s="40"/>
       <c r="I132" s="5" t="s">
+        <v>1237</v>
+      </c>
+      <c r="J132" s="5" t="s">
+        <v>1161</v>
+      </c>
+      <c r="K132" s="5" t="s">
+        <v>1167</v>
+      </c>
+      <c r="L132" s="19" t="s">
         <v>1238</v>
-      </c>
-      <c r="J132" s="5" t="s">
-        <v>1162</v>
-      </c>
-      <c r="K132" s="5" t="s">
-        <v>1168</v>
-      </c>
-      <c r="L132" s="19" t="s">
-        <v>1239</v>
       </c>
       <c r="M132" s="19"/>
       <c r="N132" s="19"/>
@@ -13034,7 +13043,7 @@
         <v>728</v>
       </c>
       <c r="X132" s="2" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="133" spans="1:24" x14ac:dyDescent="0.25">
@@ -13049,10 +13058,10 @@
         <v>72</v>
       </c>
       <c r="D133" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E133" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F133" s="6"/>
       <c r="G133" s="40" t="str">
@@ -13105,10 +13114,10 @@
         <v>73</v>
       </c>
       <c r="D134" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E134" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F134" s="6"/>
       <c r="G134" s="40" t="str">
@@ -13165,10 +13174,10 @@
         <v>729</v>
       </c>
       <c r="D135" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E135" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F135" s="6"/>
       <c r="G135" s="40" t="str">
@@ -13270,10 +13279,10 @@
         <v>730</v>
       </c>
       <c r="D137" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E137" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F137" s="6"/>
       <c r="G137" s="40" t="str">
@@ -13326,10 +13335,10 @@
         <v>731</v>
       </c>
       <c r="D138" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E138" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F138" s="6"/>
       <c r="G138" s="40" t="str">
@@ -13382,10 +13391,10 @@
         <v>75</v>
       </c>
       <c r="D139" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E139" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F139" s="6"/>
       <c r="G139" s="40" t="str">
@@ -13438,10 +13447,10 @@
         <v>76</v>
       </c>
       <c r="D140" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E140" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F140" s="6"/>
       <c r="G140" s="40" t="str">
@@ -13553,10 +13562,10 @@
         <v>732</v>
       </c>
       <c r="D142" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E142" s="26" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="F142" s="6"/>
       <c r="G142" s="40" t="str">
@@ -13616,10 +13625,10 @@
         <v>79</v>
       </c>
       <c r="D143" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E143" s="26" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="F143" s="6"/>
       <c r="G143" s="40" t="str">
@@ -13676,10 +13685,10 @@
         <v>80</v>
       </c>
       <c r="D144" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E144" s="26" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="F144" s="6"/>
       <c r="G144" s="40" t="str">
@@ -13736,10 +13745,10 @@
         <v>81</v>
       </c>
       <c r="D145" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E145" s="26" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="F145" s="6"/>
       <c r="G145" s="40" t="str">
@@ -13796,10 +13805,10 @@
         <v>82</v>
       </c>
       <c r="D146" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E146" s="26" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="F146" s="6"/>
       <c r="G146" s="40" t="str">
@@ -13852,10 +13861,10 @@
         <v>83</v>
       </c>
       <c r="D147" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E147" s="26" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="F147" s="6"/>
       <c r="G147" s="40" t="str">
@@ -13908,10 +13917,10 @@
         <v>84</v>
       </c>
       <c r="D148" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E148" s="26" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="F148" s="6"/>
       <c r="G148" s="40" t="str">
@@ -13923,16 +13932,16 @@
         <v>D06</v>
       </c>
       <c r="I148" s="57" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="J148" s="18" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K148" s="5" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="L148" s="58" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="M148" s="58"/>
       <c r="N148" s="58"/>
@@ -14030,7 +14039,7 @@
         <v>86</v>
       </c>
       <c r="D150" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E150" s="26">
         <v>99</v>
@@ -14086,7 +14095,7 @@
         <v>87</v>
       </c>
       <c r="D151" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E151" s="26">
         <v>99</v>
@@ -14142,7 +14151,7 @@
         <v>733</v>
       </c>
       <c r="D152" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E152" s="26">
         <v>99</v>
@@ -14198,7 +14207,7 @@
         <v>89</v>
       </c>
       <c r="D153" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E153" s="26">
         <v>99</v>
@@ -14254,7 +14263,7 @@
         <v>90</v>
       </c>
       <c r="D154" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E154" s="26">
         <v>99</v>
@@ -14271,7 +14280,7 @@
         <v>460</v>
       </c>
       <c r="L154" s="49" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="M154" s="49"/>
       <c r="N154" s="49"/>
@@ -14310,7 +14319,7 @@
         <v>91</v>
       </c>
       <c r="D155" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E155" s="26">
         <v>99</v>
@@ -14366,7 +14375,7 @@
         <v>92</v>
       </c>
       <c r="D156" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E156" s="26">
         <v>99</v>
@@ -14424,7 +14433,7 @@
         <v>93</v>
       </c>
       <c r="D157" s="25" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="E157" s="26"/>
       <c r="F157" s="6"/>
@@ -14482,7 +14491,7 @@
         <v>94</v>
       </c>
       <c r="D158" s="6" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="E158" s="26">
         <v>99</v>
@@ -14505,7 +14514,7 @@
         <v>464</v>
       </c>
       <c r="N158" s="49" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="O158" s="59" t="s">
         <v>464</v>
@@ -14546,10 +14555,10 @@
         <v>95</v>
       </c>
       <c r="D159" s="6" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="E159" s="26" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="F159" s="6"/>
       <c r="G159" s="40" t="str">
@@ -14613,10 +14622,10 @@
         <v>96</v>
       </c>
       <c r="D160" s="6" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="E160" s="26" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="F160" s="6"/>
       <c r="G160" s="40" t="str">
@@ -14680,10 +14689,10 @@
         <v>97</v>
       </c>
       <c r="D161" s="6" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="E161" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F161" s="6"/>
       <c r="G161" s="40" t="str">
@@ -14695,22 +14704,22 @@
         <v>C03</v>
       </c>
       <c r="I161" s="5" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="J161" s="5" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K161" s="5" t="s">
+        <v>1229</v>
+      </c>
+      <c r="L161" s="49" t="s">
         <v>1230</v>
       </c>
-      <c r="L161" s="49" t="s">
-        <v>1231</v>
-      </c>
       <c r="M161" s="49" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="N161" s="49" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="O161" s="59" t="s">
         <v>467</v>
@@ -14751,10 +14760,10 @@
         <v>98</v>
       </c>
       <c r="D162" s="6" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="E162" s="26" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F162" s="6"/>
       <c r="G162" s="40" t="str">
@@ -14774,10 +14783,10 @@
         <v>830</v>
       </c>
       <c r="M162" s="49" t="s">
+        <v>1352</v>
+      </c>
+      <c r="N162" s="49" t="s">
         <v>1353</v>
-      </c>
-      <c r="N162" s="49" t="s">
-        <v>1354</v>
       </c>
       <c r="O162" s="59" t="s">
         <v>468</v>
@@ -14805,7 +14814,7 @@
         <v>98</v>
       </c>
       <c r="X162" s="81" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="163" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
@@ -14816,10 +14825,10 @@
       <c r="B163" s="2"/>
       <c r="C163" s="36"/>
       <c r="D163" s="6" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="E163" s="26" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="F163" s="6"/>
       <c r="G163" s="40" t="str">
@@ -14831,22 +14840,22 @@
         <v>C05</v>
       </c>
       <c r="I163" s="5" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="J163" s="5" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="K163" s="5" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="L163" s="49" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="M163" s="49" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="N163" s="49" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="O163" s="59"/>
       <c r="P163" s="68"/>
@@ -14854,7 +14863,7 @@
       <c r="R163" s="59"/>
       <c r="S163" s="59"/>
       <c r="T163" s="5" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="U163" s="50"/>
       <c r="V163" s="5"/>
@@ -14873,7 +14882,7 @@
         <v>99</v>
       </c>
       <c r="D164" s="6" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="E164" s="26">
         <v>99</v>
@@ -14888,22 +14897,22 @@
         <v>C99</v>
       </c>
       <c r="I164" s="5" t="s">
+        <v>1335</v>
+      </c>
+      <c r="J164" s="5" t="s">
         <v>1336</v>
       </c>
-      <c r="J164" s="5" t="s">
+      <c r="K164" s="5" t="s">
         <v>1337</v>
       </c>
-      <c r="K164" s="5" t="s">
+      <c r="L164" s="19" t="s">
         <v>1338</v>
       </c>
-      <c r="L164" s="19" t="s">
-        <v>1339</v>
-      </c>
       <c r="M164" s="19" t="s">
+        <v>1357</v>
+      </c>
+      <c r="N164" s="19" t="s">
         <v>1358</v>
-      </c>
-      <c r="N164" s="19" t="s">
-        <v>1359</v>
       </c>
       <c r="O164" s="59" t="s">
         <v>469</v>
@@ -14919,7 +14928,7 @@
         <v>1102</v>
       </c>
       <c r="T164" s="79" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="U164" s="52" t="s">
         <v>99</v>
@@ -14931,7 +14940,7 @@
         <v>99</v>
       </c>
       <c r="X164" s="81" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="165" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
@@ -14994,7 +15003,7 @@
     <row r="166" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A166" s="44" t="str">
         <f t="shared" si="11"/>
-        <v>.....D.07. - Chronic obstructive pulmonary disease</v>
+        <v>.....D.66. - Chronic obstructive pulmonary disease</v>
       </c>
       <c r="B166" s="2">
         <v>155</v>
@@ -15002,20 +15011,20 @@
       <c r="C166" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="D166" s="6" t="s">
-        <v>1143</v>
-      </c>
-      <c r="E166" s="26" t="s">
-        <v>1151</v>
+      <c r="D166" s="27" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E166" s="83" t="s">
+        <v>1365</v>
       </c>
       <c r="F166" s="6"/>
       <c r="G166" s="40" t="str">
         <f>CONCATENATE("c",D166,E166,F166)</f>
-        <v>cD07</v>
+        <v>cD66</v>
       </c>
       <c r="H166" s="40" t="str">
         <f>CONCATENATE(D166,E166,F166)</f>
-        <v>D07</v>
+        <v>D66</v>
       </c>
       <c r="I166" s="5"/>
       <c r="J166" s="5"/>
@@ -15057,7 +15066,7 @@
     <row r="167" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A167" s="44" t="str">
         <f t="shared" si="11"/>
-        <v/>
+        <v>.....D.67. - Asthma</v>
       </c>
       <c r="B167" s="2">
         <v>156</v>
@@ -15065,18 +15074,21 @@
       <c r="C167" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="D167" s="6" t="s">
-        <v>1143</v>
-      </c>
-      <c r="E167" s="26" t="s">
-        <v>1152</v>
+      <c r="D167" s="27" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E167" s="83" t="s">
+        <v>1366</v>
       </c>
       <c r="F167" s="6"/>
       <c r="G167" s="40" t="str">
         <f>CONCATENATE("c",D167,E167,F167)</f>
-        <v>cD08</v>
-      </c>
-      <c r="H167" s="40"/>
+        <v>cD67</v>
+      </c>
+      <c r="H167" s="40" t="str">
+        <f>CONCATENATE(D167,E167,F167)</f>
+        <v>D67</v>
+      </c>
       <c r="I167" s="5"/>
       <c r="J167" s="5"/>
       <c r="K167" s="5" t="s">
@@ -15117,28 +15129,28 @@
     <row r="168" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A168" s="44" t="str">
         <f t="shared" si="11"/>
-        <v>.....D.08. - Asthma and other respiratory diseases</v>
+        <v>.....D.68. - Other respiratory diseases</v>
       </c>
       <c r="B168" s="2">
         <v>157</v>
       </c>
       <c r="C168" s="31" t="s">
-        <v>1136</v>
-      </c>
-      <c r="D168" s="6" t="s">
-        <v>1143</v>
-      </c>
-      <c r="E168" s="26" t="s">
-        <v>1152</v>
+        <v>1364</v>
+      </c>
+      <c r="D168" s="27" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E168" s="83" t="s">
+        <v>1367</v>
       </c>
       <c r="F168" s="6"/>
       <c r="G168" s="40" t="str">
         <f>CONCATENATE("c",D168,E168,F168)</f>
-        <v>cD08</v>
+        <v>cD68</v>
       </c>
       <c r="H168" s="40" t="str">
         <f>CONCATENATE(D168,E168,F168)</f>
-        <v>D08</v>
+        <v>D68</v>
       </c>
       <c r="I168" s="5"/>
       <c r="J168" s="5"/>
@@ -15164,7 +15176,7 @@
         <v>1055</v>
       </c>
       <c r="T168" s="5" t="s">
-        <v>1363</v>
+        <v>280</v>
       </c>
       <c r="U168" s="20" t="s">
         <v>103</v>
@@ -15189,10 +15201,10 @@
         <v>104</v>
       </c>
       <c r="D169" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E169" s="26" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F169" s="6"/>
       <c r="G169" s="40" t="s">
@@ -15226,10 +15238,10 @@
         <v>682</v>
       </c>
       <c r="T169" s="81" t="s">
+        <v>1342</v>
+      </c>
+      <c r="U169" s="20" t="s">
         <v>1343</v>
-      </c>
-      <c r="U169" s="20" t="s">
-        <v>1344</v>
       </c>
       <c r="V169" s="2" t="s">
         <v>281</v>
@@ -15251,10 +15263,10 @@
         <v>105</v>
       </c>
       <c r="D170" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E170" s="26" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F170" s="6"/>
       <c r="G170" s="40" t="str">
@@ -15311,10 +15323,10 @@
         <v>106</v>
       </c>
       <c r="D171" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E171" s="26" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="F171" s="6"/>
       <c r="G171" s="40" t="str">
@@ -15326,16 +15338,16 @@
         <v>D11</v>
       </c>
       <c r="I171" s="16" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="J171" s="5" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K171" s="5" t="s">
+        <v>1203</v>
+      </c>
+      <c r="L171" s="49" t="s">
         <v>1204</v>
-      </c>
-      <c r="L171" s="49" t="s">
-        <v>1205</v>
       </c>
       <c r="M171" s="49"/>
       <c r="N171" s="49"/>
@@ -15378,10 +15390,10 @@
         <v>107</v>
       </c>
       <c r="D172" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E172" s="26" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F172" s="6"/>
       <c r="G172" s="40" t="str">
@@ -15438,10 +15450,10 @@
         <v>734</v>
       </c>
       <c r="D173" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E173" s="26" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F173" s="6"/>
       <c r="G173" s="40" t="str">
@@ -15498,10 +15510,10 @@
         <v>735</v>
       </c>
       <c r="D174" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E174" s="26" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F174" s="6"/>
       <c r="G174" s="40" t="str">
@@ -15558,10 +15570,10 @@
         <v>667</v>
       </c>
       <c r="D175" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E175" s="26" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F175" s="6"/>
       <c r="G175" s="40" t="str">
@@ -15618,10 +15630,10 @@
         <v>736</v>
       </c>
       <c r="D176" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E176" s="26" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F176" s="6"/>
       <c r="G176" s="40" t="str">
@@ -15678,10 +15690,10 @@
         <v>737</v>
       </c>
       <c r="D177" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E177" s="26" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F177" s="6"/>
       <c r="G177" s="40" t="str">
@@ -15738,10 +15750,10 @@
         <v>738</v>
       </c>
       <c r="D178" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E178" s="26" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="F178" s="6"/>
       <c r="G178" s="40" t="str">
@@ -15750,16 +15762,16 @@
       </c>
       <c r="H178" s="40"/>
       <c r="I178" s="5" t="s">
+        <v>1205</v>
+      </c>
+      <c r="J178" s="5" t="s">
+        <v>1161</v>
+      </c>
+      <c r="K178" s="5" t="s">
         <v>1206</v>
       </c>
-      <c r="J178" s="5" t="s">
-        <v>1162</v>
-      </c>
-      <c r="K178" s="5" t="s">
+      <c r="L178" s="49" t="s">
         <v>1207</v>
-      </c>
-      <c r="L178" s="49" t="s">
-        <v>1208</v>
       </c>
       <c r="M178" s="49"/>
       <c r="N178" s="49"/>
@@ -15857,10 +15869,10 @@
         <v>109</v>
       </c>
       <c r="D180" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E180" s="26" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="F180" s="6"/>
       <c r="G180" s="40" t="s">
@@ -15919,10 +15931,10 @@
         <v>739</v>
       </c>
       <c r="D181" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E181" s="26" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="F181" s="6" t="s">
         <v>1126</v>
@@ -15984,10 +15996,10 @@
         <v>740</v>
       </c>
       <c r="D182" s="27" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E182" s="26" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="F182" s="6" t="s">
         <v>1127</v>
@@ -16049,10 +16061,10 @@
         <v>741</v>
       </c>
       <c r="D183" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E183" s="26" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="F183" s="6" t="s">
         <v>1130</v>
@@ -16114,7 +16126,7 @@
         <v>742</v>
       </c>
       <c r="D184" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E184" s="26">
         <v>99</v>
@@ -16170,7 +16182,7 @@
         <v>110</v>
       </c>
       <c r="D185" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E185" s="26">
         <v>99</v>
@@ -16230,7 +16242,7 @@
         <v>743</v>
       </c>
       <c r="D186" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E186" s="26">
         <v>99</v>
@@ -16290,7 +16302,7 @@
         <v>112</v>
       </c>
       <c r="D187" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E187" s="26">
         <v>99</v>
@@ -16350,7 +16362,7 @@
         <v>113</v>
       </c>
       <c r="D188" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E188" s="26">
         <v>99</v>
@@ -16410,7 +16422,7 @@
         <v>114</v>
       </c>
       <c r="D189" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E189" s="26">
         <v>99</v>
@@ -16527,7 +16539,7 @@
         <v>116</v>
       </c>
       <c r="D191" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E191" s="26">
         <v>99</v>
@@ -16587,7 +16599,7 @@
         <v>117</v>
       </c>
       <c r="D192" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E192" s="26">
         <v>99</v>
@@ -16643,7 +16655,7 @@
         <v>118</v>
       </c>
       <c r="D193" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E193" s="26">
         <v>99</v>
@@ -16699,7 +16711,7 @@
         <v>119</v>
       </c>
       <c r="D194" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E194" s="26">
         <v>99</v>
@@ -16755,7 +16767,7 @@
         <v>120</v>
       </c>
       <c r="D195" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E195" s="26">
         <v>99</v>
@@ -16767,16 +16779,16 @@
       </c>
       <c r="H195" s="40"/>
       <c r="I195" s="5" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="J195" s="5" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="K195" s="5" t="s">
+        <v>1200</v>
+      </c>
+      <c r="L195" s="49" t="s">
         <v>1201</v>
-      </c>
-      <c r="L195" s="49" t="s">
-        <v>1202</v>
       </c>
       <c r="M195" s="49"/>
       <c r="N195" s="49"/>
@@ -16819,10 +16831,10 @@
         <v>121</v>
       </c>
       <c r="D196" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E196" s="26" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="F196" s="6"/>
       <c r="G196" s="40" t="s">
@@ -16881,10 +16893,10 @@
         <v>122</v>
       </c>
       <c r="D197" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E197" s="26" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="F197" s="6"/>
       <c r="G197" s="40" t="str">
@@ -16941,10 +16953,10 @@
         <v>123</v>
       </c>
       <c r="D198" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E198" s="26" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="F198" s="6"/>
       <c r="G198" s="40" t="str">
@@ -17001,10 +17013,10 @@
         <v>124</v>
       </c>
       <c r="D199" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E199" s="26" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="F199" s="6"/>
       <c r="G199" s="40" t="str">
@@ -17061,10 +17073,10 @@
         <v>125</v>
       </c>
       <c r="D200" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E200" s="26" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="F200" s="6"/>
       <c r="G200" s="40" t="str">
@@ -17121,10 +17133,10 @@
         <v>126</v>
       </c>
       <c r="D201" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E201" s="26" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="F201" s="6"/>
       <c r="G201" s="40" t="str">
@@ -17181,10 +17193,10 @@
         <v>127</v>
       </c>
       <c r="D202" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E202" s="26" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="F202" s="6"/>
       <c r="G202" s="40" t="str">
@@ -17294,7 +17306,7 @@
         <v>129</v>
       </c>
       <c r="D204" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E204" s="26">
         <v>99</v>
@@ -17350,7 +17362,7 @@
         <v>130</v>
       </c>
       <c r="D205" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E205" s="26">
         <v>99</v>
@@ -17406,7 +17418,7 @@
         <v>131</v>
       </c>
       <c r="D206" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E206" s="26">
         <v>99</v>
@@ -17462,7 +17474,7 @@
         <v>744</v>
       </c>
       <c r="D207" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E207" s="26">
         <v>99</v>
@@ -17518,7 +17530,7 @@
         <v>132</v>
       </c>
       <c r="D208" s="25" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E208" s="26"/>
       <c r="F208" s="6"/>
@@ -17545,7 +17557,7 @@
       </c>
       <c r="Q208" s="66"/>
       <c r="R208" s="60" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="S208" s="59" t="s">
         <v>654</v>
@@ -17576,10 +17588,10 @@
         <v>133</v>
       </c>
       <c r="D209" s="6" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E209" s="26" t="s">
         <v>1144</v>
-      </c>
-      <c r="E209" s="26" t="s">
-        <v>1145</v>
       </c>
       <c r="F209" s="6"/>
       <c r="G209" s="40"/>
@@ -17636,10 +17648,10 @@
         <v>134</v>
       </c>
       <c r="D210" s="6" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E210" s="26" t="s">
         <v>1144</v>
-      </c>
-      <c r="E210" s="26" t="s">
-        <v>1145</v>
       </c>
       <c r="F210" s="6" t="s">
         <v>1126</v>
@@ -17653,16 +17665,16 @@
         <v>E01a</v>
       </c>
       <c r="I210" s="5" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="J210" s="5" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K210" s="5" t="s">
+        <v>1196</v>
+      </c>
+      <c r="L210" s="19" t="s">
         <v>1197</v>
-      </c>
-      <c r="L210" s="19" t="s">
-        <v>1198</v>
       </c>
       <c r="M210" s="19"/>
       <c r="N210" s="19"/>
@@ -17705,10 +17717,10 @@
         <v>135</v>
       </c>
       <c r="D211" s="6" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E211" s="26" t="s">
         <v>1144</v>
-      </c>
-      <c r="E211" s="26" t="s">
-        <v>1145</v>
       </c>
       <c r="F211" s="6" t="s">
         <v>1128</v>
@@ -17767,10 +17779,10 @@
         <v>136</v>
       </c>
       <c r="D212" s="6" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E212" s="26" t="s">
         <v>1144</v>
-      </c>
-      <c r="E212" s="26" t="s">
-        <v>1145</v>
       </c>
       <c r="F212" s="6" t="s">
         <v>1127</v>
@@ -17832,10 +17844,10 @@
         <v>137</v>
       </c>
       <c r="D213" s="6" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E213" s="26" t="s">
         <v>1144</v>
-      </c>
-      <c r="E213" s="26" t="s">
-        <v>1145</v>
       </c>
       <c r="F213" s="6" t="s">
         <v>1128</v>
@@ -17892,10 +17904,10 @@
         <v>745</v>
       </c>
       <c r="D214" s="6" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E214" s="26" t="s">
         <v>1144</v>
-      </c>
-      <c r="E214" s="26" t="s">
-        <v>1145</v>
       </c>
       <c r="F214" s="6" t="s">
         <v>1128</v>
@@ -17954,10 +17966,10 @@
         <v>746</v>
       </c>
       <c r="D215" s="6" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E215" s="26" t="s">
         <v>1144</v>
-      </c>
-      <c r="E215" s="26" t="s">
-        <v>1145</v>
       </c>
       <c r="F215" s="6" t="s">
         <v>1128</v>
@@ -18016,10 +18028,10 @@
         <v>747</v>
       </c>
       <c r="D216" s="6" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E216" s="26" t="s">
         <v>1144</v>
-      </c>
-      <c r="E216" s="26" t="s">
-        <v>1145</v>
       </c>
       <c r="F216" s="6" t="s">
         <v>1128</v>
@@ -18030,16 +18042,16 @@
       </c>
       <c r="H216" s="40"/>
       <c r="I216" s="5" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="J216" s="5" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="K216" s="5" t="s">
+        <v>1198</v>
+      </c>
+      <c r="L216" s="49" t="s">
         <v>1199</v>
-      </c>
-      <c r="L216" s="49" t="s">
-        <v>1200</v>
       </c>
       <c r="M216" s="49"/>
       <c r="N216" s="49"/>
@@ -18078,10 +18090,10 @@
         <v>748</v>
       </c>
       <c r="D217" s="6" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E217" s="26" t="s">
         <v>1144</v>
-      </c>
-      <c r="E217" s="26" t="s">
-        <v>1145</v>
       </c>
       <c r="F217" s="6" t="s">
         <v>1128</v>
@@ -18095,16 +18107,16 @@
         <v>E01x</v>
       </c>
       <c r="I217" s="5" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="J217" s="5" t="s">
+        <v>1262</v>
+      </c>
+      <c r="K217" s="5" t="s">
         <v>1263</v>
       </c>
-      <c r="K217" s="5" t="s">
+      <c r="L217" s="49" t="s">
         <v>1264</v>
-      </c>
-      <c r="L217" s="49" t="s">
-        <v>1265</v>
       </c>
       <c r="M217" s="49"/>
       <c r="N217" s="49"/>
@@ -18134,7 +18146,7 @@
         <v>887</v>
       </c>
       <c r="X217" s="22" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="218" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
@@ -18202,10 +18214,10 @@
         <v>140</v>
       </c>
       <c r="D219" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E219" s="26" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="F219" s="6"/>
       <c r="G219" s="40" t="str">
@@ -18217,16 +18229,16 @@
         <v>E02</v>
       </c>
       <c r="I219" s="5" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="J219" s="5" t="s">
+        <v>1214</v>
+      </c>
+      <c r="K219" s="5" t="s">
         <v>1215</v>
       </c>
-      <c r="K219" s="5" t="s">
+      <c r="L219" s="49" t="s">
         <v>1216</v>
-      </c>
-      <c r="L219" s="49" t="s">
-        <v>1217</v>
       </c>
       <c r="M219" s="49"/>
       <c r="N219" s="49"/>
@@ -18244,7 +18256,7 @@
         <v>999</v>
       </c>
       <c r="T219" s="5" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="U219" s="20" t="s">
         <v>140</v>
@@ -18269,10 +18281,10 @@
         <v>141</v>
       </c>
       <c r="D220" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E220" s="26" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F220" s="6"/>
       <c r="G220" s="40" t="str">
@@ -18284,16 +18296,16 @@
         <v>E03</v>
       </c>
       <c r="I220" s="5" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="J220" s="5" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="K220" s="5" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="L220" s="19" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="M220" s="19"/>
       <c r="N220" s="19"/>
@@ -18311,7 +18323,7 @@
         <v>998</v>
       </c>
       <c r="T220" s="5" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="U220" s="20" t="s">
         <v>141</v>
@@ -18336,10 +18348,10 @@
         <v>142</v>
       </c>
       <c r="D221" s="6" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E221" s="26" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="F221" s="6"/>
       <c r="G221" s="40" t="str">
@@ -18348,16 +18360,16 @@
       </c>
       <c r="H221" s="40"/>
       <c r="I221" s="5" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="J221" s="5" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="K221" s="5" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="L221" s="49" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="M221" s="49"/>
       <c r="N221" s="49"/>
@@ -18383,21 +18395,21 @@
         <v>142</v>
       </c>
       <c r="X221" s="22" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="222" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B222" s="82" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="C222" s="16" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="D222" s="54" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E222" s="55" t="s">
         <v>1144</v>
-      </c>
-      <c r="E222" s="55" t="s">
-        <v>1145</v>
       </c>
       <c r="G222" s="40" t="str">
         <f t="shared" si="21"/>
@@ -18405,19 +18417,19 @@
       </c>
       <c r="H222" s="40"/>
       <c r="I222" s="48" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="J222" s="48" t="s">
+        <v>1278</v>
+      </c>
+      <c r="K222" s="16" t="s">
         <v>1279</v>
       </c>
-      <c r="K222" s="16" t="s">
+      <c r="L222" s="16" t="s">
         <v>1280</v>
       </c>
-      <c r="L222" s="16" t="s">
-        <v>1281</v>
-      </c>
       <c r="T222" s="48" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="223" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
@@ -18426,10 +18438,10 @@
         <v>.....Z.01. - Symptoms, signs and ill-defined conditions, not elsewhere classified</v>
       </c>
       <c r="D223" s="56" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="E223" s="55" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G223" s="40" t="str">
         <f t="shared" si="21"/>
@@ -18440,19 +18452,19 @@
         <v>Z01</v>
       </c>
       <c r="I223" s="48" t="s">
+        <v>1224</v>
+      </c>
+      <c r="J223" s="48" t="s">
         <v>1225</v>
       </c>
-      <c r="J223" s="48" t="s">
+      <c r="K223" s="16" t="s">
         <v>1226</v>
       </c>
-      <c r="K223" s="16" t="s">
+      <c r="L223" s="16" t="s">
+        <v>1260</v>
+      </c>
+      <c r="T223" s="48" t="s">
         <v>1227</v>
-      </c>
-      <c r="L223" s="16" t="s">
-        <v>1261</v>
-      </c>
-      <c r="T223" s="48" t="s">
-        <v>1228</v>
       </c>
     </row>
     <row r="224" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
@@ -18461,10 +18473,10 @@
         <v/>
       </c>
       <c r="D224" s="56" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E224" s="55" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="G224" s="42" t="str">
         <f t="shared" si="21"/>
@@ -18472,19 +18484,19 @@
       </c>
       <c r="H224" s="40"/>
       <c r="I224" s="16" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="J224" s="48" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="K224" s="16" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="L224" s="16" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="T224" s="48" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="225" spans="1:20" x14ac:dyDescent="0.25">
@@ -18493,10 +18505,10 @@
         <v>.....Z.02. - Unknown/Missing Value</v>
       </c>
       <c r="D225" s="56" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="E225" s="55" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G225" s="43"/>
       <c r="H225" s="40" t="str">
@@ -18504,7 +18516,7 @@
         <v>Z02</v>
       </c>
       <c r="T225" s="48" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="226" spans="1:20" ht="38.25" x14ac:dyDescent="0.25">
@@ -18513,10 +18525,10 @@
         <v>.....Z.03. - Code does not map</v>
       </c>
       <c r="D226" s="56" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="E226" s="55" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G226" s="43"/>
       <c r="H226" s="40" t="str">
@@ -18524,10 +18536,10 @@
         <v>Z03</v>
       </c>
       <c r="I226" s="16" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="T226" s="48" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="227" spans="1:20" x14ac:dyDescent="0.25">
@@ -18536,7 +18548,7 @@
         <v>Z. - Unknown/Missing Value</v>
       </c>
       <c r="D227" s="56" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="G227" s="43"/>
       <c r="H227" s="40" t="str">
@@ -18544,7 +18556,7 @@
         <v>Z</v>
       </c>
       <c r="T227" s="48" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="228" spans="1:20" x14ac:dyDescent="0.25">
@@ -18553,10 +18565,10 @@
         <v>.....D.99. - Other Chronic Conditions</v>
       </c>
       <c r="D228" s="56" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E228" s="55" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="G228" s="43"/>
       <c r="H228" s="40" t="str">
@@ -18564,7 +18576,7 @@
         <v>D99</v>
       </c>
       <c r="T228" s="48" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
   </sheetData>
@@ -18805,24 +18817,24 @@
   <sheetData>
     <row r="11" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="75" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="D11" s="76" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="E11" s="76" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="12" spans="3:5" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="77" t="s">
+        <v>1330</v>
+      </c>
+      <c r="D12" s="78" t="s">
         <v>1331</v>
       </c>
-      <c r="D12" s="78" t="s">
+      <c r="E12" s="78" t="s">
         <v>1332</v>
-      </c>
-      <c r="E12" s="78" t="s">
-        <v>1333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ICD-10-CM codes for respiratory infections and maternal conditions to gbd.ICD.Map.xlsx
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/gbd.ICD.Map.xlsx
+++ b/myCBD/myInfo/gbd.ICD.Map.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\0.CBD\myCBD\myInfo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="10935"/>
   </bookViews>
@@ -14,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$A$1:$X$221</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +36,7 @@
     <author>Dauphine, David (CDPH-CHSI)</author>
   </authors>
   <commentList>
-    <comment ref="L1" authorId="0">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -55,7 +60,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C57" authorId="1">
+    <comment ref="C57" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -79,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P126" authorId="2">
+    <comment ref="P126" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -108,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2810" uniqueCount="1368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2830" uniqueCount="1381">
   <si>
     <t>I. Communicable, maternal, perinatal and nutritional conditions</t>
   </si>
@@ -4357,11 +4362,50 @@
   <si>
     <t>68</t>
   </si>
+  <si>
+    <t>J09-18, J20-22, P23</t>
+  </si>
+  <si>
+    <t>J09|J1|J2[0-2]|P23</t>
+  </si>
+  <si>
+    <t>O44.1-O46, O67, O72 (exclude O44.0)</t>
+  </si>
+  <si>
+    <t>O44.1-O46, O67, O72</t>
+  </si>
+  <si>
+    <t>O44.1|O4[5-6]|O67|O72</t>
+  </si>
+  <si>
+    <t>O44.1| O4[5-6]|O67|O72</t>
+  </si>
+  <si>
+    <t>For both mortality and CM codes, O44.0 is placenta previa specified as without hemorrhage, therefore needs to be excluded from hemorrhage definition</t>
+  </si>
+  <si>
+    <t>O10-16</t>
+  </si>
+  <si>
+    <t>For both mortality and CM codes, O12 is gestational edema and proteinuria without hypertension--therefore, should it be excluded from definition?</t>
+  </si>
+  <si>
+    <t>O00-O04, O07 (O05 and O06 aren't included as possible codes for CM)</t>
+  </si>
+  <si>
+    <t>O0[0-4]|O07</t>
+  </si>
+  <si>
+    <t>O20-O43, O47-O63, O68-O71, O73-O77, O87-O94, O98-O99</t>
+  </si>
+  <si>
+    <t>O2[0-9]|O3[0-9]|O4[0-3,7-9]|O5|O6[0-3,8-9]|O7[0-1,3-7]|O8[7-9]|O9[4,8-9]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###0.;###0."/>
   </numFmts>
@@ -5012,7 +5056,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5047,7 +5091,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5258,11 +5302,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X228"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B172" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E196" sqref="E196"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A49" sqref="A49"/>
+      <selection pane="topRight" activeCell="N62" sqref="N62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -8253,8 +8296,12 @@
       <c r="L53" s="80" t="s">
         <v>1341</v>
       </c>
-      <c r="M53" s="80"/>
-      <c r="N53" s="80"/>
+      <c r="M53" s="80" t="s">
+        <v>1368</v>
+      </c>
+      <c r="N53" s="80" t="s">
+        <v>1369</v>
+      </c>
       <c r="O53" s="59" t="s">
         <v>404</v>
       </c>
@@ -8313,6 +8360,12 @@
       <c r="L54" s="16" t="s">
         <v>365</v>
       </c>
+      <c r="M54" s="16" t="s">
+        <v>405</v>
+      </c>
+      <c r="N54" s="16" t="s">
+        <v>365</v>
+      </c>
       <c r="O54" s="59" t="s">
         <v>405</v>
       </c>
@@ -8371,6 +8424,12 @@
       <c r="L55" s="16" t="s">
         <v>366</v>
       </c>
+      <c r="M55" s="16" t="s">
+        <v>406</v>
+      </c>
+      <c r="N55" s="16" t="s">
+        <v>366</v>
+      </c>
       <c r="O55" s="59" t="s">
         <v>406</v>
       </c>
@@ -8460,7 +8519,7 @@
       </c>
       <c r="X56" s="2"/>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A57" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -8486,10 +8545,16 @@
       <c r="I57" s="5"/>
       <c r="J57" s="5"/>
       <c r="K57" s="5" t="s">
-        <v>408</v>
+        <v>1370</v>
       </c>
       <c r="L57" s="16" t="s">
-        <v>368</v>
+        <v>1373</v>
+      </c>
+      <c r="M57" s="16" t="s">
+        <v>1371</v>
+      </c>
+      <c r="N57" s="16" t="s">
+        <v>1372</v>
       </c>
       <c r="O57" s="59" t="s">
         <v>408</v>
@@ -8516,7 +8581,9 @@
       <c r="W57" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="X57" s="2"/>
+      <c r="X57" s="5" t="s">
+        <v>1374</v>
+      </c>
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58" s="44" t="str">
@@ -8549,6 +8616,12 @@
       <c r="L58" s="16" t="s">
         <v>369</v>
       </c>
+      <c r="M58" s="16" t="s">
+        <v>409</v>
+      </c>
+      <c r="N58" s="16" t="s">
+        <v>369</v>
+      </c>
       <c r="O58" s="59" t="s">
         <v>409</v>
       </c>
@@ -8576,7 +8649,7 @@
       </c>
       <c r="X58" s="2"/>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A59" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -8607,6 +8680,12 @@
       <c r="L59" s="16" t="s">
         <v>370</v>
       </c>
+      <c r="M59" s="16" t="s">
+        <v>1375</v>
+      </c>
+      <c r="N59" s="16" t="s">
+        <v>370</v>
+      </c>
       <c r="O59" s="59" t="s">
         <v>410</v>
       </c>
@@ -8632,7 +8711,9 @@
       <c r="W59" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="X59" s="2"/>
+      <c r="X59" s="5" t="s">
+        <v>1376</v>
+      </c>
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60" s="44" t="str">
@@ -8665,6 +8746,12 @@
       <c r="L60" s="16" t="s">
         <v>371</v>
       </c>
+      <c r="M60" s="16" t="s">
+        <v>411</v>
+      </c>
+      <c r="N60" s="16" t="s">
+        <v>371</v>
+      </c>
       <c r="O60" s="59" t="s">
         <v>411</v>
       </c>
@@ -8723,6 +8810,12 @@
       <c r="L61" s="16" t="s">
         <v>372</v>
       </c>
+      <c r="M61" s="16" t="s">
+        <v>1377</v>
+      </c>
+      <c r="N61" s="16" t="s">
+        <v>1378</v>
+      </c>
       <c r="O61" s="59" t="s">
         <v>412</v>
       </c>
@@ -8780,6 +8873,12 @@
       </c>
       <c r="L62" s="16" t="s">
         <v>373</v>
+      </c>
+      <c r="M62" s="16" t="s">
+        <v>1379</v>
+      </c>
+      <c r="N62" s="16" t="s">
+        <v>1380</v>
       </c>
       <c r="O62" s="59" t="s">
         <v>413</v>

</xml_diff>

<commit_message>
adding 3-year county data and assoicated organizing; starting to add "education" strata
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/gbd.ICD.Map.xlsx
+++ b/myCBD/myInfo/gbd.ICD.Map.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\0.CBD\myCBD\myInfo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0.CBD\myCBD\myInfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2830" uniqueCount="1381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2830" uniqueCount="1380">
   <si>
     <t>I. Communicable, maternal, perinatal and nutritional conditions</t>
   </si>
@@ -4394,9 +4394,6 @@
   </si>
   <si>
     <t>O2[0-9]|O3[0-9]|O4[0-3,7-9]|O5|O6[0-3,8-9]|O7[0-1,3-7]|O8[7-9]|O9[4,8-9]</t>
-  </si>
-  <si>
-    <t>O441| O4[5-6]|O67|O72</t>
   </si>
   <si>
     <t>O441|O4[5-6]|O67|O72</t>
@@ -5302,10 +5299,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection activeCell="A49" sqref="A49"/>
-      <selection pane="topRight" activeCell="M59" sqref="M59"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -8554,7 +8552,7 @@
         <v>1371</v>
       </c>
       <c r="N57" s="16" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="O57" s="59" t="s">
         <v>408</v>

</xml_diff>

<commit_message>
life table investigation AND work on seperating homicide and "legal intervention"
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/gbd.ICD.Map.xlsx
+++ b/myCBD/myInfo/gbd.ICD.Map.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0.CBD\myCBD\myInfo\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="10935"/>
   </bookViews>
@@ -17,9 +12,9 @@
     <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$A$1:$X$221</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$A$1:$X$223</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -36,7 +31,7 @@
     <author>Dauphine, David (CDPH-CHSI)</author>
   </authors>
   <commentList>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -60,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C57" authorId="1" shapeId="0">
+    <comment ref="C57" authorId="1">
       <text>
         <r>
           <rPr>
@@ -84,7 +79,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P126" authorId="2" shapeId="0">
+    <comment ref="P126" authorId="2">
       <text>
         <r>
           <rPr>
@@ -113,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2830" uniqueCount="1380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2841" uniqueCount="1385">
   <si>
     <t>I. Communicable, maternal, perinatal and nutritional conditions</t>
   </si>
@@ -3801,9 +3796,6 @@
   </si>
   <si>
     <t>U03[1,9]|X[6-7]|X8[0-4]|Y870</t>
-  </si>
-  <si>
-    <t>U010-U019, U02, X85-Y09, Y350-354, Y356-Y357, Y871, Y890</t>
   </si>
   <si>
     <t>Sudden infant death syndrome</t>
@@ -3906,15 +3898,6 @@
     <t>Change name to something like "War and Legal Executions" or "War and Capital Punishment" based on CDPH changes?</t>
   </si>
   <si>
-    <t>Y35[5,8-9]|Y36|Y891</t>
-  </si>
-  <si>
-    <t>Y355, Y358-Y359, Y36, Y891</t>
-  </si>
-  <si>
-    <t>U01[0-9]|U02|X8[5-9]|X9|Y0|Y35[0-4,6-7]|Y871|Y890</t>
-  </si>
-  <si>
     <t>C18-C21, D010-D013, D120-D122, D125-D126, D128-D129, D373-D375</t>
   </si>
   <si>
@@ -4111,12 +4094,6 @@
   </si>
   <si>
     <t>Added U031, U039 (terrorism)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Added Y350-4, 356-7, 890 (officer-involved shootings etc. from war/legal interventions to homicides) and U010-U019, U02 (terrorism) per CDPH. See 4oct2018 email regarding recommendation to Added Y358-9 (other and unspecified officer-involved deaths) to be consistent with CDPH-recommended for legal interventions. </t>
-  </si>
-  <si>
-    <t>Added Y891 (sequelae of war operations) per IHME, move Y890 (officer-involved killings) to homicides rather than here per CDPH</t>
   </si>
   <si>
     <t>Moved P043 to alcohol and P044 to drug use disorders.</t>
@@ -4398,11 +4375,50 @@
   <si>
     <t>O441|O4[5-6]|O67|O72</t>
   </si>
+  <si>
+    <t>Legal intervention</t>
+  </si>
+  <si>
+    <t>Homicide excluding legal intervention</t>
+  </si>
+  <si>
+    <t>Added Y350-4, 356-7, 890 (officer-involved shootings etc. from war/legal interventions to homicides) and U010-U019, U02 (terrorism) per CDPH. See 4oct2018 email regarding recommendation to Added Y358-9 (other and unspecified officer-involved deaths) to be consistent with CDPH-recommended for legal interventions. 
+exploring seperating "legal intervention" from other homicide
+for "210" row 223, TEMP change of E from 99 to 03, and make F c</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Y350-354, Y356-Y357, Y358-Y359,Y890</t>
+  </si>
+  <si>
+    <t>U010-U019, U02, X85-Y09, Y871</t>
+  </si>
+  <si>
+    <t>Y355,  Y36, Y891, Y38, y899</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added Y891 (sequelae of war operations) per IHME, move Y890 (officer-involved killings) to homicides rather than here per CDPH
+Y35.5 - execution
+Y36, Y37, Y89.1 - war/military
+Y38 - terrorism
+</t>
+  </si>
+  <si>
+    <t>Y355|Y36|Y37|Y891|Y38</t>
+  </si>
+  <si>
+    <t>U01[0-9]|U02|X8[5-9]|X9|Y0|Y871</t>
+  </si>
+  <si>
+    <t>Y35[0-4]|Y35[6-9]|Y890</t>
+  </si>
+  <si>
+    <t>Execution, War, Terroism</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###0.;###0."/>
   </numFmts>
@@ -5053,7 +5069,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5088,7 +5104,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5297,13 +5313,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X228"/>
+  <dimension ref="A1:X230"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="T218" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A57" sqref="A57"/>
+      <selection pane="bottomRight" activeCell="T223" sqref="T223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -5359,10 +5375,10 @@
         <v>1124</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>1321</v>
+        <v>1315</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>1267</v>
+        <v>1263</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>384</v>
@@ -5371,10 +5387,10 @@
         <v>759</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>1346</v>
+        <v>1340</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>1347</v>
+        <v>1341</v>
       </c>
       <c r="O1" s="59" t="s">
         <v>1162</v>
@@ -8161,16 +8177,16 @@
       </c>
       <c r="H51" s="40"/>
       <c r="I51" s="5" t="s">
-        <v>1287</v>
+        <v>1283</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="K51" s="5" t="s">
+        <v>1232</v>
+      </c>
+      <c r="L51" s="19" t="s">
         <v>1233</v>
-      </c>
-      <c r="L51" s="19" t="s">
-        <v>1234</v>
       </c>
       <c r="M51" s="19"/>
       <c r="N51" s="19"/>
@@ -8200,7 +8216,7 @@
         <v>880</v>
       </c>
       <c r="X51" s="5" t="s">
-        <v>1320</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="52" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
@@ -8292,13 +8308,13 @@
         <v>404</v>
       </c>
       <c r="L53" s="80" t="s">
-        <v>1341</v>
+        <v>1335</v>
       </c>
       <c r="M53" s="80" t="s">
-        <v>1368</v>
+        <v>1362</v>
       </c>
       <c r="N53" s="80" t="s">
-        <v>1369</v>
+        <v>1363</v>
       </c>
       <c r="O53" s="59" t="s">
         <v>404</v>
@@ -8543,16 +8559,16 @@
       <c r="I57" s="5"/>
       <c r="J57" s="5"/>
       <c r="K57" s="5" t="s">
-        <v>1370</v>
+        <v>1364</v>
       </c>
       <c r="L57" s="16" t="s">
-        <v>1379</v>
+        <v>1373</v>
       </c>
       <c r="M57" s="16" t="s">
-        <v>1371</v>
+        <v>1365</v>
       </c>
       <c r="N57" s="16" t="s">
-        <v>1379</v>
+        <v>1373</v>
       </c>
       <c r="O57" s="59" t="s">
         <v>408</v>
@@ -8580,7 +8596,7 @@
         <v>33</v>
       </c>
       <c r="X57" s="5" t="s">
-        <v>1372</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.25">
@@ -8679,7 +8695,7 @@
         <v>370</v>
       </c>
       <c r="M59" s="16" t="s">
-        <v>1373</v>
+        <v>1367</v>
       </c>
       <c r="N59" s="16" t="s">
         <v>370</v>
@@ -8710,7 +8726,7 @@
         <v>35</v>
       </c>
       <c r="X59" s="5" t="s">
-        <v>1374</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.25">
@@ -8809,10 +8825,10 @@
         <v>372</v>
       </c>
       <c r="M61" s="16" t="s">
-        <v>1375</v>
+        <v>1369</v>
       </c>
       <c r="N61" s="16" t="s">
-        <v>1376</v>
+        <v>1370</v>
       </c>
       <c r="O61" s="59" t="s">
         <v>412</v>
@@ -8873,10 +8889,10 @@
         <v>373</v>
       </c>
       <c r="M62" s="16" t="s">
-        <v>1377</v>
+        <v>1371</v>
       </c>
       <c r="N62" s="16" t="s">
-        <v>1378</v>
+        <v>1372</v>
       </c>
       <c r="O62" s="59" t="s">
         <v>413</v>
@@ -9165,7 +9181,7 @@
       </c>
       <c r="H67" s="40"/>
       <c r="I67" s="5" t="s">
-        <v>1315</v>
+        <v>1309</v>
       </c>
       <c r="J67" s="5" t="s">
         <v>1161</v>
@@ -9174,7 +9190,7 @@
         <v>1166</v>
       </c>
       <c r="L67" s="19" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="M67" s="19"/>
       <c r="N67" s="19"/>
@@ -9289,7 +9305,7 @@
         <v>420</v>
       </c>
       <c r="L69" s="16" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="O69" s="59" t="s">
         <v>420</v>
@@ -9580,7 +9596,7 @@
       </c>
       <c r="Q74" s="59"/>
       <c r="R74" s="60" t="s">
-        <v>1325</v>
+        <v>1319</v>
       </c>
       <c r="S74" s="59" t="s">
         <v>557</v>
@@ -9682,7 +9698,7 @@
         <v>558</v>
       </c>
       <c r="T76" s="2" t="s">
-        <v>1284</v>
+        <v>1280</v>
       </c>
       <c r="U76" s="20" t="s">
         <v>51</v>
@@ -9724,10 +9740,10 @@
       <c r="I77" s="5"/>
       <c r="J77" s="5"/>
       <c r="K77" s="5" t="s">
-        <v>1273</v>
+        <v>1269</v>
       </c>
       <c r="L77" s="49" t="s">
-        <v>1273</v>
+        <v>1269</v>
       </c>
       <c r="M77" s="49"/>
       <c r="N77" s="49"/>
@@ -9778,16 +9794,16 @@
       </c>
       <c r="H78" s="40"/>
       <c r="I78" s="18" t="s">
-        <v>1288</v>
+        <v>1284</v>
       </c>
       <c r="J78" s="17" t="s">
         <v>1161</v>
       </c>
       <c r="K78" s="5" t="s">
-        <v>1274</v>
+        <v>1270</v>
       </c>
       <c r="L78" s="19" t="s">
-        <v>1275</v>
+        <v>1271</v>
       </c>
       <c r="M78" s="19"/>
       <c r="N78" s="19"/>
@@ -9842,7 +9858,7 @@
       </c>
       <c r="H79" s="40"/>
       <c r="I79" s="19" t="s">
-        <v>1289</v>
+        <v>1285</v>
       </c>
       <c r="J79" s="17" t="s">
         <v>1161</v>
@@ -9969,7 +9985,7 @@
         <v>B02</v>
       </c>
       <c r="I81" s="18" t="s">
-        <v>1290</v>
+        <v>1286</v>
       </c>
       <c r="J81" s="17" t="s">
         <v>1161</v>
@@ -10036,7 +10052,7 @@
         <v>B03</v>
       </c>
       <c r="I82" s="18" t="s">
-        <v>1291</v>
+        <v>1287</v>
       </c>
       <c r="J82" s="17" t="s">
         <v>1161</v>
@@ -10105,16 +10121,16 @@
         <v>B04</v>
       </c>
       <c r="I83" s="16" t="s">
-        <v>1292</v>
+        <v>1288</v>
       </c>
       <c r="J83" s="17" t="s">
         <v>1161</v>
       </c>
       <c r="K83" s="5" t="s">
-        <v>1247</v>
+        <v>1243</v>
       </c>
       <c r="L83" s="49" t="s">
-        <v>1248</v>
+        <v>1244</v>
       </c>
       <c r="M83" s="49"/>
       <c r="N83" s="49"/>
@@ -10172,7 +10188,7 @@
         <v>B05</v>
       </c>
       <c r="I84" s="18" t="s">
-        <v>1293</v>
+        <v>1289</v>
       </c>
       <c r="J84" s="17" t="s">
         <v>1161</v>
@@ -10239,7 +10255,7 @@
         <v>B06</v>
       </c>
       <c r="I85" s="18" t="s">
-        <v>1294</v>
+        <v>1290</v>
       </c>
       <c r="J85" s="17" t="s">
         <v>1161</v>
@@ -10306,7 +10322,7 @@
         <v>B07</v>
       </c>
       <c r="I86" s="18" t="s">
-        <v>1295</v>
+        <v>1291</v>
       </c>
       <c r="J86" s="17" t="s">
         <v>1161</v>
@@ -10429,16 +10445,16 @@
       </c>
       <c r="H88" s="40"/>
       <c r="I88" s="18" t="s">
-        <v>1296</v>
+        <v>1292</v>
       </c>
       <c r="J88" s="17" t="s">
         <v>1161</v>
       </c>
       <c r="K88" s="5" t="s">
-        <v>1251</v>
+        <v>1247</v>
       </c>
       <c r="L88" s="49" t="s">
-        <v>1252</v>
+        <v>1248</v>
       </c>
       <c r="M88" s="49"/>
       <c r="N88" s="49"/>
@@ -10493,16 +10509,16 @@
       </c>
       <c r="H89" s="40"/>
       <c r="I89" s="18" t="s">
-        <v>1297</v>
+        <v>1293</v>
       </c>
       <c r="J89" s="17" t="s">
         <v>1161</v>
       </c>
       <c r="K89" s="5" t="s">
-        <v>1253</v>
+        <v>1249</v>
       </c>
       <c r="L89" s="49" t="s">
-        <v>1254</v>
+        <v>1250</v>
       </c>
       <c r="M89" s="49"/>
       <c r="N89" s="49"/>
@@ -10560,7 +10576,7 @@
         <v>B09</v>
       </c>
       <c r="I90" s="16" t="s">
-        <v>1298</v>
+        <v>1294</v>
       </c>
       <c r="J90" s="17" t="s">
         <v>1161</v>
@@ -10607,7 +10623,7 @@
       </c>
       <c r="B91" s="2"/>
       <c r="C91" s="37" t="s">
-        <v>1277</v>
+        <v>1273</v>
       </c>
       <c r="D91" s="6" t="s">
         <v>1139</v>
@@ -10634,11 +10650,11 @@
       <c r="R91" s="59"/>
       <c r="S91" s="59"/>
       <c r="T91" s="5" t="s">
-        <v>1276</v>
+        <v>1272</v>
       </c>
       <c r="U91" s="20"/>
       <c r="V91" s="5" t="s">
-        <v>1276</v>
+        <v>1272</v>
       </c>
       <c r="W91" s="45"/>
       <c r="X91" s="2"/>
@@ -10667,7 +10683,7 @@
       </c>
       <c r="H92" s="40"/>
       <c r="I92" s="5" t="s">
-        <v>1299</v>
+        <v>1295</v>
       </c>
       <c r="J92" s="17" t="s">
         <v>1161</v>
@@ -10731,16 +10747,16 @@
       </c>
       <c r="H93" s="40"/>
       <c r="I93" s="5" t="s">
-        <v>1300</v>
+        <v>1296</v>
       </c>
       <c r="J93" s="17" t="s">
         <v>1161</v>
       </c>
       <c r="K93" s="5" t="s">
-        <v>1255</v>
+        <v>1251</v>
       </c>
       <c r="L93" s="49" t="s">
-        <v>1270</v>
+        <v>1266</v>
       </c>
       <c r="M93" s="49"/>
       <c r="N93" s="49"/>
@@ -10798,7 +10814,7 @@
         <v>B11</v>
       </c>
       <c r="I94" s="5" t="s">
-        <v>1301</v>
+        <v>1297</v>
       </c>
       <c r="J94" s="17" t="s">
         <v>1161</v>
@@ -10865,7 +10881,7 @@
         <v>B12</v>
       </c>
       <c r="I95" s="19" t="s">
-        <v>1302</v>
+        <v>1298</v>
       </c>
       <c r="J95" s="17" t="s">
         <v>1161</v>
@@ -10929,7 +10945,7 @@
       </c>
       <c r="H96" s="40"/>
       <c r="I96" s="19" t="s">
-        <v>1303</v>
+        <v>1299</v>
       </c>
       <c r="J96" s="17" t="s">
         <v>1161</v>
@@ -10996,7 +11012,7 @@
         <v>B13</v>
       </c>
       <c r="I97" s="19" t="s">
-        <v>1304</v>
+        <v>1300</v>
       </c>
       <c r="J97" s="17" t="s">
         <v>1161</v>
@@ -11063,16 +11079,16 @@
         <v>B14</v>
       </c>
       <c r="I98" s="5" t="s">
-        <v>1305</v>
+        <v>1301</v>
       </c>
       <c r="J98" s="17" t="s">
         <v>1161</v>
       </c>
       <c r="K98" s="5" t="s">
-        <v>1256</v>
+        <v>1252</v>
       </c>
       <c r="L98" s="49" t="s">
-        <v>1257</v>
+        <v>1253</v>
       </c>
       <c r="M98" s="49"/>
       <c r="N98" s="49"/>
@@ -11130,7 +11146,7 @@
         <v>B15</v>
       </c>
       <c r="I99" s="16" t="s">
-        <v>1306</v>
+        <v>1302</v>
       </c>
       <c r="J99" s="17" t="s">
         <v>1161</v>
@@ -11194,7 +11210,7 @@
       </c>
       <c r="H100" s="40"/>
       <c r="I100" s="19" t="s">
-        <v>1307</v>
+        <v>1303</v>
       </c>
       <c r="J100" s="17" t="s">
         <v>1161</v>
@@ -11258,7 +11274,7 @@
       </c>
       <c r="H101" s="40"/>
       <c r="I101" s="19" t="s">
-        <v>1308</v>
+        <v>1304</v>
       </c>
       <c r="J101" s="17" t="s">
         <v>1161</v>
@@ -11322,7 +11338,7 @@
       </c>
       <c r="H102" s="40"/>
       <c r="I102" s="19" t="s">
-        <v>1309</v>
+        <v>1305</v>
       </c>
       <c r="J102" s="17" t="s">
         <v>1161</v>
@@ -11767,7 +11783,7 @@
         <v>B99</v>
       </c>
       <c r="I109" s="5" t="s">
-        <v>1310</v>
+        <v>1306</v>
       </c>
       <c r="J109" s="5" t="s">
         <v>1161</v>
@@ -11827,10 +11843,10 @@
       </c>
       <c r="H110" s="40"/>
       <c r="K110" s="5" t="s">
-        <v>1272</v>
+        <v>1268</v>
       </c>
       <c r="L110" s="5" t="s">
-        <v>1271</v>
+        <v>1267</v>
       </c>
       <c r="M110" s="5"/>
       <c r="N110" s="5"/>
@@ -11888,22 +11904,22 @@
         <v>D01</v>
       </c>
       <c r="I111" s="5" t="s">
-        <v>1311</v>
+        <v>1307</v>
       </c>
       <c r="J111" s="5" t="s">
         <v>1161</v>
       </c>
       <c r="K111" s="5" t="s">
-        <v>1258</v>
+        <v>1254</v>
       </c>
       <c r="L111" s="49" t="s">
-        <v>1345</v>
+        <v>1339</v>
       </c>
       <c r="M111" s="49" t="s">
-        <v>1350</v>
+        <v>1344</v>
       </c>
       <c r="N111" s="49" t="s">
-        <v>1348</v>
+        <v>1342</v>
       </c>
       <c r="O111" s="59" t="s">
         <v>975</v>
@@ -11931,7 +11947,7 @@
         <v>66</v>
       </c>
       <c r="X111" s="2" t="s">
-        <v>1349</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="112" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
@@ -11962,18 +11978,18 @@
       <c r="I112" s="5"/>
       <c r="J112" s="5"/>
       <c r="K112" s="5" t="s">
-        <v>1316</v>
+        <v>1310</v>
       </c>
       <c r="L112" s="19" t="s">
-        <v>1317</v>
+        <v>1311</v>
       </c>
       <c r="M112" s="19"/>
       <c r="N112" s="19"/>
       <c r="O112" s="59" t="s">
-        <v>1316</v>
+        <v>1310</v>
       </c>
       <c r="P112" s="66" t="s">
-        <v>1317</v>
+        <v>1311</v>
       </c>
       <c r="Q112" s="69"/>
       <c r="R112" s="59" t="s">
@@ -12302,7 +12318,7 @@
       </c>
       <c r="B118" s="2"/>
       <c r="C118" s="32" t="s">
-        <v>1360</v>
+        <v>1354</v>
       </c>
       <c r="D118" s="6" t="s">
         <v>1142</v>
@@ -12330,11 +12346,11 @@
       <c r="R118" s="59"/>
       <c r="S118" s="59"/>
       <c r="T118" s="2" t="s">
-        <v>1362</v>
+        <v>1356</v>
       </c>
       <c r="U118" s="20"/>
       <c r="V118" s="2" t="s">
-        <v>1361</v>
+        <v>1355</v>
       </c>
       <c r="W118" s="45"/>
       <c r="X118" s="2"/>
@@ -12372,7 +12388,7 @@
       <c r="R119" s="59"/>
       <c r="S119" s="59"/>
       <c r="T119" s="2" t="s">
-        <v>1363</v>
+        <v>1357</v>
       </c>
       <c r="U119" s="20"/>
       <c r="V119" s="2" t="s">
@@ -12670,13 +12686,13 @@
         <v>443</v>
       </c>
       <c r="L125" s="49" t="s">
-        <v>1351</v>
+        <v>1345</v>
       </c>
       <c r="M125" s="49" t="s">
         <v>443</v>
       </c>
       <c r="N125" s="49" t="s">
-        <v>1351</v>
+        <v>1345</v>
       </c>
       <c r="O125" s="59" t="s">
         <v>443</v>
@@ -12734,24 +12750,24 @@
         <v>D04a</v>
       </c>
       <c r="I126" s="5" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="J126" s="5" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="K126" s="5" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="L126" s="19" t="s">
-        <v>1268</v>
+        <v>1264</v>
       </c>
       <c r="M126" s="19"/>
       <c r="N126" s="19"/>
       <c r="O126" s="59" t="s">
-        <v>1326</v>
+        <v>1320</v>
       </c>
       <c r="P126" s="66" t="s">
-        <v>1269</v>
+        <v>1265</v>
       </c>
       <c r="Q126" s="69"/>
       <c r="R126" s="59" t="s">
@@ -13101,7 +13117,7 @@
       </c>
       <c r="H132" s="40"/>
       <c r="I132" s="5" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="J132" s="5" t="s">
         <v>1161</v>
@@ -13110,7 +13126,7 @@
         <v>1167</v>
       </c>
       <c r="L132" s="19" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="M132" s="19"/>
       <c r="N132" s="19"/>
@@ -13140,7 +13156,7 @@
         <v>728</v>
       </c>
       <c r="X132" s="2" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="133" spans="1:24" x14ac:dyDescent="0.25">
@@ -14029,7 +14045,7 @@
         <v>D06</v>
       </c>
       <c r="I148" s="57" t="s">
-        <v>1324</v>
+        <v>1318</v>
       </c>
       <c r="J148" s="18" t="s">
         <v>1161</v>
@@ -14038,7 +14054,7 @@
         <v>1202</v>
       </c>
       <c r="L148" s="58" t="s">
-        <v>1323</v>
+        <v>1317</v>
       </c>
       <c r="M148" s="58"/>
       <c r="N148" s="58"/>
@@ -14377,7 +14393,7 @@
         <v>460</v>
       </c>
       <c r="L154" s="49" t="s">
-        <v>1259</v>
+        <v>1255</v>
       </c>
       <c r="M154" s="49"/>
       <c r="N154" s="49"/>
@@ -14611,7 +14627,7 @@
         <v>464</v>
       </c>
       <c r="N158" s="49" t="s">
-        <v>1354</v>
+        <v>1348</v>
       </c>
       <c r="O158" s="59" t="s">
         <v>464</v>
@@ -14801,22 +14817,22 @@
         <v>C03</v>
       </c>
       <c r="I161" s="5" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="J161" s="5" t="s">
         <v>1161</v>
       </c>
       <c r="K161" s="5" t="s">
+        <v>1228</v>
+      </c>
+      <c r="L161" s="49" t="s">
         <v>1229</v>
       </c>
-      <c r="L161" s="49" t="s">
-        <v>1230</v>
-      </c>
       <c r="M161" s="49" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="N161" s="49" t="s">
-        <v>1355</v>
+        <v>1349</v>
       </c>
       <c r="O161" s="59" t="s">
         <v>467</v>
@@ -14880,10 +14896,10 @@
         <v>830</v>
       </c>
       <c r="M162" s="49" t="s">
-        <v>1352</v>
+        <v>1346</v>
       </c>
       <c r="N162" s="49" t="s">
-        <v>1353</v>
+        <v>1347</v>
       </c>
       <c r="O162" s="59" t="s">
         <v>468</v>
@@ -14911,7 +14927,7 @@
         <v>98</v>
       </c>
       <c r="X162" s="81" t="s">
-        <v>1359</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="163" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
@@ -14937,22 +14953,22 @@
         <v>C05</v>
       </c>
       <c r="I163" s="5" t="s">
-        <v>1334</v>
+        <v>1328</v>
       </c>
       <c r="J163" s="5" t="s">
         <v>1214</v>
       </c>
       <c r="K163" s="5" t="s">
-        <v>1328</v>
+        <v>1322</v>
       </c>
       <c r="L163" s="49" t="s">
-        <v>1328</v>
+        <v>1322</v>
       </c>
       <c r="M163" s="49" t="s">
-        <v>1328</v>
+        <v>1322</v>
       </c>
       <c r="N163" s="49" t="s">
-        <v>1328</v>
+        <v>1322</v>
       </c>
       <c r="O163" s="59"/>
       <c r="P163" s="68"/>
@@ -14960,7 +14976,7 @@
       <c r="R163" s="59"/>
       <c r="S163" s="59"/>
       <c r="T163" s="5" t="s">
-        <v>1339</v>
+        <v>1333</v>
       </c>
       <c r="U163" s="50"/>
       <c r="V163" s="5"/>
@@ -14994,22 +15010,22 @@
         <v>C99</v>
       </c>
       <c r="I164" s="5" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="J164" s="5" t="s">
-        <v>1336</v>
+        <v>1330</v>
       </c>
       <c r="K164" s="5" t="s">
-        <v>1337</v>
+        <v>1331</v>
       </c>
       <c r="L164" s="19" t="s">
-        <v>1338</v>
+        <v>1332</v>
       </c>
       <c r="M164" s="19" t="s">
-        <v>1357</v>
+        <v>1351</v>
       </c>
       <c r="N164" s="19" t="s">
-        <v>1358</v>
+        <v>1352</v>
       </c>
       <c r="O164" s="59" t="s">
         <v>469</v>
@@ -15025,7 +15041,7 @@
         <v>1102</v>
       </c>
       <c r="T164" s="79" t="s">
-        <v>1333</v>
+        <v>1327</v>
       </c>
       <c r="U164" s="52" t="s">
         <v>99</v>
@@ -15037,7 +15053,7 @@
         <v>99</v>
       </c>
       <c r="X164" s="81" t="s">
-        <v>1356</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="165" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
@@ -15112,7 +15128,7 @@
         <v>1142</v>
       </c>
       <c r="E166" s="83" t="s">
-        <v>1365</v>
+        <v>1359</v>
       </c>
       <c r="F166" s="6"/>
       <c r="G166" s="40" t="str">
@@ -15175,7 +15191,7 @@
         <v>1142</v>
       </c>
       <c r="E167" s="83" t="s">
-        <v>1366</v>
+        <v>1360</v>
       </c>
       <c r="F167" s="6"/>
       <c r="G167" s="40" t="str">
@@ -15232,13 +15248,13 @@
         <v>157</v>
       </c>
       <c r="C168" s="31" t="s">
-        <v>1364</v>
+        <v>1358</v>
       </c>
       <c r="D168" s="27" t="s">
         <v>1142</v>
       </c>
       <c r="E168" s="83" t="s">
-        <v>1367</v>
+        <v>1361</v>
       </c>
       <c r="F168" s="6"/>
       <c r="G168" s="40" t="str">
@@ -15335,10 +15351,10 @@
         <v>682</v>
       </c>
       <c r="T169" s="81" t="s">
-        <v>1342</v>
+        <v>1336</v>
       </c>
       <c r="U169" s="20" t="s">
-        <v>1343</v>
+        <v>1337</v>
       </c>
       <c r="V169" s="2" t="s">
         <v>281</v>
@@ -15435,7 +15451,7 @@
         <v>D11</v>
       </c>
       <c r="I171" s="16" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="J171" s="5" t="s">
         <v>1161</v>
@@ -16854,7 +16870,7 @@
     </row>
     <row r="195" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A195" s="44" t="str">
-        <f t="shared" ref="A195:A221" si="18">IF(H195&lt;&gt;"",IF(F195&lt;&gt;"",CONCATENATE("..........",D195,".",E195,".",F195,". - ",T195),IF(E195&lt;&gt;"",CONCATENATE(".....",D195,".",E195,". - ",T195),CONCATENATE(D195,". - ",T195))),"")</f>
+        <f t="shared" ref="A195:A223" si="18">IF(H195&lt;&gt;"",IF(F195&lt;&gt;"",CONCATENATE("..........",D195,".",E195,".",F195,". - ",T195),IF(E195&lt;&gt;"",CONCATENATE(".....",D195,".",E195,". - ",T195),CONCATENATE(D195,". - ",T195))),"")</f>
         <v/>
       </c>
       <c r="B195" s="2">
@@ -16876,10 +16892,10 @@
       </c>
       <c r="H195" s="40"/>
       <c r="I195" s="5" t="s">
-        <v>1319</v>
+        <v>1313</v>
       </c>
       <c r="J195" s="5" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="K195" s="5" t="s">
         <v>1200</v>
@@ -17654,7 +17670,7 @@
       </c>
       <c r="Q208" s="66"/>
       <c r="R208" s="60" t="s">
-        <v>1327</v>
+        <v>1321</v>
       </c>
       <c r="S208" s="59" t="s">
         <v>654</v>
@@ -17762,7 +17778,7 @@
         <v>E01a</v>
       </c>
       <c r="I210" s="5" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="J210" s="5" t="s">
         <v>1161</v>
@@ -18139,7 +18155,7 @@
       </c>
       <c r="H216" s="40"/>
       <c r="I216" s="5" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="J216" s="5" t="s">
         <v>1161</v>
@@ -18204,16 +18220,16 @@
         <v>E01x</v>
       </c>
       <c r="I217" s="5" t="s">
-        <v>1265</v>
+        <v>1261</v>
       </c>
       <c r="J217" s="5" t="s">
-        <v>1262</v>
+        <v>1258</v>
       </c>
       <c r="K217" s="5" t="s">
-        <v>1263</v>
+        <v>1259</v>
       </c>
       <c r="L217" s="49" t="s">
-        <v>1264</v>
+        <v>1260</v>
       </c>
       <c r="M217" s="49"/>
       <c r="N217" s="49"/>
@@ -18243,7 +18259,7 @@
         <v>887</v>
       </c>
       <c r="X217" s="22" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="218" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
@@ -18318,7 +18334,7 @@
       </c>
       <c r="F219" s="6"/>
       <c r="G219" s="40" t="str">
-        <f t="shared" ref="G219:G224" si="21">CONCATENATE("c",D219,E219,F219)</f>
+        <f t="shared" ref="G219:G226" si="21">CONCATENATE("c",D219,E219,F219)</f>
         <v>cE02</v>
       </c>
       <c r="H219" s="40" t="str">
@@ -18326,7 +18342,7 @@
         <v>E02</v>
       </c>
       <c r="I219" s="5" t="s">
-        <v>1312</v>
+        <v>1308</v>
       </c>
       <c r="J219" s="5" t="s">
         <v>1214</v>
@@ -18353,7 +18369,7 @@
         <v>999</v>
       </c>
       <c r="T219" s="5" t="s">
-        <v>1283</v>
+        <v>1279</v>
       </c>
       <c r="U219" s="20" t="s">
         <v>140</v>
@@ -18366,7 +18382,7 @@
       </c>
       <c r="X219" s="2"/>
     </row>
-    <row r="220" spans="1:24" ht="140.25" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:24" ht="229.5" x14ac:dyDescent="0.25">
       <c r="A220" s="44" t="str">
         <f t="shared" si="18"/>
         <v>.....E.03. - Homicide/Interpersonal violence</v>
@@ -18393,16 +18409,10 @@
         <v>E03</v>
       </c>
       <c r="I220" s="5" t="s">
-        <v>1313</v>
+        <v>1376</v>
       </c>
       <c r="J220" s="5" t="s">
         <v>1214</v>
-      </c>
-      <c r="K220" s="5" t="s">
-        <v>1217</v>
-      </c>
-      <c r="L220" s="19" t="s">
-        <v>1246</v>
       </c>
       <c r="M220" s="19"/>
       <c r="N220" s="19"/>
@@ -18420,7 +18430,7 @@
         <v>998</v>
       </c>
       <c r="T220" s="5" t="s">
-        <v>1282</v>
+        <v>1278</v>
       </c>
       <c r="U220" s="20" t="s">
         <v>141</v>
@@ -18433,251 +18443,350 @@
       </c>
       <c r="X220" s="2"/>
     </row>
-    <row r="221" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A221" s="44" t="str">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="B221" s="2">
-        <v>210</v>
-      </c>
-      <c r="C221" s="31" t="s">
-        <v>142</v>
-      </c>
+        <v>..........E.03.a. - Homicide excluding legal intervention</v>
+      </c>
+      <c r="B221" s="2"/>
+      <c r="C221" s="31"/>
       <c r="D221" s="6" t="s">
         <v>1143</v>
       </c>
       <c r="E221" s="26" t="s">
-        <v>1228</v>
-      </c>
-      <c r="F221" s="6"/>
+        <v>1146</v>
+      </c>
+      <c r="F221" s="6" t="s">
+        <v>1126</v>
+      </c>
       <c r="G221" s="40" t="str">
         <f t="shared" si="21"/>
-        <v>cE99</v>
-      </c>
-      <c r="H221" s="40"/>
-      <c r="I221" s="5" t="s">
-        <v>1314</v>
-      </c>
-      <c r="J221" s="5" t="s">
-        <v>1242</v>
-      </c>
+        <v>cE03a</v>
+      </c>
+      <c r="H221" s="40" t="str">
+        <f t="shared" ref="H221:H223" si="22">CONCATENATE(D221,E221,F221)</f>
+        <v>E03a</v>
+      </c>
+      <c r="I221" s="5"/>
+      <c r="J221" s="5"/>
       <c r="K221" s="5" t="s">
-        <v>1245</v>
-      </c>
-      <c r="L221" s="49" t="s">
-        <v>1244</v>
-      </c>
-      <c r="M221" s="49"/>
-      <c r="N221" s="49"/>
-      <c r="O221" s="59" t="s">
-        <v>508</v>
-      </c>
-      <c r="P221" s="68" t="s">
-        <v>877</v>
-      </c>
+        <v>1378</v>
+      </c>
+      <c r="L221" s="19" t="s">
+        <v>1382</v>
+      </c>
+      <c r="M221" s="19"/>
+      <c r="N221" s="19"/>
+      <c r="O221" s="59"/>
+      <c r="P221" s="68"/>
       <c r="Q221" s="69"/>
       <c r="R221" s="59"/>
       <c r="S221" s="59"/>
-      <c r="T221" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="U221" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="V221" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="W221" s="45" t="s">
-        <v>142</v>
-      </c>
-      <c r="X221" s="22" t="s">
-        <v>1243</v>
-      </c>
-    </row>
-    <row r="222" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B222" s="82" t="s">
-        <v>1344</v>
-      </c>
-      <c r="C222" s="16" t="s">
-        <v>1285</v>
-      </c>
-      <c r="D222" s="54" t="s">
+      <c r="T221" s="20" t="s">
+        <v>1375</v>
+      </c>
+      <c r="U221" s="46"/>
+      <c r="V221" s="5"/>
+      <c r="W221" s="45"/>
+      <c r="X221" s="2"/>
+    </row>
+    <row r="222" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A222" s="44" t="str">
+        <f t="shared" si="18"/>
+        <v>..........E.03.b. - Legal intervention</v>
+      </c>
+      <c r="B222" s="2"/>
+      <c r="C222" s="31"/>
+      <c r="D222" s="6" t="s">
         <v>1143</v>
       </c>
-      <c r="E222" s="55" t="s">
-        <v>1144</v>
+      <c r="E222" s="26" t="s">
+        <v>1146</v>
+      </c>
+      <c r="F222" s="6" t="s">
+        <v>1127</v>
       </c>
       <c r="G222" s="40" t="str">
         <f t="shared" si="21"/>
-        <v>cE01</v>
-      </c>
-      <c r="H222" s="40"/>
-      <c r="I222" s="48" t="s">
-        <v>1261</v>
-      </c>
-      <c r="J222" s="48" t="s">
-        <v>1278</v>
-      </c>
-      <c r="K222" s="16" t="s">
-        <v>1279</v>
-      </c>
-      <c r="L222" s="16" t="s">
-        <v>1280</v>
-      </c>
-      <c r="T222" s="48" t="s">
-        <v>1222</v>
-      </c>
-    </row>
-    <row r="223" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+        <v>cE03b</v>
+      </c>
+      <c r="H222" s="40" t="str">
+        <f t="shared" si="22"/>
+        <v>E03b</v>
+      </c>
+      <c r="I222" s="5"/>
+      <c r="J222" s="5"/>
+      <c r="K222" s="5" t="s">
+        <v>1377</v>
+      </c>
+      <c r="L222" s="19" t="s">
+        <v>1383</v>
+      </c>
+      <c r="M222" s="19"/>
+      <c r="N222" s="19"/>
+      <c r="O222" s="59"/>
+      <c r="P222" s="68"/>
+      <c r="Q222" s="69"/>
+      <c r="R222" s="59"/>
+      <c r="S222" s="59"/>
+      <c r="T222" s="20" t="s">
+        <v>1374</v>
+      </c>
+      <c r="U222" s="46"/>
+      <c r="V222" s="5"/>
+      <c r="W222" s="45"/>
+      <c r="X222" s="2"/>
+    </row>
+    <row r="223" spans="1:24" ht="153" x14ac:dyDescent="0.25">
       <c r="A223" s="44" t="str">
-        <f t="shared" ref="A223:A228" si="22">IF(H223&lt;&gt;"",IF(F223&lt;&gt;"",CONCATENATE("..........",D223,".",E223,".",F223,". - ",T223),IF(E223&lt;&gt;"",CONCATENATE(".....",D223,".",E223,". - ",T223),CONCATENATE(D223,". - ",T223))),"")</f>
-        <v>.....Z.01. - Symptoms, signs and ill-defined conditions, not elsewhere classified</v>
-      </c>
-      <c r="D223" s="56" t="s">
-        <v>1249</v>
-      </c>
-      <c r="E223" s="55" t="s">
-        <v>1144</v>
+        <f t="shared" si="18"/>
+        <v>..........E.03.c. - Execution, War, Terroism</v>
+      </c>
+      <c r="B223" s="2">
+        <v>210</v>
+      </c>
+      <c r="C223" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="D223" s="6" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E223" s="26" t="s">
+        <v>1146</v>
+      </c>
+      <c r="F223" s="6" t="s">
+        <v>1130</v>
       </c>
       <c r="G223" s="40" t="str">
         <f t="shared" si="21"/>
+        <v>cE03c</v>
+      </c>
+      <c r="H223" s="40" t="str">
+        <f t="shared" si="22"/>
+        <v>E03c</v>
+      </c>
+      <c r="I223" s="5" t="s">
+        <v>1380</v>
+      </c>
+      <c r="J223" s="5" t="s">
+        <v>1241</v>
+      </c>
+      <c r="K223" s="5" t="s">
+        <v>1379</v>
+      </c>
+      <c r="L223" s="49" t="s">
+        <v>1381</v>
+      </c>
+      <c r="M223" s="49"/>
+      <c r="N223" s="49"/>
+      <c r="O223" s="59" t="s">
+        <v>508</v>
+      </c>
+      <c r="P223" s="68" t="s">
+        <v>877</v>
+      </c>
+      <c r="Q223" s="69"/>
+      <c r="R223" s="59"/>
+      <c r="S223" s="59"/>
+      <c r="T223" s="5" t="s">
+        <v>1384</v>
+      </c>
+      <c r="U223" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="V223" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="W223" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="X223" s="22" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="224" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B224" s="82" t="s">
+        <v>1338</v>
+      </c>
+      <c r="C224" s="16" t="s">
+        <v>1281</v>
+      </c>
+      <c r="D224" s="54" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E224" s="55" t="s">
+        <v>1144</v>
+      </c>
+      <c r="G224" s="40" t="str">
+        <f t="shared" si="21"/>
+        <v>cE01</v>
+      </c>
+      <c r="H224" s="40"/>
+      <c r="I224" s="48" t="s">
+        <v>1257</v>
+      </c>
+      <c r="J224" s="48" t="s">
+        <v>1274</v>
+      </c>
+      <c r="K224" s="16" t="s">
+        <v>1275</v>
+      </c>
+      <c r="L224" s="16" t="s">
+        <v>1276</v>
+      </c>
+      <c r="T224" s="48" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="225" spans="1:20" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A225" s="44" t="str">
+        <f t="shared" ref="A225:A230" si="23">IF(H225&lt;&gt;"",IF(F225&lt;&gt;"",CONCATENATE("..........",D225,".",E225,".",F225,". - ",T225),IF(E225&lt;&gt;"",CONCATENATE(".....",D225,".",E225,". - ",T225),CONCATENATE(D225,". - ",T225))),"")</f>
+        <v>.....Z.01. - Symptoms, signs and ill-defined conditions, not elsewhere classified</v>
+      </c>
+      <c r="D225" s="56" t="s">
+        <v>1245</v>
+      </c>
+      <c r="E225" s="55" t="s">
+        <v>1144</v>
+      </c>
+      <c r="G225" s="40" t="str">
+        <f t="shared" si="21"/>
         <v>cZ01</v>
       </c>
-      <c r="H223" s="40" t="str">
-        <f>CONCATENATE(D223,E223,F223)</f>
+      <c r="H225" s="40" t="str">
+        <f>CONCATENATE(D225,E225,F225)</f>
         <v>Z01</v>
       </c>
-      <c r="I223" s="48" t="s">
+      <c r="I225" s="48" t="s">
+        <v>1223</v>
+      </c>
+      <c r="J225" s="48" t="s">
         <v>1224</v>
       </c>
-      <c r="J223" s="48" t="s">
+      <c r="K225" s="16" t="s">
         <v>1225</v>
       </c>
-      <c r="K223" s="16" t="s">
+      <c r="L225" s="16" t="s">
+        <v>1256</v>
+      </c>
+      <c r="T225" s="48" t="s">
         <v>1226</v>
       </c>
-      <c r="L223" s="16" t="s">
-        <v>1260</v>
-      </c>
-      <c r="T223" s="48" t="s">
-        <v>1227</v>
-      </c>
-    </row>
-    <row r="224" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A224" s="44" t="str">
-        <f t="shared" si="22"/>
+    </row>
+    <row r="226" spans="1:20" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A226" s="44" t="str">
+        <f t="shared" si="23"/>
         <v/>
       </c>
-      <c r="D224" s="56" t="s">
+      <c r="D226" s="56" t="s">
         <v>1138</v>
       </c>
-      <c r="E224" s="55" t="s">
+      <c r="E226" s="55" t="s">
         <v>1152</v>
       </c>
-      <c r="G224" s="42" t="str">
+      <c r="G226" s="42" t="str">
         <f t="shared" si="21"/>
         <v>cA09</v>
       </c>
-      <c r="H224" s="40"/>
-      <c r="I224" s="16" t="s">
-        <v>1340</v>
-      </c>
-      <c r="J224" s="48" t="s">
-        <v>1225</v>
-      </c>
-      <c r="K224" s="16" t="s">
-        <v>1219</v>
-      </c>
-      <c r="L224" s="16" t="s">
-        <v>1219</v>
-      </c>
-      <c r="T224" s="48" t="s">
+      <c r="H226" s="40"/>
+      <c r="I226" s="16" t="s">
+        <v>1334</v>
+      </c>
+      <c r="J226" s="48" t="s">
+        <v>1224</v>
+      </c>
+      <c r="K226" s="16" t="s">
         <v>1218</v>
       </c>
-    </row>
-    <row r="225" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A225" s="44" t="str">
-        <f t="shared" si="22"/>
-        <v>.....Z.02. - Unknown/Missing Value</v>
-      </c>
-      <c r="D225" s="56" t="s">
-        <v>1249</v>
-      </c>
-      <c r="E225" s="55" t="s">
-        <v>1145</v>
-      </c>
-      <c r="G225" s="43"/>
-      <c r="H225" s="40" t="str">
-        <f t="shared" ref="H225:H228" si="23">CONCATENATE(D225,E225,F225)</f>
-        <v>Z02</v>
-      </c>
-      <c r="T225" s="48" t="s">
-        <v>1322</v>
-      </c>
-    </row>
-    <row r="226" spans="1:20" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A226" s="44" t="str">
-        <f t="shared" si="22"/>
-        <v>.....Z.03. - Code does not map</v>
-      </c>
-      <c r="D226" s="56" t="s">
-        <v>1249</v>
-      </c>
-      <c r="E226" s="55" t="s">
-        <v>1146</v>
-      </c>
-      <c r="G226" s="43"/>
-      <c r="H226" s="40" t="str">
-        <f t="shared" si="23"/>
-        <v>Z03</v>
-      </c>
-      <c r="I226" s="16" t="s">
-        <v>1266</v>
+      <c r="L226" s="16" t="s">
+        <v>1218</v>
       </c>
       <c r="T226" s="48" t="s">
-        <v>1250</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="227" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A227" s="44" t="str">
-        <f t="shared" si="22"/>
-        <v>Z. - Unknown/Missing Value</v>
+        <f t="shared" si="23"/>
+        <v>.....Z.02. - Unknown/Missing Value</v>
       </c>
       <c r="D227" s="56" t="s">
-        <v>1249</v>
+        <v>1245</v>
+      </c>
+      <c r="E227" s="55" t="s">
+        <v>1145</v>
       </c>
       <c r="G227" s="43"/>
       <c r="H227" s="40" t="str">
+        <f t="shared" ref="H227:H230" si="24">CONCATENATE(D227,E227,F227)</f>
+        <v>Z02</v>
+      </c>
+      <c r="T227" s="48" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="228" spans="1:20" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A228" s="44" t="str">
         <f t="shared" si="23"/>
-        <v>Z</v>
-      </c>
-      <c r="T227" s="48" t="s">
-        <v>1322</v>
-      </c>
-    </row>
-    <row r="228" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A228" s="44" t="str">
-        <f t="shared" si="22"/>
-        <v>.....D.99. - Other Chronic Conditions</v>
+        <v>.....Z.03. - Code does not map</v>
       </c>
       <c r="D228" s="56" t="s">
-        <v>1142</v>
+        <v>1245</v>
       </c>
       <c r="E228" s="55" t="s">
-        <v>1228</v>
+        <v>1146</v>
       </c>
       <c r="G228" s="43"/>
       <c r="H228" s="40" t="str">
+        <f t="shared" si="24"/>
+        <v>Z03</v>
+      </c>
+      <c r="I228" s="16" t="s">
+        <v>1262</v>
+      </c>
+      <c r="T228" s="48" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="229" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A229" s="44" t="str">
         <f t="shared" si="23"/>
+        <v>Z. - Unknown/Missing Value</v>
+      </c>
+      <c r="D229" s="56" t="s">
+        <v>1245</v>
+      </c>
+      <c r="G229" s="43"/>
+      <c r="H229" s="40" t="str">
+        <f t="shared" si="24"/>
+        <v>Z</v>
+      </c>
+      <c r="T229" s="48" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="230" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A230" s="44" t="str">
+        <f t="shared" si="23"/>
+        <v>.....D.99. - Other Chronic Conditions</v>
+      </c>
+      <c r="D230" s="56" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E230" s="55" t="s">
+        <v>1227</v>
+      </c>
+      <c r="G230" s="43"/>
+      <c r="H230" s="40" t="str">
+        <f t="shared" si="24"/>
         <v>D99</v>
       </c>
-      <c r="T228" s="48" t="s">
-        <v>1281</v>
+      <c r="T230" s="48" t="s">
+        <v>1277</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:X221"/>
+  <autoFilter ref="A1:X223"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -18914,24 +19023,24 @@
   <sheetData>
     <row r="11" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="75" t="s">
-        <v>1329</v>
+        <v>1323</v>
       </c>
       <c r="D11" s="76" t="s">
-        <v>1328</v>
+        <v>1322</v>
       </c>
       <c r="E11" s="76" t="s">
-        <v>1328</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="12" spans="3:5" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="77" t="s">
-        <v>1330</v>
+        <v>1324</v>
       </c>
       <c r="D12" s="78" t="s">
-        <v>1331</v>
+        <v>1325</v>
       </c>
       <c r="E12" s="78" t="s">
-        <v>1332</v>
+        <v>1326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to "download handling" for charts and data; edits to multip[le figures
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/gbd.ICD.Map.xlsx
+++ b/myCBD/myInfo/gbd.ICD.Map.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0.CBD\myCBD\myInfo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="10935"/>
   </bookViews>
@@ -12,9 +17,9 @@
     <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$A$1:$X$223</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$A$1:$X$225</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +36,7 @@
     <author>Dauphine, David (CDPH-CHSI)</author>
   </authors>
   <commentList>
-    <comment ref="L1" authorId="0">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -55,7 +60,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C57" authorId="1">
+    <comment ref="C57" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -79,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P126" authorId="2">
+    <comment ref="P126" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -108,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2842" uniqueCount="1385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2852" uniqueCount="1392">
   <si>
     <t>I. Communicable, maternal, perinatal and nutritional conditions</t>
   </si>
@@ -4415,11 +4420,33 @@
 removed "cE03" code from G
 for "210" row 223, TEMP change of E from 99 to 03, and make F c</t>
   </si>
+  <si>
+    <t>W32-W34.9</t>
+  </si>
+  <si>
+    <t>W3[2-4]</t>
+  </si>
+  <si>
+    <t>Accidental Firearm</t>
+  </si>
+  <si>
+    <t>Moved W3[2-4] here from line above.</t>
+  </si>
+  <si>
+    <t>W20-W38, W40-W43, W45, W46, W49-W52, W75, W76
+not W3[2-4]</t>
+  </si>
+  <si>
+    <t>6. Accidental Firearm</t>
+  </si>
+  <si>
+    <t>W2|W3[0-1,5-8]|W4[0-3,5-6,9]|W5[0-2]|W7[5-6]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###0.;###0."/>
   </numFmts>
@@ -5070,7 +5097,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5105,7 +5132,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5314,13 +5341,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X230"/>
+  <dimension ref="A1:X232"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C215" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C212" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G221" sqref="G221"/>
+      <selection pane="bottomRight" activeCell="L215" sqref="L215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -16871,7 +16898,7 @@
     </row>
     <row r="195" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A195" s="44" t="str">
-        <f t="shared" ref="A195:A223" si="18">IF(H195&lt;&gt;"",IF(F195&lt;&gt;"",CONCATENATE("..........",D195,".",E195,".",F195,". - ",T195),IF(E195&lt;&gt;"",CONCATENATE(".....",D195,".",E195,". - ",T195),CONCATENATE(D195,". - ",T195))),"")</f>
+        <f t="shared" ref="A195:A225" si="18">IF(H195&lt;&gt;"",IF(F195&lt;&gt;"",CONCATENATE("..........",D195,".",E195,".",F195,". - ",T195),IF(E195&lt;&gt;"",CONCATENATE(".....",D195,".",E195,". - ",T195),CONCATENATE(D195,". - ",T195))),"")</f>
         <v/>
       </c>
       <c r="B195" s="2">
@@ -17771,7 +17798,7 @@
         <v>1126</v>
       </c>
       <c r="G210" s="40" t="str">
-        <f t="shared" ref="G210:G217" si="20">CONCATENATE("c",D210,E210,F210)</f>
+        <f t="shared" ref="G210:G219" si="20">CONCATENATE("c",D210,E210,F210)</f>
         <v>cE01a</v>
       </c>
       <c r="H210" s="40" t="str">
@@ -17909,7 +17936,9 @@
         <f>CONCATENATE(D212,E212,F212)</f>
         <v>E01b</v>
       </c>
-      <c r="I212" s="5"/>
+      <c r="I212" s="5" t="s">
+        <v>952</v>
+      </c>
       <c r="J212" s="5"/>
       <c r="K212" s="5" t="s">
         <v>501</v>
@@ -18068,7 +18097,7 @@
       </c>
       <c r="X214" s="2"/>
     </row>
-    <row r="215" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A215" s="44" t="str">
         <f t="shared" si="18"/>
         <v/>
@@ -18096,10 +18125,10 @@
       <c r="I215" s="5"/>
       <c r="J215" s="5"/>
       <c r="K215" s="5" t="s">
-        <v>995</v>
+        <v>1389</v>
       </c>
       <c r="L215" s="49" t="s">
-        <v>997</v>
+        <v>1391</v>
       </c>
       <c r="M215" s="49"/>
       <c r="N215" s="49"/>
@@ -18133,13 +18162,11 @@
     <row r="216" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A216" s="44" t="str">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="B216" s="2">
-        <v>205</v>
-      </c>
+        <v>..........E.01.c. - Accidental Firearm</v>
+      </c>
+      <c r="B216" s="2"/>
       <c r="C216" s="31" t="s">
-        <v>747</v>
+        <v>1390</v>
       </c>
       <c r="D216" s="6" t="s">
         <v>1143</v>
@@ -18148,60 +18175,53 @@
         <v>1144</v>
       </c>
       <c r="F216" s="6" t="s">
-        <v>1128</v>
+        <v>1130</v>
       </c>
       <c r="G216" s="40" t="str">
         <f t="shared" si="20"/>
-        <v>cE01x</v>
-      </c>
-      <c r="H216" s="40"/>
+        <v>cE01c</v>
+      </c>
+      <c r="H216" s="40" t="str">
+        <f>CONCATENATE(D216,E216,F216)</f>
+        <v>E01c</v>
+      </c>
       <c r="I216" s="5" t="s">
-        <v>1240</v>
+        <v>1388</v>
       </c>
       <c r="J216" s="5" t="s">
-        <v>1161</v>
+        <v>1214</v>
       </c>
       <c r="K216" s="5" t="s">
-        <v>1198</v>
+        <v>1385</v>
       </c>
       <c r="L216" s="49" t="s">
-        <v>1199</v>
+        <v>1386</v>
       </c>
       <c r="M216" s="49"/>
       <c r="N216" s="49"/>
-      <c r="O216" s="59" t="s">
-        <v>504</v>
-      </c>
-      <c r="P216" s="68" t="s">
-        <v>873</v>
-      </c>
-      <c r="Q216" s="69"/>
+      <c r="O216" s="59"/>
+      <c r="P216" s="68"/>
+      <c r="Q216" s="68"/>
       <c r="R216" s="59"/>
       <c r="S216" s="59"/>
       <c r="T216" s="5" t="s">
-        <v>886</v>
-      </c>
-      <c r="U216" s="20" t="s">
-        <v>747</v>
-      </c>
-      <c r="V216" s="5" t="s">
-        <v>886</v>
-      </c>
-      <c r="W216" s="45" t="s">
-        <v>747</v>
-      </c>
+        <v>1387</v>
+      </c>
+      <c r="U216" s="20"/>
+      <c r="V216" s="5"/>
+      <c r="W216" s="45"/>
       <c r="X216" s="2"/>
     </row>
-    <row r="217" spans="1:24" ht="102" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A217" s="44" t="str">
         <f t="shared" si="18"/>
-        <v>..........E.01.x. - Other unintentional injuries</v>
+        <v/>
       </c>
       <c r="B217" s="2">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C217" s="31" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="D217" s="6" t="s">
         <v>1143</v>
@@ -18216,64 +18236,47 @@
         <f t="shared" si="20"/>
         <v>cE01x</v>
       </c>
-      <c r="H217" s="40" t="str">
-        <f>CONCATENATE(D217,E217,F217)</f>
-        <v>E01x</v>
-      </c>
+      <c r="H217" s="40"/>
       <c r="I217" s="5" t="s">
-        <v>1261</v>
+        <v>1240</v>
       </c>
       <c r="J217" s="5" t="s">
-        <v>1258</v>
+        <v>1161</v>
       </c>
       <c r="K217" s="5" t="s">
-        <v>1259</v>
+        <v>1198</v>
       </c>
       <c r="L217" s="49" t="s">
-        <v>1260</v>
+        <v>1199</v>
       </c>
       <c r="M217" s="49"/>
       <c r="N217" s="49"/>
       <c r="O217" s="59" t="s">
-        <v>996</v>
+        <v>504</v>
       </c>
       <c r="P217" s="68" t="s">
-        <v>1113</v>
-      </c>
-      <c r="Q217" s="68"/>
-      <c r="R217" s="59" t="s">
-        <v>662</v>
-      </c>
-      <c r="S217" s="59" t="s">
-        <v>1003</v>
-      </c>
+        <v>873</v>
+      </c>
+      <c r="Q217" s="69"/>
+      <c r="R217" s="59"/>
+      <c r="S217" s="59"/>
       <c r="T217" s="5" t="s">
-        <v>315</v>
+        <v>886</v>
       </c>
       <c r="U217" s="20" t="s">
-        <v>887</v>
+        <v>747</v>
       </c>
       <c r="V217" s="5" t="s">
-        <v>315</v>
+        <v>886</v>
       </c>
       <c r="W217" s="45" t="s">
-        <v>887</v>
-      </c>
-      <c r="X217" s="22" t="s">
-        <v>1282</v>
-      </c>
-    </row>
-    <row r="218" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A218" s="44" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="B218" s="2">
-        <v>207</v>
-      </c>
-      <c r="C218" s="35" t="s">
-        <v>139</v>
-      </c>
+        <v>747</v>
+      </c>
+      <c r="X217" s="2"/>
+    </row>
+    <row r="218" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B218" s="2"/>
+      <c r="C218" s="31"/>
       <c r="D218" s="6"/>
       <c r="E218" s="26"/>
       <c r="F218" s="6"/>
@@ -18281,512 +18284,616 @@
       <c r="H218" s="40"/>
       <c r="I218" s="5"/>
       <c r="J218" s="5"/>
-      <c r="K218" s="5" t="s">
-        <v>952</v>
-      </c>
-      <c r="L218" s="19" t="s">
-        <v>952</v>
-      </c>
-      <c r="M218" s="19"/>
-      <c r="N218" s="19"/>
-      <c r="O218" s="59" t="s">
-        <v>505</v>
-      </c>
-      <c r="P218" s="66" t="s">
-        <v>874</v>
-      </c>
-      <c r="Q218" s="67"/>
-      <c r="R218" s="59" t="s">
-        <v>664</v>
-      </c>
-      <c r="S218" s="59" t="s">
-        <v>663</v>
-      </c>
-      <c r="T218" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="U218" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="V218" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="W218" s="45" t="s">
-        <v>139</v>
-      </c>
+      <c r="K218" s="5"/>
+      <c r="L218" s="49"/>
+      <c r="M218" s="49"/>
+      <c r="N218" s="49"/>
+      <c r="O218" s="59"/>
+      <c r="P218" s="68"/>
+      <c r="Q218" s="69"/>
+      <c r="R218" s="59"/>
+      <c r="S218" s="59"/>
+      <c r="T218" s="5"/>
+      <c r="U218" s="20"/>
+      <c r="V218" s="5"/>
+      <c r="W218" s="45"/>
       <c r="X218" s="2"/>
     </row>
-    <row r="219" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:24" ht="102" x14ac:dyDescent="0.25">
       <c r="A219" s="44" t="str">
         <f t="shared" si="18"/>
-        <v>.....E.02. - Suicide/Self-harm</v>
+        <v>..........E.01.x. - Other unintentional injuries</v>
       </c>
       <c r="B219" s="2">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C219" s="31" t="s">
-        <v>140</v>
+        <v>748</v>
       </c>
       <c r="D219" s="6" t="s">
         <v>1143</v>
       </c>
       <c r="E219" s="26" t="s">
-        <v>1145</v>
-      </c>
-      <c r="F219" s="6"/>
+        <v>1144</v>
+      </c>
+      <c r="F219" s="6" t="s">
+        <v>1128</v>
+      </c>
       <c r="G219" s="40" t="str">
-        <f t="shared" ref="G219:G226" si="21">CONCATENATE("c",D219,E219,F219)</f>
-        <v>cE02</v>
+        <f t="shared" si="20"/>
+        <v>cE01x</v>
       </c>
       <c r="H219" s="40" t="str">
         <f>CONCATENATE(D219,E219,F219)</f>
-        <v>E02</v>
+        <v>E01x</v>
       </c>
       <c r="I219" s="5" t="s">
-        <v>1308</v>
+        <v>1261</v>
       </c>
       <c r="J219" s="5" t="s">
-        <v>1214</v>
+        <v>1258</v>
       </c>
       <c r="K219" s="5" t="s">
-        <v>1215</v>
+        <v>1259</v>
       </c>
       <c r="L219" s="49" t="s">
-        <v>1216</v>
+        <v>1260</v>
       </c>
       <c r="M219" s="49"/>
       <c r="N219" s="49"/>
       <c r="O219" s="59" t="s">
-        <v>506</v>
+        <v>996</v>
       </c>
       <c r="P219" s="68" t="s">
-        <v>875</v>
-      </c>
-      <c r="Q219" s="69"/>
+        <v>1113</v>
+      </c>
+      <c r="Q219" s="68"/>
       <c r="R219" s="59" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="S219" s="59" t="s">
-        <v>999</v>
+        <v>1003</v>
       </c>
       <c r="T219" s="5" t="s">
-        <v>1279</v>
+        <v>315</v>
       </c>
       <c r="U219" s="20" t="s">
-        <v>140</v>
+        <v>887</v>
       </c>
       <c r="V219" s="5" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="W219" s="45" t="s">
-        <v>140</v>
-      </c>
-      <c r="X219" s="2"/>
-    </row>
-    <row r="220" spans="1:24" ht="255" x14ac:dyDescent="0.25">
+        <v>887</v>
+      </c>
+      <c r="X219" s="22" t="s">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="220" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A220" s="44" t="str">
         <f t="shared" si="18"/>
-        <v>.....E.03. - Homicide/Interpersonal violence</v>
+        <v/>
       </c>
       <c r="B220" s="2">
-        <v>209</v>
-      </c>
-      <c r="C220" s="31" t="s">
-        <v>141</v>
-      </c>
-      <c r="D220" s="6" t="s">
-        <v>1143</v>
-      </c>
-      <c r="E220" s="26" t="s">
-        <v>1146</v>
-      </c>
+        <v>207</v>
+      </c>
+      <c r="C220" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="D220" s="6"/>
+      <c r="E220" s="26"/>
       <c r="F220" s="6"/>
-      <c r="G220" s="40" t="s">
+      <c r="G220" s="40"/>
+      <c r="H220" s="40"/>
+      <c r="I220" s="5"/>
+      <c r="J220" s="5"/>
+      <c r="K220" s="5" t="s">
         <v>952</v>
       </c>
-      <c r="H220" s="40" t="str">
-        <f>CONCATENATE(D220,E220,F220)</f>
-        <v>E03</v>
-      </c>
-      <c r="I220" s="5" t="s">
-        <v>1384</v>
-      </c>
-      <c r="J220" s="5" t="s">
-        <v>1214</v>
+      <c r="L220" s="19" t="s">
+        <v>952</v>
       </c>
       <c r="M220" s="19"/>
       <c r="N220" s="19"/>
       <c r="O220" s="59" t="s">
-        <v>507</v>
-      </c>
-      <c r="P220" s="68" t="s">
-        <v>876</v>
-      </c>
-      <c r="Q220" s="69"/>
+        <v>505</v>
+      </c>
+      <c r="P220" s="66" t="s">
+        <v>874</v>
+      </c>
+      <c r="Q220" s="67"/>
       <c r="R220" s="59" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="S220" s="59" t="s">
-        <v>998</v>
-      </c>
-      <c r="T220" s="5" t="s">
-        <v>1278</v>
+        <v>663</v>
+      </c>
+      <c r="T220" s="2" t="s">
+        <v>316</v>
       </c>
       <c r="U220" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="V220" s="5" t="s">
-        <v>318</v>
+        <v>139</v>
+      </c>
+      <c r="V220" s="2" t="s">
+        <v>316</v>
       </c>
       <c r="W220" s="45" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="X220" s="2"/>
     </row>
-    <row r="221" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A221" s="44" t="str">
         <f t="shared" si="18"/>
-        <v>..........E.03.a. - Homicide excluding legal intervention</v>
-      </c>
-      <c r="B221" s="2"/>
-      <c r="C221" s="31"/>
+        <v>.....E.02. - Suicide/Self-harm</v>
+      </c>
+      <c r="B221" s="2">
+        <v>208</v>
+      </c>
+      <c r="C221" s="31" t="s">
+        <v>140</v>
+      </c>
       <c r="D221" s="6" t="s">
         <v>1143</v>
       </c>
       <c r="E221" s="26" t="s">
+        <v>1145</v>
+      </c>
+      <c r="F221" s="6"/>
+      <c r="G221" s="40" t="str">
+        <f t="shared" ref="G221:G228" si="21">CONCATENATE("c",D221,E221,F221)</f>
+        <v>cE02</v>
+      </c>
+      <c r="H221" s="40" t="str">
+        <f>CONCATENATE(D221,E221,F221)</f>
+        <v>E02</v>
+      </c>
+      <c r="I221" s="5" t="s">
+        <v>1308</v>
+      </c>
+      <c r="J221" s="5" t="s">
+        <v>1214</v>
+      </c>
+      <c r="K221" s="5" t="s">
+        <v>1215</v>
+      </c>
+      <c r="L221" s="49" t="s">
+        <v>1216</v>
+      </c>
+      <c r="M221" s="49"/>
+      <c r="N221" s="49"/>
+      <c r="O221" s="59" t="s">
+        <v>506</v>
+      </c>
+      <c r="P221" s="68" t="s">
+        <v>875</v>
+      </c>
+      <c r="Q221" s="69"/>
+      <c r="R221" s="59" t="s">
+        <v>665</v>
+      </c>
+      <c r="S221" s="59" t="s">
+        <v>999</v>
+      </c>
+      <c r="T221" s="5" t="s">
+        <v>1279</v>
+      </c>
+      <c r="U221" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="V221" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="W221" s="45" t="s">
+        <v>140</v>
+      </c>
+      <c r="X221" s="2"/>
+    </row>
+    <row r="222" spans="1:24" ht="255" x14ac:dyDescent="0.25">
+      <c r="A222" s="44" t="str">
+        <f t="shared" si="18"/>
+        <v>.....E.03. - Homicide/Interpersonal violence</v>
+      </c>
+      <c r="B222" s="2">
+        <v>209</v>
+      </c>
+      <c r="C222" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="D222" s="6" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E222" s="26" t="s">
         <v>1146</v>
       </c>
-      <c r="F221" s="6" t="s">
+      <c r="F222" s="6"/>
+      <c r="G222" s="40" t="s">
+        <v>952</v>
+      </c>
+      <c r="H222" s="40" t="str">
+        <f>CONCATENATE(D222,E222,F222)</f>
+        <v>E03</v>
+      </c>
+      <c r="I222" s="5" t="s">
+        <v>1384</v>
+      </c>
+      <c r="J222" s="5" t="s">
+        <v>1214</v>
+      </c>
+      <c r="M222" s="19"/>
+      <c r="N222" s="19"/>
+      <c r="O222" s="59" t="s">
+        <v>507</v>
+      </c>
+      <c r="P222" s="68" t="s">
+        <v>876</v>
+      </c>
+      <c r="Q222" s="69"/>
+      <c r="R222" s="59" t="s">
+        <v>666</v>
+      </c>
+      <c r="S222" s="59" t="s">
+        <v>998</v>
+      </c>
+      <c r="T222" s="5" t="s">
+        <v>1278</v>
+      </c>
+      <c r="U222" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="V222" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="W222" s="45" t="s">
+        <v>141</v>
+      </c>
+      <c r="X222" s="2"/>
+    </row>
+    <row r="223" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A223" s="44" t="str">
+        <f t="shared" si="18"/>
+        <v>..........E.03.a. - Homicide excluding legal intervention</v>
+      </c>
+      <c r="B223" s="2"/>
+      <c r="C223" s="31"/>
+      <c r="D223" s="6" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E223" s="26" t="s">
+        <v>1146</v>
+      </c>
+      <c r="F223" s="6" t="s">
         <v>1126</v>
       </c>
-      <c r="G221" s="40" t="str">
+      <c r="G223" s="40" t="str">
         <f t="shared" si="21"/>
         <v>cE03a</v>
       </c>
-      <c r="H221" s="40" t="str">
-        <f t="shared" ref="H221:H223" si="22">CONCATENATE(D221,E221,F221)</f>
+      <c r="H223" s="40" t="str">
+        <f t="shared" ref="H223:H225" si="22">CONCATENATE(D223,E223,F223)</f>
         <v>E03a</v>
       </c>
-      <c r="I221" s="5"/>
-      <c r="J221" s="5"/>
-      <c r="K221" s="5" t="s">
+      <c r="I223" s="5"/>
+      <c r="J223" s="5"/>
+      <c r="K223" s="5" t="s">
         <v>1377</v>
       </c>
-      <c r="L221" s="19" t="s">
+      <c r="L223" s="19" t="s">
         <v>1381</v>
       </c>
-      <c r="M221" s="19"/>
-      <c r="N221" s="19"/>
-      <c r="O221" s="59"/>
-      <c r="P221" s="68"/>
-      <c r="Q221" s="69"/>
-      <c r="R221" s="59"/>
-      <c r="S221" s="59"/>
-      <c r="T221" s="20" t="s">
-        <v>1375</v>
-      </c>
-      <c r="U221" s="46"/>
-      <c r="V221" s="5"/>
-      <c r="W221" s="45"/>
-      <c r="X221" s="2"/>
-    </row>
-    <row r="222" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A222" s="44" t="str">
-        <f t="shared" si="18"/>
-        <v>..........E.03.b. - Legal intervention</v>
-      </c>
-      <c r="B222" s="2"/>
-      <c r="C222" s="31"/>
-      <c r="D222" s="6" t="s">
-        <v>1143</v>
-      </c>
-      <c r="E222" s="26" t="s">
-        <v>1146</v>
-      </c>
-      <c r="F222" s="6" t="s">
-        <v>1127</v>
-      </c>
-      <c r="G222" s="40" t="str">
-        <f t="shared" si="21"/>
-        <v>cE03b</v>
-      </c>
-      <c r="H222" s="40" t="str">
-        <f t="shared" si="22"/>
-        <v>E03b</v>
-      </c>
-      <c r="I222" s="5"/>
-      <c r="J222" s="5"/>
-      <c r="K222" s="5" t="s">
-        <v>1376</v>
-      </c>
-      <c r="L222" s="19" t="s">
-        <v>1382</v>
-      </c>
-      <c r="M222" s="19"/>
-      <c r="N222" s="19"/>
-      <c r="O222" s="59"/>
-      <c r="P222" s="68"/>
-      <c r="Q222" s="69"/>
-      <c r="R222" s="59"/>
-      <c r="S222" s="59"/>
-      <c r="T222" s="20" t="s">
-        <v>1374</v>
-      </c>
-      <c r="U222" s="46"/>
-      <c r="V222" s="5"/>
-      <c r="W222" s="45"/>
-      <c r="X222" s="2"/>
-    </row>
-    <row r="223" spans="1:24" ht="153" x14ac:dyDescent="0.25">
-      <c r="A223" s="44" t="str">
-        <f t="shared" si="18"/>
-        <v>..........E.03.c. - Execution, War, Terroism</v>
-      </c>
-      <c r="B223" s="2">
-        <v>210</v>
-      </c>
-      <c r="C223" s="31" t="s">
-        <v>142</v>
-      </c>
-      <c r="D223" s="6" t="s">
-        <v>1143</v>
-      </c>
-      <c r="E223" s="26" t="s">
-        <v>1146</v>
-      </c>
-      <c r="F223" s="6" t="s">
-        <v>1130</v>
-      </c>
-      <c r="G223" s="40" t="str">
-        <f t="shared" si="21"/>
-        <v>cE03c</v>
-      </c>
-      <c r="H223" s="40" t="str">
-        <f t="shared" si="22"/>
-        <v>E03c</v>
-      </c>
-      <c r="I223" s="5" t="s">
-        <v>1379</v>
-      </c>
-      <c r="J223" s="5" t="s">
-        <v>1241</v>
-      </c>
-      <c r="K223" s="5" t="s">
-        <v>1378</v>
-      </c>
-      <c r="L223" s="49" t="s">
-        <v>1380</v>
-      </c>
-      <c r="M223" s="49"/>
-      <c r="N223" s="49"/>
-      <c r="O223" s="59" t="s">
-        <v>508</v>
-      </c>
-      <c r="P223" s="68" t="s">
-        <v>877</v>
-      </c>
+      <c r="M223" s="19"/>
+      <c r="N223" s="19"/>
+      <c r="O223" s="59"/>
+      <c r="P223" s="68"/>
       <c r="Q223" s="69"/>
       <c r="R223" s="59"/>
       <c r="S223" s="59"/>
-      <c r="T223" s="5" t="s">
-        <v>1383</v>
-      </c>
-      <c r="U223" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="V223" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="W223" s="45" t="s">
-        <v>142</v>
-      </c>
-      <c r="X223" s="22" t="s">
-        <v>1242</v>
-      </c>
-    </row>
-    <row r="224" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B224" s="82" t="s">
-        <v>1338</v>
-      </c>
-      <c r="C224" s="16" t="s">
-        <v>1281</v>
-      </c>
-      <c r="D224" s="54" t="s">
+      <c r="T223" s="20" t="s">
+        <v>1375</v>
+      </c>
+      <c r="U223" s="46"/>
+      <c r="V223" s="5"/>
+      <c r="W223" s="45"/>
+      <c r="X223" s="2"/>
+    </row>
+    <row r="224" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A224" s="44" t="str">
+        <f t="shared" si="18"/>
+        <v>..........E.03.b. - Legal intervention</v>
+      </c>
+      <c r="B224" s="2"/>
+      <c r="C224" s="31"/>
+      <c r="D224" s="6" t="s">
         <v>1143</v>
       </c>
-      <c r="E224" s="55" t="s">
-        <v>1144</v>
+      <c r="E224" s="26" t="s">
+        <v>1146</v>
+      </c>
+      <c r="F224" s="6" t="s">
+        <v>1127</v>
       </c>
       <c r="G224" s="40" t="str">
         <f t="shared" si="21"/>
-        <v>cE01</v>
-      </c>
-      <c r="H224" s="40"/>
-      <c r="I224" s="48" t="s">
-        <v>1257</v>
-      </c>
-      <c r="J224" s="48" t="s">
-        <v>1274</v>
-      </c>
-      <c r="K224" s="16" t="s">
-        <v>1275</v>
-      </c>
-      <c r="L224" s="16" t="s">
-        <v>1276</v>
-      </c>
-      <c r="T224" s="48" t="s">
-        <v>1221</v>
-      </c>
-    </row>
-    <row r="225" spans="1:20" ht="25.5" x14ac:dyDescent="0.25">
+        <v>cE03b</v>
+      </c>
+      <c r="H224" s="40" t="str">
+        <f t="shared" si="22"/>
+        <v>E03b</v>
+      </c>
+      <c r="I224" s="5"/>
+      <c r="J224" s="5"/>
+      <c r="K224" s="5" t="s">
+        <v>1376</v>
+      </c>
+      <c r="L224" s="19" t="s">
+        <v>1382</v>
+      </c>
+      <c r="M224" s="19"/>
+      <c r="N224" s="19"/>
+      <c r="O224" s="59"/>
+      <c r="P224" s="68"/>
+      <c r="Q224" s="69"/>
+      <c r="R224" s="59"/>
+      <c r="S224" s="59"/>
+      <c r="T224" s="20" t="s">
+        <v>1374</v>
+      </c>
+      <c r="U224" s="46"/>
+      <c r="V224" s="5"/>
+      <c r="W224" s="45"/>
+      <c r="X224" s="2"/>
+    </row>
+    <row r="225" spans="1:24" ht="153" x14ac:dyDescent="0.25">
       <c r="A225" s="44" t="str">
-        <f t="shared" ref="A225:A230" si="23">IF(H225&lt;&gt;"",IF(F225&lt;&gt;"",CONCATENATE("..........",D225,".",E225,".",F225,". - ",T225),IF(E225&lt;&gt;"",CONCATENATE(".....",D225,".",E225,". - ",T225),CONCATENATE(D225,". - ",T225))),"")</f>
-        <v>.....Z.01. - Symptoms, signs and ill-defined conditions, not elsewhere classified</v>
-      </c>
-      <c r="D225" s="56" t="s">
-        <v>1245</v>
-      </c>
-      <c r="E225" s="55" t="s">
-        <v>1144</v>
+        <f t="shared" si="18"/>
+        <v>..........E.03.c. - Execution, War, Terroism</v>
+      </c>
+      <c r="B225" s="2">
+        <v>210</v>
+      </c>
+      <c r="C225" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="D225" s="6" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E225" s="26" t="s">
+        <v>1146</v>
+      </c>
+      <c r="F225" s="6" t="s">
+        <v>1130</v>
       </c>
       <c r="G225" s="40" t="str">
         <f t="shared" si="21"/>
+        <v>cE03c</v>
+      </c>
+      <c r="H225" s="40" t="str">
+        <f t="shared" si="22"/>
+        <v>E03c</v>
+      </c>
+      <c r="I225" s="5" t="s">
+        <v>1379</v>
+      </c>
+      <c r="J225" s="5" t="s">
+        <v>1241</v>
+      </c>
+      <c r="K225" s="5" t="s">
+        <v>1378</v>
+      </c>
+      <c r="L225" s="49" t="s">
+        <v>1380</v>
+      </c>
+      <c r="M225" s="49"/>
+      <c r="N225" s="49"/>
+      <c r="O225" s="59" t="s">
+        <v>508</v>
+      </c>
+      <c r="P225" s="68" t="s">
+        <v>877</v>
+      </c>
+      <c r="Q225" s="69"/>
+      <c r="R225" s="59"/>
+      <c r="S225" s="59"/>
+      <c r="T225" s="5" t="s">
+        <v>1383</v>
+      </c>
+      <c r="U225" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="V225" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="W225" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="X225" s="22" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="226" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B226" s="82" t="s">
+        <v>1338</v>
+      </c>
+      <c r="C226" s="16" t="s">
+        <v>1281</v>
+      </c>
+      <c r="D226" s="54" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E226" s="55" t="s">
+        <v>1144</v>
+      </c>
+      <c r="G226" s="40" t="str">
+        <f t="shared" si="21"/>
+        <v>cE01</v>
+      </c>
+      <c r="H226" s="40"/>
+      <c r="I226" s="48" t="s">
+        <v>1257</v>
+      </c>
+      <c r="J226" s="48" t="s">
+        <v>1274</v>
+      </c>
+      <c r="K226" s="16" t="s">
+        <v>1275</v>
+      </c>
+      <c r="L226" s="16" t="s">
+        <v>1276</v>
+      </c>
+      <c r="T226" s="48" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="227" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A227" s="44" t="str">
+        <f t="shared" ref="A227:A232" si="23">IF(H227&lt;&gt;"",IF(F227&lt;&gt;"",CONCATENATE("..........",D227,".",E227,".",F227,". - ",T227),IF(E227&lt;&gt;"",CONCATENATE(".....",D227,".",E227,". - ",T227),CONCATENATE(D227,". - ",T227))),"")</f>
+        <v>.....Z.01. - Symptoms, signs and ill-defined conditions, not elsewhere classified</v>
+      </c>
+      <c r="D227" s="56" t="s">
+        <v>1245</v>
+      </c>
+      <c r="E227" s="55" t="s">
+        <v>1144</v>
+      </c>
+      <c r="G227" s="40" t="str">
+        <f t="shared" si="21"/>
         <v>cZ01</v>
       </c>
-      <c r="H225" s="40" t="str">
-        <f>CONCATENATE(D225,E225,F225)</f>
+      <c r="H227" s="40" t="str">
+        <f>CONCATENATE(D227,E227,F227)</f>
         <v>Z01</v>
       </c>
-      <c r="I225" s="48" t="s">
+      <c r="I227" s="48" t="s">
         <v>1223</v>
       </c>
-      <c r="J225" s="48" t="s">
+      <c r="J227" s="48" t="s">
         <v>1224</v>
       </c>
-      <c r="K225" s="16" t="s">
+      <c r="K227" s="16" t="s">
         <v>1225</v>
       </c>
-      <c r="L225" s="16" t="s">
+      <c r="L227" s="16" t="s">
         <v>1256</v>
       </c>
-      <c r="T225" s="48" t="s">
+      <c r="T227" s="48" t="s">
         <v>1226</v>
       </c>
     </row>
-    <row r="226" spans="1:20" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A226" s="44" t="str">
+    <row r="228" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A228" s="44" t="str">
         <f t="shared" si="23"/>
         <v/>
       </c>
-      <c r="D226" s="56" t="s">
+      <c r="D228" s="56" t="s">
         <v>1138</v>
       </c>
-      <c r="E226" s="55" t="s">
+      <c r="E228" s="55" t="s">
         <v>1152</v>
       </c>
-      <c r="G226" s="42" t="str">
+      <c r="G228" s="42" t="str">
         <f t="shared" si="21"/>
         <v>cA09</v>
       </c>
-      <c r="H226" s="40"/>
-      <c r="I226" s="16" t="s">
+      <c r="H228" s="40"/>
+      <c r="I228" s="16" t="s">
         <v>1334</v>
       </c>
-      <c r="J226" s="48" t="s">
+      <c r="J228" s="48" t="s">
         <v>1224</v>
       </c>
-      <c r="K226" s="16" t="s">
+      <c r="K228" s="16" t="s">
         <v>1218</v>
       </c>
-      <c r="L226" s="16" t="s">
+      <c r="L228" s="16" t="s">
         <v>1218</v>
       </c>
-      <c r="T226" s="48" t="s">
+      <c r="T228" s="48" t="s">
         <v>1217</v>
       </c>
     </row>
-    <row r="227" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A227" s="44" t="str">
+    <row r="229" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A229" s="44" t="str">
         <f t="shared" si="23"/>
         <v>.....Z.02. - Unknown/Missing Value</v>
       </c>
-      <c r="D227" s="56" t="s">
+      <c r="D229" s="56" t="s">
         <v>1245</v>
       </c>
-      <c r="E227" s="55" t="s">
+      <c r="E229" s="55" t="s">
         <v>1145</v>
       </c>
-      <c r="G227" s="43"/>
-      <c r="H227" s="40" t="str">
-        <f t="shared" ref="H227:H230" si="24">CONCATENATE(D227,E227,F227)</f>
+      <c r="G229" s="43"/>
+      <c r="H229" s="40" t="str">
+        <f t="shared" ref="H229:H232" si="24">CONCATENATE(D229,E229,F229)</f>
         <v>Z02</v>
       </c>
-      <c r="T227" s="48" t="s">
+      <c r="T229" s="48" t="s">
         <v>1316</v>
       </c>
     </row>
-    <row r="228" spans="1:20" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A228" s="44" t="str">
+    <row r="230" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A230" s="44" t="str">
         <f t="shared" si="23"/>
         <v>.....Z.03. - Code does not map</v>
       </c>
-      <c r="D228" s="56" t="s">
+      <c r="D230" s="56" t="s">
         <v>1245</v>
       </c>
-      <c r="E228" s="55" t="s">
+      <c r="E230" s="55" t="s">
         <v>1146</v>
-      </c>
-      <c r="G228" s="43"/>
-      <c r="H228" s="40" t="str">
-        <f t="shared" si="24"/>
-        <v>Z03</v>
-      </c>
-      <c r="I228" s="16" t="s">
-        <v>1262</v>
-      </c>
-      <c r="T228" s="48" t="s">
-        <v>1246</v>
-      </c>
-    </row>
-    <row r="229" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A229" s="44" t="str">
-        <f t="shared" si="23"/>
-        <v>Z. - Unknown/Missing Value</v>
-      </c>
-      <c r="D229" s="56" t="s">
-        <v>1245</v>
-      </c>
-      <c r="G229" s="43"/>
-      <c r="H229" s="40" t="str">
-        <f t="shared" si="24"/>
-        <v>Z</v>
-      </c>
-      <c r="T229" s="48" t="s">
-        <v>1316</v>
-      </c>
-    </row>
-    <row r="230" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A230" s="44" t="str">
-        <f t="shared" si="23"/>
-        <v>.....D.99. - Other Chronic Conditions</v>
-      </c>
-      <c r="D230" s="56" t="s">
-        <v>1142</v>
-      </c>
-      <c r="E230" s="55" t="s">
-        <v>1227</v>
       </c>
       <c r="G230" s="43"/>
       <c r="H230" s="40" t="str">
         <f t="shared" si="24"/>
+        <v>Z03</v>
+      </c>
+      <c r="I230" s="16" t="s">
+        <v>1262</v>
+      </c>
+      <c r="T230" s="48" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="231" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A231" s="44" t="str">
+        <f t="shared" si="23"/>
+        <v>Z. - Unknown/Missing Value</v>
+      </c>
+      <c r="D231" s="56" t="s">
+        <v>1245</v>
+      </c>
+      <c r="G231" s="43"/>
+      <c r="H231" s="40" t="str">
+        <f t="shared" si="24"/>
+        <v>Z</v>
+      </c>
+      <c r="T231" s="48" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="232" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A232" s="44" t="str">
+        <f t="shared" si="23"/>
+        <v>.....D.99. - Other Chronic Conditions</v>
+      </c>
+      <c r="D232" s="56" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E232" s="55" t="s">
+        <v>1227</v>
+      </c>
+      <c r="G232" s="43"/>
+      <c r="H232" s="40" t="str">
+        <f t="shared" si="24"/>
         <v>D99</v>
       </c>
-      <c r="T230" s="48" t="s">
+      <c r="T232" s="48" t="s">
         <v>1277</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:X223"/>
+  <autoFilter ref="A1:X225"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
new CAUSE dropdown format; other minor edits
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/gbd.ICD.Map.xlsx
+++ b/myCBD/myInfo/gbd.ICD.Map.xlsx
@@ -5344,10 +5344,10 @@
   <dimension ref="A1:X232"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C212" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B220" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L215" sqref="L215"/>
+      <selection pane="bottomRight" activeCell="A228" sqref="A228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -5499,7 +5499,7 @@
     </row>
     <row r="3" spans="1:24" ht="66" x14ac:dyDescent="0.25">
       <c r="A3" s="44" t="str">
-        <f t="shared" ref="A3:A66" si="0">IF(H3&lt;&gt;"",IF(F3&lt;&gt;"",CONCATENATE("..........",D3,".",E3,".",F3,". - ",T3),IF(E3&lt;&gt;"",CONCATENATE(".....",D3,".",E3,". - ",T3),CONCATENATE(D3,". - ",T3))),"")</f>
+        <f>IF(H3&lt;&gt;"",IF(F3&lt;&gt;"",CONCATENATE("...",D3,".",E3,".",F3,". - ",T3),IF(E3&lt;&gt;"",CONCATENATE("..",D3,".",E3,". - ",T3),CONCATENATE(D3,". - ",T3))),"")</f>
         <v>A. - Communicable, maternal, perinatal and nutritional conditions</v>
       </c>
       <c r="B3" s="2">
@@ -5551,10 +5551,10 @@
       </c>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="44" t="str">
-        <f t="shared" si="0"/>
-        <v>.....A.99. - Other Infectious Diseases</v>
+        <f t="shared" ref="A4:A67" si="0">IF(H4&lt;&gt;"",IF(F4&lt;&gt;"",CONCATENATE("...",D4,".",E4,".",F4,". - ",T4),IF(E4&lt;&gt;"",CONCATENATE("..",D4,".",E4,". - ",T4),CONCATENATE(D4,". - ",T4))),"")</f>
+        <v>..A.99. - Other Infectious Diseases</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="29" t="s">
@@ -5644,10 +5644,10 @@
       </c>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="44" t="str">
         <f t="shared" si="0"/>
-        <v>.....A.01. - Tuberculosis</v>
+        <v>..A.01. - Tuberculosis</v>
       </c>
       <c r="B6" s="2">
         <v>3</v>
@@ -5708,7 +5708,7 @@
     <row r="7" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="44" t="str">
         <f t="shared" si="0"/>
-        <v>.....A.02. - HIV/ and other Sexually transmitted diseases (STDs)</v>
+        <v>..A.02. - HIV/ and other Sexually transmitted diseases (STDs)</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="32" t="s">
@@ -5750,7 +5750,7 @@
     <row r="8" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="44" t="str">
         <f t="shared" si="0"/>
-        <v>..........A.02.a. - Sexually transmitted diseases (STDs) excluding HIV</v>
+        <v>...A.02.a. - Sexually transmitted diseases (STDs) excluding HIV</v>
       </c>
       <c r="B8" s="2">
         <v>4</v>
@@ -5811,7 +5811,7 @@
       </c>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -5871,7 +5871,7 @@
       </c>
       <c r="X9" s="2"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A10" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -5931,7 +5931,7 @@
       </c>
       <c r="X10" s="2"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -5991,7 +5991,7 @@
       </c>
       <c r="X11" s="2"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6049,7 +6049,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A13" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6109,10 +6109,10 @@
       </c>
       <c r="X13" s="2"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="str">
         <f t="shared" si="0"/>
-        <v>..........A.02.b. - HIV/AIDS</v>
+        <v>...A.02.b. - HIV/AIDS</v>
       </c>
       <c r="B14" s="2">
         <v>10</v>
@@ -6171,7 +6171,7 @@
       </c>
       <c r="X14" s="2"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A15" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6227,7 +6227,7 @@
       </c>
       <c r="X15" s="2"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A16" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6287,7 +6287,7 @@
       </c>
       <c r="X16" s="2"/>
     </row>
-    <row r="17" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A17" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6345,7 +6345,7 @@
       </c>
       <c r="X17" s="2"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A18" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6397,7 +6397,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A19" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6455,7 +6455,7 @@
       </c>
       <c r="X19" s="2"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A20" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6513,7 +6513,7 @@
       </c>
       <c r="X20" s="2"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A21" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6571,7 +6571,7 @@
       </c>
       <c r="X21" s="2"/>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A22" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6629,10 +6629,10 @@
       </c>
       <c r="X22" s="2"/>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A23" s="44" t="str">
         <f t="shared" si="0"/>
-        <v>.....A.04. - Meningitis</v>
+        <v>..A.04. - Meningitis</v>
       </c>
       <c r="B23" s="2">
         <v>19</v>
@@ -6690,10 +6690,10 @@
       </c>
       <c r="X23" s="2"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A24" s="44" t="str">
         <f t="shared" si="0"/>
-        <v>.....A.05. - Encephalitis</v>
+        <v>..A.05. - Encephalitis</v>
       </c>
       <c r="B24" s="2">
         <v>20</v>
@@ -6751,10 +6751,10 @@
       </c>
       <c r="X24" s="2"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A25" s="44" t="str">
         <f t="shared" si="0"/>
-        <v>.....A.06. - Hepatitis</v>
+        <v>..A.06. - Hepatitis</v>
       </c>
       <c r="B25" s="2">
         <v>21</v>
@@ -6805,7 +6805,7 @@
       </c>
       <c r="X25" s="2"/>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A26" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6862,7 +6862,7 @@
     <row r="27" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A27" s="44" t="str">
         <f t="shared" si="0"/>
-        <v>..........A.06.a. - Acute hepatitis B</v>
+        <v>...A.06.a. - Acute hepatitis B</v>
       </c>
       <c r="B27" s="2">
         <v>23</v>
@@ -6918,7 +6918,7 @@
       </c>
       <c r="X27" s="2"/>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A28" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -6946,10 +6946,10 @@
       <c r="W28" s="45"/>
       <c r="X28" s="2"/>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A29" s="44" t="str">
         <f t="shared" si="0"/>
-        <v>..........A.06.b. - Acute hepatitis C</v>
+        <v>...A.06.b. - Acute hepatitis C</v>
       </c>
       <c r="B29" s="2">
         <v>24</v>
@@ -7005,7 +7005,7 @@
       </c>
       <c r="X29" s="2"/>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A30" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -7059,7 +7059,7 @@
       </c>
       <c r="X30" s="2"/>
     </row>
-    <row r="31" spans="1:24" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A31" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -7110,7 +7110,7 @@
       </c>
       <c r="X31" s="2"/>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A32" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -7168,7 +7168,7 @@
       </c>
       <c r="X32" s="2"/>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A33" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -7226,7 +7226,7 @@
       </c>
       <c r="X33" s="2"/>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A34" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -7284,7 +7284,7 @@
       </c>
       <c r="X34" s="2"/>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A35" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -7342,7 +7342,7 @@
       </c>
       <c r="X35" s="2"/>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A36" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -7400,7 +7400,7 @@
       </c>
       <c r="X36" s="2"/>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A37" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -7454,7 +7454,7 @@
       </c>
       <c r="X37" s="2"/>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A38" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -7508,7 +7508,7 @@
       </c>
       <c r="X38" s="2"/>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A39" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -7566,7 +7566,7 @@
       </c>
       <c r="X39" s="2"/>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A40" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -7624,7 +7624,7 @@
       </c>
       <c r="X40" s="2"/>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A41" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -7678,7 +7678,7 @@
       </c>
       <c r="X41" s="2"/>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A42" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -7736,7 +7736,7 @@
       </c>
       <c r="X42" s="2"/>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A43" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -7790,7 +7790,7 @@
       </c>
       <c r="X43" s="2"/>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A44" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -7848,7 +7848,7 @@
       </c>
       <c r="X44" s="2"/>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A45" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -7906,7 +7906,7 @@
       </c>
       <c r="X45" s="2"/>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A46" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -7961,7 +7961,7 @@
       </c>
       <c r="X46" s="2"/>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A47" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -8019,7 +8019,7 @@
       </c>
       <c r="X47" s="2"/>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A48" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -8073,7 +8073,7 @@
       </c>
       <c r="X48" s="2"/>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A49" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -8127,7 +8127,7 @@
       </c>
       <c r="X49" s="2"/>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A50" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -8247,10 +8247,10 @@
         <v>1314</v>
       </c>
     </row>
-    <row r="52" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A52" s="44" t="str">
         <f t="shared" si="0"/>
-        <v>.....A.07. - Respiratory infections</v>
+        <v>..A.07. - Respiratory infections</v>
       </c>
       <c r="B52" s="2">
         <v>47</v>
@@ -8307,7 +8307,7 @@
       </c>
       <c r="X52" s="2"/>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A53" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -8371,7 +8371,7 @@
       </c>
       <c r="X53" s="2"/>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A54" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -8435,7 +8435,7 @@
       </c>
       <c r="X54" s="2"/>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A55" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -8499,10 +8499,10 @@
       </c>
       <c r="X55" s="2"/>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A56" s="44" t="str">
         <f t="shared" si="0"/>
-        <v>.....A.08. - Maternal conditions</v>
+        <v>..A.08. - Maternal conditions</v>
       </c>
       <c r="B56" s="2">
         <v>51</v>
@@ -8627,7 +8627,7 @@
         <v>1366</v>
       </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A58" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -8757,7 +8757,7 @@
         <v>1368</v>
       </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A60" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -8821,7 +8821,7 @@
       </c>
       <c r="X60" s="2"/>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A61" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -8949,10 +8949,10 @@
       </c>
       <c r="X62" s="2"/>
     </row>
-    <row r="63" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A63" s="44" t="str">
         <f t="shared" si="0"/>
-        <v>.....A.09. - Neonatal conditions</v>
+        <v>..A.09. - Neonatal conditions</v>
       </c>
       <c r="B63" s="2">
         <v>58</v>
@@ -9011,7 +9011,7 @@
       </c>
       <c r="X63" s="2"/>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A64" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -9127,7 +9127,7 @@
       </c>
       <c r="X65" s="2"/>
     </row>
-    <row r="66" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A66" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -9187,7 +9187,7 @@
     </row>
     <row r="67" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A67" s="44" t="str">
-        <f t="shared" ref="A67:A130" si="4">IF(H67&lt;&gt;"",IF(F67&lt;&gt;"",CONCATENATE("..........",D67,".",E67,".",F67,". - ",T67),IF(E67&lt;&gt;"",CONCATENATE(".....",D67,".",E67,". - ",T67),CONCATENATE(D67,". - ",T67))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B67" s="2">
@@ -9249,9 +9249,9 @@
       </c>
       <c r="X67" s="2"/>
     </row>
-    <row r="68" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A68" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="A68:A131" si="4">IF(H68&lt;&gt;"",IF(F68&lt;&gt;"",CONCATENATE("...",D68,".",E68,".",F68,". - ",T68),IF(E68&lt;&gt;"",CONCATENATE("..",D68,".",E68,". - ",T68),CONCATENATE(D68,". - ",T68))),"")</f>
         <v/>
       </c>
       <c r="B68" s="2">
@@ -9304,7 +9304,7 @@
       </c>
       <c r="X68" s="2"/>
     </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A69" s="44" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -9362,7 +9362,7 @@
       </c>
       <c r="X69" s="2"/>
     </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A70" s="44" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -9420,7 +9420,7 @@
       </c>
       <c r="X70" s="2"/>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A71" s="44" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -9474,7 +9474,7 @@
       </c>
       <c r="X71" s="2"/>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A72" s="44" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -9532,7 +9532,7 @@
       </c>
       <c r="X72" s="2"/>
     </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A73" s="44" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -9643,7 +9643,7 @@
       </c>
       <c r="X74" s="2"/>
     </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A75" s="44" t="str">
         <f t="shared" si="4"/>
         <v>D. - Other Chronic</v>
@@ -9739,10 +9739,10 @@
       </c>
       <c r="X76" s="2"/>
     </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A77" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>.....B.01. - Mouth and oropharynx cancers</v>
+        <v>..B.01. - Mouth and oropharynx cancers</v>
       </c>
       <c r="B77" s="2">
         <v>71</v>
@@ -9862,7 +9862,7 @@
       </c>
       <c r="X78" s="2"/>
     </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A79" s="44" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -9926,7 +9926,7 @@
       </c>
       <c r="X79" s="2"/>
     </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A80" s="44" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -9986,10 +9986,10 @@
       </c>
       <c r="X80" s="2"/>
     </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A81" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>.....B.02. - Oesophagus cancer</v>
+        <v>..B.02. - Oesophagus cancer</v>
       </c>
       <c r="B81" s="2">
         <v>75</v>
@@ -10053,10 +10053,10 @@
       </c>
       <c r="X81" s="2"/>
     </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A82" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>.....B.03. - Stomach cancer</v>
+        <v>..B.03. - Stomach cancer</v>
       </c>
       <c r="B82" s="2">
         <v>76</v>
@@ -10125,7 +10125,7 @@
     <row r="83" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A83" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>.....B.04. - Colon and rectum cancers</v>
+        <v>..B.04. - Colon and rectum cancers</v>
       </c>
       <c r="B83" s="2">
         <v>77</v>
@@ -10189,10 +10189,10 @@
       </c>
       <c r="X83" s="2"/>
     </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A84" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>.....B.05. - Liver cancer</v>
+        <v>..B.05. - Liver cancer</v>
       </c>
       <c r="B84" s="2">
         <v>78</v>
@@ -10256,10 +10256,10 @@
       </c>
       <c r="X84" s="2"/>
     </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A85" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>.....B.06. - Pancreas cancer</v>
+        <v>..B.06. - Pancreas cancer</v>
       </c>
       <c r="B85" s="2">
         <v>79</v>
@@ -10323,10 +10323,10 @@
       </c>
       <c r="X85" s="2"/>
     </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A86" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>.....B.07. - Trachea, bronchus and lung cancers</v>
+        <v>..B.07. - Trachea, bronchus and lung cancers</v>
       </c>
       <c r="B86" s="2">
         <v>80</v>
@@ -10390,10 +10390,10 @@
       </c>
       <c r="X86" s="2"/>
     </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A87" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>.....B.08. - Melanoma and other skin cancers</v>
+        <v>..B.08. - Melanoma and other skin cancers</v>
       </c>
       <c r="B87" s="2">
         <v>81</v>
@@ -10513,7 +10513,7 @@
       </c>
       <c r="X88" s="2"/>
     </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A89" s="44" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10577,10 +10577,10 @@
       </c>
       <c r="X89" s="2"/>
     </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A90" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>.....B.09. - Breast cancer</v>
+        <v>..B.09. - Breast cancer</v>
       </c>
       <c r="B90" s="2">
         <v>84</v>
@@ -10644,10 +10644,10 @@
       </c>
       <c r="X90" s="2"/>
     </row>
-    <row r="91" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A91" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>.....B.10. - Uterine cancer</v>
+        <v>..B.10. - Uterine cancer</v>
       </c>
       <c r="B91" s="2"/>
       <c r="C91" s="37" t="s">
@@ -10687,7 +10687,7 @@
       <c r="W91" s="45"/>
       <c r="X91" s="2"/>
     </row>
-    <row r="92" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A92" s="44" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10815,10 +10815,10 @@
       </c>
       <c r="X93" s="2"/>
     </row>
-    <row r="94" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A94" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>.....B.11. - Ovary cancer</v>
+        <v>..B.11. - Ovary cancer</v>
       </c>
       <c r="B94" s="2">
         <v>87</v>
@@ -10882,10 +10882,10 @@
       </c>
       <c r="X94" s="2"/>
     </row>
-    <row r="95" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A95" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>.....B.12. - Prostate cancer</v>
+        <v>..B.12. - Prostate cancer</v>
       </c>
       <c r="B95" s="2">
         <v>88</v>
@@ -10949,7 +10949,7 @@
       </c>
       <c r="X95" s="2"/>
     </row>
-    <row r="96" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A96" s="44" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -11016,7 +11016,7 @@
     <row r="97" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A97" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>.....B.13. - Kidney, renal pelvis and ureter cancer</v>
+        <v>..B.13. - Kidney, renal pelvis and ureter cancer</v>
       </c>
       <c r="B97" s="2">
         <v>90</v>
@@ -11080,10 +11080,10 @@
       </c>
       <c r="X97" s="2"/>
     </row>
-    <row r="98" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A98" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>.....B.14. - Bladder cancer</v>
+        <v>..B.14. - Bladder cancer</v>
       </c>
       <c r="B98" s="2">
         <v>91</v>
@@ -11150,7 +11150,7 @@
     <row r="99" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A99" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>.....B.15. - Brain and nervous system cancers</v>
+        <v>..B.15. - Brain and nervous system cancers</v>
       </c>
       <c r="B99" s="2">
         <v>92</v>
@@ -11214,7 +11214,7 @@
       </c>
       <c r="X99" s="2"/>
     </row>
-    <row r="100" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A100" s="44" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -11278,7 +11278,7 @@
       </c>
       <c r="X100" s="2"/>
     </row>
-    <row r="101" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A101" s="44" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -11342,7 +11342,7 @@
       </c>
       <c r="X101" s="2"/>
     </row>
-    <row r="102" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A102" s="44" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -11406,7 +11406,7 @@
       </c>
       <c r="X102" s="2"/>
     </row>
-    <row r="103" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A103" s="44" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -11466,10 +11466,10 @@
       </c>
       <c r="X103" s="2"/>
     </row>
-    <row r="104" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A104" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>.....B.16. - Lymphomas and multiple myeloma</v>
+        <v>..B.16. - Lymphomas and multiple myeloma</v>
       </c>
       <c r="B104" s="2">
         <v>97</v>
@@ -11526,10 +11526,10 @@
       </c>
       <c r="X104" s="2"/>
     </row>
-    <row r="105" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A105" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>..........B.16.a. - Hodgkin lymphoma</v>
+        <v>...B.16.a. - Hodgkin lymphoma</v>
       </c>
       <c r="B105" s="2">
         <v>98</v>
@@ -11591,10 +11591,10 @@
       </c>
       <c r="X105" s="2"/>
     </row>
-    <row r="106" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A106" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>..........B.16.b. - Non-Hodgkin lymphoma</v>
+        <v>...B.16.b. - Non-Hodgkin lymphoma</v>
       </c>
       <c r="B106" s="2">
         <v>99</v>
@@ -11656,10 +11656,10 @@
       </c>
       <c r="X106" s="2"/>
     </row>
-    <row r="107" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A107" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>..........B.16.c. - Multiple myeloma</v>
+        <v>...B.16.c. - Multiple myeloma</v>
       </c>
       <c r="B107" s="2">
         <v>100</v>
@@ -11721,10 +11721,10 @@
       </c>
       <c r="X107" s="2"/>
     </row>
-    <row r="108" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A108" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>.....B.17. - Leukaemia</v>
+        <v>..B.17. - Leukaemia</v>
       </c>
       <c r="B108" s="2">
         <v>101</v>
@@ -11787,7 +11787,7 @@
     <row r="109" spans="1:24" ht="51" x14ac:dyDescent="0.25">
       <c r="A109" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>.....B.99. - Other malignant neoplasms</v>
+        <v>..B.99. - Other malignant neoplasms</v>
       </c>
       <c r="B109" s="2">
         <v>102</v>
@@ -11908,7 +11908,7 @@
     <row r="111" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A111" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>.....D.01. - Diabetes mellitus</v>
+        <v>..D.01. - Diabetes mellitus</v>
       </c>
       <c r="B111" s="2">
         <v>104</v>
@@ -11981,7 +11981,7 @@
     <row r="112" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A112" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>.....D.02. - Endocrine, blood, immune disorders</v>
+        <v>..D.02. - Endocrine, blood, immune disorders</v>
       </c>
       <c r="B112" s="2">
         <v>105</v>
@@ -12040,7 +12040,7 @@
       </c>
       <c r="X112" s="2"/>
     </row>
-    <row r="113" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A113" s="44" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -12100,7 +12100,7 @@
       </c>
       <c r="X113" s="2"/>
     </row>
-    <row r="114" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A114" s="44" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -12280,7 +12280,7 @@
       </c>
       <c r="X116" s="2"/>
     </row>
-    <row r="117" spans="1:24" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A117" s="44" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -12342,7 +12342,7 @@
     <row r="118" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A118" s="44" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">.....D.03. - Mental Health disorders </v>
+        <v xml:space="preserve">..D.03. - Mental Health disorders </v>
       </c>
       <c r="B118" s="2"/>
       <c r="C118" s="32" t="s">
@@ -12383,10 +12383,10 @@
       <c r="W118" s="45"/>
       <c r="X118" s="2"/>
     </row>
-    <row r="119" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A119" s="44" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">.....D.04. - Substance use </v>
+        <v xml:space="preserve">..D.04. - Substance use </v>
       </c>
       <c r="B119" s="2"/>
       <c r="C119" s="32" t="s">
@@ -12425,7 +12425,7 @@
       <c r="W119" s="45"/>
       <c r="X119" s="2"/>
     </row>
-    <row r="120" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A120" s="44" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -12456,7 +12456,7 @@
       <c r="W120" s="45"/>
       <c r="X120" s="2"/>
     </row>
-    <row r="121" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A121" s="44" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -12505,7 +12505,7 @@
       </c>
       <c r="X121" s="2"/>
     </row>
-    <row r="122" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A122" s="44" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -12565,7 +12565,7 @@
       </c>
       <c r="X122" s="2"/>
     </row>
-    <row r="123" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A123" s="44" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -12625,7 +12625,7 @@
       </c>
       <c r="X123" s="2"/>
     </row>
-    <row r="124" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A124" s="44" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -12685,7 +12685,7 @@
       </c>
       <c r="X124" s="2"/>
     </row>
-    <row r="125" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A125" s="44" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -12752,7 +12752,7 @@
     <row r="126" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A126" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>..........D.04.a. - Alcohol use disorders</v>
+        <v>...D.04.a. - Alcohol use disorders</v>
       </c>
       <c r="B126" s="2">
         <v>116</v>
@@ -12818,7 +12818,7 @@
       </c>
       <c r="X126" s="2"/>
     </row>
-    <row r="127" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A127" s="44" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -12871,10 +12871,10 @@
       </c>
       <c r="X127" s="2"/>
     </row>
-    <row r="128" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A128" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>..........D.04.b. - Opioid use disorders</v>
+        <v>...D.04.b. - Opioid use disorders</v>
       </c>
       <c r="B128" s="2">
         <v>118</v>
@@ -12936,10 +12936,10 @@
       </c>
       <c r="X128" s="2"/>
     </row>
-    <row r="129" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A129" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>..........D.04.c. - Cocaine use disorders</v>
+        <v>...D.04.c. - Cocaine use disorders</v>
       </c>
       <c r="B129" s="2">
         <v>119</v>
@@ -13001,10 +13001,10 @@
       </c>
       <c r="X129" s="2"/>
     </row>
-    <row r="130" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A130" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>..........D.04.d. - Amphetamine use disorders</v>
+        <v>...D.04.d. - Amphetamine use disorders</v>
       </c>
       <c r="B130" s="2">
         <v>120</v>
@@ -13066,9 +13066,9 @@
       </c>
       <c r="X130" s="2"/>
     </row>
-    <row r="131" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A131" s="44" t="str">
-        <f t="shared" ref="A131:A194" si="11">IF(H131&lt;&gt;"",IF(F131&lt;&gt;"",CONCATENATE("..........",D131,".",E131,".",F131,". - ",T131),IF(E131&lt;&gt;"",CONCATENATE(".....",D131,".",E131,". - ",T131),CONCATENATE(D131,". - ",T131))),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="B131" s="2">
@@ -13121,9 +13121,9 @@
       </c>
       <c r="X131" s="2"/>
     </row>
-    <row r="132" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A132" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="A132:A195" si="11">IF(H132&lt;&gt;"",IF(F132&lt;&gt;"",CONCATENATE("...",D132,".",E132,".",F132,". - ",T132),IF(E132&lt;&gt;"",CONCATENATE("..",D132,".",E132,". - ",T132),CONCATENATE(D132,". - ",T132))),"")</f>
         <v/>
       </c>
       <c r="B132" s="2">
@@ -13187,7 +13187,7 @@
         <v>1238</v>
       </c>
     </row>
-    <row r="133" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A133" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -13243,7 +13243,7 @@
       </c>
       <c r="X133" s="2"/>
     </row>
-    <row r="134" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A134" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -13303,7 +13303,7 @@
       </c>
       <c r="X134" s="2"/>
     </row>
-    <row r="135" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A135" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -13359,7 +13359,7 @@
       </c>
       <c r="X135" s="2"/>
     </row>
-    <row r="136" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A136" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -13408,7 +13408,7 @@
       </c>
       <c r="X136" s="2"/>
     </row>
-    <row r="137" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A137" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -13464,7 +13464,7 @@
       </c>
       <c r="X137" s="2"/>
     </row>
-    <row r="138" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A138" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -13520,7 +13520,7 @@
       </c>
       <c r="X138" s="2"/>
     </row>
-    <row r="139" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A139" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -13632,7 +13632,7 @@
       </c>
       <c r="X140" s="2"/>
     </row>
-    <row r="141" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A141" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -13691,10 +13691,10 @@
         <v>607</v>
       </c>
     </row>
-    <row r="142" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A142" s="44" t="str">
         <f t="shared" si="11"/>
-        <v>.....D.05. - Alzheimer’s disease and other dementias</v>
+        <v>..D.05. - Alzheimer’s disease and other dementias</v>
       </c>
       <c r="B142" s="2">
         <v>132</v>
@@ -13754,7 +13754,7 @@
       </c>
       <c r="X142" s="2"/>
     </row>
-    <row r="143" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A143" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -13814,7 +13814,7 @@
       </c>
       <c r="X143" s="2"/>
     </row>
-    <row r="144" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A144" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -13874,7 +13874,7 @@
       </c>
       <c r="X144" s="2"/>
     </row>
-    <row r="145" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A145" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -13934,7 +13934,7 @@
       </c>
       <c r="X145" s="2"/>
     </row>
-    <row r="146" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A146" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -13990,7 +13990,7 @@
       </c>
       <c r="X146" s="2"/>
     </row>
-    <row r="147" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A147" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -14049,7 +14049,7 @@
     <row r="148" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A148" s="44" t="str">
         <f t="shared" si="11"/>
-        <v>.....D.06. - Other neurological conditions</v>
+        <v>..D.06. - Other neurological conditions</v>
       </c>
       <c r="B148" s="2">
         <v>138</v>
@@ -14113,7 +14113,7 @@
       </c>
       <c r="X148" s="2"/>
     </row>
-    <row r="149" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A149" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -14168,7 +14168,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="150" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A150" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -14224,7 +14224,7 @@
       </c>
       <c r="X150" s="2"/>
     </row>
-    <row r="151" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A151" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -14280,7 +14280,7 @@
       </c>
       <c r="X151" s="2"/>
     </row>
-    <row r="152" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A152" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -14336,7 +14336,7 @@
       </c>
       <c r="X152" s="2"/>
     </row>
-    <row r="153" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A153" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -14392,7 +14392,7 @@
       </c>
       <c r="X153" s="2"/>
     </row>
-    <row r="154" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A154" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -14448,7 +14448,7 @@
       </c>
       <c r="X154" s="2"/>
     </row>
-    <row r="155" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A155" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -14620,7 +14620,7 @@
       </c>
       <c r="X157" s="2"/>
     </row>
-    <row r="158" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A158" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -14684,10 +14684,10 @@
       </c>
       <c r="X158" s="2"/>
     </row>
-    <row r="159" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A159" s="44" t="str">
         <f t="shared" si="11"/>
-        <v>.....C.01. - Hypertensive heart disease</v>
+        <v>..C.01. - Hypertensive heart disease</v>
       </c>
       <c r="B159" s="2">
         <v>149</v>
@@ -14751,10 +14751,10 @@
       </c>
       <c r="X159" s="2"/>
     </row>
-    <row r="160" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A160" s="44" t="str">
         <f t="shared" si="11"/>
-        <v>.....C.02. - Ischaemic heart disease</v>
+        <v>..C.02. - Ischaemic heart disease</v>
       </c>
       <c r="B160" s="2">
         <v>150</v>
@@ -14821,7 +14821,7 @@
     <row r="161" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A161" s="44" t="str">
         <f t="shared" si="11"/>
-        <v>.....C.03. - Stroke</v>
+        <v>..C.03. - Stroke</v>
       </c>
       <c r="B161" s="2">
         <v>151</v>
@@ -14892,7 +14892,7 @@
     <row r="162" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A162" s="44" t="str">
         <f t="shared" si="11"/>
-        <v>.....C.04. - Cardiomyopathy, myocarditis, endocarditis</v>
+        <v>..C.04. - Cardiomyopathy, myocarditis, endocarditis</v>
       </c>
       <c r="B162" s="2">
         <v>152</v>
@@ -14961,7 +14961,7 @@
     <row r="163" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A163" s="44" t="str">
         <f t="shared" si="11"/>
-        <v>.....C.05. -  Congestive heart failure</v>
+        <v>..C.05. -  Congestive heart failure</v>
       </c>
       <c r="B163" s="2"/>
       <c r="C163" s="36"/>
@@ -15014,7 +15014,7 @@
     <row r="164" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A164" s="44" t="str">
         <f t="shared" si="11"/>
-        <v>.....C.99. - Other or unspecified cardiovascular diseases</v>
+        <v>..C.99. - Other or unspecified cardiovascular diseases</v>
       </c>
       <c r="B164" s="2">
         <v>153</v>
@@ -15084,7 +15084,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="165" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A165" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -15141,10 +15141,10 @@
       </c>
       <c r="X165" s="2"/>
     </row>
-    <row r="166" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A166" s="44" t="str">
         <f t="shared" si="11"/>
-        <v>.....D.66. - Chronic obstructive pulmonary disease</v>
+        <v>..D.66. - Chronic obstructive pulmonary disease</v>
       </c>
       <c r="B166" s="2">
         <v>155</v>
@@ -15204,10 +15204,10 @@
       </c>
       <c r="X166" s="2"/>
     </row>
-    <row r="167" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A167" s="44" t="str">
         <f t="shared" si="11"/>
-        <v>.....D.67. - Asthma</v>
+        <v>..D.67. - Asthma</v>
       </c>
       <c r="B167" s="2">
         <v>156</v>
@@ -15267,10 +15267,10 @@
       </c>
       <c r="X167" s="2"/>
     </row>
-    <row r="168" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A168" s="44" t="str">
         <f t="shared" si="11"/>
-        <v>.....D.68. - Other respiratory diseases</v>
+        <v>..D.68. - Other respiratory diseases</v>
       </c>
       <c r="B168" s="2">
         <v>157</v>
@@ -15330,10 +15330,10 @@
       </c>
       <c r="X168" s="2"/>
     </row>
-    <row r="169" spans="1:24" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A169" s="44" t="str">
         <f t="shared" si="11"/>
-        <v>.....D.09. - Digestive diseases (excluding cirrhosis)</v>
+        <v>..D.09. - Digestive diseases (excluding cirrhosis)</v>
       </c>
       <c r="B169" s="2">
         <v>158</v>
@@ -15392,7 +15392,7 @@
       </c>
       <c r="X169" s="2"/>
     </row>
-    <row r="170" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A170" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -15455,7 +15455,7 @@
     <row r="171" spans="1:24" s="48" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A171" s="44" t="str">
         <f t="shared" si="11"/>
-        <v>.....D.11. - Cirrhosis of the liver</v>
+        <v>..D.11. - Cirrhosis of the liver</v>
       </c>
       <c r="B171" s="2">
         <v>160</v>
@@ -15519,7 +15519,7 @@
       </c>
       <c r="X171" s="2"/>
     </row>
-    <row r="172" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A172" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -15579,7 +15579,7 @@
       </c>
       <c r="X172" s="2"/>
     </row>
-    <row r="173" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A173" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -15699,7 +15699,7 @@
       </c>
       <c r="X174" s="2"/>
     </row>
-    <row r="175" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A175" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -15759,7 +15759,7 @@
       </c>
       <c r="X175" s="2"/>
     </row>
-    <row r="176" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A176" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -15819,7 +15819,7 @@
       </c>
       <c r="X176" s="2"/>
     </row>
-    <row r="177" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A177" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -15998,10 +15998,10 @@
       </c>
       <c r="X179" s="2"/>
     </row>
-    <row r="180" spans="1:24" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A180" s="44" t="str">
         <f t="shared" si="11"/>
-        <v>.....D.10. - Kidney diseases</v>
+        <v>..D.10. - Kidney diseases</v>
       </c>
       <c r="B180" s="2">
         <v>169</v>
@@ -16060,10 +16060,10 @@
       </c>
       <c r="X180" s="2"/>
     </row>
-    <row r="181" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A181" s="44" t="str">
         <f t="shared" si="11"/>
-        <v>..........D.10.a. - Acute glomerulonephritis</v>
+        <v>...D.10.a. - Acute glomerulonephritis</v>
       </c>
       <c r="B181" s="2">
         <v>170</v>
@@ -16128,7 +16128,7 @@
     <row r="182" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A182" s="44" t="str">
         <f t="shared" si="11"/>
-        <v>..........D.10.b. - Chronic kidney diesease due to diabetes</v>
+        <v>...D.10.b. - Chronic kidney diesease due to diabetes</v>
       </c>
       <c r="B182" s="2">
         <v>171</v>
@@ -16190,10 +16190,10 @@
       </c>
       <c r="X182" s="2"/>
     </row>
-    <row r="183" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A183" s="44" t="str">
         <f t="shared" si="11"/>
-        <v>..........D.10.c. - Other chronic kidney disease</v>
+        <v>...D.10.c. - Other chronic kidney disease</v>
       </c>
       <c r="B183" s="2">
         <v>172</v>
@@ -16255,7 +16255,7 @@
       </c>
       <c r="X183" s="2"/>
     </row>
-    <row r="184" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A184" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -16311,7 +16311,7 @@
       </c>
       <c r="X184" s="2"/>
     </row>
-    <row r="185" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A185" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -16431,7 +16431,7 @@
       </c>
       <c r="X186" s="2"/>
     </row>
-    <row r="187" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A187" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -16491,7 +16491,7 @@
       </c>
       <c r="X187" s="2"/>
     </row>
-    <row r="188" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A188" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -16551,7 +16551,7 @@
       </c>
       <c r="X188" s="2"/>
     </row>
-    <row r="189" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A189" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -16609,7 +16609,7 @@
       </c>
       <c r="X189" s="2"/>
     </row>
-    <row r="190" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A190" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -16668,7 +16668,7 @@
       </c>
       <c r="X190" s="2"/>
     </row>
-    <row r="191" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A191" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -16728,7 +16728,7 @@
       </c>
       <c r="X191" s="2"/>
     </row>
-    <row r="192" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A192" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -16784,7 +16784,7 @@
       </c>
       <c r="X192" s="2"/>
     </row>
-    <row r="193" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A193" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -16840,7 +16840,7 @@
       </c>
       <c r="X193" s="2"/>
     </row>
-    <row r="194" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A194" s="44" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -16898,7 +16898,7 @@
     </row>
     <row r="195" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A195" s="44" t="str">
-        <f t="shared" ref="A195:A225" si="18">IF(H195&lt;&gt;"",IF(F195&lt;&gt;"",CONCATENATE("..........",D195,".",E195,".",F195,". - ",T195),IF(E195&lt;&gt;"",CONCATENATE(".....",D195,".",E195,". - ",T195),CONCATENATE(D195,". - ",T195))),"")</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="B195" s="2">
@@ -16960,10 +16960,10 @@
       </c>
       <c r="X195" s="2"/>
     </row>
-    <row r="196" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A196" s="44" t="str">
-        <f t="shared" si="18"/>
-        <v>.....D.12. - Congenital anomalies</v>
+        <f t="shared" ref="A196:A232" si="18">IF(H196&lt;&gt;"",IF(F196&lt;&gt;"",CONCATENATE("...",D196,".",E196,".",F196,". - ",T196),IF(E196&lt;&gt;"",CONCATENATE("..",D196,".",E196,". - ",T196),CONCATENATE(D196,". - ",T196))),"")</f>
+        <v>..D.12. - Congenital anomalies</v>
       </c>
       <c r="B196" s="2">
         <v>185</v>
@@ -17022,7 +17022,7 @@
       </c>
       <c r="X196" s="2"/>
     </row>
-    <row r="197" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A197" s="44" t="str">
         <f t="shared" si="18"/>
         <v/>
@@ -17082,7 +17082,7 @@
       </c>
       <c r="X197" s="2"/>
     </row>
-    <row r="198" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A198" s="44" t="str">
         <f t="shared" si="18"/>
         <v/>
@@ -17142,7 +17142,7 @@
       </c>
       <c r="X198" s="2"/>
     </row>
-    <row r="199" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A199" s="44" t="str">
         <f t="shared" si="18"/>
         <v/>
@@ -17202,7 +17202,7 @@
       </c>
       <c r="X199" s="2"/>
     </row>
-    <row r="200" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A200" s="44" t="str">
         <f t="shared" si="18"/>
         <v/>
@@ -17262,7 +17262,7 @@
       </c>
       <c r="X200" s="2"/>
     </row>
-    <row r="201" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A201" s="44" t="str">
         <f t="shared" si="18"/>
         <v/>
@@ -17382,7 +17382,7 @@
       </c>
       <c r="X202" s="2"/>
     </row>
-    <row r="203" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A203" s="44" t="str">
         <f t="shared" si="18"/>
         <v/>
@@ -17435,7 +17435,7 @@
       </c>
       <c r="X203" s="2"/>
     </row>
-    <row r="204" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A204" s="44" t="str">
         <f t="shared" si="18"/>
         <v/>
@@ -17491,7 +17491,7 @@
       </c>
       <c r="X204" s="2"/>
     </row>
-    <row r="205" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A205" s="44" t="str">
         <f t="shared" si="18"/>
         <v/>
@@ -17547,7 +17547,7 @@
       </c>
       <c r="X205" s="2"/>
     </row>
-    <row r="206" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A206" s="44" t="str">
         <f t="shared" si="18"/>
         <v/>
@@ -17603,7 +17603,7 @@
       </c>
       <c r="X206" s="2"/>
     </row>
-    <row r="207" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A207" s="44" t="str">
         <f t="shared" si="18"/>
         <v/>
@@ -17720,7 +17720,7 @@
     <row r="209" spans="1:24" ht="41.25" x14ac:dyDescent="0.25">
       <c r="A209" s="44" t="str">
         <f t="shared" si="18"/>
-        <v>.....E.01. - Unintentional injuries</v>
+        <v>..E.01. - Unintentional injuries</v>
       </c>
       <c r="B209" s="2">
         <v>198</v>
@@ -17780,7 +17780,7 @@
     <row r="210" spans="1:24" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A210" s="44" t="str">
         <f t="shared" si="18"/>
-        <v>..........E.01.a. - Road injury</v>
+        <v>...E.01.a. - Road injury</v>
       </c>
       <c r="B210" s="2">
         <v>199</v>
@@ -17846,7 +17846,7 @@
       </c>
       <c r="X210" s="2"/>
     </row>
-    <row r="211" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A211" s="44" t="str">
         <f t="shared" si="18"/>
         <v/>
@@ -17908,10 +17908,10 @@
       </c>
       <c r="X211" s="2"/>
     </row>
-    <row r="212" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A212" s="44" t="str">
         <f t="shared" si="18"/>
-        <v>..........E.01.b. - Falls</v>
+        <v>...E.01.b. - Falls</v>
       </c>
       <c r="B212" s="2">
         <v>201</v>
@@ -17975,7 +17975,7 @@
       </c>
       <c r="X212" s="2"/>
     </row>
-    <row r="213" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A213" s="44" t="str">
         <f t="shared" si="18"/>
         <v/>
@@ -18035,7 +18035,7 @@
       </c>
       <c r="X213" s="2"/>
     </row>
-    <row r="214" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A214" s="44" t="str">
         <f t="shared" si="18"/>
         <v/>
@@ -18162,7 +18162,7 @@
     <row r="216" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A216" s="44" t="str">
         <f t="shared" si="18"/>
-        <v>..........E.01.c. - Accidental Firearm</v>
+        <v>...E.01.c. - Accidental Firearm</v>
       </c>
       <c r="B216" s="2"/>
       <c r="C216" s="31" t="s">
@@ -18274,7 +18274,11 @@
       </c>
       <c r="X217" s="2"/>
     </row>
-    <row r="218" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A218" s="44" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
       <c r="B218" s="2"/>
       <c r="C218" s="31"/>
       <c r="D218" s="6"/>
@@ -18302,7 +18306,7 @@
     <row r="219" spans="1:24" ht="102" x14ac:dyDescent="0.25">
       <c r="A219" s="44" t="str">
         <f t="shared" si="18"/>
-        <v>..........E.01.x. - Other unintentional injuries</v>
+        <v>...E.01.x. - Other unintentional injuries</v>
       </c>
       <c r="B219" s="2">
         <v>206</v>
@@ -18370,7 +18374,7 @@
         <v>1282</v>
       </c>
     </row>
-    <row r="220" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A220" s="44" t="str">
         <f t="shared" si="18"/>
         <v/>
@@ -18426,7 +18430,7 @@
     <row r="221" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A221" s="44" t="str">
         <f t="shared" si="18"/>
-        <v>.....E.02. - Suicide/Self-harm</v>
+        <v>..E.02. - Suicide/Self-harm</v>
       </c>
       <c r="B221" s="2">
         <v>208</v>
@@ -18493,7 +18497,7 @@
     <row r="222" spans="1:24" ht="255" x14ac:dyDescent="0.25">
       <c r="A222" s="44" t="str">
         <f t="shared" si="18"/>
-        <v>.....E.03. - Homicide/Interpersonal violence</v>
+        <v>..E.03. - Homicide/Interpersonal violence</v>
       </c>
       <c r="B222" s="2">
         <v>209</v>
@@ -18550,10 +18554,10 @@
       </c>
       <c r="X222" s="2"/>
     </row>
-    <row r="223" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A223" s="44" t="str">
         <f t="shared" si="18"/>
-        <v>..........E.03.a. - Homicide excluding legal intervention</v>
+        <v>...E.03.a. - Homicide excluding legal intervention</v>
       </c>
       <c r="B223" s="2"/>
       <c r="C223" s="31"/>
@@ -18600,7 +18604,7 @@
     <row r="224" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A224" s="44" t="str">
         <f t="shared" si="18"/>
-        <v>..........E.03.b. - Legal intervention</v>
+        <v>...E.03.b. - Legal intervention</v>
       </c>
       <c r="B224" s="2"/>
       <c r="C224" s="31"/>
@@ -18647,7 +18651,7 @@
     <row r="225" spans="1:24" ht="153" x14ac:dyDescent="0.25">
       <c r="A225" s="44" t="str">
         <f t="shared" si="18"/>
-        <v>..........E.03.c. - Execution, War, Terroism</v>
+        <v>...E.03.c. - Execution, War, Terroism</v>
       </c>
       <c r="B225" s="2">
         <v>210</v>
@@ -18712,6 +18716,10 @@
       </c>
     </row>
     <row r="226" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A226" s="44" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
       <c r="B226" s="82" t="s">
         <v>1338</v>
       </c>
@@ -18747,8 +18755,8 @@
     </row>
     <row r="227" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A227" s="44" t="str">
-        <f t="shared" ref="A227:A232" si="23">IF(H227&lt;&gt;"",IF(F227&lt;&gt;"",CONCATENATE("..........",D227,".",E227,".",F227,". - ",T227),IF(E227&lt;&gt;"",CONCATENATE(".....",D227,".",E227,". - ",T227),CONCATENATE(D227,". - ",T227))),"")</f>
-        <v>.....Z.01. - Symptoms, signs and ill-defined conditions, not elsewhere classified</v>
+        <f t="shared" si="18"/>
+        <v>..Z.01. - Symptoms, signs and ill-defined conditions, not elsewhere classified</v>
       </c>
       <c r="D227" s="56" t="s">
         <v>1245</v>
@@ -18782,7 +18790,7 @@
     </row>
     <row r="228" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A228" s="44" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="D228" s="56" t="s">
@@ -18812,10 +18820,10 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="229" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A229" s="44" t="str">
-        <f t="shared" si="23"/>
-        <v>.....Z.02. - Unknown/Missing Value</v>
+        <f t="shared" si="18"/>
+        <v>..Z.02. - Unknown/Missing Value</v>
       </c>
       <c r="D229" s="56" t="s">
         <v>1245</v>
@@ -18825,7 +18833,7 @@
       </c>
       <c r="G229" s="43"/>
       <c r="H229" s="40" t="str">
-        <f t="shared" ref="H229:H232" si="24">CONCATENATE(D229,E229,F229)</f>
+        <f t="shared" ref="H229:H232" si="23">CONCATENATE(D229,E229,F229)</f>
         <v>Z02</v>
       </c>
       <c r="T229" s="48" t="s">
@@ -18834,8 +18842,8 @@
     </row>
     <row r="230" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A230" s="44" t="str">
-        <f t="shared" si="23"/>
-        <v>.....Z.03. - Code does not map</v>
+        <f t="shared" si="18"/>
+        <v>..Z.03. - Code does not map</v>
       </c>
       <c r="D230" s="56" t="s">
         <v>1245</v>
@@ -18845,7 +18853,7 @@
       </c>
       <c r="G230" s="43"/>
       <c r="H230" s="40" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>Z03</v>
       </c>
       <c r="I230" s="16" t="s">
@@ -18855,9 +18863,9 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="231" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A231" s="44" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v>Z. - Unknown/Missing Value</v>
       </c>
       <c r="D231" s="56" t="s">
@@ -18865,17 +18873,17 @@
       </c>
       <c r="G231" s="43"/>
       <c r="H231" s="40" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>Z</v>
       </c>
       <c r="T231" s="48" t="s">
         <v>1316</v>
       </c>
     </row>
-    <row r="232" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A232" s="44" t="str">
-        <f t="shared" si="23"/>
-        <v>.....D.99. - Other Chronic Conditions</v>
+        <f t="shared" si="18"/>
+        <v>..D.99. - Other Chronic Conditions</v>
       </c>
       <c r="D232" s="56" t="s">
         <v>1142</v>
@@ -18885,7 +18893,7 @@
       </c>
       <c r="G232" s="43"/>
       <c r="H232" s="40" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>D99</v>
       </c>
       <c r="T232" s="48" t="s">

</xml_diff>

<commit_message>
cause list revisions (kidney disase) for OSHPD; other minor edits
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/gbd.ICD.Map.xlsx
+++ b/myCBD/myInfo/gbd.ICD.Map.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0.CBD\myCBD\myInfo\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="10935"/>
   </bookViews>
@@ -19,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$A$1:$X$225</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -36,7 +31,7 @@
     <author>Dauphine, David (CDPH-CHSI)</author>
   </authors>
   <commentList>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -60,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C57" authorId="1" shapeId="0">
+    <comment ref="C57" authorId="1">
       <text>
         <r>
           <rPr>
@@ -84,7 +79,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P126" authorId="2" shapeId="0">
+    <comment ref="P126" authorId="2">
       <text>
         <r>
           <rPr>
@@ -113,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2852" uniqueCount="1392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2858" uniqueCount="1392">
   <si>
     <t>I. Communicable, maternal, perinatal and nutritional conditions</t>
   </si>
@@ -4446,7 +4441,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###0.;###0."/>
   </numFmts>
@@ -5097,7 +5092,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5132,7 +5127,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5344,15 +5339,15 @@
   <dimension ref="A1:X232"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B220" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B171" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A228" sqref="A228"/>
+      <selection pane="bottomRight" activeCell="M182" sqref="M182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.85546875" style="44" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" style="44" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" style="46" customWidth="1"/>
     <col min="3" max="3" width="35.7109375" style="44" customWidth="1"/>
     <col min="4" max="4" width="4.42578125" style="56" customWidth="1"/>
@@ -5363,7 +5358,9 @@
     <col min="9" max="9" width="28.85546875" style="16" customWidth="1"/>
     <col min="10" max="10" width="10" style="48" customWidth="1"/>
     <col min="11" max="11" width="29.85546875" style="16" customWidth="1"/>
-    <col min="12" max="14" width="71.28515625" style="16" customWidth="1"/>
+    <col min="12" max="12" width="33.42578125" style="16" customWidth="1"/>
+    <col min="13" max="13" width="27.5703125" style="16" customWidth="1"/>
+    <col min="14" max="14" width="71.28515625" style="16" customWidth="1"/>
     <col min="15" max="15" width="16.42578125" style="72" customWidth="1"/>
     <col min="16" max="16" width="35.140625" style="72" customWidth="1"/>
     <col min="17" max="17" width="38.42578125" style="73" customWidth="1"/>
@@ -8310,7 +8307,7 @@
     <row r="53" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A53" s="44" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>...A.07.a. - Lower respiratory infections</v>
       </c>
       <c r="B53" s="2">
         <v>48</v>
@@ -8324,12 +8321,17 @@
       <c r="E53" s="26" t="s">
         <v>1150</v>
       </c>
-      <c r="F53" s="6"/>
+      <c r="F53" s="6" t="s">
+        <v>1126</v>
+      </c>
       <c r="G53" s="40" t="str">
         <f>CONCATENATE("c",D53,E53,F53)</f>
-        <v>cA07</v>
-      </c>
-      <c r="H53" s="40"/>
+        <v>cA07a</v>
+      </c>
+      <c r="H53" s="40" t="str">
+        <f t="shared" ref="H53:H54" si="3">CONCATENATE(D53,E53,F53)</f>
+        <v>A07a</v>
+      </c>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
       <c r="K53" s="5" t="s">
@@ -8374,7 +8376,7 @@
     <row r="54" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A54" s="44" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>...A.07.b. - Upper respiratory infections</v>
       </c>
       <c r="B54" s="2">
         <v>49</v>
@@ -8388,12 +8390,17 @@
       <c r="E54" s="26" t="s">
         <v>1150</v>
       </c>
-      <c r="F54" s="6"/>
+      <c r="F54" s="6" t="s">
+        <v>1127</v>
+      </c>
       <c r="G54" s="40" t="str">
         <f>CONCATENATE("c",D54,E54,F54)</f>
-        <v>cA07</v>
-      </c>
-      <c r="H54" s="40"/>
+        <v>cA07b</v>
+      </c>
+      <c r="H54" s="40" t="str">
+        <f t="shared" si="3"/>
+        <v>A07b</v>
+      </c>
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
       <c r="K54" s="5" t="s">
@@ -8580,7 +8587,7 @@
       </c>
       <c r="F57" s="6"/>
       <c r="G57" s="40" t="str">
-        <f t="shared" ref="G57:G62" si="3">CONCATENATE("c",D57,E57,F57)</f>
+        <f t="shared" ref="G57:G62" si="4">CONCATENATE("c",D57,E57,F57)</f>
         <v>cA08</v>
       </c>
       <c r="H57" s="40"/>
@@ -8646,7 +8653,7 @@
       </c>
       <c r="F58" s="6"/>
       <c r="G58" s="40" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>cA08</v>
       </c>
       <c r="H58" s="40"/>
@@ -8710,7 +8717,7 @@
       </c>
       <c r="F59" s="6"/>
       <c r="G59" s="40" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>cA08</v>
       </c>
       <c r="H59" s="40"/>
@@ -8776,7 +8783,7 @@
       </c>
       <c r="F60" s="6"/>
       <c r="G60" s="40" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>cA08</v>
       </c>
       <c r="H60" s="40"/>
@@ -8840,7 +8847,7 @@
       </c>
       <c r="F61" s="6"/>
       <c r="G61" s="40" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>cA08</v>
       </c>
       <c r="H61" s="40"/>
@@ -8904,7 +8911,7 @@
       </c>
       <c r="F62" s="6"/>
       <c r="G62" s="40" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>cA08</v>
       </c>
       <c r="H62" s="40"/>
@@ -9011,7 +9018,7 @@
       </c>
       <c r="X63" s="2"/>
     </row>
-    <row r="64" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -9127,7 +9134,7 @@
       </c>
       <c r="X65" s="2"/>
     </row>
-    <row r="66" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A66" s="44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -9249,9 +9256,9 @@
       </c>
       <c r="X67" s="2"/>
     </row>
-    <row r="68" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A68" s="44" t="str">
-        <f t="shared" ref="A68:A131" si="4">IF(H68&lt;&gt;"",IF(F68&lt;&gt;"",CONCATENATE("...",D68,".",E68,".",F68,". - ",T68),IF(E68&lt;&gt;"",CONCATENATE("..",D68,".",E68,". - ",T68),CONCATENATE(D68,". - ",T68))),"")</f>
+        <f t="shared" ref="A68:A131" si="5">IF(H68&lt;&gt;"",IF(F68&lt;&gt;"",CONCATENATE("...",D68,".",E68,".",F68,". - ",T68),IF(E68&lt;&gt;"",CONCATENATE("..",D68,".",E68,". - ",T68),CONCATENATE(D68,". - ",T68))),"")</f>
         <v/>
       </c>
       <c r="B68" s="2">
@@ -9304,9 +9311,9 @@
       </c>
       <c r="X68" s="2"/>
     </row>
-    <row r="69" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A69" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B69" s="2">
@@ -9362,9 +9369,9 @@
       </c>
       <c r="X69" s="2"/>
     </row>
-    <row r="70" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A70" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B70" s="2">
@@ -9420,9 +9427,9 @@
       </c>
       <c r="X70" s="2"/>
     </row>
-    <row r="71" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A71" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B71" s="2">
@@ -9474,9 +9481,9 @@
       </c>
       <c r="X71" s="2"/>
     </row>
-    <row r="72" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A72" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B72" s="2">
@@ -9532,9 +9539,9 @@
       </c>
       <c r="X72" s="2"/>
     </row>
-    <row r="73" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A73" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B73" s="2">
@@ -9592,7 +9599,7 @@
     </row>
     <row r="74" spans="1:24" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A74" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B74" s="2">
@@ -9643,9 +9650,9 @@
       </c>
       <c r="X74" s="2"/>
     </row>
-    <row r="75" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A75" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>D. - Other Chronic</v>
       </c>
       <c r="B75" s="2"/>
@@ -9683,7 +9690,7 @@
     </row>
     <row r="76" spans="1:24" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A76" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>B. - Cancer/Malignant neoplasms</v>
       </c>
       <c r="B76" s="2">
@@ -9739,9 +9746,9 @@
       </c>
       <c r="X76" s="2"/>
     </row>
-    <row r="77" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A77" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>..B.01. - Mouth and oropharynx cancers</v>
       </c>
       <c r="B77" s="2">
@@ -9758,7 +9765,7 @@
       </c>
       <c r="F77" s="6"/>
       <c r="G77" s="40" t="str">
-        <f t="shared" ref="G77:G86" si="5">CONCATENATE("c",D77,E77,F77)</f>
+        <f t="shared" ref="G77:G86" si="6">CONCATENATE("c",D77,E77,F77)</f>
         <v>cB01</v>
       </c>
       <c r="H77" s="40" t="str">
@@ -9800,7 +9807,7 @@
     </row>
     <row r="78" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A78" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B78" s="2">
@@ -9817,7 +9824,7 @@
       </c>
       <c r="F78" s="6"/>
       <c r="G78" s="40" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>cB01</v>
       </c>
       <c r="H78" s="40"/>
@@ -9862,9 +9869,9 @@
       </c>
       <c r="X78" s="2"/>
     </row>
-    <row r="79" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A79" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B79" s="2">
@@ -9881,7 +9888,7 @@
       </c>
       <c r="F79" s="6"/>
       <c r="G79" s="40" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>cB01</v>
       </c>
       <c r="H79" s="40"/>
@@ -9926,9 +9933,9 @@
       </c>
       <c r="X79" s="2"/>
     </row>
-    <row r="80" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A80" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B80" s="2">
@@ -9945,7 +9952,7 @@
       </c>
       <c r="F80" s="6"/>
       <c r="G80" s="40" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>cB01</v>
       </c>
       <c r="H80" s="40"/>
@@ -9986,9 +9993,9 @@
       </c>
       <c r="X80" s="2"/>
     </row>
-    <row r="81" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A81" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>..B.02. - Oesophagus cancer</v>
       </c>
       <c r="B81" s="2">
@@ -10005,11 +10012,11 @@
       </c>
       <c r="F81" s="6"/>
       <c r="G81" s="40" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>cB02</v>
       </c>
       <c r="H81" s="40" t="str">
-        <f t="shared" ref="H81:H87" si="6">CONCATENATE(D81,E81,F81)</f>
+        <f t="shared" ref="H81:H87" si="7">CONCATENATE(D81,E81,F81)</f>
         <v>B02</v>
       </c>
       <c r="I81" s="18" t="s">
@@ -10053,9 +10060,9 @@
       </c>
       <c r="X81" s="2"/>
     </row>
-    <row r="82" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A82" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>..B.03. - Stomach cancer</v>
       </c>
       <c r="B82" s="2">
@@ -10072,11 +10079,11 @@
       </c>
       <c r="F82" s="6"/>
       <c r="G82" s="40" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>cB03</v>
       </c>
       <c r="H82" s="40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>B03</v>
       </c>
       <c r="I82" s="18" t="s">
@@ -10124,7 +10131,7 @@
     </row>
     <row r="83" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A83" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>..B.04. - Colon and rectum cancers</v>
       </c>
       <c r="B83" s="2">
@@ -10141,11 +10148,11 @@
       </c>
       <c r="F83" s="6"/>
       <c r="G83" s="40" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>cB04</v>
       </c>
       <c r="H83" s="40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>B04</v>
       </c>
       <c r="I83" s="16" t="s">
@@ -10189,9 +10196,9 @@
       </c>
       <c r="X83" s="2"/>
     </row>
-    <row r="84" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A84" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>..B.05. - Liver cancer</v>
       </c>
       <c r="B84" s="2">
@@ -10208,11 +10215,11 @@
       </c>
       <c r="F84" s="6"/>
       <c r="G84" s="40" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>cB05</v>
       </c>
       <c r="H84" s="40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>B05</v>
       </c>
       <c r="I84" s="18" t="s">
@@ -10256,9 +10263,9 @@
       </c>
       <c r="X84" s="2"/>
     </row>
-    <row r="85" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A85" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>..B.06. - Pancreas cancer</v>
       </c>
       <c r="B85" s="2">
@@ -10275,11 +10282,11 @@
       </c>
       <c r="F85" s="6"/>
       <c r="G85" s="40" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>cB06</v>
       </c>
       <c r="H85" s="40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>B06</v>
       </c>
       <c r="I85" s="18" t="s">
@@ -10323,9 +10330,9 @@
       </c>
       <c r="X85" s="2"/>
     </row>
-    <row r="86" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A86" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>..B.07. - Trachea, bronchus and lung cancers</v>
       </c>
       <c r="B86" s="2">
@@ -10342,11 +10349,11 @@
       </c>
       <c r="F86" s="6"/>
       <c r="G86" s="40" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>cB07</v>
       </c>
       <c r="H86" s="40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>B07</v>
       </c>
       <c r="I86" s="18" t="s">
@@ -10390,9 +10397,9 @@
       </c>
       <c r="X86" s="2"/>
     </row>
-    <row r="87" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A87" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>..B.08. - Melanoma and other skin cancers</v>
       </c>
       <c r="B87" s="2">
@@ -10412,7 +10419,7 @@
         <v>952</v>
       </c>
       <c r="H87" s="40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>B08</v>
       </c>
       <c r="J87" s="17" t="s">
@@ -10451,7 +10458,7 @@
     </row>
     <row r="88" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A88" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B88" s="2">
@@ -10468,7 +10475,7 @@
       </c>
       <c r="F88" s="6"/>
       <c r="G88" s="40" t="str">
-        <f t="shared" ref="G88:G103" si="7">CONCATENATE("c",D88,E88,F88)</f>
+        <f t="shared" ref="G88:G103" si="8">CONCATENATE("c",D88,E88,F88)</f>
         <v>cB08</v>
       </c>
       <c r="H88" s="40"/>
@@ -10513,9 +10520,9 @@
       </c>
       <c r="X88" s="2"/>
     </row>
-    <row r="89" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A89" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B89" s="2">
@@ -10532,7 +10539,7 @@
       </c>
       <c r="F89" s="6"/>
       <c r="G89" s="40" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>cB08</v>
       </c>
       <c r="H89" s="40"/>
@@ -10577,9 +10584,9 @@
       </c>
       <c r="X89" s="2"/>
     </row>
-    <row r="90" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A90" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>..B.09. - Breast cancer</v>
       </c>
       <c r="B90" s="2">
@@ -10596,7 +10603,7 @@
       </c>
       <c r="F90" s="6"/>
       <c r="G90" s="40" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>cB09</v>
       </c>
       <c r="H90" s="40" t="str">
@@ -10644,9 +10651,9 @@
       </c>
       <c r="X90" s="2"/>
     </row>
-    <row r="91" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A91" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>..B.10. - Uterine cancer</v>
       </c>
       <c r="B91" s="2"/>
@@ -10687,9 +10694,9 @@
       <c r="W91" s="45"/>
       <c r="X91" s="2"/>
     </row>
-    <row r="92" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A92" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B92" s="2">
@@ -10753,7 +10760,7 @@
     </row>
     <row r="93" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A93" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B93" s="2">
@@ -10770,7 +10777,7 @@
       </c>
       <c r="F93" s="6"/>
       <c r="G93" s="40" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>cB10</v>
       </c>
       <c r="H93" s="40"/>
@@ -10815,9 +10822,9 @@
       </c>
       <c r="X93" s="2"/>
     </row>
-    <row r="94" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A94" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>..B.11. - Ovary cancer</v>
       </c>
       <c r="B94" s="2">
@@ -10834,7 +10841,7 @@
       </c>
       <c r="F94" s="6"/>
       <c r="G94" s="40" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>cB11</v>
       </c>
       <c r="H94" s="40" t="str">
@@ -10882,9 +10889,9 @@
       </c>
       <c r="X94" s="2"/>
     </row>
-    <row r="95" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A95" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>..B.12. - Prostate cancer</v>
       </c>
       <c r="B95" s="2">
@@ -10901,7 +10908,7 @@
       </c>
       <c r="F95" s="6"/>
       <c r="G95" s="40" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>cB12</v>
       </c>
       <c r="H95" s="40" t="str">
@@ -10949,9 +10956,9 @@
       </c>
       <c r="X95" s="2"/>
     </row>
-    <row r="96" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A96" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B96" s="2">
@@ -10968,7 +10975,7 @@
       </c>
       <c r="F96" s="6"/>
       <c r="G96" s="40" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>cB99</v>
       </c>
       <c r="H96" s="40"/>
@@ -11015,7 +11022,7 @@
     </row>
     <row r="97" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A97" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>..B.13. - Kidney, renal pelvis and ureter cancer</v>
       </c>
       <c r="B97" s="2">
@@ -11032,7 +11039,7 @@
       </c>
       <c r="F97" s="6"/>
       <c r="G97" s="40" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>cB13</v>
       </c>
       <c r="H97" s="40" t="str">
@@ -11080,9 +11087,9 @@
       </c>
       <c r="X97" s="2"/>
     </row>
-    <row r="98" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A98" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>..B.14. - Bladder cancer</v>
       </c>
       <c r="B98" s="2">
@@ -11099,7 +11106,7 @@
       </c>
       <c r="F98" s="6"/>
       <c r="G98" s="40" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>cB14</v>
       </c>
       <c r="H98" s="40" t="str">
@@ -11149,7 +11156,7 @@
     </row>
     <row r="99" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A99" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>..B.15. - Brain and nervous system cancers</v>
       </c>
       <c r="B99" s="2">
@@ -11166,7 +11173,7 @@
       </c>
       <c r="F99" s="6"/>
       <c r="G99" s="40" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>cB15</v>
       </c>
       <c r="H99" s="40" t="str">
@@ -11214,9 +11221,9 @@
       </c>
       <c r="X99" s="2"/>
     </row>
-    <row r="100" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A100" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B100" s="2">
@@ -11233,7 +11240,7 @@
       </c>
       <c r="F100" s="6"/>
       <c r="G100" s="40" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>cB99</v>
       </c>
       <c r="H100" s="40"/>
@@ -11278,9 +11285,9 @@
       </c>
       <c r="X100" s="2"/>
     </row>
-    <row r="101" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A101" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B101" s="2">
@@ -11297,7 +11304,7 @@
       </c>
       <c r="F101" s="6"/>
       <c r="G101" s="40" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>cB99</v>
       </c>
       <c r="H101" s="40"/>
@@ -11342,9 +11349,9 @@
       </c>
       <c r="X101" s="2"/>
     </row>
-    <row r="102" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A102" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B102" s="2">
@@ -11361,7 +11368,7 @@
       </c>
       <c r="F102" s="6"/>
       <c r="G102" s="40" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>cB99</v>
       </c>
       <c r="H102" s="40"/>
@@ -11406,9 +11413,9 @@
       </c>
       <c r="X102" s="2"/>
     </row>
-    <row r="103" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A103" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B103" s="2">
@@ -11425,7 +11432,7 @@
       </c>
       <c r="F103" s="6"/>
       <c r="G103" s="40" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>cB99</v>
       </c>
       <c r="H103" s="40"/>
@@ -11466,9 +11473,9 @@
       </c>
       <c r="X103" s="2"/>
     </row>
-    <row r="104" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A104" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>..B.16. - Lymphomas and multiple myeloma</v>
       </c>
       <c r="B104" s="2">
@@ -11486,7 +11493,7 @@
       <c r="F104" s="6"/>
       <c r="G104" s="40"/>
       <c r="H104" s="40" t="str">
-        <f t="shared" ref="H104:H109" si="8">CONCATENATE(D104,E104,F104)</f>
+        <f t="shared" ref="H104:H109" si="9">CONCATENATE(D104,E104,F104)</f>
         <v>B16</v>
       </c>
       <c r="I104" s="5"/>
@@ -11526,9 +11533,9 @@
       </c>
       <c r="X104" s="2"/>
     </row>
-    <row r="105" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A105" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>...B.16.a. - Hodgkin lymphoma</v>
       </c>
       <c r="B105" s="2">
@@ -11547,11 +11554,11 @@
         <v>1126</v>
       </c>
       <c r="G105" s="40" t="str">
-        <f t="shared" ref="G105:G111" si="9">CONCATENATE("c",D105,E105,F105)</f>
+        <f t="shared" ref="G105:G111" si="10">CONCATENATE("c",D105,E105,F105)</f>
         <v>cB16a</v>
       </c>
       <c r="H105" s="40" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>B16a</v>
       </c>
       <c r="I105" s="5"/>
@@ -11591,9 +11598,9 @@
       </c>
       <c r="X105" s="2"/>
     </row>
-    <row r="106" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A106" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>...B.16.b. - Non-Hodgkin lymphoma</v>
       </c>
       <c r="B106" s="2">
@@ -11612,11 +11619,11 @@
         <v>1127</v>
       </c>
       <c r="G106" s="40" t="str">
+        <f t="shared" si="10"/>
+        <v>cB16b</v>
+      </c>
+      <c r="H106" s="40" t="str">
         <f t="shared" si="9"/>
-        <v>cB16b</v>
-      </c>
-      <c r="H106" s="40" t="str">
-        <f t="shared" si="8"/>
         <v>B16b</v>
       </c>
       <c r="I106" s="5"/>
@@ -11656,9 +11663,9 @@
       </c>
       <c r="X106" s="2"/>
     </row>
-    <row r="107" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A107" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>...B.16.c. - Multiple myeloma</v>
       </c>
       <c r="B107" s="2">
@@ -11677,11 +11684,11 @@
         <v>1130</v>
       </c>
       <c r="G107" s="40" t="str">
+        <f t="shared" si="10"/>
+        <v>cB16c</v>
+      </c>
+      <c r="H107" s="40" t="str">
         <f t="shared" si="9"/>
-        <v>cB16c</v>
-      </c>
-      <c r="H107" s="40" t="str">
-        <f t="shared" si="8"/>
         <v>B16c</v>
       </c>
       <c r="I107" s="5"/>
@@ -11721,9 +11728,9 @@
       </c>
       <c r="X107" s="2"/>
     </row>
-    <row r="108" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A108" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>..B.17. - Leukaemia</v>
       </c>
       <c r="B108" s="2">
@@ -11740,11 +11747,11 @@
       </c>
       <c r="F108" s="6"/>
       <c r="G108" s="40" t="str">
+        <f t="shared" si="10"/>
+        <v>cB17</v>
+      </c>
+      <c r="H108" s="40" t="str">
         <f t="shared" si="9"/>
-        <v>cB17</v>
-      </c>
-      <c r="H108" s="40" t="str">
-        <f t="shared" si="8"/>
         <v>B17</v>
       </c>
       <c r="I108" s="5"/>
@@ -11786,7 +11793,7 @@
     </row>
     <row r="109" spans="1:24" ht="51" x14ac:dyDescent="0.25">
       <c r="A109" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>..B.99. - Other malignant neoplasms</v>
       </c>
       <c r="B109" s="2">
@@ -11803,11 +11810,11 @@
       </c>
       <c r="F109" s="6"/>
       <c r="G109" s="40" t="str">
+        <f t="shared" si="10"/>
+        <v>cB99</v>
+      </c>
+      <c r="H109" s="40" t="str">
         <f t="shared" si="9"/>
-        <v>cB99</v>
-      </c>
-      <c r="H109" s="40" t="str">
-        <f t="shared" si="8"/>
         <v>B99</v>
       </c>
       <c r="I109" s="5" t="s">
@@ -11849,7 +11856,7 @@
     </row>
     <row r="110" spans="1:24" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A110" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B110" s="2">
@@ -11866,7 +11873,7 @@
       </c>
       <c r="F110" s="6"/>
       <c r="G110" s="40" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>cD99</v>
       </c>
       <c r="H110" s="40"/>
@@ -11907,7 +11914,7 @@
     </row>
     <row r="111" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A111" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>..D.01. - Diabetes mellitus</v>
       </c>
       <c r="B111" s="2">
@@ -11924,7 +11931,7 @@
       </c>
       <c r="F111" s="6"/>
       <c r="G111" s="40" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>cD01</v>
       </c>
       <c r="H111" s="40" t="str">
@@ -11980,7 +11987,7 @@
     </row>
     <row r="112" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A112" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>..D.02. - Endocrine, blood, immune disorders</v>
       </c>
       <c r="B112" s="2">
@@ -12040,9 +12047,9 @@
       </c>
       <c r="X112" s="2"/>
     </row>
-    <row r="113" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A113" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B113" s="2">
@@ -12100,9 +12107,9 @@
       </c>
       <c r="X113" s="2"/>
     </row>
-    <row r="114" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A114" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B114" s="2">
@@ -12162,7 +12169,7 @@
     </row>
     <row r="115" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A115" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B115" s="2">
@@ -12222,7 +12229,7 @@
     </row>
     <row r="116" spans="1:24" ht="33" x14ac:dyDescent="0.25">
       <c r="A116" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B116" s="2">
@@ -12280,9 +12287,9 @@
       </c>
       <c r="X116" s="2"/>
     </row>
-    <row r="117" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:24" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A117" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B117" s="2">
@@ -12341,7 +12348,7 @@
     </row>
     <row r="118" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A118" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">..D.03. - Mental Health disorders </v>
       </c>
       <c r="B118" s="2"/>
@@ -12383,9 +12390,9 @@
       <c r="W118" s="45"/>
       <c r="X118" s="2"/>
     </row>
-    <row r="119" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A119" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">..D.04. - Substance use </v>
       </c>
       <c r="B119" s="2"/>
@@ -12425,9 +12432,9 @@
       <c r="W119" s="45"/>
       <c r="X119" s="2"/>
     </row>
-    <row r="120" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A120" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B120" s="2"/>
@@ -12456,9 +12463,9 @@
       <c r="W120" s="45"/>
       <c r="X120" s="2"/>
     </row>
-    <row r="121" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A121" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B121" s="2">
@@ -12505,9 +12512,9 @@
       </c>
       <c r="X121" s="2"/>
     </row>
-    <row r="122" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A122" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B122" s="2">
@@ -12565,9 +12572,9 @@
       </c>
       <c r="X122" s="2"/>
     </row>
-    <row r="123" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A123" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B123" s="2">
@@ -12625,9 +12632,9 @@
       </c>
       <c r="X123" s="2"/>
     </row>
-    <row r="124" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A124" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B124" s="2">
@@ -12685,9 +12692,9 @@
       </c>
       <c r="X124" s="2"/>
     </row>
-    <row r="125" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A125" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B125" s="2">
@@ -12751,7 +12758,7 @@
     </row>
     <row r="126" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A126" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>...D.04.a. - Alcohol use disorders</v>
       </c>
       <c r="B126" s="2">
@@ -12818,9 +12825,9 @@
       </c>
       <c r="X126" s="2"/>
     </row>
-    <row r="127" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A127" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B127" s="2">
@@ -12871,9 +12878,9 @@
       </c>
       <c r="X127" s="2"/>
     </row>
-    <row r="128" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A128" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>...D.04.b. - Opioid use disorders</v>
       </c>
       <c r="B128" s="2">
@@ -12892,7 +12899,7 @@
         <v>1127</v>
       </c>
       <c r="G128" s="40" t="str">
-        <f t="shared" ref="G128:G135" si="10">CONCATENATE("c",D128,E128,F128)</f>
+        <f t="shared" ref="G128:G135" si="11">CONCATENATE("c",D128,E128,F128)</f>
         <v>cD04b</v>
       </c>
       <c r="H128" s="40" t="str">
@@ -12936,9 +12943,9 @@
       </c>
       <c r="X128" s="2"/>
     </row>
-    <row r="129" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A129" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>...D.04.c. - Cocaine use disorders</v>
       </c>
       <c r="B129" s="2">
@@ -12957,7 +12964,7 @@
         <v>1130</v>
       </c>
       <c r="G129" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>cD04c</v>
       </c>
       <c r="H129" s="40" t="str">
@@ -13001,9 +13008,9 @@
       </c>
       <c r="X129" s="2"/>
     </row>
-    <row r="130" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A130" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>...D.04.d. - Amphetamine use disorders</v>
       </c>
       <c r="B130" s="2">
@@ -13022,7 +13029,7 @@
         <v>1154</v>
       </c>
       <c r="G130" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>cD04d</v>
       </c>
       <c r="H130" s="40" t="str">
@@ -13066,9 +13073,9 @@
       </c>
       <c r="X130" s="2"/>
     </row>
-    <row r="131" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A131" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B131" s="2">
@@ -13085,7 +13092,7 @@
       </c>
       <c r="F131" s="6"/>
       <c r="G131" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>cD04</v>
       </c>
       <c r="H131" s="40"/>
@@ -13121,9 +13128,9 @@
       </c>
       <c r="X131" s="2"/>
     </row>
-    <row r="132" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A132" s="44" t="str">
-        <f t="shared" ref="A132:A195" si="11">IF(H132&lt;&gt;"",IF(F132&lt;&gt;"",CONCATENATE("...",D132,".",E132,".",F132,". - ",T132),IF(E132&lt;&gt;"",CONCATENATE("..",D132,".",E132,". - ",T132),CONCATENATE(D132,". - ",T132))),"")</f>
+        <f t="shared" ref="A132:A195" si="12">IF(H132&lt;&gt;"",IF(F132&lt;&gt;"",CONCATENATE("...",D132,".",E132,".",F132,". - ",T132),IF(E132&lt;&gt;"",CONCATENATE("..",D132,".",E132,". - ",T132),CONCATENATE(D132,". - ",T132))),"")</f>
         <v/>
       </c>
       <c r="B132" s="2">
@@ -13140,7 +13147,7 @@
       </c>
       <c r="F132" s="6"/>
       <c r="G132" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>cD04</v>
       </c>
       <c r="H132" s="40"/>
@@ -13187,9 +13194,9 @@
         <v>1238</v>
       </c>
     </row>
-    <row r="133" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A133" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B133" s="2">
@@ -13206,7 +13213,7 @@
       </c>
       <c r="F133" s="6"/>
       <c r="G133" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>cD03</v>
       </c>
       <c r="H133" s="40"/>
@@ -13243,9 +13250,9 @@
       </c>
       <c r="X133" s="2"/>
     </row>
-    <row r="134" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A134" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B134" s="2">
@@ -13262,7 +13269,7 @@
       </c>
       <c r="F134" s="6"/>
       <c r="G134" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>cD03</v>
       </c>
       <c r="H134" s="40"/>
@@ -13303,9 +13310,9 @@
       </c>
       <c r="X134" s="2"/>
     </row>
-    <row r="135" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A135" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B135" s="2">
@@ -13322,7 +13329,7 @@
       </c>
       <c r="F135" s="6"/>
       <c r="G135" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>cD03</v>
       </c>
       <c r="H135" s="40"/>
@@ -13359,9 +13366,9 @@
       </c>
       <c r="X135" s="2"/>
     </row>
-    <row r="136" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A136" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B136" s="2">
@@ -13408,9 +13415,9 @@
       </c>
       <c r="X136" s="2"/>
     </row>
-    <row r="137" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A137" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B137" s="2">
@@ -13464,9 +13471,9 @@
       </c>
       <c r="X137" s="2"/>
     </row>
-    <row r="138" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A138" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B138" s="2">
@@ -13520,9 +13527,9 @@
       </c>
       <c r="X138" s="2"/>
     </row>
-    <row r="139" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A139" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B139" s="2">
@@ -13578,7 +13585,7 @@
     </row>
     <row r="140" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A140" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B140" s="2">
@@ -13632,9 +13639,9 @@
       </c>
       <c r="X140" s="2"/>
     </row>
-    <row r="141" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A141" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B141" s="2">
@@ -13691,9 +13698,9 @@
         <v>607</v>
       </c>
     </row>
-    <row r="142" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:24" ht="102" x14ac:dyDescent="0.25">
       <c r="A142" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>..D.05. - Alzheimer’s disease and other dementias</v>
       </c>
       <c r="B142" s="2">
@@ -13710,7 +13717,7 @@
       </c>
       <c r="F142" s="6"/>
       <c r="G142" s="40" t="str">
-        <f t="shared" ref="G142:G148" si="12">CONCATENATE("c",D142,E142,F142)</f>
+        <f t="shared" ref="G142:G148" si="13">CONCATENATE("c",D142,E142,F142)</f>
         <v>cD05</v>
       </c>
       <c r="H142" s="40" t="str">
@@ -13754,9 +13761,9 @@
       </c>
       <c r="X142" s="2"/>
     </row>
-    <row r="143" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A143" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B143" s="2">
@@ -13773,7 +13780,7 @@
       </c>
       <c r="F143" s="6"/>
       <c r="G143" s="40" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>cD06</v>
       </c>
       <c r="H143" s="40"/>
@@ -13814,9 +13821,9 @@
       </c>
       <c r="X143" s="2"/>
     </row>
-    <row r="144" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A144" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B144" s="2">
@@ -13833,7 +13840,7 @@
       </c>
       <c r="F144" s="6"/>
       <c r="G144" s="40" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>cD06</v>
       </c>
       <c r="H144" s="40"/>
@@ -13874,9 +13881,9 @@
       </c>
       <c r="X144" s="2"/>
     </row>
-    <row r="145" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A145" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B145" s="2">
@@ -13893,7 +13900,7 @@
       </c>
       <c r="F145" s="6"/>
       <c r="G145" s="40" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>cD06</v>
       </c>
       <c r="H145" s="40"/>
@@ -13934,9 +13941,9 @@
       </c>
       <c r="X145" s="2"/>
     </row>
-    <row r="146" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A146" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B146" s="2">
@@ -13953,7 +13960,7 @@
       </c>
       <c r="F146" s="6"/>
       <c r="G146" s="40" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>cD06</v>
       </c>
       <c r="H146" s="40"/>
@@ -13990,9 +13997,9 @@
       </c>
       <c r="X146" s="2"/>
     </row>
-    <row r="147" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A147" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B147" s="2">
@@ -14009,7 +14016,7 @@
       </c>
       <c r="F147" s="6"/>
       <c r="G147" s="40" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>cD06</v>
       </c>
       <c r="H147" s="40"/>
@@ -14048,7 +14055,7 @@
     </row>
     <row r="148" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A148" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>..D.06. - Other neurological conditions</v>
       </c>
       <c r="B148" s="2">
@@ -14065,7 +14072,7 @@
       </c>
       <c r="F148" s="6"/>
       <c r="G148" s="40" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>cD06</v>
       </c>
       <c r="H148" s="40" t="str">
@@ -14113,9 +14120,9 @@
       </c>
       <c r="X148" s="2"/>
     </row>
-    <row r="149" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A149" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B149" s="2">
@@ -14168,9 +14175,9 @@
         <v>614</v>
       </c>
     </row>
-    <row r="150" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A150" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B150" s="2">
@@ -14187,7 +14194,7 @@
       </c>
       <c r="F150" s="6"/>
       <c r="G150" s="40" t="str">
-        <f t="shared" ref="G150:G156" si="13">CONCATENATE("c",D150,E150,F150)</f>
+        <f t="shared" ref="G150:G156" si="14">CONCATENATE("c",D150,E150,F150)</f>
         <v>cD99</v>
       </c>
       <c r="H150" s="40"/>
@@ -14224,9 +14231,9 @@
       </c>
       <c r="X150" s="2"/>
     </row>
-    <row r="151" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A151" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B151" s="2">
@@ -14243,7 +14250,7 @@
       </c>
       <c r="F151" s="6"/>
       <c r="G151" s="40" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>cD99</v>
       </c>
       <c r="H151" s="40"/>
@@ -14280,9 +14287,9 @@
       </c>
       <c r="X151" s="2"/>
     </row>
-    <row r="152" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A152" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B152" s="2">
@@ -14299,7 +14306,7 @@
       </c>
       <c r="F152" s="6"/>
       <c r="G152" s="40" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>cD99</v>
       </c>
       <c r="H152" s="40"/>
@@ -14336,9 +14343,9 @@
       </c>
       <c r="X152" s="2"/>
     </row>
-    <row r="153" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A153" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B153" s="2">
@@ -14355,7 +14362,7 @@
       </c>
       <c r="F153" s="6"/>
       <c r="G153" s="40" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>cD99</v>
       </c>
       <c r="H153" s="40"/>
@@ -14392,9 +14399,9 @@
       </c>
       <c r="X153" s="2"/>
     </row>
-    <row r="154" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A154" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B154" s="2">
@@ -14411,7 +14418,7 @@
       </c>
       <c r="F154" s="6"/>
       <c r="G154" s="40" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>cD99</v>
       </c>
       <c r="H154" s="40"/>
@@ -14448,9 +14455,9 @@
       </c>
       <c r="X154" s="2"/>
     </row>
-    <row r="155" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A155" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B155" s="2">
@@ -14467,7 +14474,7 @@
       </c>
       <c r="F155" s="6"/>
       <c r="G155" s="40" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>cD99</v>
       </c>
       <c r="H155" s="40"/>
@@ -14506,7 +14513,7 @@
     </row>
     <row r="156" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A156" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B156" s="2">
@@ -14523,7 +14530,7 @@
       </c>
       <c r="F156" s="6"/>
       <c r="G156" s="40" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>cD99</v>
       </c>
       <c r="H156" s="40"/>
@@ -14564,7 +14571,7 @@
     </row>
     <row r="157" spans="1:24" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A157" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>C. - Cardiovascular diseases</v>
       </c>
       <c r="B157" s="2">
@@ -14620,9 +14627,9 @@
       </c>
       <c r="X157" s="2"/>
     </row>
-    <row r="158" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A158" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B158" s="2">
@@ -14639,7 +14646,7 @@
       </c>
       <c r="F158" s="6"/>
       <c r="G158" s="40" t="str">
-        <f t="shared" ref="G158:G164" si="14">CONCATENATE("c",D158,E158,F158)</f>
+        <f t="shared" ref="G158:G164" si="15">CONCATENATE("c",D158,E158,F158)</f>
         <v>cC99</v>
       </c>
       <c r="H158" s="40"/>
@@ -14684,9 +14691,9 @@
       </c>
       <c r="X158" s="2"/>
     </row>
-    <row r="159" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A159" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>..C.01. - Hypertensive heart disease</v>
       </c>
       <c r="B159" s="2">
@@ -14703,11 +14710,11 @@
       </c>
       <c r="F159" s="6"/>
       <c r="G159" s="40" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>cC01</v>
       </c>
       <c r="H159" s="40" t="str">
-        <f t="shared" ref="H159:H164" si="15">CONCATENATE(D159,E159,F159)</f>
+        <f t="shared" ref="H159:H164" si="16">CONCATENATE(D159,E159,F159)</f>
         <v>C01</v>
       </c>
       <c r="I159" s="5"/>
@@ -14751,9 +14758,9 @@
       </c>
       <c r="X159" s="2"/>
     </row>
-    <row r="160" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A160" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>..C.02. - Ischaemic heart disease</v>
       </c>
       <c r="B160" s="2">
@@ -14770,11 +14777,11 @@
       </c>
       <c r="F160" s="6"/>
       <c r="G160" s="40" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>cC02</v>
       </c>
       <c r="H160" s="40" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C02</v>
       </c>
       <c r="I160" s="5"/>
@@ -14820,7 +14827,7 @@
     </row>
     <row r="161" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A161" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>..C.03. - Stroke</v>
       </c>
       <c r="B161" s="2">
@@ -14837,11 +14844,11 @@
       </c>
       <c r="F161" s="6"/>
       <c r="G161" s="40" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>cC03</v>
       </c>
       <c r="H161" s="40" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C03</v>
       </c>
       <c r="I161" s="5" t="s">
@@ -14891,7 +14898,7 @@
     </row>
     <row r="162" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A162" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>..C.04. - Cardiomyopathy, myocarditis, endocarditis</v>
       </c>
       <c r="B162" s="2">
@@ -14908,11 +14915,11 @@
       </c>
       <c r="F162" s="6"/>
       <c r="G162" s="40" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>cC04</v>
       </c>
       <c r="H162" s="40" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C04</v>
       </c>
       <c r="I162" s="5"/>
@@ -14960,7 +14967,7 @@
     </row>
     <row r="163" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A163" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>..C.05. -  Congestive heart failure</v>
       </c>
       <c r="B163" s="2"/>
@@ -14973,11 +14980,11 @@
       </c>
       <c r="F163" s="6"/>
       <c r="G163" s="40" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>cC05</v>
       </c>
       <c r="H163" s="40" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C05</v>
       </c>
       <c r="I163" s="5" t="s">
@@ -15013,7 +15020,7 @@
     </row>
     <row r="164" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A164" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>..C.99. - Other or unspecified cardiovascular diseases</v>
       </c>
       <c r="B164" s="2">
@@ -15030,11 +15037,11 @@
       </c>
       <c r="F164" s="6"/>
       <c r="G164" s="40" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>cC99</v>
       </c>
       <c r="H164" s="40" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C99</v>
       </c>
       <c r="I164" s="5" t="s">
@@ -15084,9 +15091,9 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="165" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A165" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B165" s="2">
@@ -15141,9 +15148,9 @@
       </c>
       <c r="X165" s="2"/>
     </row>
-    <row r="166" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A166" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>..D.66. - Chronic obstructive pulmonary disease</v>
       </c>
       <c r="B166" s="2">
@@ -15204,9 +15211,9 @@
       </c>
       <c r="X166" s="2"/>
     </row>
-    <row r="167" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A167" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>..D.67. - Asthma</v>
       </c>
       <c r="B167" s="2">
@@ -15267,9 +15274,9 @@
       </c>
       <c r="X167" s="2"/>
     </row>
-    <row r="168" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A168" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>..D.68. - Other respiratory diseases</v>
       </c>
       <c r="B168" s="2">
@@ -15330,9 +15337,9 @@
       </c>
       <c r="X168" s="2"/>
     </row>
-    <row r="169" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:24" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A169" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>..D.09. - Digestive diseases (excluding cirrhosis)</v>
       </c>
       <c r="B169" s="2">
@@ -15392,9 +15399,9 @@
       </c>
       <c r="X169" s="2"/>
     </row>
-    <row r="170" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A170" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B170" s="2">
@@ -15411,7 +15418,7 @@
       </c>
       <c r="F170" s="6"/>
       <c r="G170" s="40" t="str">
-        <f t="shared" ref="G170:G178" si="16">CONCATENATE("c",D170,E170,F170)</f>
+        <f t="shared" ref="G170:G178" si="17">CONCATENATE("c",D170,E170,F170)</f>
         <v>cD09</v>
       </c>
       <c r="H170" s="40"/>
@@ -15454,7 +15461,7 @@
     </row>
     <row r="171" spans="1:24" s="48" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A171" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>..D.11. - Cirrhosis of the liver</v>
       </c>
       <c r="B171" s="2">
@@ -15471,7 +15478,7 @@
       </c>
       <c r="F171" s="6"/>
       <c r="G171" s="40" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>cD11</v>
       </c>
       <c r="H171" s="40" t="str">
@@ -15519,9 +15526,9 @@
       </c>
       <c r="X171" s="2"/>
     </row>
-    <row r="172" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A172" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B172" s="2">
@@ -15538,7 +15545,7 @@
       </c>
       <c r="F172" s="6"/>
       <c r="G172" s="40" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>cD09</v>
       </c>
       <c r="H172" s="40"/>
@@ -15579,9 +15586,9 @@
       </c>
       <c r="X172" s="2"/>
     </row>
-    <row r="173" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A173" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B173" s="2">
@@ -15598,7 +15605,7 @@
       </c>
       <c r="F173" s="6"/>
       <c r="G173" s="40" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>cD09</v>
       </c>
       <c r="H173" s="40"/>
@@ -15641,7 +15648,7 @@
     </row>
     <row r="174" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A174" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B174" s="2">
@@ -15658,7 +15665,7 @@
       </c>
       <c r="F174" s="6"/>
       <c r="G174" s="40" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>cD09</v>
       </c>
       <c r="H174" s="40"/>
@@ -15699,9 +15706,9 @@
       </c>
       <c r="X174" s="2"/>
     </row>
-    <row r="175" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A175" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B175" s="2">
@@ -15718,7 +15725,7 @@
       </c>
       <c r="F175" s="6"/>
       <c r="G175" s="40" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>cD09</v>
       </c>
       <c r="H175" s="40"/>
@@ -15759,9 +15766,9 @@
       </c>
       <c r="X175" s="2"/>
     </row>
-    <row r="176" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A176" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B176" s="2">
@@ -15778,7 +15785,7 @@
       </c>
       <c r="F176" s="6"/>
       <c r="G176" s="40" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>cD09</v>
       </c>
       <c r="H176" s="40"/>
@@ -15819,9 +15826,9 @@
       </c>
       <c r="X176" s="2"/>
     </row>
-    <row r="177" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A177" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B177" s="2">
@@ -15838,7 +15845,7 @@
       </c>
       <c r="F177" s="6"/>
       <c r="G177" s="40" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>cD09</v>
       </c>
       <c r="H177" s="40"/>
@@ -15881,7 +15888,7 @@
     </row>
     <row r="178" spans="1:24" ht="51" x14ac:dyDescent="0.25">
       <c r="A178" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B178" s="2">
@@ -15898,7 +15905,7 @@
       </c>
       <c r="F178" s="6"/>
       <c r="G178" s="40" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>cD09</v>
       </c>
       <c r="H178" s="40"/>
@@ -15945,7 +15952,7 @@
     </row>
     <row r="179" spans="1:24" ht="33" x14ac:dyDescent="0.25">
       <c r="A179" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B179" s="2">
@@ -15998,9 +16005,9 @@
       </c>
       <c r="X179" s="2"/>
     </row>
-    <row r="180" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:24" ht="51" x14ac:dyDescent="0.25">
       <c r="A180" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>..D.10. - Kidney diseases</v>
       </c>
       <c r="B180" s="2">
@@ -16032,7 +16039,9 @@
         <v>952</v>
       </c>
       <c r="M180" s="49"/>
-      <c r="N180" s="49"/>
+      <c r="N180" s="49" t="s">
+        <v>952</v>
+      </c>
       <c r="O180" s="59" t="s">
         <v>954</v>
       </c>
@@ -16060,9 +16069,9 @@
       </c>
       <c r="X180" s="2"/>
     </row>
-    <row r="181" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A181" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>...D.10.a. - Acute glomerulonephritis</v>
       </c>
       <c r="B181" s="2">
@@ -16081,7 +16090,7 @@
         <v>1126</v>
       </c>
       <c r="G181" s="40" t="str">
-        <f t="shared" ref="G181:G189" si="17">CONCATENATE("c",D181,E181,F181)</f>
+        <f t="shared" ref="G181:G189" si="18">CONCATENATE("c",D181,E181,F181)</f>
         <v>cD10a</v>
       </c>
       <c r="H181" s="40" t="str">
@@ -16097,7 +16106,9 @@
         <v>847</v>
       </c>
       <c r="M181" s="49"/>
-      <c r="N181" s="49"/>
+      <c r="N181" s="49" t="s">
+        <v>847</v>
+      </c>
       <c r="O181" s="59" t="s">
         <v>955</v>
       </c>
@@ -16125,9 +16136,9 @@
       </c>
       <c r="X181" s="2"/>
     </row>
-    <row r="182" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:24" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A182" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>...D.10.b. - Chronic kidney diesease due to diabetes</v>
       </c>
       <c r="B182" s="2">
@@ -16146,7 +16157,7 @@
         <v>1127</v>
       </c>
       <c r="G182" s="40" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>cD10b</v>
       </c>
       <c r="H182" s="40" t="str">
@@ -16162,7 +16173,9 @@
         <v>848</v>
       </c>
       <c r="M182" s="49"/>
-      <c r="N182" s="49"/>
+      <c r="N182" s="49" t="s">
+        <v>848</v>
+      </c>
       <c r="O182" s="59" t="s">
         <v>956</v>
       </c>
@@ -16190,9 +16203,9 @@
       </c>
       <c r="X182" s="2"/>
     </row>
-    <row r="183" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:24" ht="102" x14ac:dyDescent="0.25">
       <c r="A183" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>...D.10.c. - Other chronic kidney disease</v>
       </c>
       <c r="B183" s="2">
@@ -16211,7 +16224,7 @@
         <v>1130</v>
       </c>
       <c r="G183" s="40" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>cD10c</v>
       </c>
       <c r="H183" s="40" t="str">
@@ -16227,7 +16240,9 @@
         <v>959</v>
       </c>
       <c r="M183" s="49"/>
-      <c r="N183" s="49"/>
+      <c r="N183" s="49" t="s">
+        <v>959</v>
+      </c>
       <c r="O183" s="59" t="s">
         <v>957</v>
       </c>
@@ -16255,9 +16270,9 @@
       </c>
       <c r="X183" s="2"/>
     </row>
-    <row r="184" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A184" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B184" s="2">
@@ -16274,7 +16289,7 @@
       </c>
       <c r="F184" s="6"/>
       <c r="G184" s="40" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>cD99</v>
       </c>
       <c r="H184" s="40"/>
@@ -16311,9 +16326,9 @@
       </c>
       <c r="X184" s="2"/>
     </row>
-    <row r="185" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A185" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B185" s="2">
@@ -16330,7 +16345,7 @@
       </c>
       <c r="F185" s="6"/>
       <c r="G185" s="40" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>cD99</v>
       </c>
       <c r="H185" s="40"/>
@@ -16373,7 +16388,7 @@
     </row>
     <row r="186" spans="1:24" ht="33" x14ac:dyDescent="0.25">
       <c r="A186" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B186" s="2">
@@ -16390,7 +16405,7 @@
       </c>
       <c r="F186" s="6"/>
       <c r="G186" s="40" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>cD99</v>
       </c>
       <c r="H186" s="40"/>
@@ -16431,9 +16446,9 @@
       </c>
       <c r="X186" s="2"/>
     </row>
-    <row r="187" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A187" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B187" s="2">
@@ -16450,7 +16465,7 @@
       </c>
       <c r="F187" s="6"/>
       <c r="G187" s="40" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>cD99</v>
       </c>
       <c r="H187" s="40"/>
@@ -16491,9 +16506,9 @@
       </c>
       <c r="X187" s="2"/>
     </row>
-    <row r="188" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A188" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B188" s="2">
@@ -16510,7 +16525,7 @@
       </c>
       <c r="F188" s="6"/>
       <c r="G188" s="40" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>cD99</v>
       </c>
       <c r="H188" s="40"/>
@@ -16551,9 +16566,9 @@
       </c>
       <c r="X188" s="2"/>
     </row>
-    <row r="189" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A189" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B189" s="2">
@@ -16570,7 +16585,7 @@
       </c>
       <c r="F189" s="6"/>
       <c r="G189" s="40" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>cD99</v>
       </c>
       <c r="H189" s="40"/>
@@ -16609,9 +16624,9 @@
       </c>
       <c r="X189" s="2"/>
     </row>
-    <row r="190" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A190" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B190" s="2">
@@ -16668,9 +16683,9 @@
       </c>
       <c r="X190" s="2"/>
     </row>
-    <row r="191" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A191" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B191" s="2">
@@ -16728,9 +16743,9 @@
       </c>
       <c r="X191" s="2"/>
     </row>
-    <row r="192" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A192" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B192" s="2">
@@ -16784,9 +16799,9 @@
       </c>
       <c r="X192" s="2"/>
     </row>
-    <row r="193" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A193" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B193" s="2">
@@ -16840,9 +16855,9 @@
       </c>
       <c r="X193" s="2"/>
     </row>
-    <row r="194" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A194" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B194" s="2">
@@ -16898,7 +16913,7 @@
     </row>
     <row r="195" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A195" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B195" s="2">
@@ -16960,9 +16975,9 @@
       </c>
       <c r="X195" s="2"/>
     </row>
-    <row r="196" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A196" s="44" t="str">
-        <f t="shared" ref="A196:A232" si="18">IF(H196&lt;&gt;"",IF(F196&lt;&gt;"",CONCATENATE("...",D196,".",E196,".",F196,". - ",T196),IF(E196&lt;&gt;"",CONCATENATE("..",D196,".",E196,". - ",T196),CONCATENATE(D196,". - ",T196))),"")</f>
+        <f t="shared" ref="A196:A232" si="19">IF(H196&lt;&gt;"",IF(F196&lt;&gt;"",CONCATENATE("...",D196,".",E196,".",F196,". - ",T196),IF(E196&lt;&gt;"",CONCATENATE("..",D196,".",E196,". - ",T196),CONCATENATE(D196,". - ",T196))),"")</f>
         <v>..D.12. - Congenital anomalies</v>
       </c>
       <c r="B196" s="2">
@@ -17022,9 +17037,9 @@
       </c>
       <c r="X196" s="2"/>
     </row>
-    <row r="197" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A197" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B197" s="2">
@@ -17041,7 +17056,7 @@
       </c>
       <c r="F197" s="6"/>
       <c r="G197" s="40" t="str">
-        <f t="shared" ref="G197:G202" si="19">CONCATENATE("c",D197,E197,F197)</f>
+        <f t="shared" ref="G197:G202" si="20">CONCATENATE("c",D197,E197,F197)</f>
         <v>cD12</v>
       </c>
       <c r="H197" s="40"/>
@@ -17082,9 +17097,9 @@
       </c>
       <c r="X197" s="2"/>
     </row>
-    <row r="198" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A198" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B198" s="2">
@@ -17101,7 +17116,7 @@
       </c>
       <c r="F198" s="6"/>
       <c r="G198" s="40" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>cD12</v>
       </c>
       <c r="H198" s="40"/>
@@ -17142,9 +17157,9 @@
       </c>
       <c r="X198" s="2"/>
     </row>
-    <row r="199" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A199" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B199" s="2">
@@ -17161,7 +17176,7 @@
       </c>
       <c r="F199" s="6"/>
       <c r="G199" s="40" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>cD12</v>
       </c>
       <c r="H199" s="40"/>
@@ -17202,9 +17217,9 @@
       </c>
       <c r="X199" s="2"/>
     </row>
-    <row r="200" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A200" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B200" s="2">
@@ -17221,7 +17236,7 @@
       </c>
       <c r="F200" s="6"/>
       <c r="G200" s="40" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>cD12</v>
       </c>
       <c r="H200" s="40"/>
@@ -17262,9 +17277,9 @@
       </c>
       <c r="X200" s="2"/>
     </row>
-    <row r="201" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A201" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B201" s="2">
@@ -17281,7 +17296,7 @@
       </c>
       <c r="F201" s="6"/>
       <c r="G201" s="40" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>cD12</v>
       </c>
       <c r="H201" s="40"/>
@@ -17324,7 +17339,7 @@
     </row>
     <row r="202" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A202" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B202" s="2">
@@ -17341,7 +17356,7 @@
       </c>
       <c r="F202" s="6"/>
       <c r="G202" s="40" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>cD12</v>
       </c>
       <c r="H202" s="40"/>
@@ -17382,9 +17397,9 @@
       </c>
       <c r="X202" s="2"/>
     </row>
-    <row r="203" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A203" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B203" s="2">
@@ -17435,9 +17450,9 @@
       </c>
       <c r="X203" s="2"/>
     </row>
-    <row r="204" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A204" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B204" s="2">
@@ -17491,9 +17506,9 @@
       </c>
       <c r="X204" s="2"/>
     </row>
-    <row r="205" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A205" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B205" s="2">
@@ -17547,9 +17562,9 @@
       </c>
       <c r="X205" s="2"/>
     </row>
-    <row r="206" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A206" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B206" s="2">
@@ -17603,9 +17618,9 @@
       </c>
       <c r="X206" s="2"/>
     </row>
-    <row r="207" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A207" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B207" s="2">
@@ -17661,7 +17676,7 @@
     </row>
     <row r="208" spans="1:24" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A208" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>E. - Injuries</v>
       </c>
       <c r="B208" s="2">
@@ -17717,9 +17732,9 @@
       </c>
       <c r="X208" s="2"/>
     </row>
-    <row r="209" spans="1:24" ht="41.25" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A209" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>..E.01. - Unintentional injuries</v>
       </c>
       <c r="B209" s="2">
@@ -17777,9 +17792,9 @@
       </c>
       <c r="X209" s="2"/>
     </row>
-    <row r="210" spans="1:24" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:24" ht="51" x14ac:dyDescent="0.25">
       <c r="A210" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>...E.01.a. - Road injury</v>
       </c>
       <c r="B210" s="2">
@@ -17798,7 +17813,7 @@
         <v>1126</v>
       </c>
       <c r="G210" s="40" t="str">
-        <f t="shared" ref="G210:G219" si="20">CONCATENATE("c",D210,E210,F210)</f>
+        <f t="shared" ref="G210:G219" si="21">CONCATENATE("c",D210,E210,F210)</f>
         <v>cE01a</v>
       </c>
       <c r="H210" s="40" t="str">
@@ -17846,9 +17861,9 @@
       </c>
       <c r="X210" s="2"/>
     </row>
-    <row r="211" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A211" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B211" s="2">
@@ -17867,7 +17882,7 @@
         <v>1128</v>
       </c>
       <c r="G211" s="40" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>cE01x</v>
       </c>
       <c r="H211" s="40"/>
@@ -17908,9 +17923,9 @@
       </c>
       <c r="X211" s="2"/>
     </row>
-    <row r="212" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A212" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>...E.01.b. - Falls</v>
       </c>
       <c r="B212" s="2">
@@ -17929,7 +17944,7 @@
         <v>1127</v>
       </c>
       <c r="G212" s="40" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>cE01b</v>
       </c>
       <c r="H212" s="40" t="str">
@@ -17975,9 +17990,9 @@
       </c>
       <c r="X212" s="2"/>
     </row>
-    <row r="213" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A213" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B213" s="2">
@@ -17996,7 +18011,7 @@
         <v>1128</v>
       </c>
       <c r="G213" s="40" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>cE01x</v>
       </c>
       <c r="H213" s="40"/>
@@ -18035,9 +18050,9 @@
       </c>
       <c r="X213" s="2"/>
     </row>
-    <row r="214" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A214" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B214" s="2">
@@ -18056,7 +18071,7 @@
         <v>1128</v>
       </c>
       <c r="G214" s="40" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>cE01x</v>
       </c>
       <c r="H214" s="40"/>
@@ -18099,7 +18114,7 @@
     </row>
     <row r="215" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A215" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B215" s="2">
@@ -18118,7 +18133,7 @@
         <v>1128</v>
       </c>
       <c r="G215" s="40" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>cE01x</v>
       </c>
       <c r="H215" s="40"/>
@@ -18159,9 +18174,9 @@
       </c>
       <c r="X215" s="2"/>
     </row>
-    <row r="216" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A216" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>...E.01.c. - Accidental Firearm</v>
       </c>
       <c r="B216" s="2"/>
@@ -18178,7 +18193,7 @@
         <v>1130</v>
       </c>
       <c r="G216" s="40" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>cE01c</v>
       </c>
       <c r="H216" s="40" t="str">
@@ -18214,7 +18229,7 @@
     </row>
     <row r="217" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A217" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B217" s="2">
@@ -18233,7 +18248,7 @@
         <v>1128</v>
       </c>
       <c r="G217" s="40" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>cE01x</v>
       </c>
       <c r="H217" s="40"/>
@@ -18274,9 +18289,9 @@
       </c>
       <c r="X217" s="2"/>
     </row>
-    <row r="218" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A218" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B218" s="2"/>
@@ -18305,7 +18320,7 @@
     </row>
     <row r="219" spans="1:24" ht="102" x14ac:dyDescent="0.25">
       <c r="A219" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>...E.01.x. - Other unintentional injuries</v>
       </c>
       <c r="B219" s="2">
@@ -18324,7 +18339,7 @@
         <v>1128</v>
       </c>
       <c r="G219" s="40" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>cE01x</v>
       </c>
       <c r="H219" s="40" t="str">
@@ -18374,9 +18389,9 @@
         <v>1282</v>
       </c>
     </row>
-    <row r="220" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A220" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B220" s="2">
@@ -18427,9 +18442,9 @@
       </c>
       <c r="X220" s="2"/>
     </row>
-    <row r="221" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:24" ht="51" x14ac:dyDescent="0.25">
       <c r="A221" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>..E.02. - Suicide/Self-harm</v>
       </c>
       <c r="B221" s="2">
@@ -18446,7 +18461,7 @@
       </c>
       <c r="F221" s="6"/>
       <c r="G221" s="40" t="str">
-        <f t="shared" ref="G221:G228" si="21">CONCATENATE("c",D221,E221,F221)</f>
+        <f t="shared" ref="G221:G228" si="22">CONCATENATE("c",D221,E221,F221)</f>
         <v>cE02</v>
       </c>
       <c r="H221" s="40" t="str">
@@ -18496,7 +18511,7 @@
     </row>
     <row r="222" spans="1:24" ht="255" x14ac:dyDescent="0.25">
       <c r="A222" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>..E.03. - Homicide/Interpersonal violence</v>
       </c>
       <c r="B222" s="2">
@@ -18554,9 +18569,9 @@
       </c>
       <c r="X222" s="2"/>
     </row>
-    <row r="223" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:24" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A223" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>...E.03.a. - Homicide excluding legal intervention</v>
       </c>
       <c r="B223" s="2"/>
@@ -18571,11 +18586,11 @@
         <v>1126</v>
       </c>
       <c r="G223" s="40" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>cE03a</v>
       </c>
       <c r="H223" s="40" t="str">
-        <f t="shared" ref="H223:H225" si="22">CONCATENATE(D223,E223,F223)</f>
+        <f t="shared" ref="H223:H225" si="23">CONCATENATE(D223,E223,F223)</f>
         <v>E03a</v>
       </c>
       <c r="I223" s="5"/>
@@ -18601,9 +18616,9 @@
       <c r="W223" s="45"/>
       <c r="X223" s="2"/>
     </row>
-    <row r="224" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A224" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>...E.03.b. - Legal intervention</v>
       </c>
       <c r="B224" s="2"/>
@@ -18618,11 +18633,11 @@
         <v>1127</v>
       </c>
       <c r="G224" s="40" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>cE03b</v>
       </c>
       <c r="H224" s="40" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>E03b</v>
       </c>
       <c r="I224" s="5"/>
@@ -18650,7 +18665,7 @@
     </row>
     <row r="225" spans="1:24" ht="153" x14ac:dyDescent="0.25">
       <c r="A225" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>...E.03.c. - Execution, War, Terroism</v>
       </c>
       <c r="B225" s="2">
@@ -18669,11 +18684,11 @@
         <v>1130</v>
       </c>
       <c r="G225" s="40" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>cE03c</v>
       </c>
       <c r="H225" s="40" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>E03c</v>
       </c>
       <c r="I225" s="5" t="s">
@@ -18717,7 +18732,7 @@
     </row>
     <row r="226" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A226" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B226" s="82" t="s">
@@ -18733,7 +18748,7 @@
         <v>1144</v>
       </c>
       <c r="G226" s="40" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>cE01</v>
       </c>
       <c r="H226" s="40"/>
@@ -18753,9 +18768,9 @@
         <v>1221</v>
       </c>
     </row>
-    <row r="227" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:24" ht="178.5" x14ac:dyDescent="0.25">
       <c r="A227" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>..Z.01. - Symptoms, signs and ill-defined conditions, not elsewhere classified</v>
       </c>
       <c r="D227" s="56" t="s">
@@ -18765,7 +18780,7 @@
         <v>1144</v>
       </c>
       <c r="G227" s="40" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>cZ01</v>
       </c>
       <c r="H227" s="40" t="str">
@@ -18790,7 +18805,7 @@
     </row>
     <row r="228" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A228" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="D228" s="56" t="s">
@@ -18800,7 +18815,7 @@
         <v>1152</v>
       </c>
       <c r="G228" s="42" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>cA09</v>
       </c>
       <c r="H228" s="40"/>
@@ -18820,9 +18835,9 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="229" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A229" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>..Z.02. - Unknown/Missing Value</v>
       </c>
       <c r="D229" s="56" t="s">
@@ -18833,16 +18848,16 @@
       </c>
       <c r="G229" s="43"/>
       <c r="H229" s="40" t="str">
-        <f t="shared" ref="H229:H232" si="23">CONCATENATE(D229,E229,F229)</f>
+        <f t="shared" ref="H229:H232" si="24">CONCATENATE(D229,E229,F229)</f>
         <v>Z02</v>
       </c>
       <c r="T229" s="48" t="s">
         <v>1316</v>
       </c>
     </row>
-    <row r="230" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A230" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>..Z.03. - Code does not map</v>
       </c>
       <c r="D230" s="56" t="s">
@@ -18853,7 +18868,7 @@
       </c>
       <c r="G230" s="43"/>
       <c r="H230" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>Z03</v>
       </c>
       <c r="I230" s="16" t="s">
@@ -18863,9 +18878,9 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="231" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A231" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>Z. - Unknown/Missing Value</v>
       </c>
       <c r="D231" s="56" t="s">
@@ -18873,16 +18888,16 @@
       </c>
       <c r="G231" s="43"/>
       <c r="H231" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>Z</v>
       </c>
       <c r="T231" s="48" t="s">
         <v>1316</v>
       </c>
     </row>
-    <row r="232" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A232" s="44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>..D.99. - Other Chronic Conditions</v>
       </c>
       <c r="D232" s="56" t="s">
@@ -18893,7 +18908,7 @@
       </c>
       <c r="G232" s="43"/>
       <c r="H232" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>D99</v>
       </c>
       <c r="T232" s="48" t="s">

</xml_diff>

<commit_message>
tab text and data clean up
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/gbd.ICD.Map.xlsx
+++ b/myCBD/myInfo/gbd.ICD.Map.xlsx
@@ -5339,10 +5339,10 @@
   <dimension ref="A1:X232"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B171" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H155" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M182" sqref="M182"/>
+      <selection pane="bottomRight" activeCell="N157" sqref="N157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -5448,7 +5448,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="44" t="str">
         <f>V2</f>
         <v>All CAUSES</v>
@@ -5494,7 +5494,7 @@
       </c>
       <c r="X2" s="6"/>
     </row>
-    <row r="3" spans="1:24" ht="66" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="153" x14ac:dyDescent="0.25">
       <c r="A3" s="44" t="str">
         <f>IF(H3&lt;&gt;"",IF(F3&lt;&gt;"",CONCATENATE("...",D3,".",E3,".",F3,". - ",T3),IF(E3&lt;&gt;"",CONCATENATE("..",D3,".",E3,". - ",T3),CONCATENATE(D3,". - ",T3))),"")</f>
         <v>A. - Communicable, maternal, perinatal and nutritional conditions</v>
@@ -5548,9 +5548,9 @@
       </c>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A4" s="44" t="str">
-        <f t="shared" ref="A4:A67" si="0">IF(H4&lt;&gt;"",IF(F4&lt;&gt;"",CONCATENATE("...",D4,".",E4,".",F4,". - ",T4),IF(E4&lt;&gt;"",CONCATENATE("..",D4,".",E4,". - ",T4),CONCATENATE(D4,". - ",T4))),"")</f>
+        <f>IF(H4&lt;&gt;"",IF(F4&lt;&gt;"",CONCATENATE("...",D4,".",E4,".",F4,". - ",T4),IF(E4&lt;&gt;"",CONCATENATE("..",D4,".",E4,". - ",T4),CONCATENATE(D4,". - ",T4))),"")</f>
         <v>..A.99. - Other Infectious Diseases</v>
       </c>
       <c r="B4" s="2"/>
@@ -5592,7 +5592,7 @@
     </row>
     <row r="5" spans="1:24" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A5" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H5&lt;&gt;"",IF(F5&lt;&gt;"",CONCATENATE("...",D5,".",E5,".",F5,". - ",T5),IF(E5&lt;&gt;"",CONCATENATE("..",D5,".",E5,". - ",T5),CONCATENATE(D5,". - ",T5))),"")</f>
         <v/>
       </c>
       <c r="B5" s="2">
@@ -5641,9 +5641,9 @@
       </c>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A6" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H6&lt;&gt;"",IF(F6&lt;&gt;"",CONCATENATE("...",D6,".",E6,".",F6,". - ",T6),IF(E6&lt;&gt;"",CONCATENATE("..",D6,".",E6,". - ",T6),CONCATENATE(D6,". - ",T6))),"")</f>
         <v>..A.01. - Tuberculosis</v>
       </c>
       <c r="B6" s="2">
@@ -5702,9 +5702,9 @@
       </c>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A7" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H7&lt;&gt;"",IF(F7&lt;&gt;"",CONCATENATE("...",D7,".",E7,".",F7,". - ",T7),IF(E7&lt;&gt;"",CONCATENATE("..",D7,".",E7,". - ",T7),CONCATENATE(D7,". - ",T7))),"")</f>
         <v>..A.02. - HIV/ and other Sexually transmitted diseases (STDs)</v>
       </c>
       <c r="B7" s="2"/>
@@ -5744,9 +5744,9 @@
       <c r="W7" s="45"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A8" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H8&lt;&gt;"",IF(F8&lt;&gt;"",CONCATENATE("...",D8,".",E8,".",F8,". - ",T8),IF(E8&lt;&gt;"",CONCATENATE("..",D8,".",E8,". - ",T8),CONCATENATE(D8,". - ",T8))),"")</f>
         <v>...A.02.a. - Sexually transmitted diseases (STDs) excluding HIV</v>
       </c>
       <c r="B8" s="2">
@@ -5808,9 +5808,9 @@
       </c>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H9&lt;&gt;"",IF(F9&lt;&gt;"",CONCATENATE("...",D9,".",E9,".",F9,". - ",T9),IF(E9&lt;&gt;"",CONCATENATE("..",D9,".",E9,". - ",T9),CONCATENATE(D9,". - ",T9))),"")</f>
         <v/>
       </c>
       <c r="B9" s="2">
@@ -5868,9 +5868,9 @@
       </c>
       <c r="X9" s="2"/>
     </row>
-    <row r="10" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H10&lt;&gt;"",IF(F10&lt;&gt;"",CONCATENATE("...",D10,".",E10,".",F10,". - ",T10),IF(E10&lt;&gt;"",CONCATENATE("..",D10,".",E10,". - ",T10),CONCATENATE(D10,". - ",T10))),"")</f>
         <v/>
       </c>
       <c r="B10" s="2">
@@ -5928,9 +5928,9 @@
       </c>
       <c r="X10" s="2"/>
     </row>
-    <row r="11" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H11&lt;&gt;"",IF(F11&lt;&gt;"",CONCATENATE("...",D11,".",E11,".",F11,". - ",T11),IF(E11&lt;&gt;"",CONCATENATE("..",D11,".",E11,". - ",T11),CONCATENATE(D11,". - ",T11))),"")</f>
         <v/>
       </c>
       <c r="B11" s="2">
@@ -5988,9 +5988,9 @@
       </c>
       <c r="X11" s="2"/>
     </row>
-    <row r="12" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H12&lt;&gt;"",IF(F12&lt;&gt;"",CONCATENATE("...",D12,".",E12,".",F12,". - ",T12),IF(E12&lt;&gt;"",CONCATENATE("..",D12,".",E12,". - ",T12),CONCATENATE(D12,". - ",T12))),"")</f>
         <v/>
       </c>
       <c r="B12" s="2">
@@ -6046,9 +6046,9 @@
         <v>516</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H13&lt;&gt;"",IF(F13&lt;&gt;"",CONCATENATE("...",D13,".",E13,".",F13,". - ",T13),IF(E13&lt;&gt;"",CONCATENATE("..",D13,".",E13,". - ",T13),CONCATENATE(D13,". - ",T13))),"")</f>
         <v/>
       </c>
       <c r="B13" s="2">
@@ -6106,9 +6106,9 @@
       </c>
       <c r="X13" s="2"/>
     </row>
-    <row r="14" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" ht="51" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H14&lt;&gt;"",IF(F14&lt;&gt;"",CONCATENATE("...",D14,".",E14,".",F14,". - ",T14),IF(E14&lt;&gt;"",CONCATENATE("..",D14,".",E14,". - ",T14),CONCATENATE(D14,". - ",T14))),"")</f>
         <v>...A.02.b. - HIV/AIDS</v>
       </c>
       <c r="B14" s="2">
@@ -6168,9 +6168,9 @@
       </c>
       <c r="X14" s="2"/>
     </row>
-    <row r="15" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H15&lt;&gt;"",IF(F15&lt;&gt;"",CONCATENATE("...",D15,".",E15,".",F15,". - ",T15),IF(E15&lt;&gt;"",CONCATENATE("..",D15,".",E15,". - ",T15),CONCATENATE(D15,". - ",T15))),"")</f>
         <v/>
       </c>
       <c r="B15" s="2">
@@ -6224,9 +6224,9 @@
       </c>
       <c r="X15" s="2"/>
     </row>
-    <row r="16" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H16&lt;&gt;"",IF(F16&lt;&gt;"",CONCATENATE("...",D16,".",E16,".",F16,". - ",T16),IF(E16&lt;&gt;"",CONCATENATE("..",D16,".",E16,". - ",T16),CONCATENATE(D16,". - ",T16))),"")</f>
         <v/>
       </c>
       <c r="B16" s="2">
@@ -6284,9 +6284,9 @@
       </c>
       <c r="X16" s="2"/>
     </row>
-    <row r="17" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H17&lt;&gt;"",IF(F17&lt;&gt;"",CONCATENATE("...",D17,".",E17,".",F17,". - ",T17),IF(E17&lt;&gt;"",CONCATENATE("..",D17,".",E17,". - ",T17),CONCATENATE(D17,". - ",T17))),"")</f>
         <v/>
       </c>
       <c r="B17" s="2">
@@ -6342,9 +6342,9 @@
       </c>
       <c r="X17" s="2"/>
     </row>
-    <row r="18" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H18&lt;&gt;"",IF(F18&lt;&gt;"",CONCATENATE("...",D18,".",E18,".",F18,". - ",T18),IF(E18&lt;&gt;"",CONCATENATE("..",D18,".",E18,". - ",T18),CONCATENATE(D18,". - ",T18))),"")</f>
         <v/>
       </c>
       <c r="B18" s="2">
@@ -6394,9 +6394,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H19&lt;&gt;"",IF(F19&lt;&gt;"",CONCATENATE("...",D19,".",E19,".",F19,". - ",T19),IF(E19&lt;&gt;"",CONCATENATE("..",D19,".",E19,". - ",T19),CONCATENATE(D19,". - ",T19))),"")</f>
         <v/>
       </c>
       <c r="B19" s="2">
@@ -6413,7 +6413,7 @@
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="40" t="str">
-        <f t="shared" ref="G19:G24" si="1">CONCATENATE("c",D19,E19,F19)</f>
+        <f t="shared" ref="G19:G24" si="0">CONCATENATE("c",D19,E19,F19)</f>
         <v>cA99</v>
       </c>
       <c r="H19" s="40"/>
@@ -6452,9 +6452,9 @@
       </c>
       <c r="X19" s="2"/>
     </row>
-    <row r="20" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H20&lt;&gt;"",IF(F20&lt;&gt;"",CONCATENATE("...",D20,".",E20,".",F20,". - ",T20),IF(E20&lt;&gt;"",CONCATENATE("..",D20,".",E20,". - ",T20),CONCATENATE(D20,". - ",T20))),"")</f>
         <v/>
       </c>
       <c r="B20" s="2">
@@ -6471,7 +6471,7 @@
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>cA99</v>
       </c>
       <c r="H20" s="40"/>
@@ -6510,9 +6510,9 @@
       </c>
       <c r="X20" s="2"/>
     </row>
-    <row r="21" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H21&lt;&gt;"",IF(F21&lt;&gt;"",CONCATENATE("...",D21,".",E21,".",F21,". - ",T21),IF(E21&lt;&gt;"",CONCATENATE("..",D21,".",E21,". - ",T21),CONCATENATE(D21,". - ",T21))),"")</f>
         <v/>
       </c>
       <c r="B21" s="2">
@@ -6529,7 +6529,7 @@
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>cA99</v>
       </c>
       <c r="H21" s="40"/>
@@ -6568,9 +6568,9 @@
       </c>
       <c r="X21" s="2"/>
     </row>
-    <row r="22" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H22&lt;&gt;"",IF(F22&lt;&gt;"",CONCATENATE("...",D22,".",E22,".",F22,". - ",T22),IF(E22&lt;&gt;"",CONCATENATE("..",D22,".",E22,". - ",T22),CONCATENATE(D22,". - ",T22))),"")</f>
         <v/>
       </c>
       <c r="B22" s="2">
@@ -6587,7 +6587,7 @@
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>cA99</v>
       </c>
       <c r="H22" s="40"/>
@@ -6626,9 +6626,9 @@
       </c>
       <c r="X22" s="2"/>
     </row>
-    <row r="23" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A23" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H23&lt;&gt;"",IF(F23&lt;&gt;"",CONCATENATE("...",D23,".",E23,".",F23,". - ",T23),IF(E23&lt;&gt;"",CONCATENATE("..",D23,".",E23,". - ",T23),CONCATENATE(D23,". - ",T23))),"")</f>
         <v>..A.04. - Meningitis</v>
       </c>
       <c r="B23" s="2">
@@ -6645,7 +6645,7 @@
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>cA04</v>
       </c>
       <c r="H23" s="40" t="str">
@@ -6687,9 +6687,9 @@
       </c>
       <c r="X23" s="2"/>
     </row>
-    <row r="24" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A24" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H24&lt;&gt;"",IF(F24&lt;&gt;"",CONCATENATE("...",D24,".",E24,".",F24,". - ",T24),IF(E24&lt;&gt;"",CONCATENATE("..",D24,".",E24,". - ",T24),CONCATENATE(D24,". - ",T24))),"")</f>
         <v>..A.05. - Encephalitis</v>
       </c>
       <c r="B24" s="2">
@@ -6706,7 +6706,7 @@
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>cA05</v>
       </c>
       <c r="H24" s="40" t="str">
@@ -6748,9 +6748,9 @@
       </c>
       <c r="X24" s="2"/>
     </row>
-    <row r="25" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A25" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H25&lt;&gt;"",IF(F25&lt;&gt;"",CONCATENATE("...",D25,".",E25,".",F25,". - ",T25),IF(E25&lt;&gt;"",CONCATENATE("..",D25,".",E25,". - ",T25),CONCATENATE(D25,". - ",T25))),"")</f>
         <v>..A.06. - Hepatitis</v>
       </c>
       <c r="B25" s="2">
@@ -6802,9 +6802,9 @@
       </c>
       <c r="X25" s="2"/>
     </row>
-    <row r="26" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H26&lt;&gt;"",IF(F26&lt;&gt;"",CONCATENATE("...",D26,".",E26,".",F26,". - ",T26),IF(E26&lt;&gt;"",CONCATENATE("..",D26,".",E26,". - ",T26),CONCATENATE(D26,". - ",T26))),"")</f>
         <v/>
       </c>
       <c r="B26" s="2">
@@ -6856,9 +6856,9 @@
       </c>
       <c r="X26" s="2"/>
     </row>
-    <row r="27" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A27" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H27&lt;&gt;"",IF(F27&lt;&gt;"",CONCATENATE("...",D27,".",E27,".",F27,". - ",T27),IF(E27&lt;&gt;"",CONCATENATE("..",D27,".",E27,". - ",T27),CONCATENATE(D27,". - ",T27))),"")</f>
         <v>...A.06.a. - Acute hepatitis B</v>
       </c>
       <c r="B27" s="2">
@@ -6915,9 +6915,9 @@
       </c>
       <c r="X27" s="2"/>
     </row>
-    <row r="28" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H28&lt;&gt;"",IF(F28&lt;&gt;"",CONCATENATE("...",D28,".",E28,".",F28,". - ",T28),IF(E28&lt;&gt;"",CONCATENATE("..",D28,".",E28,". - ",T28),CONCATENATE(D28,". - ",T28))),"")</f>
         <v/>
       </c>
       <c r="B28" s="2"/>
@@ -6943,9 +6943,9 @@
       <c r="W28" s="45"/>
       <c r="X28" s="2"/>
     </row>
-    <row r="29" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A29" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H29&lt;&gt;"",IF(F29&lt;&gt;"",CONCATENATE("...",D29,".",E29,".",F29,". - ",T29),IF(E29&lt;&gt;"",CONCATENATE("..",D29,".",E29,". - ",T29),CONCATENATE(D29,". - ",T29))),"")</f>
         <v>...A.06.b. - Acute hepatitis C</v>
       </c>
       <c r="B29" s="2">
@@ -7002,9 +7002,9 @@
       </c>
       <c r="X29" s="2"/>
     </row>
-    <row r="30" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H30&lt;&gt;"",IF(F30&lt;&gt;"",CONCATENATE("...",D30,".",E30,".",F30,". - ",T30),IF(E30&lt;&gt;"",CONCATENATE("..",D30,".",E30,". - ",T30),CONCATENATE(D30,". - ",T30))),"")</f>
         <v/>
       </c>
       <c r="B30" s="2">
@@ -7056,9 +7056,9 @@
       </c>
       <c r="X30" s="2"/>
     </row>
-    <row r="31" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A31" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H31&lt;&gt;"",IF(F31&lt;&gt;"",CONCATENATE("...",D31,".",E31,".",F31,". - ",T31),IF(E31&lt;&gt;"",CONCATENATE("..",D31,".",E31,". - ",T31),CONCATENATE(D31,". - ",T31))),"")</f>
         <v/>
       </c>
       <c r="B31" s="2">
@@ -7107,9 +7107,9 @@
       </c>
       <c r="X31" s="2"/>
     </row>
-    <row r="32" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H32&lt;&gt;"",IF(F32&lt;&gt;"",CONCATENATE("...",D32,".",E32,".",F32,". - ",T32),IF(E32&lt;&gt;"",CONCATENATE("..",D32,".",E32,". - ",T32),CONCATENATE(D32,". - ",T32))),"")</f>
         <v/>
       </c>
       <c r="B32" s="2">
@@ -7126,7 +7126,7 @@
       </c>
       <c r="F32" s="6"/>
       <c r="G32" s="40" t="str">
-        <f t="shared" ref="G32:G45" si="2">CONCATENATE("c",D32,E32,F32)</f>
+        <f t="shared" ref="G32:G45" si="1">CONCATENATE("c",D32,E32,F32)</f>
         <v>cA99</v>
       </c>
       <c r="H32" s="40"/>
@@ -7165,9 +7165,9 @@
       </c>
       <c r="X32" s="2"/>
     </row>
-    <row r="33" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H33&lt;&gt;"",IF(F33&lt;&gt;"",CONCATENATE("...",D33,".",E33,".",F33,". - ",T33),IF(E33&lt;&gt;"",CONCATENATE("..",D33,".",E33,". - ",T33),CONCATENATE(D33,". - ",T33))),"")</f>
         <v/>
       </c>
       <c r="B33" s="2">
@@ -7184,7 +7184,7 @@
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>cA99</v>
       </c>
       <c r="H33" s="40"/>
@@ -7223,9 +7223,9 @@
       </c>
       <c r="X33" s="2"/>
     </row>
-    <row r="34" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H34&lt;&gt;"",IF(F34&lt;&gt;"",CONCATENATE("...",D34,".",E34,".",F34,". - ",T34),IF(E34&lt;&gt;"",CONCATENATE("..",D34,".",E34,". - ",T34),CONCATENATE(D34,". - ",T34))),"")</f>
         <v/>
       </c>
       <c r="B34" s="2">
@@ -7242,7 +7242,7 @@
       </c>
       <c r="F34" s="6"/>
       <c r="G34" s="40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>cA99</v>
       </c>
       <c r="H34" s="40"/>
@@ -7281,9 +7281,9 @@
       </c>
       <c r="X34" s="2"/>
     </row>
-    <row r="35" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H35&lt;&gt;"",IF(F35&lt;&gt;"",CONCATENATE("...",D35,".",E35,".",F35,". - ",T35),IF(E35&lt;&gt;"",CONCATENATE("..",D35,".",E35,". - ",T35),CONCATENATE(D35,". - ",T35))),"")</f>
         <v/>
       </c>
       <c r="B35" s="2">
@@ -7300,7 +7300,7 @@
       </c>
       <c r="F35" s="6"/>
       <c r="G35" s="40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>cA99</v>
       </c>
       <c r="H35" s="40"/>
@@ -7339,9 +7339,9 @@
       </c>
       <c r="X35" s="2"/>
     </row>
-    <row r="36" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H36&lt;&gt;"",IF(F36&lt;&gt;"",CONCATENATE("...",D36,".",E36,".",F36,". - ",T36),IF(E36&lt;&gt;"",CONCATENATE("..",D36,".",E36,". - ",T36),CONCATENATE(D36,". - ",T36))),"")</f>
         <v/>
       </c>
       <c r="B36" s="2">
@@ -7358,7 +7358,7 @@
       </c>
       <c r="F36" s="6"/>
       <c r="G36" s="40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>cA99</v>
       </c>
       <c r="H36" s="40"/>
@@ -7397,9 +7397,9 @@
       </c>
       <c r="X36" s="2"/>
     </row>
-    <row r="37" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H37&lt;&gt;"",IF(F37&lt;&gt;"",CONCATENATE("...",D37,".",E37,".",F37,". - ",T37),IF(E37&lt;&gt;"",CONCATENATE("..",D37,".",E37,". - ",T37),CONCATENATE(D37,". - ",T37))),"")</f>
         <v/>
       </c>
       <c r="B37" s="2">
@@ -7416,7 +7416,7 @@
       </c>
       <c r="F37" s="6"/>
       <c r="G37" s="40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>cA99</v>
       </c>
       <c r="H37" s="40"/>
@@ -7451,9 +7451,9 @@
       </c>
       <c r="X37" s="2"/>
     </row>
-    <row r="38" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H38&lt;&gt;"",IF(F38&lt;&gt;"",CONCATENATE("...",D38,".",E38,".",F38,". - ",T38),IF(E38&lt;&gt;"",CONCATENATE("..",D38,".",E38,". - ",T38),CONCATENATE(D38,". - ",T38))),"")</f>
         <v/>
       </c>
       <c r="B38" s="2">
@@ -7470,7 +7470,7 @@
       </c>
       <c r="F38" s="6"/>
       <c r="G38" s="40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>cA99</v>
       </c>
       <c r="H38" s="40"/>
@@ -7505,9 +7505,9 @@
       </c>
       <c r="X38" s="2"/>
     </row>
-    <row r="39" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H39&lt;&gt;"",IF(F39&lt;&gt;"",CONCATENATE("...",D39,".",E39,".",F39,". - ",T39),IF(E39&lt;&gt;"",CONCATENATE("..",D39,".",E39,". - ",T39),CONCATENATE(D39,". - ",T39))),"")</f>
         <v/>
       </c>
       <c r="B39" s="2">
@@ -7524,7 +7524,7 @@
       </c>
       <c r="F39" s="6"/>
       <c r="G39" s="40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>cA99</v>
       </c>
       <c r="H39" s="40"/>
@@ -7563,9 +7563,9 @@
       </c>
       <c r="X39" s="2"/>
     </row>
-    <row r="40" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H40&lt;&gt;"",IF(F40&lt;&gt;"",CONCATENATE("...",D40,".",E40,".",F40,". - ",T40),IF(E40&lt;&gt;"",CONCATENATE("..",D40,".",E40,". - ",T40),CONCATENATE(D40,". - ",T40))),"")</f>
         <v/>
       </c>
       <c r="B40" s="2">
@@ -7582,7 +7582,7 @@
       </c>
       <c r="F40" s="6"/>
       <c r="G40" s="40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>cA99</v>
       </c>
       <c r="H40" s="40"/>
@@ -7621,9 +7621,9 @@
       </c>
       <c r="X40" s="2"/>
     </row>
-    <row r="41" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H41&lt;&gt;"",IF(F41&lt;&gt;"",CONCATENATE("...",D41,".",E41,".",F41,". - ",T41),IF(E41&lt;&gt;"",CONCATENATE("..",D41,".",E41,". - ",T41),CONCATENATE(D41,". - ",T41))),"")</f>
         <v/>
       </c>
       <c r="B41" s="2">
@@ -7640,7 +7640,7 @@
       </c>
       <c r="F41" s="6"/>
       <c r="G41" s="40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>cA99</v>
       </c>
       <c r="H41" s="40"/>
@@ -7675,9 +7675,9 @@
       </c>
       <c r="X41" s="2"/>
     </row>
-    <row r="42" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H42&lt;&gt;"",IF(F42&lt;&gt;"",CONCATENATE("...",D42,".",E42,".",F42,". - ",T42),IF(E42&lt;&gt;"",CONCATENATE("..",D42,".",E42,". - ",T42),CONCATENATE(D42,". - ",T42))),"")</f>
         <v/>
       </c>
       <c r="B42" s="2">
@@ -7694,7 +7694,7 @@
       </c>
       <c r="F42" s="6"/>
       <c r="G42" s="40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>cA99</v>
       </c>
       <c r="H42" s="40"/>
@@ -7733,9 +7733,9 @@
       </c>
       <c r="X42" s="2"/>
     </row>
-    <row r="43" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H43&lt;&gt;"",IF(F43&lt;&gt;"",CONCATENATE("...",D43,".",E43,".",F43,". - ",T43),IF(E43&lt;&gt;"",CONCATENATE("..",D43,".",E43,". - ",T43),CONCATENATE(D43,". - ",T43))),"")</f>
         <v/>
       </c>
       <c r="B43" s="2">
@@ -7752,7 +7752,7 @@
       </c>
       <c r="F43" s="6"/>
       <c r="G43" s="40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>cA99</v>
       </c>
       <c r="H43" s="40"/>
@@ -7787,9 +7787,9 @@
       </c>
       <c r="X43" s="2"/>
     </row>
-    <row r="44" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H44&lt;&gt;"",IF(F44&lt;&gt;"",CONCATENATE("...",D44,".",E44,".",F44,". - ",T44),IF(E44&lt;&gt;"",CONCATENATE("..",D44,".",E44,". - ",T44),CONCATENATE(D44,". - ",T44))),"")</f>
         <v/>
       </c>
       <c r="B44" s="2">
@@ -7806,7 +7806,7 @@
       </c>
       <c r="F44" s="6"/>
       <c r="G44" s="40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>cA99</v>
       </c>
       <c r="H44" s="40"/>
@@ -7845,9 +7845,9 @@
       </c>
       <c r="X44" s="2"/>
     </row>
-    <row r="45" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H45&lt;&gt;"",IF(F45&lt;&gt;"",CONCATENATE("...",D45,".",E45,".",F45,". - ",T45),IF(E45&lt;&gt;"",CONCATENATE("..",D45,".",E45,". - ",T45),CONCATENATE(D45,". - ",T45))),"")</f>
         <v/>
       </c>
       <c r="B45" s="2">
@@ -7864,7 +7864,7 @@
       </c>
       <c r="F45" s="6"/>
       <c r="G45" s="40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>cA99</v>
       </c>
       <c r="H45" s="40"/>
@@ -7903,9 +7903,9 @@
       </c>
       <c r="X45" s="2"/>
     </row>
-    <row r="46" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H46&lt;&gt;"",IF(F46&lt;&gt;"",CONCATENATE("...",D46,".",E46,".",F46,". - ",T46),IF(E46&lt;&gt;"",CONCATENATE("..",D46,".",E46,". - ",T46),CONCATENATE(D46,". - ",T46))),"")</f>
         <v/>
       </c>
       <c r="B46" s="2">
@@ -7958,9 +7958,9 @@
       </c>
       <c r="X46" s="2"/>
     </row>
-    <row r="47" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H47&lt;&gt;"",IF(F47&lt;&gt;"",CONCATENATE("...",D47,".",E47,".",F47,". - ",T47),IF(E47&lt;&gt;"",CONCATENATE("..",D47,".",E47,". - ",T47),CONCATENATE(D47,". - ",T47))),"")</f>
         <v/>
       </c>
       <c r="B47" s="2">
@@ -8016,9 +8016,9 @@
       </c>
       <c r="X47" s="2"/>
     </row>
-    <row r="48" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H48&lt;&gt;"",IF(F48&lt;&gt;"",CONCATENATE("...",D48,".",E48,".",F48,". - ",T48),IF(E48&lt;&gt;"",CONCATENATE("..",D48,".",E48,". - ",T48),CONCATENATE(D48,". - ",T48))),"")</f>
         <v/>
       </c>
       <c r="B48" s="2">
@@ -8070,9 +8070,9 @@
       </c>
       <c r="X48" s="2"/>
     </row>
-    <row r="49" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H49&lt;&gt;"",IF(F49&lt;&gt;"",CONCATENATE("...",D49,".",E49,".",F49,". - ",T49),IF(E49&lt;&gt;"",CONCATENATE("..",D49,".",E49,". - ",T49),CONCATENATE(D49,". - ",T49))),"")</f>
         <v/>
       </c>
       <c r="B49" s="2">
@@ -8124,9 +8124,9 @@
       </c>
       <c r="X49" s="2"/>
     </row>
-    <row r="50" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H50&lt;&gt;"",IF(F50&lt;&gt;"",CONCATENATE("...",D50,".",E50,".",F50,". - ",T50),IF(E50&lt;&gt;"",CONCATENATE("..",D50,".",E50,". - ",T50),CONCATENATE(D50,". - ",T50))),"")</f>
         <v/>
       </c>
       <c r="B50" s="2">
@@ -8180,7 +8180,7 @@
     </row>
     <row r="51" spans="1:24" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A51" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H51&lt;&gt;"",IF(F51&lt;&gt;"",CONCATENATE("...",D51,".",E51,".",F51,". - ",T51),IF(E51&lt;&gt;"",CONCATENATE("..",D51,".",E51,". - ",T51),CONCATENATE(D51,". - ",T51))),"")</f>
         <v/>
       </c>
       <c r="B51" s="2">
@@ -8244,9 +8244,9 @@
         <v>1314</v>
       </c>
     </row>
-    <row r="52" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A52" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H52&lt;&gt;"",IF(F52&lt;&gt;"",CONCATENATE("...",D52,".",E52,".",F52,". - ",T52),IF(E52&lt;&gt;"",CONCATENATE("..",D52,".",E52,". - ",T52),CONCATENATE(D52,". - ",T52))),"")</f>
         <v>..A.07. - Respiratory infections</v>
       </c>
       <c r="B52" s="2">
@@ -8304,9 +8304,9 @@
       </c>
       <c r="X52" s="2"/>
     </row>
-    <row r="53" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A53" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H53&lt;&gt;"",IF(F53&lt;&gt;"",CONCATENATE("...",D53,".",E53,".",F53,". - ",T53),IF(E53&lt;&gt;"",CONCATENATE("..",D53,".",E53,". - ",T53),CONCATENATE(D53,". - ",T53))),"")</f>
         <v>...A.07.a. - Lower respiratory infections</v>
       </c>
       <c r="B53" s="2">
@@ -8329,7 +8329,7 @@
         <v>cA07a</v>
       </c>
       <c r="H53" s="40" t="str">
-        <f t="shared" ref="H53:H54" si="3">CONCATENATE(D53,E53,F53)</f>
+        <f t="shared" ref="H53:H54" si="2">CONCATENATE(D53,E53,F53)</f>
         <v>A07a</v>
       </c>
       <c r="I53" s="5"/>
@@ -8373,9 +8373,9 @@
       </c>
       <c r="X53" s="2"/>
     </row>
-    <row r="54" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A54" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H54&lt;&gt;"",IF(F54&lt;&gt;"",CONCATENATE("...",D54,".",E54,".",F54,". - ",T54),IF(E54&lt;&gt;"",CONCATENATE("..",D54,".",E54,". - ",T54),CONCATENATE(D54,". - ",T54))),"")</f>
         <v>...A.07.b. - Upper respiratory infections</v>
       </c>
       <c r="B54" s="2">
@@ -8398,7 +8398,7 @@
         <v>cA07b</v>
       </c>
       <c r="H54" s="40" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>A07b</v>
       </c>
       <c r="I54" s="5"/>
@@ -8442,9 +8442,9 @@
       </c>
       <c r="X54" s="2"/>
     </row>
-    <row r="55" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H55&lt;&gt;"",IF(F55&lt;&gt;"",CONCATENATE("...",D55,".",E55,".",F55,". - ",T55),IF(E55&lt;&gt;"",CONCATENATE("..",D55,".",E55,". - ",T55),CONCATENATE(D55,". - ",T55))),"")</f>
         <v/>
       </c>
       <c r="B55" s="2">
@@ -8506,9 +8506,9 @@
       </c>
       <c r="X55" s="2"/>
     </row>
-    <row r="56" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A56" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H56&lt;&gt;"",IF(F56&lt;&gt;"",CONCATENATE("...",D56,".",E56,".",F56,". - ",T56),IF(E56&lt;&gt;"",CONCATENATE("..",D56,".",E56,". - ",T56),CONCATENATE(D56,". - ",T56))),"")</f>
         <v>..A.08. - Maternal conditions</v>
       </c>
       <c r="B56" s="2">
@@ -8570,7 +8570,7 @@
     </row>
     <row r="57" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A57" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H57&lt;&gt;"",IF(F57&lt;&gt;"",CONCATENATE("...",D57,".",E57,".",F57,". - ",T57),IF(E57&lt;&gt;"",CONCATENATE("..",D57,".",E57,". - ",T57),CONCATENATE(D57,". - ",T57))),"")</f>
         <v/>
       </c>
       <c r="B57" s="2">
@@ -8587,7 +8587,7 @@
       </c>
       <c r="F57" s="6"/>
       <c r="G57" s="40" t="str">
-        <f t="shared" ref="G57:G62" si="4">CONCATENATE("c",D57,E57,F57)</f>
+        <f t="shared" ref="G57:G62" si="3">CONCATENATE("c",D57,E57,F57)</f>
         <v>cA08</v>
       </c>
       <c r="H57" s="40"/>
@@ -8634,9 +8634,9 @@
         <v>1366</v>
       </c>
     </row>
-    <row r="58" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H58&lt;&gt;"",IF(F58&lt;&gt;"",CONCATENATE("...",D58,".",E58,".",F58,". - ",T58),IF(E58&lt;&gt;"",CONCATENATE("..",D58,".",E58,". - ",T58),CONCATENATE(D58,". - ",T58))),"")</f>
         <v/>
       </c>
       <c r="B58" s="2">
@@ -8653,7 +8653,7 @@
       </c>
       <c r="F58" s="6"/>
       <c r="G58" s="40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>cA08</v>
       </c>
       <c r="H58" s="40"/>
@@ -8700,7 +8700,7 @@
     </row>
     <row r="59" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A59" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H59&lt;&gt;"",IF(F59&lt;&gt;"",CONCATENATE("...",D59,".",E59,".",F59,". - ",T59),IF(E59&lt;&gt;"",CONCATENATE("..",D59,".",E59,". - ",T59),CONCATENATE(D59,". - ",T59))),"")</f>
         <v/>
       </c>
       <c r="B59" s="2">
@@ -8717,7 +8717,7 @@
       </c>
       <c r="F59" s="6"/>
       <c r="G59" s="40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>cA08</v>
       </c>
       <c r="H59" s="40"/>
@@ -8764,9 +8764,9 @@
         <v>1368</v>
       </c>
     </row>
-    <row r="60" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H60&lt;&gt;"",IF(F60&lt;&gt;"",CONCATENATE("...",D60,".",E60,".",F60,". - ",T60),IF(E60&lt;&gt;"",CONCATENATE("..",D60,".",E60,". - ",T60),CONCATENATE(D60,". - ",T60))),"")</f>
         <v/>
       </c>
       <c r="B60" s="2">
@@ -8783,7 +8783,7 @@
       </c>
       <c r="F60" s="6"/>
       <c r="G60" s="40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>cA08</v>
       </c>
       <c r="H60" s="40"/>
@@ -8828,9 +8828,9 @@
       </c>
       <c r="X60" s="2"/>
     </row>
-    <row r="61" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A61" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H61&lt;&gt;"",IF(F61&lt;&gt;"",CONCATENATE("...",D61,".",E61,".",F61,". - ",T61),IF(E61&lt;&gt;"",CONCATENATE("..",D61,".",E61,". - ",T61),CONCATENATE(D61,". - ",T61))),"")</f>
         <v/>
       </c>
       <c r="B61" s="2">
@@ -8847,7 +8847,7 @@
       </c>
       <c r="F61" s="6"/>
       <c r="G61" s="40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>cA08</v>
       </c>
       <c r="H61" s="40"/>
@@ -8894,7 +8894,7 @@
     </row>
     <row r="62" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A62" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H62&lt;&gt;"",IF(F62&lt;&gt;"",CONCATENATE("...",D62,".",E62,".",F62,". - ",T62),IF(E62&lt;&gt;"",CONCATENATE("..",D62,".",E62,". - ",T62),CONCATENATE(D62,". - ",T62))),"")</f>
         <v/>
       </c>
       <c r="B62" s="2">
@@ -8911,7 +8911,7 @@
       </c>
       <c r="F62" s="6"/>
       <c r="G62" s="40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>cA08</v>
       </c>
       <c r="H62" s="40"/>
@@ -8956,9 +8956,9 @@
       </c>
       <c r="X62" s="2"/>
     </row>
-    <row r="63" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A63" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H63&lt;&gt;"",IF(F63&lt;&gt;"",CONCATENATE("...",D63,".",E63,".",F63,". - ",T63),IF(E63&lt;&gt;"",CONCATENATE("..",D63,".",E63,". - ",T63),CONCATENATE(D63,". - ",T63))),"")</f>
         <v>..A.09. - Neonatal conditions</v>
       </c>
       <c r="B63" s="2">
@@ -9020,7 +9020,7 @@
     </row>
     <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H64&lt;&gt;"",IF(F64&lt;&gt;"",CONCATENATE("...",D64,".",E64,".",F64,". - ",T64),IF(E64&lt;&gt;"",CONCATENATE("..",D64,".",E64,". - ",T64),CONCATENATE(D64,". - ",T64))),"")</f>
         <v/>
       </c>
       <c r="B64" s="2">
@@ -9078,7 +9078,7 @@
     </row>
     <row r="65" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A65" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H65&lt;&gt;"",IF(F65&lt;&gt;"",CONCATENATE("...",D65,".",E65,".",F65,". - ",T65),IF(E65&lt;&gt;"",CONCATENATE("..",D65,".",E65,". - ",T65),CONCATENATE(D65,". - ",T65))),"")</f>
         <v/>
       </c>
       <c r="B65" s="2">
@@ -9136,7 +9136,7 @@
     </row>
     <row r="66" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A66" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H66&lt;&gt;"",IF(F66&lt;&gt;"",CONCATENATE("...",D66,".",E66,".",F66,". - ",T66),IF(E66&lt;&gt;"",CONCATENATE("..",D66,".",E66,". - ",T66),CONCATENATE(D66,". - ",T66))),"")</f>
         <v/>
       </c>
       <c r="B66" s="2">
@@ -9194,7 +9194,7 @@
     </row>
     <row r="67" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A67" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(H67&lt;&gt;"",IF(F67&lt;&gt;"",CONCATENATE("...",D67,".",E67,".",F67,". - ",T67),IF(E67&lt;&gt;"",CONCATENATE("..",D67,".",E67,". - ",T67),CONCATENATE(D67,". - ",T67))),"")</f>
         <v/>
       </c>
       <c r="B67" s="2">
@@ -9258,7 +9258,7 @@
     </row>
     <row r="68" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A68" s="44" t="str">
-        <f t="shared" ref="A68:A131" si="5">IF(H68&lt;&gt;"",IF(F68&lt;&gt;"",CONCATENATE("...",D68,".",E68,".",F68,". - ",T68),IF(E68&lt;&gt;"",CONCATENATE("..",D68,".",E68,". - ",T68),CONCATENATE(D68,". - ",T68))),"")</f>
+        <f>IF(H68&lt;&gt;"",IF(F68&lt;&gt;"",CONCATENATE("...",D68,".",E68,".",F68,". - ",T68),IF(E68&lt;&gt;"",CONCATENATE("..",D68,".",E68,". - ",T68),CONCATENATE(D68,". - ",T68))),"")</f>
         <v/>
       </c>
       <c r="B68" s="2">
@@ -9313,7 +9313,7 @@
     </row>
     <row r="69" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A69" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H69&lt;&gt;"",IF(F69&lt;&gt;"",CONCATENATE("...",D69,".",E69,".",F69,". - ",T69),IF(E69&lt;&gt;"",CONCATENATE("..",D69,".",E69,". - ",T69),CONCATENATE(D69,". - ",T69))),"")</f>
         <v/>
       </c>
       <c r="B69" s="2">
@@ -9371,7 +9371,7 @@
     </row>
     <row r="70" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A70" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H70&lt;&gt;"",IF(F70&lt;&gt;"",CONCATENATE("...",D70,".",E70,".",F70,". - ",T70),IF(E70&lt;&gt;"",CONCATENATE("..",D70,".",E70,". - ",T70),CONCATENATE(D70,". - ",T70))),"")</f>
         <v/>
       </c>
       <c r="B70" s="2">
@@ -9429,7 +9429,7 @@
     </row>
     <row r="71" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A71" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H71&lt;&gt;"",IF(F71&lt;&gt;"",CONCATENATE("...",D71,".",E71,".",F71,". - ",T71),IF(E71&lt;&gt;"",CONCATENATE("..",D71,".",E71,". - ",T71),CONCATENATE(D71,". - ",T71))),"")</f>
         <v/>
       </c>
       <c r="B71" s="2">
@@ -9483,7 +9483,7 @@
     </row>
     <row r="72" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A72" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H72&lt;&gt;"",IF(F72&lt;&gt;"",CONCATENATE("...",D72,".",E72,".",F72,". - ",T72),IF(E72&lt;&gt;"",CONCATENATE("..",D72,".",E72,". - ",T72),CONCATENATE(D72,". - ",T72))),"")</f>
         <v/>
       </c>
       <c r="B72" s="2">
@@ -9541,7 +9541,7 @@
     </row>
     <row r="73" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A73" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H73&lt;&gt;"",IF(F73&lt;&gt;"",CONCATENATE("...",D73,".",E73,".",F73,". - ",T73),IF(E73&lt;&gt;"",CONCATENATE("..",D73,".",E73,". - ",T73),CONCATENATE(D73,". - ",T73))),"")</f>
         <v/>
       </c>
       <c r="B73" s="2">
@@ -9599,7 +9599,7 @@
     </row>
     <row r="74" spans="1:24" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A74" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H74&lt;&gt;"",IF(F74&lt;&gt;"",CONCATENATE("...",D74,".",E74,".",F74,". - ",T74),IF(E74&lt;&gt;"",CONCATENATE("..",D74,".",E74,". - ",T74),CONCATENATE(D74,". - ",T74))),"")</f>
         <v/>
       </c>
       <c r="B74" s="2">
@@ -9650,9 +9650,9 @@
       </c>
       <c r="X74" s="2"/>
     </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:24" ht="51" x14ac:dyDescent="0.25">
       <c r="A75" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H75&lt;&gt;"",IF(F75&lt;&gt;"",CONCATENATE("...",D75,".",E75,".",F75,". - ",T75),IF(E75&lt;&gt;"",CONCATENATE("..",D75,".",E75,". - ",T75),CONCATENATE(D75,". - ",T75))),"")</f>
         <v>D. - Other Chronic</v>
       </c>
       <c r="B75" s="2"/>
@@ -9688,9 +9688,9 @@
       </c>
       <c r="X75" s="2"/>
     </row>
-    <row r="76" spans="1:24" ht="57.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A76" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H76&lt;&gt;"",IF(F76&lt;&gt;"",CONCATENATE("...",D76,".",E76,".",F76,". - ",T76),IF(E76&lt;&gt;"",CONCATENATE("..",D76,".",E76,". - ",T76),CONCATENATE(D76,". - ",T76))),"")</f>
         <v>B. - Cancer/Malignant neoplasms</v>
       </c>
       <c r="B76" s="2">
@@ -9746,9 +9746,9 @@
       </c>
       <c r="X76" s="2"/>
     </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:24" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A77" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H77&lt;&gt;"",IF(F77&lt;&gt;"",CONCATENATE("...",D77,".",E77,".",F77,". - ",T77),IF(E77&lt;&gt;"",CONCATENATE("..",D77,".",E77,". - ",T77),CONCATENATE(D77,". - ",T77))),"")</f>
         <v>..B.01. - Mouth and oropharynx cancers</v>
       </c>
       <c r="B77" s="2">
@@ -9765,7 +9765,7 @@
       </c>
       <c r="F77" s="6"/>
       <c r="G77" s="40" t="str">
-        <f t="shared" ref="G77:G86" si="6">CONCATENATE("c",D77,E77,F77)</f>
+        <f t="shared" ref="G77:G86" si="4">CONCATENATE("c",D77,E77,F77)</f>
         <v>cB01</v>
       </c>
       <c r="H77" s="40" t="str">
@@ -9807,7 +9807,7 @@
     </row>
     <row r="78" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A78" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H78&lt;&gt;"",IF(F78&lt;&gt;"",CONCATENATE("...",D78,".",E78,".",F78,". - ",T78),IF(E78&lt;&gt;"",CONCATENATE("..",D78,".",E78,". - ",T78),CONCATENATE(D78,". - ",T78))),"")</f>
         <v/>
       </c>
       <c r="B78" s="2">
@@ -9824,7 +9824,7 @@
       </c>
       <c r="F78" s="6"/>
       <c r="G78" s="40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>cB01</v>
       </c>
       <c r="H78" s="40"/>
@@ -9871,7 +9871,7 @@
     </row>
     <row r="79" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A79" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H79&lt;&gt;"",IF(F79&lt;&gt;"",CONCATENATE("...",D79,".",E79,".",F79,". - ",T79),IF(E79&lt;&gt;"",CONCATENATE("..",D79,".",E79,". - ",T79),CONCATENATE(D79,". - ",T79))),"")</f>
         <v/>
       </c>
       <c r="B79" s="2">
@@ -9888,7 +9888,7 @@
       </c>
       <c r="F79" s="6"/>
       <c r="G79" s="40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>cB01</v>
       </c>
       <c r="H79" s="40"/>
@@ -9935,7 +9935,7 @@
     </row>
     <row r="80" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A80" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H80&lt;&gt;"",IF(F80&lt;&gt;"",CONCATENATE("...",D80,".",E80,".",F80,". - ",T80),IF(E80&lt;&gt;"",CONCATENATE("..",D80,".",E80,". - ",T80),CONCATENATE(D80,". - ",T80))),"")</f>
         <v/>
       </c>
       <c r="B80" s="2">
@@ -9952,7 +9952,7 @@
       </c>
       <c r="F80" s="6"/>
       <c r="G80" s="40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>cB01</v>
       </c>
       <c r="H80" s="40"/>
@@ -9993,9 +9993,9 @@
       </c>
       <c r="X80" s="2"/>
     </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:24" ht="51" x14ac:dyDescent="0.25">
       <c r="A81" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H81&lt;&gt;"",IF(F81&lt;&gt;"",CONCATENATE("...",D81,".",E81,".",F81,". - ",T81),IF(E81&lt;&gt;"",CONCATENATE("..",D81,".",E81,". - ",T81),CONCATENATE(D81,". - ",T81))),"")</f>
         <v>..B.02. - Oesophagus cancer</v>
       </c>
       <c r="B81" s="2">
@@ -10012,11 +10012,11 @@
       </c>
       <c r="F81" s="6"/>
       <c r="G81" s="40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>cB02</v>
       </c>
       <c r="H81" s="40" t="str">
-        <f t="shared" ref="H81:H87" si="7">CONCATENATE(D81,E81,F81)</f>
+        <f t="shared" ref="H81:H87" si="5">CONCATENATE(D81,E81,F81)</f>
         <v>B02</v>
       </c>
       <c r="I81" s="18" t="s">
@@ -10060,9 +10060,9 @@
       </c>
       <c r="X81" s="2"/>
     </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:24" ht="51" x14ac:dyDescent="0.25">
       <c r="A82" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H82&lt;&gt;"",IF(F82&lt;&gt;"",CONCATENATE("...",D82,".",E82,".",F82,". - ",T82),IF(E82&lt;&gt;"",CONCATENATE("..",D82,".",E82,". - ",T82),CONCATENATE(D82,". - ",T82))),"")</f>
         <v>..B.03. - Stomach cancer</v>
       </c>
       <c r="B82" s="2">
@@ -10079,11 +10079,11 @@
       </c>
       <c r="F82" s="6"/>
       <c r="G82" s="40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>cB03</v>
       </c>
       <c r="H82" s="40" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>B03</v>
       </c>
       <c r="I82" s="18" t="s">
@@ -10129,9 +10129,9 @@
         <v>952</v>
       </c>
     </row>
-    <row r="83" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A83" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H83&lt;&gt;"",IF(F83&lt;&gt;"",CONCATENATE("...",D83,".",E83,".",F83,". - ",T83),IF(E83&lt;&gt;"",CONCATENATE("..",D83,".",E83,". - ",T83),CONCATENATE(D83,". - ",T83))),"")</f>
         <v>..B.04. - Colon and rectum cancers</v>
       </c>
       <c r="B83" s="2">
@@ -10148,11 +10148,11 @@
       </c>
       <c r="F83" s="6"/>
       <c r="G83" s="40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>cB04</v>
       </c>
       <c r="H83" s="40" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>B04</v>
       </c>
       <c r="I83" s="16" t="s">
@@ -10196,9 +10196,9 @@
       </c>
       <c r="X83" s="2"/>
     </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A84" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H84&lt;&gt;"",IF(F84&lt;&gt;"",CONCATENATE("...",D84,".",E84,".",F84,". - ",T84),IF(E84&lt;&gt;"",CONCATENATE("..",D84,".",E84,". - ",T84),CONCATENATE(D84,". - ",T84))),"")</f>
         <v>..B.05. - Liver cancer</v>
       </c>
       <c r="B84" s="2">
@@ -10215,11 +10215,11 @@
       </c>
       <c r="F84" s="6"/>
       <c r="G84" s="40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>cB05</v>
       </c>
       <c r="H84" s="40" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>B05</v>
       </c>
       <c r="I84" s="18" t="s">
@@ -10263,9 +10263,9 @@
       </c>
       <c r="X84" s="2"/>
     </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:24" ht="51" x14ac:dyDescent="0.25">
       <c r="A85" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H85&lt;&gt;"",IF(F85&lt;&gt;"",CONCATENATE("...",D85,".",E85,".",F85,". - ",T85),IF(E85&lt;&gt;"",CONCATENATE("..",D85,".",E85,". - ",T85),CONCATENATE(D85,". - ",T85))),"")</f>
         <v>..B.06. - Pancreas cancer</v>
       </c>
       <c r="B85" s="2">
@@ -10282,11 +10282,11 @@
       </c>
       <c r="F85" s="6"/>
       <c r="G85" s="40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>cB06</v>
       </c>
       <c r="H85" s="40" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>B06</v>
       </c>
       <c r="I85" s="18" t="s">
@@ -10330,9 +10330,9 @@
       </c>
       <c r="X85" s="2"/>
     </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:24" ht="102" x14ac:dyDescent="0.25">
       <c r="A86" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H86&lt;&gt;"",IF(F86&lt;&gt;"",CONCATENATE("...",D86,".",E86,".",F86,". - ",T86),IF(E86&lt;&gt;"",CONCATENATE("..",D86,".",E86,". - ",T86),CONCATENATE(D86,". - ",T86))),"")</f>
         <v>..B.07. - Trachea, bronchus and lung cancers</v>
       </c>
       <c r="B86" s="2">
@@ -10349,11 +10349,11 @@
       </c>
       <c r="F86" s="6"/>
       <c r="G86" s="40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>cB07</v>
       </c>
       <c r="H86" s="40" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>B07</v>
       </c>
       <c r="I86" s="18" t="s">
@@ -10397,9 +10397,9 @@
       </c>
       <c r="X86" s="2"/>
     </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:24" ht="102" x14ac:dyDescent="0.25">
       <c r="A87" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H87&lt;&gt;"",IF(F87&lt;&gt;"",CONCATENATE("...",D87,".",E87,".",F87,". - ",T87),IF(E87&lt;&gt;"",CONCATENATE("..",D87,".",E87,". - ",T87),CONCATENATE(D87,". - ",T87))),"")</f>
         <v>..B.08. - Melanoma and other skin cancers</v>
       </c>
       <c r="B87" s="2">
@@ -10419,7 +10419,7 @@
         <v>952</v>
       </c>
       <c r="H87" s="40" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>B08</v>
       </c>
       <c r="J87" s="17" t="s">
@@ -10458,7 +10458,7 @@
     </row>
     <row r="88" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A88" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H88&lt;&gt;"",IF(F88&lt;&gt;"",CONCATENATE("...",D88,".",E88,".",F88,". - ",T88),IF(E88&lt;&gt;"",CONCATENATE("..",D88,".",E88,". - ",T88),CONCATENATE(D88,". - ",T88))),"")</f>
         <v/>
       </c>
       <c r="B88" s="2">
@@ -10475,7 +10475,7 @@
       </c>
       <c r="F88" s="6"/>
       <c r="G88" s="40" t="str">
-        <f t="shared" ref="G88:G103" si="8">CONCATENATE("c",D88,E88,F88)</f>
+        <f t="shared" ref="G88:G103" si="6">CONCATENATE("c",D88,E88,F88)</f>
         <v>cB08</v>
       </c>
       <c r="H88" s="40"/>
@@ -10522,7 +10522,7 @@
     </row>
     <row r="89" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A89" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H89&lt;&gt;"",IF(F89&lt;&gt;"",CONCATENATE("...",D89,".",E89,".",F89,". - ",T89),IF(E89&lt;&gt;"",CONCATENATE("..",D89,".",E89,". - ",T89),CONCATENATE(D89,". - ",T89))),"")</f>
         <v/>
       </c>
       <c r="B89" s="2">
@@ -10539,7 +10539,7 @@
       </c>
       <c r="F89" s="6"/>
       <c r="G89" s="40" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>cB08</v>
       </c>
       <c r="H89" s="40"/>
@@ -10584,9 +10584,9 @@
       </c>
       <c r="X89" s="2"/>
     </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A90" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H90&lt;&gt;"",IF(F90&lt;&gt;"",CONCATENATE("...",D90,".",E90,".",F90,". - ",T90),IF(E90&lt;&gt;"",CONCATENATE("..",D90,".",E90,". - ",T90),CONCATENATE(D90,". - ",T90))),"")</f>
         <v>..B.09. - Breast cancer</v>
       </c>
       <c r="B90" s="2">
@@ -10603,7 +10603,7 @@
       </c>
       <c r="F90" s="6"/>
       <c r="G90" s="40" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>cB09</v>
       </c>
       <c r="H90" s="40" t="str">
@@ -10651,9 +10651,9 @@
       </c>
       <c r="X90" s="2"/>
     </row>
-    <row r="91" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:24" ht="51" x14ac:dyDescent="0.25">
       <c r="A91" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H91&lt;&gt;"",IF(F91&lt;&gt;"",CONCATENATE("...",D91,".",E91,".",F91,". - ",T91),IF(E91&lt;&gt;"",CONCATENATE("..",D91,".",E91,". - ",T91),CONCATENATE(D91,". - ",T91))),"")</f>
         <v>..B.10. - Uterine cancer</v>
       </c>
       <c r="B91" s="2"/>
@@ -10696,7 +10696,7 @@
     </row>
     <row r="92" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A92" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H92&lt;&gt;"",IF(F92&lt;&gt;"",CONCATENATE("...",D92,".",E92,".",F92,". - ",T92),IF(E92&lt;&gt;"",CONCATENATE("..",D92,".",E92,". - ",T92),CONCATENATE(D92,". - ",T92))),"")</f>
         <v/>
       </c>
       <c r="B92" s="2">
@@ -10760,7 +10760,7 @@
     </row>
     <row r="93" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A93" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H93&lt;&gt;"",IF(F93&lt;&gt;"",CONCATENATE("...",D93,".",E93,".",F93,". - ",T93),IF(E93&lt;&gt;"",CONCATENATE("..",D93,".",E93,". - ",T93),CONCATENATE(D93,". - ",T93))),"")</f>
         <v/>
       </c>
       <c r="B93" s="2">
@@ -10777,7 +10777,7 @@
       </c>
       <c r="F93" s="6"/>
       <c r="G93" s="40" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>cB10</v>
       </c>
       <c r="H93" s="40"/>
@@ -10822,9 +10822,9 @@
       </c>
       <c r="X93" s="2"/>
     </row>
-    <row r="94" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A94" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H94&lt;&gt;"",IF(F94&lt;&gt;"",CONCATENATE("...",D94,".",E94,".",F94,". - ",T94),IF(E94&lt;&gt;"",CONCATENATE("..",D94,".",E94,". - ",T94),CONCATENATE(D94,". - ",T94))),"")</f>
         <v>..B.11. - Ovary cancer</v>
       </c>
       <c r="B94" s="2">
@@ -10841,7 +10841,7 @@
       </c>
       <c r="F94" s="6"/>
       <c r="G94" s="40" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>cB11</v>
       </c>
       <c r="H94" s="40" t="str">
@@ -10889,9 +10889,9 @@
       </c>
       <c r="X94" s="2"/>
     </row>
-    <row r="95" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:24" ht="51" x14ac:dyDescent="0.25">
       <c r="A95" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H95&lt;&gt;"",IF(F95&lt;&gt;"",CONCATENATE("...",D95,".",E95,".",F95,". - ",T95),IF(E95&lt;&gt;"",CONCATENATE("..",D95,".",E95,". - ",T95),CONCATENATE(D95,". - ",T95))),"")</f>
         <v>..B.12. - Prostate cancer</v>
       </c>
       <c r="B95" s="2">
@@ -10908,7 +10908,7 @@
       </c>
       <c r="F95" s="6"/>
       <c r="G95" s="40" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>cB12</v>
       </c>
       <c r="H95" s="40" t="str">
@@ -10958,7 +10958,7 @@
     </row>
     <row r="96" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A96" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H96&lt;&gt;"",IF(F96&lt;&gt;"",CONCATENATE("...",D96,".",E96,".",F96,". - ",T96),IF(E96&lt;&gt;"",CONCATENATE("..",D96,".",E96,". - ",T96),CONCATENATE(D96,". - ",T96))),"")</f>
         <v/>
       </c>
       <c r="B96" s="2">
@@ -10975,7 +10975,7 @@
       </c>
       <c r="F96" s="6"/>
       <c r="G96" s="40" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>cB99</v>
       </c>
       <c r="H96" s="40"/>
@@ -11020,9 +11020,9 @@
       </c>
       <c r="X96" s="2"/>
     </row>
-    <row r="97" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:24" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A97" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H97&lt;&gt;"",IF(F97&lt;&gt;"",CONCATENATE("...",D97,".",E97,".",F97,". - ",T97),IF(E97&lt;&gt;"",CONCATENATE("..",D97,".",E97,". - ",T97),CONCATENATE(D97,". - ",T97))),"")</f>
         <v>..B.13. - Kidney, renal pelvis and ureter cancer</v>
       </c>
       <c r="B97" s="2">
@@ -11039,7 +11039,7 @@
       </c>
       <c r="F97" s="6"/>
       <c r="G97" s="40" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>cB13</v>
       </c>
       <c r="H97" s="40" t="str">
@@ -11087,9 +11087,9 @@
       </c>
       <c r="X97" s="2"/>
     </row>
-    <row r="98" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:24" ht="51" x14ac:dyDescent="0.25">
       <c r="A98" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H98&lt;&gt;"",IF(F98&lt;&gt;"",CONCATENATE("...",D98,".",E98,".",F98,". - ",T98),IF(E98&lt;&gt;"",CONCATENATE("..",D98,".",E98,". - ",T98),CONCATENATE(D98,". - ",T98))),"")</f>
         <v>..B.14. - Bladder cancer</v>
       </c>
       <c r="B98" s="2">
@@ -11106,7 +11106,7 @@
       </c>
       <c r="F98" s="6"/>
       <c r="G98" s="40" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>cB14</v>
       </c>
       <c r="H98" s="40" t="str">
@@ -11154,9 +11154,9 @@
       </c>
       <c r="X98" s="2"/>
     </row>
-    <row r="99" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:24" ht="102" x14ac:dyDescent="0.25">
       <c r="A99" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H99&lt;&gt;"",IF(F99&lt;&gt;"",CONCATENATE("...",D99,".",E99,".",F99,". - ",T99),IF(E99&lt;&gt;"",CONCATENATE("..",D99,".",E99,". - ",T99),CONCATENATE(D99,". - ",T99))),"")</f>
         <v>..B.15. - Brain and nervous system cancers</v>
       </c>
       <c r="B99" s="2">
@@ -11173,7 +11173,7 @@
       </c>
       <c r="F99" s="6"/>
       <c r="G99" s="40" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>cB15</v>
       </c>
       <c r="H99" s="40" t="str">
@@ -11223,7 +11223,7 @@
     </row>
     <row r="100" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A100" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H100&lt;&gt;"",IF(F100&lt;&gt;"",CONCATENATE("...",D100,".",E100,".",F100,". - ",T100),IF(E100&lt;&gt;"",CONCATENATE("..",D100,".",E100,". - ",T100),CONCATENATE(D100,". - ",T100))),"")</f>
         <v/>
       </c>
       <c r="B100" s="2">
@@ -11240,7 +11240,7 @@
       </c>
       <c r="F100" s="6"/>
       <c r="G100" s="40" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>cB99</v>
       </c>
       <c r="H100" s="40"/>
@@ -11287,7 +11287,7 @@
     </row>
     <row r="101" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A101" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H101&lt;&gt;"",IF(F101&lt;&gt;"",CONCATENATE("...",D101,".",E101,".",F101,". - ",T101),IF(E101&lt;&gt;"",CONCATENATE("..",D101,".",E101,". - ",T101),CONCATENATE(D101,". - ",T101))),"")</f>
         <v/>
       </c>
       <c r="B101" s="2">
@@ -11304,7 +11304,7 @@
       </c>
       <c r="F101" s="6"/>
       <c r="G101" s="40" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>cB99</v>
       </c>
       <c r="H101" s="40"/>
@@ -11351,7 +11351,7 @@
     </row>
     <row r="102" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A102" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H102&lt;&gt;"",IF(F102&lt;&gt;"",CONCATENATE("...",D102,".",E102,".",F102,". - ",T102),IF(E102&lt;&gt;"",CONCATENATE("..",D102,".",E102,". - ",T102),CONCATENATE(D102,". - ",T102))),"")</f>
         <v/>
       </c>
       <c r="B102" s="2">
@@ -11368,7 +11368,7 @@
       </c>
       <c r="F102" s="6"/>
       <c r="G102" s="40" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>cB99</v>
       </c>
       <c r="H102" s="40"/>
@@ -11415,7 +11415,7 @@
     </row>
     <row r="103" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A103" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H103&lt;&gt;"",IF(F103&lt;&gt;"",CONCATENATE("...",D103,".",E103,".",F103,". - ",T103),IF(E103&lt;&gt;"",CONCATENATE("..",D103,".",E103,". - ",T103),CONCATENATE(D103,". - ",T103))),"")</f>
         <v/>
       </c>
       <c r="B103" s="2">
@@ -11432,7 +11432,7 @@
       </c>
       <c r="F103" s="6"/>
       <c r="G103" s="40" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>cB99</v>
       </c>
       <c r="H103" s="40"/>
@@ -11473,9 +11473,9 @@
       </c>
       <c r="X103" s="2"/>
     </row>
-    <row r="104" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:24" ht="102" x14ac:dyDescent="0.25">
       <c r="A104" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H104&lt;&gt;"",IF(F104&lt;&gt;"",CONCATENATE("...",D104,".",E104,".",F104,". - ",T104),IF(E104&lt;&gt;"",CONCATENATE("..",D104,".",E104,". - ",T104),CONCATENATE(D104,". - ",T104))),"")</f>
         <v>..B.16. - Lymphomas and multiple myeloma</v>
       </c>
       <c r="B104" s="2">
@@ -11493,7 +11493,7 @@
       <c r="F104" s="6"/>
       <c r="G104" s="40"/>
       <c r="H104" s="40" t="str">
-        <f t="shared" ref="H104:H109" si="9">CONCATENATE(D104,E104,F104)</f>
+        <f t="shared" ref="H104:H109" si="7">CONCATENATE(D104,E104,F104)</f>
         <v>B16</v>
       </c>
       <c r="I104" s="5"/>
@@ -11533,9 +11533,9 @@
       </c>
       <c r="X104" s="2"/>
     </row>
-    <row r="105" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A105" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H105&lt;&gt;"",IF(F105&lt;&gt;"",CONCATENATE("...",D105,".",E105,".",F105,". - ",T105),IF(E105&lt;&gt;"",CONCATENATE("..",D105,".",E105,". - ",T105),CONCATENATE(D105,". - ",T105))),"")</f>
         <v>...B.16.a. - Hodgkin lymphoma</v>
       </c>
       <c r="B105" s="2">
@@ -11554,11 +11554,11 @@
         <v>1126</v>
       </c>
       <c r="G105" s="40" t="str">
-        <f t="shared" ref="G105:G111" si="10">CONCATENATE("c",D105,E105,F105)</f>
+        <f t="shared" ref="G105:G111" si="8">CONCATENATE("c",D105,E105,F105)</f>
         <v>cB16a</v>
       </c>
       <c r="H105" s="40" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>B16a</v>
       </c>
       <c r="I105" s="5"/>
@@ -11598,9 +11598,9 @@
       </c>
       <c r="X105" s="2"/>
     </row>
-    <row r="106" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:24" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A106" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H106&lt;&gt;"",IF(F106&lt;&gt;"",CONCATENATE("...",D106,".",E106,".",F106,". - ",T106),IF(E106&lt;&gt;"",CONCATENATE("..",D106,".",E106,". - ",T106),CONCATENATE(D106,". - ",T106))),"")</f>
         <v>...B.16.b. - Non-Hodgkin lymphoma</v>
       </c>
       <c r="B106" s="2">
@@ -11619,11 +11619,11 @@
         <v>1127</v>
       </c>
       <c r="G106" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>cB16b</v>
       </c>
       <c r="H106" s="40" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>B16b</v>
       </c>
       <c r="I106" s="5"/>
@@ -11663,9 +11663,9 @@
       </c>
       <c r="X106" s="2"/>
     </row>
-    <row r="107" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A107" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H107&lt;&gt;"",IF(F107&lt;&gt;"",CONCATENATE("...",D107,".",E107,".",F107,". - ",T107),IF(E107&lt;&gt;"",CONCATENATE("..",D107,".",E107,". - ",T107),CONCATENATE(D107,". - ",T107))),"")</f>
         <v>...B.16.c. - Multiple myeloma</v>
       </c>
       <c r="B107" s="2">
@@ -11684,11 +11684,11 @@
         <v>1130</v>
       </c>
       <c r="G107" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>cB16c</v>
       </c>
       <c r="H107" s="40" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>B16c</v>
       </c>
       <c r="I107" s="5"/>
@@ -11728,9 +11728,9 @@
       </c>
       <c r="X107" s="2"/>
     </row>
-    <row r="108" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A108" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H108&lt;&gt;"",IF(F108&lt;&gt;"",CONCATENATE("...",D108,".",E108,".",F108,". - ",T108),IF(E108&lt;&gt;"",CONCATENATE("..",D108,".",E108,". - ",T108),CONCATENATE(D108,". - ",T108))),"")</f>
         <v>..B.17. - Leukaemia</v>
       </c>
       <c r="B108" s="2">
@@ -11747,11 +11747,11 @@
       </c>
       <c r="F108" s="6"/>
       <c r="G108" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>cB17</v>
       </c>
       <c r="H108" s="40" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>B17</v>
       </c>
       <c r="I108" s="5"/>
@@ -11791,9 +11791,9 @@
       </c>
       <c r="X108" s="2"/>
     </row>
-    <row r="109" spans="1:24" ht="51" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A109" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H109&lt;&gt;"",IF(F109&lt;&gt;"",CONCATENATE("...",D109,".",E109,".",F109,". - ",T109),IF(E109&lt;&gt;"",CONCATENATE("..",D109,".",E109,". - ",T109),CONCATENATE(D109,". - ",T109))),"")</f>
         <v>..B.99. - Other malignant neoplasms</v>
       </c>
       <c r="B109" s="2">
@@ -11810,11 +11810,11 @@
       </c>
       <c r="F109" s="6"/>
       <c r="G109" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>cB99</v>
       </c>
       <c r="H109" s="40" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>B99</v>
       </c>
       <c r="I109" s="5" t="s">
@@ -11856,7 +11856,7 @@
     </row>
     <row r="110" spans="1:24" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A110" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H110&lt;&gt;"",IF(F110&lt;&gt;"",CONCATENATE("...",D110,".",E110,".",F110,". - ",T110),IF(E110&lt;&gt;"",CONCATENATE("..",D110,".",E110,". - ",T110),CONCATENATE(D110,". - ",T110))),"")</f>
         <v/>
       </c>
       <c r="B110" s="2">
@@ -11873,7 +11873,7 @@
       </c>
       <c r="F110" s="6"/>
       <c r="G110" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>cD99</v>
       </c>
       <c r="H110" s="40"/>
@@ -11912,9 +11912,9 @@
       </c>
       <c r="X110" s="2"/>
     </row>
-    <row r="111" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A111" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H111&lt;&gt;"",IF(F111&lt;&gt;"",CONCATENATE("...",D111,".",E111,".",F111,". - ",T111),IF(E111&lt;&gt;"",CONCATENATE("..",D111,".",E111,". - ",T111),CONCATENATE(D111,". - ",T111))),"")</f>
         <v>..D.01. - Diabetes mellitus</v>
       </c>
       <c r="B111" s="2">
@@ -11931,7 +11931,7 @@
       </c>
       <c r="F111" s="6"/>
       <c r="G111" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>cD01</v>
       </c>
       <c r="H111" s="40" t="str">
@@ -11985,9 +11985,9 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="112" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:24" ht="102" x14ac:dyDescent="0.25">
       <c r="A112" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H112&lt;&gt;"",IF(F112&lt;&gt;"",CONCATENATE("...",D112,".",E112,".",F112,". - ",T112),IF(E112&lt;&gt;"",CONCATENATE("..",D112,".",E112,". - ",T112),CONCATENATE(D112,". - ",T112))),"")</f>
         <v>..D.02. - Endocrine, blood, immune disorders</v>
       </c>
       <c r="B112" s="2">
@@ -12049,7 +12049,7 @@
     </row>
     <row r="113" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A113" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H113&lt;&gt;"",IF(F113&lt;&gt;"",CONCATENATE("...",D113,".",E113,".",F113,". - ",T113),IF(E113&lt;&gt;"",CONCATENATE("..",D113,".",E113,". - ",T113),CONCATENATE(D113,". - ",T113))),"")</f>
         <v/>
       </c>
       <c r="B113" s="2">
@@ -12109,7 +12109,7 @@
     </row>
     <row r="114" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A114" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H114&lt;&gt;"",IF(F114&lt;&gt;"",CONCATENATE("...",D114,".",E114,".",F114,". - ",T114),IF(E114&lt;&gt;"",CONCATENATE("..",D114,".",E114,". - ",T114),CONCATENATE(D114,". - ",T114))),"")</f>
         <v/>
       </c>
       <c r="B114" s="2">
@@ -12169,7 +12169,7 @@
     </row>
     <row r="115" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A115" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H115&lt;&gt;"",IF(F115&lt;&gt;"",CONCATENATE("...",D115,".",E115,".",F115,". - ",T115),IF(E115&lt;&gt;"",CONCATENATE("..",D115,".",E115,". - ",T115),CONCATENATE(D115,". - ",T115))),"")</f>
         <v/>
       </c>
       <c r="B115" s="2">
@@ -12227,9 +12227,9 @@
       </c>
       <c r="X115" s="2"/>
     </row>
-    <row r="116" spans="1:24" ht="33" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A116" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H116&lt;&gt;"",IF(F116&lt;&gt;"",CONCATENATE("...",D116,".",E116,".",F116,". - ",T116),IF(E116&lt;&gt;"",CONCATENATE("..",D116,".",E116,". - ",T116),CONCATENATE(D116,". - ",T116))),"")</f>
         <v/>
       </c>
       <c r="B116" s="2">
@@ -12289,7 +12289,7 @@
     </row>
     <row r="117" spans="1:24" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A117" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H117&lt;&gt;"",IF(F117&lt;&gt;"",CONCATENATE("...",D117,".",E117,".",F117,". - ",T117),IF(E117&lt;&gt;"",CONCATENATE("..",D117,".",E117,". - ",T117),CONCATENATE(D117,". - ",T117))),"")</f>
         <v/>
       </c>
       <c r="B117" s="2">
@@ -12346,9 +12346,9 @@
       </c>
       <c r="X117" s="2"/>
     </row>
-    <row r="118" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A118" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H118&lt;&gt;"",IF(F118&lt;&gt;"",CONCATENATE("...",D118,".",E118,".",F118,". - ",T118),IF(E118&lt;&gt;"",CONCATENATE("..",D118,".",E118,". - ",T118),CONCATENATE(D118,". - ",T118))),"")</f>
         <v xml:space="preserve">..D.03. - Mental Health disorders </v>
       </c>
       <c r="B118" s="2"/>
@@ -12390,9 +12390,9 @@
       <c r="W118" s="45"/>
       <c r="X118" s="2"/>
     </row>
-    <row r="119" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:24" ht="51" x14ac:dyDescent="0.25">
       <c r="A119" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H119&lt;&gt;"",IF(F119&lt;&gt;"",CONCATENATE("...",D119,".",E119,".",F119,". - ",T119),IF(E119&lt;&gt;"",CONCATENATE("..",D119,".",E119,". - ",T119),CONCATENATE(D119,". - ",T119))),"")</f>
         <v xml:space="preserve">..D.04. - Substance use </v>
       </c>
       <c r="B119" s="2"/>
@@ -12434,7 +12434,7 @@
     </row>
     <row r="120" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A120" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H120&lt;&gt;"",IF(F120&lt;&gt;"",CONCATENATE("...",D120,".",E120,".",F120,". - ",T120),IF(E120&lt;&gt;"",CONCATENATE("..",D120,".",E120,". - ",T120),CONCATENATE(D120,". - ",T120))),"")</f>
         <v/>
       </c>
       <c r="B120" s="2"/>
@@ -12465,7 +12465,7 @@
     </row>
     <row r="121" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A121" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H121&lt;&gt;"",IF(F121&lt;&gt;"",CONCATENATE("...",D121,".",E121,".",F121,". - ",T121),IF(E121&lt;&gt;"",CONCATENATE("..",D121,".",E121,". - ",T121),CONCATENATE(D121,". - ",T121))),"")</f>
         <v/>
       </c>
       <c r="B121" s="2">
@@ -12514,7 +12514,7 @@
     </row>
     <row r="122" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A122" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H122&lt;&gt;"",IF(F122&lt;&gt;"",CONCATENATE("...",D122,".",E122,".",F122,". - ",T122),IF(E122&lt;&gt;"",CONCATENATE("..",D122,".",E122,". - ",T122),CONCATENATE(D122,". - ",T122))),"")</f>
         <v/>
       </c>
       <c r="B122" s="2">
@@ -12574,7 +12574,7 @@
     </row>
     <row r="123" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A123" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H123&lt;&gt;"",IF(F123&lt;&gt;"",CONCATENATE("...",D123,".",E123,".",F123,". - ",T123),IF(E123&lt;&gt;"",CONCATENATE("..",D123,".",E123,". - ",T123),CONCATENATE(D123,". - ",T123))),"")</f>
         <v/>
       </c>
       <c r="B123" s="2">
@@ -12634,7 +12634,7 @@
     </row>
     <row r="124" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A124" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H124&lt;&gt;"",IF(F124&lt;&gt;"",CONCATENATE("...",D124,".",E124,".",F124,". - ",T124),IF(E124&lt;&gt;"",CONCATENATE("..",D124,".",E124,". - ",T124),CONCATENATE(D124,". - ",T124))),"")</f>
         <v/>
       </c>
       <c r="B124" s="2">
@@ -12694,7 +12694,7 @@
     </row>
     <row r="125" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A125" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H125&lt;&gt;"",IF(F125&lt;&gt;"",CONCATENATE("...",D125,".",E125,".",F125,". - ",T125),IF(E125&lt;&gt;"",CONCATENATE("..",D125,".",E125,". - ",T125),CONCATENATE(D125,". - ",T125))),"")</f>
         <v/>
       </c>
       <c r="B125" s="2">
@@ -12756,9 +12756,9 @@
       </c>
       <c r="X125" s="2"/>
     </row>
-    <row r="126" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A126" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H126&lt;&gt;"",IF(F126&lt;&gt;"",CONCATENATE("...",D126,".",E126,".",F126,". - ",T126),IF(E126&lt;&gt;"",CONCATENATE("..",D126,".",E126,". - ",T126),CONCATENATE(D126,". - ",T126))),"")</f>
         <v>...D.04.a. - Alcohol use disorders</v>
       </c>
       <c r="B126" s="2">
@@ -12827,7 +12827,7 @@
     </row>
     <row r="127" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A127" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H127&lt;&gt;"",IF(F127&lt;&gt;"",CONCATENATE("...",D127,".",E127,".",F127,". - ",T127),IF(E127&lt;&gt;"",CONCATENATE("..",D127,".",E127,". - ",T127),CONCATENATE(D127,". - ",T127))),"")</f>
         <v/>
       </c>
       <c r="B127" s="2">
@@ -12878,9 +12878,9 @@
       </c>
       <c r="X127" s="2"/>
     </row>
-    <row r="128" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A128" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H128&lt;&gt;"",IF(F128&lt;&gt;"",CONCATENATE("...",D128,".",E128,".",F128,". - ",T128),IF(E128&lt;&gt;"",CONCATENATE("..",D128,".",E128,". - ",T128),CONCATENATE(D128,". - ",T128))),"")</f>
         <v>...D.04.b. - Opioid use disorders</v>
       </c>
       <c r="B128" s="2">
@@ -12899,7 +12899,7 @@
         <v>1127</v>
       </c>
       <c r="G128" s="40" t="str">
-        <f t="shared" ref="G128:G135" si="11">CONCATENATE("c",D128,E128,F128)</f>
+        <f t="shared" ref="G128:G135" si="9">CONCATENATE("c",D128,E128,F128)</f>
         <v>cD04b</v>
       </c>
       <c r="H128" s="40" t="str">
@@ -12943,9 +12943,9 @@
       </c>
       <c r="X128" s="2"/>
     </row>
-    <row r="129" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A129" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H129&lt;&gt;"",IF(F129&lt;&gt;"",CONCATENATE("...",D129,".",E129,".",F129,". - ",T129),IF(E129&lt;&gt;"",CONCATENATE("..",D129,".",E129,". - ",T129),CONCATENATE(D129,". - ",T129))),"")</f>
         <v>...D.04.c. - Cocaine use disorders</v>
       </c>
       <c r="B129" s="2">
@@ -12964,7 +12964,7 @@
         <v>1130</v>
       </c>
       <c r="G129" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>cD04c</v>
       </c>
       <c r="H129" s="40" t="str">
@@ -13008,9 +13008,9 @@
       </c>
       <c r="X129" s="2"/>
     </row>
-    <row r="130" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:24" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A130" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H130&lt;&gt;"",IF(F130&lt;&gt;"",CONCATENATE("...",D130,".",E130,".",F130,". - ",T130),IF(E130&lt;&gt;"",CONCATENATE("..",D130,".",E130,". - ",T130),CONCATENATE(D130,". - ",T130))),"")</f>
         <v>...D.04.d. - Amphetamine use disorders</v>
       </c>
       <c r="B130" s="2">
@@ -13029,7 +13029,7 @@
         <v>1154</v>
       </c>
       <c r="G130" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>cD04d</v>
       </c>
       <c r="H130" s="40" t="str">
@@ -13075,7 +13075,7 @@
     </row>
     <row r="131" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A131" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H131&lt;&gt;"",IF(F131&lt;&gt;"",CONCATENATE("...",D131,".",E131,".",F131,". - ",T131),IF(E131&lt;&gt;"",CONCATENATE("..",D131,".",E131,". - ",T131),CONCATENATE(D131,". - ",T131))),"")</f>
         <v/>
       </c>
       <c r="B131" s="2">
@@ -13092,7 +13092,7 @@
       </c>
       <c r="F131" s="6"/>
       <c r="G131" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>cD04</v>
       </c>
       <c r="H131" s="40"/>
@@ -13130,7 +13130,7 @@
     </row>
     <row r="132" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A132" s="44" t="str">
-        <f t="shared" ref="A132:A195" si="12">IF(H132&lt;&gt;"",IF(F132&lt;&gt;"",CONCATENATE("...",D132,".",E132,".",F132,". - ",T132),IF(E132&lt;&gt;"",CONCATENATE("..",D132,".",E132,". - ",T132),CONCATENATE(D132,". - ",T132))),"")</f>
+        <f>IF(H132&lt;&gt;"",IF(F132&lt;&gt;"",CONCATENATE("...",D132,".",E132,".",F132,". - ",T132),IF(E132&lt;&gt;"",CONCATENATE("..",D132,".",E132,". - ",T132),CONCATENATE(D132,". - ",T132))),"")</f>
         <v/>
       </c>
       <c r="B132" s="2">
@@ -13147,7 +13147,7 @@
       </c>
       <c r="F132" s="6"/>
       <c r="G132" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>cD04</v>
       </c>
       <c r="H132" s="40"/>
@@ -13196,7 +13196,7 @@
     </row>
     <row r="133" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A133" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H133&lt;&gt;"",IF(F133&lt;&gt;"",CONCATENATE("...",D133,".",E133,".",F133,". - ",T133),IF(E133&lt;&gt;"",CONCATENATE("..",D133,".",E133,". - ",T133),CONCATENATE(D133,". - ",T133))),"")</f>
         <v/>
       </c>
       <c r="B133" s="2">
@@ -13213,7 +13213,7 @@
       </c>
       <c r="F133" s="6"/>
       <c r="G133" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>cD03</v>
       </c>
       <c r="H133" s="40"/>
@@ -13252,7 +13252,7 @@
     </row>
     <row r="134" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A134" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H134&lt;&gt;"",IF(F134&lt;&gt;"",CONCATENATE("...",D134,".",E134,".",F134,". - ",T134),IF(E134&lt;&gt;"",CONCATENATE("..",D134,".",E134,". - ",T134),CONCATENATE(D134,". - ",T134))),"")</f>
         <v/>
       </c>
       <c r="B134" s="2">
@@ -13269,7 +13269,7 @@
       </c>
       <c r="F134" s="6"/>
       <c r="G134" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>cD03</v>
       </c>
       <c r="H134" s="40"/>
@@ -13312,7 +13312,7 @@
     </row>
     <row r="135" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A135" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H135&lt;&gt;"",IF(F135&lt;&gt;"",CONCATENATE("...",D135,".",E135,".",F135,". - ",T135),IF(E135&lt;&gt;"",CONCATENATE("..",D135,".",E135,". - ",T135),CONCATENATE(D135,". - ",T135))),"")</f>
         <v/>
       </c>
       <c r="B135" s="2">
@@ -13329,7 +13329,7 @@
       </c>
       <c r="F135" s="6"/>
       <c r="G135" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>cD03</v>
       </c>
       <c r="H135" s="40"/>
@@ -13368,7 +13368,7 @@
     </row>
     <row r="136" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A136" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H136&lt;&gt;"",IF(F136&lt;&gt;"",CONCATENATE("...",D136,".",E136,".",F136,". - ",T136),IF(E136&lt;&gt;"",CONCATENATE("..",D136,".",E136,". - ",T136),CONCATENATE(D136,". - ",T136))),"")</f>
         <v/>
       </c>
       <c r="B136" s="2">
@@ -13417,7 +13417,7 @@
     </row>
     <row r="137" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A137" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H137&lt;&gt;"",IF(F137&lt;&gt;"",CONCATENATE("...",D137,".",E137,".",F137,". - ",T137),IF(E137&lt;&gt;"",CONCATENATE("..",D137,".",E137,". - ",T137),CONCATENATE(D137,". - ",T137))),"")</f>
         <v/>
       </c>
       <c r="B137" s="2">
@@ -13473,7 +13473,7 @@
     </row>
     <row r="138" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A138" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H138&lt;&gt;"",IF(F138&lt;&gt;"",CONCATENATE("...",D138,".",E138,".",F138,". - ",T138),IF(E138&lt;&gt;"",CONCATENATE("..",D138,".",E138,". - ",T138),CONCATENATE(D138,". - ",T138))),"")</f>
         <v/>
       </c>
       <c r="B138" s="2">
@@ -13529,7 +13529,7 @@
     </row>
     <row r="139" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A139" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H139&lt;&gt;"",IF(F139&lt;&gt;"",CONCATENATE("...",D139,".",E139,".",F139,". - ",T139),IF(E139&lt;&gt;"",CONCATENATE("..",D139,".",E139,". - ",T139),CONCATENATE(D139,". - ",T139))),"")</f>
         <v/>
       </c>
       <c r="B139" s="2">
@@ -13585,7 +13585,7 @@
     </row>
     <row r="140" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A140" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H140&lt;&gt;"",IF(F140&lt;&gt;"",CONCATENATE("...",D140,".",E140,".",F140,". - ",T140),IF(E140&lt;&gt;"",CONCATENATE("..",D140,".",E140,". - ",T140),CONCATENATE(D140,". - ",T140))),"")</f>
         <v/>
       </c>
       <c r="B140" s="2">
@@ -13641,7 +13641,7 @@
     </row>
     <row r="141" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A141" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H141&lt;&gt;"",IF(F141&lt;&gt;"",CONCATENATE("...",D141,".",E141,".",F141,". - ",T141),IF(E141&lt;&gt;"",CONCATENATE("..",D141,".",E141,". - ",T141),CONCATENATE(D141,". - ",T141))),"")</f>
         <v/>
       </c>
       <c r="B141" s="2">
@@ -13700,7 +13700,7 @@
     </row>
     <row r="142" spans="1:24" ht="102" x14ac:dyDescent="0.25">
       <c r="A142" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H142&lt;&gt;"",IF(F142&lt;&gt;"",CONCATENATE("...",D142,".",E142,".",F142,". - ",T142),IF(E142&lt;&gt;"",CONCATENATE("..",D142,".",E142,". - ",T142),CONCATENATE(D142,". - ",T142))),"")</f>
         <v>..D.05. - Alzheimer’s disease and other dementias</v>
       </c>
       <c r="B142" s="2">
@@ -13717,7 +13717,7 @@
       </c>
       <c r="F142" s="6"/>
       <c r="G142" s="40" t="str">
-        <f t="shared" ref="G142:G148" si="13">CONCATENATE("c",D142,E142,F142)</f>
+        <f t="shared" ref="G142:G148" si="10">CONCATENATE("c",D142,E142,F142)</f>
         <v>cD05</v>
       </c>
       <c r="H142" s="40" t="str">
@@ -13763,7 +13763,7 @@
     </row>
     <row r="143" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A143" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H143&lt;&gt;"",IF(F143&lt;&gt;"",CONCATENATE("...",D143,".",E143,".",F143,". - ",T143),IF(E143&lt;&gt;"",CONCATENATE("..",D143,".",E143,". - ",T143),CONCATENATE(D143,". - ",T143))),"")</f>
         <v/>
       </c>
       <c r="B143" s="2">
@@ -13780,7 +13780,7 @@
       </c>
       <c r="F143" s="6"/>
       <c r="G143" s="40" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>cD06</v>
       </c>
       <c r="H143" s="40"/>
@@ -13823,7 +13823,7 @@
     </row>
     <row r="144" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A144" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H144&lt;&gt;"",IF(F144&lt;&gt;"",CONCATENATE("...",D144,".",E144,".",F144,". - ",T144),IF(E144&lt;&gt;"",CONCATENATE("..",D144,".",E144,". - ",T144),CONCATENATE(D144,". - ",T144))),"")</f>
         <v/>
       </c>
       <c r="B144" s="2">
@@ -13840,7 +13840,7 @@
       </c>
       <c r="F144" s="6"/>
       <c r="G144" s="40" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>cD06</v>
       </c>
       <c r="H144" s="40"/>
@@ -13883,7 +13883,7 @@
     </row>
     <row r="145" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A145" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H145&lt;&gt;"",IF(F145&lt;&gt;"",CONCATENATE("...",D145,".",E145,".",F145,". - ",T145),IF(E145&lt;&gt;"",CONCATENATE("..",D145,".",E145,". - ",T145),CONCATENATE(D145,". - ",T145))),"")</f>
         <v/>
       </c>
       <c r="B145" s="2">
@@ -13900,7 +13900,7 @@
       </c>
       <c r="F145" s="6"/>
       <c r="G145" s="40" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>cD06</v>
       </c>
       <c r="H145" s="40"/>
@@ -13943,7 +13943,7 @@
     </row>
     <row r="146" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A146" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H146&lt;&gt;"",IF(F146&lt;&gt;"",CONCATENATE("...",D146,".",E146,".",F146,". - ",T146),IF(E146&lt;&gt;"",CONCATENATE("..",D146,".",E146,". - ",T146),CONCATENATE(D146,". - ",T146))),"")</f>
         <v/>
       </c>
       <c r="B146" s="2">
@@ -13960,7 +13960,7 @@
       </c>
       <c r="F146" s="6"/>
       <c r="G146" s="40" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>cD06</v>
       </c>
       <c r="H146" s="40"/>
@@ -13999,7 +13999,7 @@
     </row>
     <row r="147" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A147" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H147&lt;&gt;"",IF(F147&lt;&gt;"",CONCATENATE("...",D147,".",E147,".",F147,". - ",T147),IF(E147&lt;&gt;"",CONCATENATE("..",D147,".",E147,". - ",T147),CONCATENATE(D147,". - ",T147))),"")</f>
         <v/>
       </c>
       <c r="B147" s="2">
@@ -14016,7 +14016,7 @@
       </c>
       <c r="F147" s="6"/>
       <c r="G147" s="40" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>cD06</v>
       </c>
       <c r="H147" s="40"/>
@@ -14053,9 +14053,9 @@
       </c>
       <c r="X147" s="2"/>
     </row>
-    <row r="148" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A148" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H148&lt;&gt;"",IF(F148&lt;&gt;"",CONCATENATE("...",D148,".",E148,".",F148,". - ",T148),IF(E148&lt;&gt;"",CONCATENATE("..",D148,".",E148,". - ",T148),CONCATENATE(D148,". - ",T148))),"")</f>
         <v>..D.06. - Other neurological conditions</v>
       </c>
       <c r="B148" s="2">
@@ -14072,7 +14072,7 @@
       </c>
       <c r="F148" s="6"/>
       <c r="G148" s="40" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>cD06</v>
       </c>
       <c r="H148" s="40" t="str">
@@ -14122,7 +14122,7 @@
     </row>
     <row r="149" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A149" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H149&lt;&gt;"",IF(F149&lt;&gt;"",CONCATENATE("...",D149,".",E149,".",F149,". - ",T149),IF(E149&lt;&gt;"",CONCATENATE("..",D149,".",E149,". - ",T149),CONCATENATE(D149,". - ",T149))),"")</f>
         <v/>
       </c>
       <c r="B149" s="2">
@@ -14177,7 +14177,7 @@
     </row>
     <row r="150" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A150" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H150&lt;&gt;"",IF(F150&lt;&gt;"",CONCATENATE("...",D150,".",E150,".",F150,". - ",T150),IF(E150&lt;&gt;"",CONCATENATE("..",D150,".",E150,". - ",T150),CONCATENATE(D150,". - ",T150))),"")</f>
         <v/>
       </c>
       <c r="B150" s="2">
@@ -14194,7 +14194,7 @@
       </c>
       <c r="F150" s="6"/>
       <c r="G150" s="40" t="str">
-        <f t="shared" ref="G150:G156" si="14">CONCATENATE("c",D150,E150,F150)</f>
+        <f t="shared" ref="G150:G156" si="11">CONCATENATE("c",D150,E150,F150)</f>
         <v>cD99</v>
       </c>
       <c r="H150" s="40"/>
@@ -14233,7 +14233,7 @@
     </row>
     <row r="151" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A151" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H151&lt;&gt;"",IF(F151&lt;&gt;"",CONCATENATE("...",D151,".",E151,".",F151,". - ",T151),IF(E151&lt;&gt;"",CONCATENATE("..",D151,".",E151,". - ",T151),CONCATENATE(D151,". - ",T151))),"")</f>
         <v/>
       </c>
       <c r="B151" s="2">
@@ -14250,7 +14250,7 @@
       </c>
       <c r="F151" s="6"/>
       <c r="G151" s="40" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>cD99</v>
       </c>
       <c r="H151" s="40"/>
@@ -14289,7 +14289,7 @@
     </row>
     <row r="152" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A152" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H152&lt;&gt;"",IF(F152&lt;&gt;"",CONCATENATE("...",D152,".",E152,".",F152,". - ",T152),IF(E152&lt;&gt;"",CONCATENATE("..",D152,".",E152,". - ",T152),CONCATENATE(D152,". - ",T152))),"")</f>
         <v/>
       </c>
       <c r="B152" s="2">
@@ -14306,7 +14306,7 @@
       </c>
       <c r="F152" s="6"/>
       <c r="G152" s="40" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>cD99</v>
       </c>
       <c r="H152" s="40"/>
@@ -14345,7 +14345,7 @@
     </row>
     <row r="153" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A153" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H153&lt;&gt;"",IF(F153&lt;&gt;"",CONCATENATE("...",D153,".",E153,".",F153,". - ",T153),IF(E153&lt;&gt;"",CONCATENATE("..",D153,".",E153,". - ",T153),CONCATENATE(D153,". - ",T153))),"")</f>
         <v/>
       </c>
       <c r="B153" s="2">
@@ -14362,7 +14362,7 @@
       </c>
       <c r="F153" s="6"/>
       <c r="G153" s="40" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>cD99</v>
       </c>
       <c r="H153" s="40"/>
@@ -14401,7 +14401,7 @@
     </row>
     <row r="154" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A154" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H154&lt;&gt;"",IF(F154&lt;&gt;"",CONCATENATE("...",D154,".",E154,".",F154,". - ",T154),IF(E154&lt;&gt;"",CONCATENATE("..",D154,".",E154,". - ",T154),CONCATENATE(D154,". - ",T154))),"")</f>
         <v/>
       </c>
       <c r="B154" s="2">
@@ -14418,7 +14418,7 @@
       </c>
       <c r="F154" s="6"/>
       <c r="G154" s="40" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>cD99</v>
       </c>
       <c r="H154" s="40"/>
@@ -14457,7 +14457,7 @@
     </row>
     <row r="155" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A155" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H155&lt;&gt;"",IF(F155&lt;&gt;"",CONCATENATE("...",D155,".",E155,".",F155,". - ",T155),IF(E155&lt;&gt;"",CONCATENATE("..",D155,".",E155,". - ",T155),CONCATENATE(D155,". - ",T155))),"")</f>
         <v/>
       </c>
       <c r="B155" s="2">
@@ -14474,7 +14474,7 @@
       </c>
       <c r="F155" s="6"/>
       <c r="G155" s="40" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>cD99</v>
       </c>
       <c r="H155" s="40"/>
@@ -14513,7 +14513,7 @@
     </row>
     <row r="156" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A156" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H156&lt;&gt;"",IF(F156&lt;&gt;"",CONCATENATE("...",D156,".",E156,".",F156,". - ",T156),IF(E156&lt;&gt;"",CONCATENATE("..",D156,".",E156,". - ",T156),CONCATENATE(D156,". - ",T156))),"")</f>
         <v/>
       </c>
       <c r="B156" s="2">
@@ -14530,7 +14530,7 @@
       </c>
       <c r="F156" s="6"/>
       <c r="G156" s="40" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>cD99</v>
       </c>
       <c r="H156" s="40"/>
@@ -14569,9 +14569,9 @@
         <v>615</v>
       </c>
     </row>
-    <row r="157" spans="1:24" ht="57.75" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A157" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H157&lt;&gt;"",IF(F157&lt;&gt;"",CONCATENATE("...",D157,".",E157,".",F157,". - ",T157),IF(E157&lt;&gt;"",CONCATENATE("..",D157,".",E157,". - ",T157),CONCATENATE(D157,". - ",T157))),"")</f>
         <v>C. - Cardiovascular diseases</v>
       </c>
       <c r="B157" s="2">
@@ -14629,7 +14629,7 @@
     </row>
     <row r="158" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A158" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H158&lt;&gt;"",IF(F158&lt;&gt;"",CONCATENATE("...",D158,".",E158,".",F158,". - ",T158),IF(E158&lt;&gt;"",CONCATENATE("..",D158,".",E158,". - ",T158),CONCATENATE(D158,". - ",T158))),"")</f>
         <v/>
       </c>
       <c r="B158" s="2">
@@ -14646,7 +14646,7 @@
       </c>
       <c r="F158" s="6"/>
       <c r="G158" s="40" t="str">
-        <f t="shared" ref="G158:G164" si="15">CONCATENATE("c",D158,E158,F158)</f>
+        <f t="shared" ref="G158:G164" si="12">CONCATENATE("c",D158,E158,F158)</f>
         <v>cC99</v>
       </c>
       <c r="H158" s="40"/>
@@ -14691,9 +14691,9 @@
       </c>
       <c r="X158" s="2"/>
     </row>
-    <row r="159" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A159" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H159&lt;&gt;"",IF(F159&lt;&gt;"",CONCATENATE("...",D159,".",E159,".",F159,". - ",T159),IF(E159&lt;&gt;"",CONCATENATE("..",D159,".",E159,". - ",T159),CONCATENATE(D159,". - ",T159))),"")</f>
         <v>..C.01. - Hypertensive heart disease</v>
       </c>
       <c r="B159" s="2">
@@ -14710,11 +14710,11 @@
       </c>
       <c r="F159" s="6"/>
       <c r="G159" s="40" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>cC01</v>
       </c>
       <c r="H159" s="40" t="str">
-        <f t="shared" ref="H159:H164" si="16">CONCATENATE(D159,E159,F159)</f>
+        <f t="shared" ref="H159:H164" si="13">CONCATENATE(D159,E159,F159)</f>
         <v>C01</v>
       </c>
       <c r="I159" s="5"/>
@@ -14758,9 +14758,9 @@
       </c>
       <c r="X159" s="2"/>
     </row>
-    <row r="160" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A160" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H160&lt;&gt;"",IF(F160&lt;&gt;"",CONCATENATE("...",D160,".",E160,".",F160,". - ",T160),IF(E160&lt;&gt;"",CONCATENATE("..",D160,".",E160,". - ",T160),CONCATENATE(D160,". - ",T160))),"")</f>
         <v>..C.02. - Ischaemic heart disease</v>
       </c>
       <c r="B160" s="2">
@@ -14777,11 +14777,11 @@
       </c>
       <c r="F160" s="6"/>
       <c r="G160" s="40" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>cC02</v>
       </c>
       <c r="H160" s="40" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>C02</v>
       </c>
       <c r="I160" s="5"/>
@@ -14827,7 +14827,7 @@
     </row>
     <row r="161" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A161" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H161&lt;&gt;"",IF(F161&lt;&gt;"",CONCATENATE("...",D161,".",E161,".",F161,". - ",T161),IF(E161&lt;&gt;"",CONCATENATE("..",D161,".",E161,". - ",T161),CONCATENATE(D161,". - ",T161))),"")</f>
         <v>..C.03. - Stroke</v>
       </c>
       <c r="B161" s="2">
@@ -14844,11 +14844,11 @@
       </c>
       <c r="F161" s="6"/>
       <c r="G161" s="40" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>cC03</v>
       </c>
       <c r="H161" s="40" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>C03</v>
       </c>
       <c r="I161" s="5" t="s">
@@ -14896,9 +14896,9 @@
       </c>
       <c r="X161" s="2"/>
     </row>
-    <row r="162" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:24" ht="102" x14ac:dyDescent="0.25">
       <c r="A162" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H162&lt;&gt;"",IF(F162&lt;&gt;"",CONCATENATE("...",D162,".",E162,".",F162,". - ",T162),IF(E162&lt;&gt;"",CONCATENATE("..",D162,".",E162,". - ",T162),CONCATENATE(D162,". - ",T162))),"")</f>
         <v>..C.04. - Cardiomyopathy, myocarditis, endocarditis</v>
       </c>
       <c r="B162" s="2">
@@ -14915,11 +14915,11 @@
       </c>
       <c r="F162" s="6"/>
       <c r="G162" s="40" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>cC04</v>
       </c>
       <c r="H162" s="40" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>C04</v>
       </c>
       <c r="I162" s="5"/>
@@ -14965,9 +14965,9 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="163" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A163" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H163&lt;&gt;"",IF(F163&lt;&gt;"",CONCATENATE("...",D163,".",E163,".",F163,". - ",T163),IF(E163&lt;&gt;"",CONCATENATE("..",D163,".",E163,". - ",T163),CONCATENATE(D163,". - ",T163))),"")</f>
         <v>..C.05. -  Congestive heart failure</v>
       </c>
       <c r="B163" s="2"/>
@@ -14980,11 +14980,11 @@
       </c>
       <c r="F163" s="6"/>
       <c r="G163" s="40" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>cC05</v>
       </c>
       <c r="H163" s="40" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>C05</v>
       </c>
       <c r="I163" s="5" t="s">
@@ -15018,9 +15018,9 @@
       <c r="W163" s="51"/>
       <c r="X163" s="2"/>
     </row>
-    <row r="164" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:24" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A164" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H164&lt;&gt;"",IF(F164&lt;&gt;"",CONCATENATE("...",D164,".",E164,".",F164,". - ",T164),IF(E164&lt;&gt;"",CONCATENATE("..",D164,".",E164,". - ",T164),CONCATENATE(D164,". - ",T164))),"")</f>
         <v>..C.99. - Other or unspecified cardiovascular diseases</v>
       </c>
       <c r="B164" s="2">
@@ -15037,11 +15037,11 @@
       </c>
       <c r="F164" s="6"/>
       <c r="G164" s="40" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>cC99</v>
       </c>
       <c r="H164" s="40" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>C99</v>
       </c>
       <c r="I164" s="5" t="s">
@@ -15093,7 +15093,7 @@
     </row>
     <row r="165" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A165" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H165&lt;&gt;"",IF(F165&lt;&gt;"",CONCATENATE("...",D165,".",E165,".",F165,". - ",T165),IF(E165&lt;&gt;"",CONCATENATE("..",D165,".",E165,". - ",T165),CONCATENATE(D165,". - ",T165))),"")</f>
         <v/>
       </c>
       <c r="B165" s="2">
@@ -15148,9 +15148,9 @@
       </c>
       <c r="X165" s="2"/>
     </row>
-    <row r="166" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:24" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A166" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H166&lt;&gt;"",IF(F166&lt;&gt;"",CONCATENATE("...",D166,".",E166,".",F166,". - ",T166),IF(E166&lt;&gt;"",CONCATENATE("..",D166,".",E166,". - ",T166),CONCATENATE(D166,". - ",T166))),"")</f>
         <v>..D.66. - Chronic obstructive pulmonary disease</v>
       </c>
       <c r="B166" s="2">
@@ -15211,9 +15211,9 @@
       </c>
       <c r="X166" s="2"/>
     </row>
-    <row r="167" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A167" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H167&lt;&gt;"",IF(F167&lt;&gt;"",CONCATENATE("...",D167,".",E167,".",F167,". - ",T167),IF(E167&lt;&gt;"",CONCATENATE("..",D167,".",E167,". - ",T167),CONCATENATE(D167,". - ",T167))),"")</f>
         <v>..D.67. - Asthma</v>
       </c>
       <c r="B167" s="2">
@@ -15274,9 +15274,9 @@
       </c>
       <c r="X167" s="2"/>
     </row>
-    <row r="168" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A168" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H168&lt;&gt;"",IF(F168&lt;&gt;"",CONCATENATE("...",D168,".",E168,".",F168,". - ",T168),IF(E168&lt;&gt;"",CONCATENATE("..",D168,".",E168,". - ",T168),CONCATENATE(D168,". - ",T168))),"")</f>
         <v>..D.68. - Other respiratory diseases</v>
       </c>
       <c r="B168" s="2">
@@ -15337,9 +15337,9 @@
       </c>
       <c r="X168" s="2"/>
     </row>
-    <row r="169" spans="1:24" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:24" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A169" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H169&lt;&gt;"",IF(F169&lt;&gt;"",CONCATENATE("...",D169,".",E169,".",F169,". - ",T169),IF(E169&lt;&gt;"",CONCATENATE("..",D169,".",E169,". - ",T169),CONCATENATE(D169,". - ",T169))),"")</f>
         <v>..D.09. - Digestive diseases (excluding cirrhosis)</v>
       </c>
       <c r="B169" s="2">
@@ -15401,7 +15401,7 @@
     </row>
     <row r="170" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A170" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H170&lt;&gt;"",IF(F170&lt;&gt;"",CONCATENATE("...",D170,".",E170,".",F170,". - ",T170),IF(E170&lt;&gt;"",CONCATENATE("..",D170,".",E170,". - ",T170),CONCATENATE(D170,". - ",T170))),"")</f>
         <v/>
       </c>
       <c r="B170" s="2">
@@ -15418,7 +15418,7 @@
       </c>
       <c r="F170" s="6"/>
       <c r="G170" s="40" t="str">
-        <f t="shared" ref="G170:G178" si="17">CONCATENATE("c",D170,E170,F170)</f>
+        <f t="shared" ref="G170:G178" si="14">CONCATENATE("c",D170,E170,F170)</f>
         <v>cD09</v>
       </c>
       <c r="H170" s="40"/>
@@ -15459,9 +15459,9 @@
       </c>
       <c r="X170" s="2"/>
     </row>
-    <row r="171" spans="1:24" s="48" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:24" s="48" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A171" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H171&lt;&gt;"",IF(F171&lt;&gt;"",CONCATENATE("...",D171,".",E171,".",F171,". - ",T171),IF(E171&lt;&gt;"",CONCATENATE("..",D171,".",E171,". - ",T171),CONCATENATE(D171,". - ",T171))),"")</f>
         <v>..D.11. - Cirrhosis of the liver</v>
       </c>
       <c r="B171" s="2">
@@ -15478,7 +15478,7 @@
       </c>
       <c r="F171" s="6"/>
       <c r="G171" s="40" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="14"/>
         <v>cD11</v>
       </c>
       <c r="H171" s="40" t="str">
@@ -15528,7 +15528,7 @@
     </row>
     <row r="172" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A172" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H172&lt;&gt;"",IF(F172&lt;&gt;"",CONCATENATE("...",D172,".",E172,".",F172,". - ",T172),IF(E172&lt;&gt;"",CONCATENATE("..",D172,".",E172,". - ",T172),CONCATENATE(D172,". - ",T172))),"")</f>
         <v/>
       </c>
       <c r="B172" s="2">
@@ -15545,7 +15545,7 @@
       </c>
       <c r="F172" s="6"/>
       <c r="G172" s="40" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="14"/>
         <v>cD09</v>
       </c>
       <c r="H172" s="40"/>
@@ -15588,7 +15588,7 @@
     </row>
     <row r="173" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A173" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H173&lt;&gt;"",IF(F173&lt;&gt;"",CONCATENATE("...",D173,".",E173,".",F173,". - ",T173),IF(E173&lt;&gt;"",CONCATENATE("..",D173,".",E173,". - ",T173),CONCATENATE(D173,". - ",T173))),"")</f>
         <v/>
       </c>
       <c r="B173" s="2">
@@ -15605,7 +15605,7 @@
       </c>
       <c r="F173" s="6"/>
       <c r="G173" s="40" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="14"/>
         <v>cD09</v>
       </c>
       <c r="H173" s="40"/>
@@ -15648,7 +15648,7 @@
     </row>
     <row r="174" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A174" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H174&lt;&gt;"",IF(F174&lt;&gt;"",CONCATENATE("...",D174,".",E174,".",F174,". - ",T174),IF(E174&lt;&gt;"",CONCATENATE("..",D174,".",E174,". - ",T174),CONCATENATE(D174,". - ",T174))),"")</f>
         <v/>
       </c>
       <c r="B174" s="2">
@@ -15665,7 +15665,7 @@
       </c>
       <c r="F174" s="6"/>
       <c r="G174" s="40" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="14"/>
         <v>cD09</v>
       </c>
       <c r="H174" s="40"/>
@@ -15708,7 +15708,7 @@
     </row>
     <row r="175" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A175" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H175&lt;&gt;"",IF(F175&lt;&gt;"",CONCATENATE("...",D175,".",E175,".",F175,". - ",T175),IF(E175&lt;&gt;"",CONCATENATE("..",D175,".",E175,". - ",T175),CONCATENATE(D175,". - ",T175))),"")</f>
         <v/>
       </c>
       <c r="B175" s="2">
@@ -15725,7 +15725,7 @@
       </c>
       <c r="F175" s="6"/>
       <c r="G175" s="40" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="14"/>
         <v>cD09</v>
       </c>
       <c r="H175" s="40"/>
@@ -15768,7 +15768,7 @@
     </row>
     <row r="176" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A176" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H176&lt;&gt;"",IF(F176&lt;&gt;"",CONCATENATE("...",D176,".",E176,".",F176,". - ",T176),IF(E176&lt;&gt;"",CONCATENATE("..",D176,".",E176,". - ",T176),CONCATENATE(D176,". - ",T176))),"")</f>
         <v/>
       </c>
       <c r="B176" s="2">
@@ -15785,7 +15785,7 @@
       </c>
       <c r="F176" s="6"/>
       <c r="G176" s="40" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="14"/>
         <v>cD09</v>
       </c>
       <c r="H176" s="40"/>
@@ -15828,7 +15828,7 @@
     </row>
     <row r="177" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A177" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H177&lt;&gt;"",IF(F177&lt;&gt;"",CONCATENATE("...",D177,".",E177,".",F177,". - ",T177),IF(E177&lt;&gt;"",CONCATENATE("..",D177,".",E177,". - ",T177),CONCATENATE(D177,". - ",T177))),"")</f>
         <v/>
       </c>
       <c r="B177" s="2">
@@ -15845,7 +15845,7 @@
       </c>
       <c r="F177" s="6"/>
       <c r="G177" s="40" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="14"/>
         <v>cD09</v>
       </c>
       <c r="H177" s="40"/>
@@ -15888,7 +15888,7 @@
     </row>
     <row r="178" spans="1:24" ht="51" x14ac:dyDescent="0.25">
       <c r="A178" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H178&lt;&gt;"",IF(F178&lt;&gt;"",CONCATENATE("...",D178,".",E178,".",F178,". - ",T178),IF(E178&lt;&gt;"",CONCATENATE("..",D178,".",E178,". - ",T178),CONCATENATE(D178,". - ",T178))),"")</f>
         <v/>
       </c>
       <c r="B178" s="2">
@@ -15905,7 +15905,7 @@
       </c>
       <c r="F178" s="6"/>
       <c r="G178" s="40" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="14"/>
         <v>cD09</v>
       </c>
       <c r="H178" s="40"/>
@@ -15952,7 +15952,7 @@
     </row>
     <row r="179" spans="1:24" ht="33" x14ac:dyDescent="0.25">
       <c r="A179" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H179&lt;&gt;"",IF(F179&lt;&gt;"",CONCATENATE("...",D179,".",E179,".",F179,". - ",T179),IF(E179&lt;&gt;"",CONCATENATE("..",D179,".",E179,". - ",T179),CONCATENATE(D179,". - ",T179))),"")</f>
         <v/>
       </c>
       <c r="B179" s="2">
@@ -16007,7 +16007,7 @@
     </row>
     <row r="180" spans="1:24" ht="51" x14ac:dyDescent="0.25">
       <c r="A180" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H180&lt;&gt;"",IF(F180&lt;&gt;"",CONCATENATE("...",D180,".",E180,".",F180,". - ",T180),IF(E180&lt;&gt;"",CONCATENATE("..",D180,".",E180,". - ",T180),CONCATENATE(D180,". - ",T180))),"")</f>
         <v>..D.10. - Kidney diseases</v>
       </c>
       <c r="B180" s="2">
@@ -16071,7 +16071,7 @@
     </row>
     <row r="181" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A181" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H181&lt;&gt;"",IF(F181&lt;&gt;"",CONCATENATE("...",D181,".",E181,".",F181,". - ",T181),IF(E181&lt;&gt;"",CONCATENATE("..",D181,".",E181,". - ",T181),CONCATENATE(D181,". - ",T181))),"")</f>
         <v>...D.10.a. - Acute glomerulonephritis</v>
       </c>
       <c r="B181" s="2">
@@ -16090,7 +16090,7 @@
         <v>1126</v>
       </c>
       <c r="G181" s="40" t="str">
-        <f t="shared" ref="G181:G189" si="18">CONCATENATE("c",D181,E181,F181)</f>
+        <f t="shared" ref="G181:G189" si="15">CONCATENATE("c",D181,E181,F181)</f>
         <v>cD10a</v>
       </c>
       <c r="H181" s="40" t="str">
@@ -16138,7 +16138,7 @@
     </row>
     <row r="182" spans="1:24" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A182" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H182&lt;&gt;"",IF(F182&lt;&gt;"",CONCATENATE("...",D182,".",E182,".",F182,". - ",T182),IF(E182&lt;&gt;"",CONCATENATE("..",D182,".",E182,". - ",T182),CONCATENATE(D182,". - ",T182))),"")</f>
         <v>...D.10.b. - Chronic kidney diesease due to diabetes</v>
       </c>
       <c r="B182" s="2">
@@ -16157,7 +16157,7 @@
         <v>1127</v>
       </c>
       <c r="G182" s="40" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>cD10b</v>
       </c>
       <c r="H182" s="40" t="str">
@@ -16205,7 +16205,7 @@
     </row>
     <row r="183" spans="1:24" ht="102" x14ac:dyDescent="0.25">
       <c r="A183" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H183&lt;&gt;"",IF(F183&lt;&gt;"",CONCATENATE("...",D183,".",E183,".",F183,". - ",T183),IF(E183&lt;&gt;"",CONCATENATE("..",D183,".",E183,". - ",T183),CONCATENATE(D183,". - ",T183))),"")</f>
         <v>...D.10.c. - Other chronic kidney disease</v>
       </c>
       <c r="B183" s="2">
@@ -16224,7 +16224,7 @@
         <v>1130</v>
       </c>
       <c r="G183" s="40" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>cD10c</v>
       </c>
       <c r="H183" s="40" t="str">
@@ -16272,7 +16272,7 @@
     </row>
     <row r="184" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A184" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H184&lt;&gt;"",IF(F184&lt;&gt;"",CONCATENATE("...",D184,".",E184,".",F184,". - ",T184),IF(E184&lt;&gt;"",CONCATENATE("..",D184,".",E184,". - ",T184),CONCATENATE(D184,". - ",T184))),"")</f>
         <v/>
       </c>
       <c r="B184" s="2">
@@ -16289,7 +16289,7 @@
       </c>
       <c r="F184" s="6"/>
       <c r="G184" s="40" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>cD99</v>
       </c>
       <c r="H184" s="40"/>
@@ -16328,7 +16328,7 @@
     </row>
     <row r="185" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A185" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H185&lt;&gt;"",IF(F185&lt;&gt;"",CONCATENATE("...",D185,".",E185,".",F185,". - ",T185),IF(E185&lt;&gt;"",CONCATENATE("..",D185,".",E185,". - ",T185),CONCATENATE(D185,". - ",T185))),"")</f>
         <v/>
       </c>
       <c r="B185" s="2">
@@ -16345,7 +16345,7 @@
       </c>
       <c r="F185" s="6"/>
       <c r="G185" s="40" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>cD99</v>
       </c>
       <c r="H185" s="40"/>
@@ -16388,7 +16388,7 @@
     </row>
     <row r="186" spans="1:24" ht="33" x14ac:dyDescent="0.25">
       <c r="A186" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H186&lt;&gt;"",IF(F186&lt;&gt;"",CONCATENATE("...",D186,".",E186,".",F186,". - ",T186),IF(E186&lt;&gt;"",CONCATENATE("..",D186,".",E186,". - ",T186),CONCATENATE(D186,". - ",T186))),"")</f>
         <v/>
       </c>
       <c r="B186" s="2">
@@ -16405,7 +16405,7 @@
       </c>
       <c r="F186" s="6"/>
       <c r="G186" s="40" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>cD99</v>
       </c>
       <c r="H186" s="40"/>
@@ -16448,7 +16448,7 @@
     </row>
     <row r="187" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A187" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H187&lt;&gt;"",IF(F187&lt;&gt;"",CONCATENATE("...",D187,".",E187,".",F187,". - ",T187),IF(E187&lt;&gt;"",CONCATENATE("..",D187,".",E187,". - ",T187),CONCATENATE(D187,". - ",T187))),"")</f>
         <v/>
       </c>
       <c r="B187" s="2">
@@ -16465,7 +16465,7 @@
       </c>
       <c r="F187" s="6"/>
       <c r="G187" s="40" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>cD99</v>
       </c>
       <c r="H187" s="40"/>
@@ -16508,7 +16508,7 @@
     </row>
     <row r="188" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A188" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H188&lt;&gt;"",IF(F188&lt;&gt;"",CONCATENATE("...",D188,".",E188,".",F188,". - ",T188),IF(E188&lt;&gt;"",CONCATENATE("..",D188,".",E188,". - ",T188),CONCATENATE(D188,". - ",T188))),"")</f>
         <v/>
       </c>
       <c r="B188" s="2">
@@ -16525,7 +16525,7 @@
       </c>
       <c r="F188" s="6"/>
       <c r="G188" s="40" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>cD99</v>
       </c>
       <c r="H188" s="40"/>
@@ -16568,7 +16568,7 @@
     </row>
     <row r="189" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A189" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H189&lt;&gt;"",IF(F189&lt;&gt;"",CONCATENATE("...",D189,".",E189,".",F189,". - ",T189),IF(E189&lt;&gt;"",CONCATENATE("..",D189,".",E189,". - ",T189),CONCATENATE(D189,". - ",T189))),"")</f>
         <v/>
       </c>
       <c r="B189" s="2">
@@ -16585,7 +16585,7 @@
       </c>
       <c r="F189" s="6"/>
       <c r="G189" s="40" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>cD99</v>
       </c>
       <c r="H189" s="40"/>
@@ -16626,7 +16626,7 @@
     </row>
     <row r="190" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A190" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H190&lt;&gt;"",IF(F190&lt;&gt;"",CONCATENATE("...",D190,".",E190,".",F190,". - ",T190),IF(E190&lt;&gt;"",CONCATENATE("..",D190,".",E190,". - ",T190),CONCATENATE(D190,". - ",T190))),"")</f>
         <v/>
       </c>
       <c r="B190" s="2">
@@ -16685,7 +16685,7 @@
     </row>
     <row r="191" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A191" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H191&lt;&gt;"",IF(F191&lt;&gt;"",CONCATENATE("...",D191,".",E191,".",F191,". - ",T191),IF(E191&lt;&gt;"",CONCATENATE("..",D191,".",E191,". - ",T191),CONCATENATE(D191,". - ",T191))),"")</f>
         <v/>
       </c>
       <c r="B191" s="2">
@@ -16745,7 +16745,7 @@
     </row>
     <row r="192" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A192" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H192&lt;&gt;"",IF(F192&lt;&gt;"",CONCATENATE("...",D192,".",E192,".",F192,". - ",T192),IF(E192&lt;&gt;"",CONCATENATE("..",D192,".",E192,". - ",T192),CONCATENATE(D192,". - ",T192))),"")</f>
         <v/>
       </c>
       <c r="B192" s="2">
@@ -16801,7 +16801,7 @@
     </row>
     <row r="193" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A193" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H193&lt;&gt;"",IF(F193&lt;&gt;"",CONCATENATE("...",D193,".",E193,".",F193,". - ",T193),IF(E193&lt;&gt;"",CONCATENATE("..",D193,".",E193,". - ",T193),CONCATENATE(D193,". - ",T193))),"")</f>
         <v/>
       </c>
       <c r="B193" s="2">
@@ -16857,7 +16857,7 @@
     </row>
     <row r="194" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A194" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H194&lt;&gt;"",IF(F194&lt;&gt;"",CONCATENATE("...",D194,".",E194,".",F194,". - ",T194),IF(E194&lt;&gt;"",CONCATENATE("..",D194,".",E194,". - ",T194),CONCATENATE(D194,". - ",T194))),"")</f>
         <v/>
       </c>
       <c r="B194" s="2">
@@ -16913,7 +16913,7 @@
     </row>
     <row r="195" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A195" s="44" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(H195&lt;&gt;"",IF(F195&lt;&gt;"",CONCATENATE("...",D195,".",E195,".",F195,". - ",T195),IF(E195&lt;&gt;"",CONCATENATE("..",D195,".",E195,". - ",T195),CONCATENATE(D195,". - ",T195))),"")</f>
         <v/>
       </c>
       <c r="B195" s="2">
@@ -16977,7 +16977,7 @@
     </row>
     <row r="196" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A196" s="44" t="str">
-        <f t="shared" ref="A196:A232" si="19">IF(H196&lt;&gt;"",IF(F196&lt;&gt;"",CONCATENATE("...",D196,".",E196,".",F196,". - ",T196),IF(E196&lt;&gt;"",CONCATENATE("..",D196,".",E196,". - ",T196),CONCATENATE(D196,". - ",T196))),"")</f>
+        <f>IF(H196&lt;&gt;"",IF(F196&lt;&gt;"",CONCATENATE("...",D196,".",E196,".",F196,". - ",T196),IF(E196&lt;&gt;"",CONCATENATE("..",D196,".",E196,". - ",T196),CONCATENATE(D196,". - ",T196))),"")</f>
         <v>..D.12. - Congenital anomalies</v>
       </c>
       <c r="B196" s="2">
@@ -17039,7 +17039,7 @@
     </row>
     <row r="197" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A197" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H197&lt;&gt;"",IF(F197&lt;&gt;"",CONCATENATE("...",D197,".",E197,".",F197,". - ",T197),IF(E197&lt;&gt;"",CONCATENATE("..",D197,".",E197,". - ",T197),CONCATENATE(D197,". - ",T197))),"")</f>
         <v/>
       </c>
       <c r="B197" s="2">
@@ -17056,7 +17056,7 @@
       </c>
       <c r="F197" s="6"/>
       <c r="G197" s="40" t="str">
-        <f t="shared" ref="G197:G202" si="20">CONCATENATE("c",D197,E197,F197)</f>
+        <f t="shared" ref="G197:G202" si="16">CONCATENATE("c",D197,E197,F197)</f>
         <v>cD12</v>
       </c>
       <c r="H197" s="40"/>
@@ -17099,7 +17099,7 @@
     </row>
     <row r="198" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A198" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H198&lt;&gt;"",IF(F198&lt;&gt;"",CONCATENATE("...",D198,".",E198,".",F198,". - ",T198),IF(E198&lt;&gt;"",CONCATENATE("..",D198,".",E198,". - ",T198),CONCATENATE(D198,". - ",T198))),"")</f>
         <v/>
       </c>
       <c r="B198" s="2">
@@ -17116,7 +17116,7 @@
       </c>
       <c r="F198" s="6"/>
       <c r="G198" s="40" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>cD12</v>
       </c>
       <c r="H198" s="40"/>
@@ -17159,7 +17159,7 @@
     </row>
     <row r="199" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A199" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H199&lt;&gt;"",IF(F199&lt;&gt;"",CONCATENATE("...",D199,".",E199,".",F199,". - ",T199),IF(E199&lt;&gt;"",CONCATENATE("..",D199,".",E199,". - ",T199),CONCATENATE(D199,". - ",T199))),"")</f>
         <v/>
       </c>
       <c r="B199" s="2">
@@ -17176,7 +17176,7 @@
       </c>
       <c r="F199" s="6"/>
       <c r="G199" s="40" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>cD12</v>
       </c>
       <c r="H199" s="40"/>
@@ -17219,7 +17219,7 @@
     </row>
     <row r="200" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A200" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H200&lt;&gt;"",IF(F200&lt;&gt;"",CONCATENATE("...",D200,".",E200,".",F200,". - ",T200),IF(E200&lt;&gt;"",CONCATENATE("..",D200,".",E200,". - ",T200),CONCATENATE(D200,". - ",T200))),"")</f>
         <v/>
       </c>
       <c r="B200" s="2">
@@ -17236,7 +17236,7 @@
       </c>
       <c r="F200" s="6"/>
       <c r="G200" s="40" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>cD12</v>
       </c>
       <c r="H200" s="40"/>
@@ -17279,7 +17279,7 @@
     </row>
     <row r="201" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A201" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H201&lt;&gt;"",IF(F201&lt;&gt;"",CONCATENATE("...",D201,".",E201,".",F201,". - ",T201),IF(E201&lt;&gt;"",CONCATENATE("..",D201,".",E201,". - ",T201),CONCATENATE(D201,". - ",T201))),"")</f>
         <v/>
       </c>
       <c r="B201" s="2">
@@ -17296,7 +17296,7 @@
       </c>
       <c r="F201" s="6"/>
       <c r="G201" s="40" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>cD12</v>
       </c>
       <c r="H201" s="40"/>
@@ -17339,7 +17339,7 @@
     </row>
     <row r="202" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A202" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H202&lt;&gt;"",IF(F202&lt;&gt;"",CONCATENATE("...",D202,".",E202,".",F202,". - ",T202),IF(E202&lt;&gt;"",CONCATENATE("..",D202,".",E202,". - ",T202),CONCATENATE(D202,". - ",T202))),"")</f>
         <v/>
       </c>
       <c r="B202" s="2">
@@ -17356,7 +17356,7 @@
       </c>
       <c r="F202" s="6"/>
       <c r="G202" s="40" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>cD12</v>
       </c>
       <c r="H202" s="40"/>
@@ -17399,7 +17399,7 @@
     </row>
     <row r="203" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A203" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H203&lt;&gt;"",IF(F203&lt;&gt;"",CONCATENATE("...",D203,".",E203,".",F203,". - ",T203),IF(E203&lt;&gt;"",CONCATENATE("..",D203,".",E203,". - ",T203),CONCATENATE(D203,". - ",T203))),"")</f>
         <v/>
       </c>
       <c r="B203" s="2">
@@ -17452,7 +17452,7 @@
     </row>
     <row r="204" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A204" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H204&lt;&gt;"",IF(F204&lt;&gt;"",CONCATENATE("...",D204,".",E204,".",F204,". - ",T204),IF(E204&lt;&gt;"",CONCATENATE("..",D204,".",E204,". - ",T204),CONCATENATE(D204,". - ",T204))),"")</f>
         <v/>
       </c>
       <c r="B204" s="2">
@@ -17508,7 +17508,7 @@
     </row>
     <row r="205" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A205" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H205&lt;&gt;"",IF(F205&lt;&gt;"",CONCATENATE("...",D205,".",E205,".",F205,". - ",T205),IF(E205&lt;&gt;"",CONCATENATE("..",D205,".",E205,". - ",T205),CONCATENATE(D205,". - ",T205))),"")</f>
         <v/>
       </c>
       <c r="B205" s="2">
@@ -17564,7 +17564,7 @@
     </row>
     <row r="206" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A206" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H206&lt;&gt;"",IF(F206&lt;&gt;"",CONCATENATE("...",D206,".",E206,".",F206,". - ",T206),IF(E206&lt;&gt;"",CONCATENATE("..",D206,".",E206,". - ",T206),CONCATENATE(D206,". - ",T206))),"")</f>
         <v/>
       </c>
       <c r="B206" s="2">
@@ -17620,7 +17620,7 @@
     </row>
     <row r="207" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A207" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H207&lt;&gt;"",IF(F207&lt;&gt;"",CONCATENATE("...",D207,".",E207,".",F207,". - ",T207),IF(E207&lt;&gt;"",CONCATENATE("..",D207,".",E207,". - ",T207),CONCATENATE(D207,". - ",T207))),"")</f>
         <v/>
       </c>
       <c r="B207" s="2">
@@ -17676,7 +17676,7 @@
     </row>
     <row r="208" spans="1:24" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A208" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H208&lt;&gt;"",IF(F208&lt;&gt;"",CONCATENATE("...",D208,".",E208,".",F208,". - ",T208),IF(E208&lt;&gt;"",CONCATENATE("..",D208,".",E208,". - ",T208),CONCATENATE(D208,". - ",T208))),"")</f>
         <v>E. - Injuries</v>
       </c>
       <c r="B208" s="2">
@@ -17734,7 +17734,7 @@
     </row>
     <row r="209" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A209" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H209&lt;&gt;"",IF(F209&lt;&gt;"",CONCATENATE("...",D209,".",E209,".",F209,". - ",T209),IF(E209&lt;&gt;"",CONCATENATE("..",D209,".",E209,". - ",T209),CONCATENATE(D209,". - ",T209))),"")</f>
         <v>..E.01. - Unintentional injuries</v>
       </c>
       <c r="B209" s="2">
@@ -17794,7 +17794,7 @@
     </row>
     <row r="210" spans="1:24" ht="51" x14ac:dyDescent="0.25">
       <c r="A210" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H210&lt;&gt;"",IF(F210&lt;&gt;"",CONCATENATE("...",D210,".",E210,".",F210,". - ",T210),IF(E210&lt;&gt;"",CONCATENATE("..",D210,".",E210,". - ",T210),CONCATENATE(D210,". - ",T210))),"")</f>
         <v>...E.01.a. - Road injury</v>
       </c>
       <c r="B210" s="2">
@@ -17813,7 +17813,7 @@
         <v>1126</v>
       </c>
       <c r="G210" s="40" t="str">
-        <f t="shared" ref="G210:G219" si="21">CONCATENATE("c",D210,E210,F210)</f>
+        <f t="shared" ref="G210:G219" si="17">CONCATENATE("c",D210,E210,F210)</f>
         <v>cE01a</v>
       </c>
       <c r="H210" s="40" t="str">
@@ -17863,7 +17863,7 @@
     </row>
     <row r="211" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A211" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H211&lt;&gt;"",IF(F211&lt;&gt;"",CONCATENATE("...",D211,".",E211,".",F211,". - ",T211),IF(E211&lt;&gt;"",CONCATENATE("..",D211,".",E211,". - ",T211),CONCATENATE(D211,". - ",T211))),"")</f>
         <v/>
       </c>
       <c r="B211" s="2">
@@ -17882,7 +17882,7 @@
         <v>1128</v>
       </c>
       <c r="G211" s="40" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>cE01x</v>
       </c>
       <c r="H211" s="40"/>
@@ -17925,7 +17925,7 @@
     </row>
     <row r="212" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A212" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H212&lt;&gt;"",IF(F212&lt;&gt;"",CONCATENATE("...",D212,".",E212,".",F212,". - ",T212),IF(E212&lt;&gt;"",CONCATENATE("..",D212,".",E212,". - ",T212),CONCATENATE(D212,". - ",T212))),"")</f>
         <v>...E.01.b. - Falls</v>
       </c>
       <c r="B212" s="2">
@@ -17944,7 +17944,7 @@
         <v>1127</v>
       </c>
       <c r="G212" s="40" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>cE01b</v>
       </c>
       <c r="H212" s="40" t="str">
@@ -17992,7 +17992,7 @@
     </row>
     <row r="213" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A213" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H213&lt;&gt;"",IF(F213&lt;&gt;"",CONCATENATE("...",D213,".",E213,".",F213,". - ",T213),IF(E213&lt;&gt;"",CONCATENATE("..",D213,".",E213,". - ",T213),CONCATENATE(D213,". - ",T213))),"")</f>
         <v/>
       </c>
       <c r="B213" s="2">
@@ -18011,7 +18011,7 @@
         <v>1128</v>
       </c>
       <c r="G213" s="40" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>cE01x</v>
       </c>
       <c r="H213" s="40"/>
@@ -18052,7 +18052,7 @@
     </row>
     <row r="214" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A214" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H214&lt;&gt;"",IF(F214&lt;&gt;"",CONCATENATE("...",D214,".",E214,".",F214,". - ",T214),IF(E214&lt;&gt;"",CONCATENATE("..",D214,".",E214,". - ",T214),CONCATENATE(D214,". - ",T214))),"")</f>
         <v/>
       </c>
       <c r="B214" s="2">
@@ -18071,7 +18071,7 @@
         <v>1128</v>
       </c>
       <c r="G214" s="40" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>cE01x</v>
       </c>
       <c r="H214" s="40"/>
@@ -18114,7 +18114,7 @@
     </row>
     <row r="215" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A215" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H215&lt;&gt;"",IF(F215&lt;&gt;"",CONCATENATE("...",D215,".",E215,".",F215,". - ",T215),IF(E215&lt;&gt;"",CONCATENATE("..",D215,".",E215,". - ",T215),CONCATENATE(D215,". - ",T215))),"")</f>
         <v/>
       </c>
       <c r="B215" s="2">
@@ -18133,7 +18133,7 @@
         <v>1128</v>
       </c>
       <c r="G215" s="40" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>cE01x</v>
       </c>
       <c r="H215" s="40"/>
@@ -18176,7 +18176,7 @@
     </row>
     <row r="216" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A216" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H216&lt;&gt;"",IF(F216&lt;&gt;"",CONCATENATE("...",D216,".",E216,".",F216,". - ",T216),IF(E216&lt;&gt;"",CONCATENATE("..",D216,".",E216,". - ",T216),CONCATENATE(D216,". - ",T216))),"")</f>
         <v>...E.01.c. - Accidental Firearm</v>
       </c>
       <c r="B216" s="2"/>
@@ -18193,7 +18193,7 @@
         <v>1130</v>
       </c>
       <c r="G216" s="40" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>cE01c</v>
       </c>
       <c r="H216" s="40" t="str">
@@ -18229,7 +18229,7 @@
     </row>
     <row r="217" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A217" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H217&lt;&gt;"",IF(F217&lt;&gt;"",CONCATENATE("...",D217,".",E217,".",F217,". - ",T217),IF(E217&lt;&gt;"",CONCATENATE("..",D217,".",E217,". - ",T217),CONCATENATE(D217,". - ",T217))),"")</f>
         <v/>
       </c>
       <c r="B217" s="2">
@@ -18248,7 +18248,7 @@
         <v>1128</v>
       </c>
       <c r="G217" s="40" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>cE01x</v>
       </c>
       <c r="H217" s="40"/>
@@ -18291,7 +18291,7 @@
     </row>
     <row r="218" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A218" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H218&lt;&gt;"",IF(F218&lt;&gt;"",CONCATENATE("...",D218,".",E218,".",F218,". - ",T218),IF(E218&lt;&gt;"",CONCATENATE("..",D218,".",E218,". - ",T218),CONCATENATE(D218,". - ",T218))),"")</f>
         <v/>
       </c>
       <c r="B218" s="2"/>
@@ -18320,7 +18320,7 @@
     </row>
     <row r="219" spans="1:24" ht="102" x14ac:dyDescent="0.25">
       <c r="A219" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H219&lt;&gt;"",IF(F219&lt;&gt;"",CONCATENATE("...",D219,".",E219,".",F219,". - ",T219),IF(E219&lt;&gt;"",CONCATENATE("..",D219,".",E219,". - ",T219),CONCATENATE(D219,". - ",T219))),"")</f>
         <v>...E.01.x. - Other unintentional injuries</v>
       </c>
       <c r="B219" s="2">
@@ -18339,7 +18339,7 @@
         <v>1128</v>
       </c>
       <c r="G219" s="40" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>cE01x</v>
       </c>
       <c r="H219" s="40" t="str">
@@ -18391,7 +18391,7 @@
     </row>
     <row r="220" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A220" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H220&lt;&gt;"",IF(F220&lt;&gt;"",CONCATENATE("...",D220,".",E220,".",F220,". - ",T220),IF(E220&lt;&gt;"",CONCATENATE("..",D220,".",E220,". - ",T220),CONCATENATE(D220,". - ",T220))),"")</f>
         <v/>
       </c>
       <c r="B220" s="2">
@@ -18444,7 +18444,7 @@
     </row>
     <row r="221" spans="1:24" ht="51" x14ac:dyDescent="0.25">
       <c r="A221" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H221&lt;&gt;"",IF(F221&lt;&gt;"",CONCATENATE("...",D221,".",E221,".",F221,". - ",T221),IF(E221&lt;&gt;"",CONCATENATE("..",D221,".",E221,". - ",T221),CONCATENATE(D221,". - ",T221))),"")</f>
         <v>..E.02. - Suicide/Self-harm</v>
       </c>
       <c r="B221" s="2">
@@ -18461,7 +18461,7 @@
       </c>
       <c r="F221" s="6"/>
       <c r="G221" s="40" t="str">
-        <f t="shared" ref="G221:G228" si="22">CONCATENATE("c",D221,E221,F221)</f>
+        <f t="shared" ref="G221:G228" si="18">CONCATENATE("c",D221,E221,F221)</f>
         <v>cE02</v>
       </c>
       <c r="H221" s="40" t="str">
@@ -18511,7 +18511,7 @@
     </row>
     <row r="222" spans="1:24" ht="255" x14ac:dyDescent="0.25">
       <c r="A222" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H222&lt;&gt;"",IF(F222&lt;&gt;"",CONCATENATE("...",D222,".",E222,".",F222,". - ",T222),IF(E222&lt;&gt;"",CONCATENATE("..",D222,".",E222,". - ",T222),CONCATENATE(D222,". - ",T222))),"")</f>
         <v>..E.03. - Homicide/Interpersonal violence</v>
       </c>
       <c r="B222" s="2">
@@ -18571,7 +18571,7 @@
     </row>
     <row r="223" spans="1:24" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A223" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H223&lt;&gt;"",IF(F223&lt;&gt;"",CONCATENATE("...",D223,".",E223,".",F223,". - ",T223),IF(E223&lt;&gt;"",CONCATENATE("..",D223,".",E223,". - ",T223),CONCATENATE(D223,". - ",T223))),"")</f>
         <v>...E.03.a. - Homicide excluding legal intervention</v>
       </c>
       <c r="B223" s="2"/>
@@ -18586,11 +18586,11 @@
         <v>1126</v>
       </c>
       <c r="G223" s="40" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v>cE03a</v>
       </c>
       <c r="H223" s="40" t="str">
-        <f t="shared" ref="H223:H225" si="23">CONCATENATE(D223,E223,F223)</f>
+        <f t="shared" ref="H223:H225" si="19">CONCATENATE(D223,E223,F223)</f>
         <v>E03a</v>
       </c>
       <c r="I223" s="5"/>
@@ -18618,7 +18618,7 @@
     </row>
     <row r="224" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A224" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H224&lt;&gt;"",IF(F224&lt;&gt;"",CONCATENATE("...",D224,".",E224,".",F224,". - ",T224),IF(E224&lt;&gt;"",CONCATENATE("..",D224,".",E224,". - ",T224),CONCATENATE(D224,". - ",T224))),"")</f>
         <v>...E.03.b. - Legal intervention</v>
       </c>
       <c r="B224" s="2"/>
@@ -18633,11 +18633,11 @@
         <v>1127</v>
       </c>
       <c r="G224" s="40" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v>cE03b</v>
       </c>
       <c r="H224" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="19"/>
         <v>E03b</v>
       </c>
       <c r="I224" s="5"/>
@@ -18665,7 +18665,7 @@
     </row>
     <row r="225" spans="1:24" ht="153" x14ac:dyDescent="0.25">
       <c r="A225" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H225&lt;&gt;"",IF(F225&lt;&gt;"",CONCATENATE("...",D225,".",E225,".",F225,". - ",T225),IF(E225&lt;&gt;"",CONCATENATE("..",D225,".",E225,". - ",T225),CONCATENATE(D225,". - ",T225))),"")</f>
         <v>...E.03.c. - Execution, War, Terroism</v>
       </c>
       <c r="B225" s="2">
@@ -18684,11 +18684,11 @@
         <v>1130</v>
       </c>
       <c r="G225" s="40" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v>cE03c</v>
       </c>
       <c r="H225" s="40" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="19"/>
         <v>E03c</v>
       </c>
       <c r="I225" s="5" t="s">
@@ -18732,7 +18732,7 @@
     </row>
     <row r="226" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A226" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H226&lt;&gt;"",IF(F226&lt;&gt;"",CONCATENATE("...",D226,".",E226,".",F226,". - ",T226),IF(E226&lt;&gt;"",CONCATENATE("..",D226,".",E226,". - ",T226),CONCATENATE(D226,". - ",T226))),"")</f>
         <v/>
       </c>
       <c r="B226" s="82" t="s">
@@ -18748,7 +18748,7 @@
         <v>1144</v>
       </c>
       <c r="G226" s="40" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v>cE01</v>
       </c>
       <c r="H226" s="40"/>
@@ -18770,7 +18770,7 @@
     </row>
     <row r="227" spans="1:24" ht="178.5" x14ac:dyDescent="0.25">
       <c r="A227" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H227&lt;&gt;"",IF(F227&lt;&gt;"",CONCATENATE("...",D227,".",E227,".",F227,". - ",T227),IF(E227&lt;&gt;"",CONCATENATE("..",D227,".",E227,". - ",T227),CONCATENATE(D227,". - ",T227))),"")</f>
         <v>..Z.01. - Symptoms, signs and ill-defined conditions, not elsewhere classified</v>
       </c>
       <c r="D227" s="56" t="s">
@@ -18780,7 +18780,7 @@
         <v>1144</v>
       </c>
       <c r="G227" s="40" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v>cZ01</v>
       </c>
       <c r="H227" s="40" t="str">
@@ -18805,7 +18805,7 @@
     </row>
     <row r="228" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A228" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H228&lt;&gt;"",IF(F228&lt;&gt;"",CONCATENATE("...",D228,".",E228,".",F228,". - ",T228),IF(E228&lt;&gt;"",CONCATENATE("..",D228,".",E228,". - ",T228),CONCATENATE(D228,". - ",T228))),"")</f>
         <v/>
       </c>
       <c r="D228" s="56" t="s">
@@ -18815,7 +18815,7 @@
         <v>1152</v>
       </c>
       <c r="G228" s="42" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v>cA09</v>
       </c>
       <c r="H228" s="40"/>
@@ -18837,7 +18837,7 @@
     </row>
     <row r="229" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A229" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H229&lt;&gt;"",IF(F229&lt;&gt;"",CONCATENATE("...",D229,".",E229,".",F229,". - ",T229),IF(E229&lt;&gt;"",CONCATENATE("..",D229,".",E229,". - ",T229),CONCATENATE(D229,". - ",T229))),"")</f>
         <v>..Z.02. - Unknown/Missing Value</v>
       </c>
       <c r="D229" s="56" t="s">
@@ -18848,7 +18848,7 @@
       </c>
       <c r="G229" s="43"/>
       <c r="H229" s="40" t="str">
-        <f t="shared" ref="H229:H232" si="24">CONCATENATE(D229,E229,F229)</f>
+        <f t="shared" ref="H229:H232" si="20">CONCATENATE(D229,E229,F229)</f>
         <v>Z02</v>
       </c>
       <c r="T229" s="48" t="s">
@@ -18857,7 +18857,7 @@
     </row>
     <row r="230" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A230" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H230&lt;&gt;"",IF(F230&lt;&gt;"",CONCATENATE("...",D230,".",E230,".",F230,". - ",T230),IF(E230&lt;&gt;"",CONCATENATE("..",D230,".",E230,". - ",T230),CONCATENATE(D230,". - ",T230))),"")</f>
         <v>..Z.03. - Code does not map</v>
       </c>
       <c r="D230" s="56" t="s">
@@ -18868,7 +18868,7 @@
       </c>
       <c r="G230" s="43"/>
       <c r="H230" s="40" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="20"/>
         <v>Z03</v>
       </c>
       <c r="I230" s="16" t="s">
@@ -18880,7 +18880,7 @@
     </row>
     <row r="231" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A231" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H231&lt;&gt;"",IF(F231&lt;&gt;"",CONCATENATE("...",D231,".",E231,".",F231,". - ",T231),IF(E231&lt;&gt;"",CONCATENATE("..",D231,".",E231,". - ",T231),CONCATENATE(D231,". - ",T231))),"")</f>
         <v>Z. - Unknown/Missing Value</v>
       </c>
       <c r="D231" s="56" t="s">
@@ -18888,7 +18888,7 @@
       </c>
       <c r="G231" s="43"/>
       <c r="H231" s="40" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="20"/>
         <v>Z</v>
       </c>
       <c r="T231" s="48" t="s">
@@ -18897,7 +18897,7 @@
     </row>
     <row r="232" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A232" s="44" t="str">
-        <f t="shared" si="19"/>
+        <f>IF(H232&lt;&gt;"",IF(F232&lt;&gt;"",CONCATENATE("...",D232,".",E232,".",F232,". - ",T232),IF(E232&lt;&gt;"",CONCATENATE("..",D232,".",E232,". - ",T232),CONCATENATE(D232,". - ",T232))),"")</f>
         <v>..D.99. - Other Chronic Conditions</v>
       </c>
       <c r="D232" s="56" t="s">
@@ -18908,7 +18908,7 @@
       </c>
       <c r="G232" s="43"/>
       <c r="H232" s="40" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="20"/>
         <v>D99</v>
       </c>
       <c r="T232" s="48" t="s">

</xml_diff>

<commit_message>
CCS coding work; disparity chart enhancements; other edits
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/gbd.ICD.Map.xlsx
+++ b/myCBD/myInfo/gbd.ICD.Map.xlsx
@@ -5338,16 +5338,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X232"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H155" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B226" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N157" sqref="N157"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:A232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="44" customWidth="1"/>
+    <col min="1" max="1" width="57" style="44" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" style="46" customWidth="1"/>
     <col min="3" max="3" width="35.7109375" style="44" customWidth="1"/>
     <col min="4" max="4" width="4.42578125" style="56" customWidth="1"/>
@@ -5450,8 +5450,8 @@
     </row>
     <row r="2" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="44" t="str">
-        <f>V2</f>
-        <v>All CAUSES</v>
+        <f>CONCATENATE(".",V2)</f>
+        <v>.All CAUSES</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -5496,8 +5496,8 @@
     </row>
     <row r="3" spans="1:24" ht="153" x14ac:dyDescent="0.25">
       <c r="A3" s="44" t="str">
-        <f>IF(H3&lt;&gt;"",IF(F3&lt;&gt;"",CONCATENATE("...",D3,".",E3,".",F3,". - ",T3),IF(E3&lt;&gt;"",CONCATENATE("..",D3,".",E3,". - ",T3),CONCATENATE(D3,". - ",T3))),"")</f>
-        <v>A. - Communicable, maternal, perinatal and nutritional conditions</v>
+        <f>IF(H3&lt;&gt;"",IF(F3&lt;&gt;"",CONCATENATE("....",D3,".",E3,".",F3,". - ",T3),IF(E3&lt;&gt;"",CONCATENATE("...",D3,".",E3,". - ",T3),CONCATENATE("..",D3,". - ",T3))),"")</f>
+        <v>..A. - Communicable, maternal, perinatal and nutritional conditions</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -5548,10 +5548,10 @@
       </c>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="44" t="str">
-        <f>IF(H4&lt;&gt;"",IF(F4&lt;&gt;"",CONCATENATE("...",D4,".",E4,".",F4,". - ",T4),IF(E4&lt;&gt;"",CONCATENATE("..",D4,".",E4,". - ",T4),CONCATENATE(D4,". - ",T4))),"")</f>
-        <v>..A.99. - Other Infectious Diseases</v>
+        <f t="shared" ref="A4:A67" si="0">IF(H4&lt;&gt;"",IF(F4&lt;&gt;"",CONCATENATE("....",D4,".",E4,".",F4,". - ",T4),IF(E4&lt;&gt;"",CONCATENATE("...",D4,".",E4,". - ",T4),CONCATENATE("..",D4,". - ",T4))),"")</f>
+        <v>...A.99. - Other Infectious Diseases</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="29" t="s">
@@ -5592,7 +5592,7 @@
     </row>
     <row r="5" spans="1:24" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A5" s="44" t="str">
-        <f>IF(H5&lt;&gt;"",IF(F5&lt;&gt;"",CONCATENATE("...",D5,".",E5,".",F5,". - ",T5),IF(E5&lt;&gt;"",CONCATENATE("..",D5,".",E5,". - ",T5),CONCATENATE(D5,". - ",T5))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B5" s="2">
@@ -5641,10 +5641,10 @@
       </c>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="44" t="str">
-        <f>IF(H6&lt;&gt;"",IF(F6&lt;&gt;"",CONCATENATE("...",D6,".",E6,".",F6,". - ",T6),IF(E6&lt;&gt;"",CONCATENATE("..",D6,".",E6,". - ",T6),CONCATENATE(D6,". - ",T6))),"")</f>
-        <v>..A.01. - Tuberculosis</v>
+        <f t="shared" si="0"/>
+        <v>...A.01. - Tuberculosis</v>
       </c>
       <c r="B6" s="2">
         <v>3</v>
@@ -5702,10 +5702,10 @@
       </c>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="140.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="44" t="str">
-        <f>IF(H7&lt;&gt;"",IF(F7&lt;&gt;"",CONCATENATE("...",D7,".",E7,".",F7,". - ",T7),IF(E7&lt;&gt;"",CONCATENATE("..",D7,".",E7,". - ",T7),CONCATENATE(D7,". - ",T7))),"")</f>
-        <v>..A.02. - HIV/ and other Sexually transmitted diseases (STDs)</v>
+        <f t="shared" si="0"/>
+        <v>...A.02. - HIV/ and other Sexually transmitted diseases (STDs)</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="32" t="s">
@@ -5744,10 +5744,10 @@
       <c r="W7" s="45"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="140.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="44" t="str">
-        <f>IF(H8&lt;&gt;"",IF(F8&lt;&gt;"",CONCATENATE("...",D8,".",E8,".",F8,". - ",T8),IF(E8&lt;&gt;"",CONCATENATE("..",D8,".",E8,". - ",T8),CONCATENATE(D8,". - ",T8))),"")</f>
-        <v>...A.02.a. - Sexually transmitted diseases (STDs) excluding HIV</v>
+        <f t="shared" si="0"/>
+        <v>....A.02.a. - Sexually transmitted diseases (STDs) excluding HIV</v>
       </c>
       <c r="B8" s="2">
         <v>4</v>
@@ -5810,7 +5810,7 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="44" t="str">
-        <f>IF(H9&lt;&gt;"",IF(F9&lt;&gt;"",CONCATENATE("...",D9,".",E9,".",F9,". - ",T9),IF(E9&lt;&gt;"",CONCATENATE("..",D9,".",E9,". - ",T9),CONCATENATE(D9,". - ",T9))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B9" s="2">
@@ -5870,7 +5870,7 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="44" t="str">
-        <f>IF(H10&lt;&gt;"",IF(F10&lt;&gt;"",CONCATENATE("...",D10,".",E10,".",F10,". - ",T10),IF(E10&lt;&gt;"",CONCATENATE("..",D10,".",E10,". - ",T10),CONCATENATE(D10,". - ",T10))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B10" s="2">
@@ -5930,7 +5930,7 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="str">
-        <f>IF(H11&lt;&gt;"",IF(F11&lt;&gt;"",CONCATENATE("...",D11,".",E11,".",F11,". - ",T11),IF(E11&lt;&gt;"",CONCATENATE("..",D11,".",E11,". - ",T11),CONCATENATE(D11,". - ",T11))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B11" s="2">
@@ -5990,7 +5990,7 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="str">
-        <f>IF(H12&lt;&gt;"",IF(F12&lt;&gt;"",CONCATENATE("...",D12,".",E12,".",F12,". - ",T12),IF(E12&lt;&gt;"",CONCATENATE("..",D12,".",E12,". - ",T12),CONCATENATE(D12,". - ",T12))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B12" s="2">
@@ -6046,9 +6046,9 @@
         <v>516</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="44" t="str">
-        <f>IF(H13&lt;&gt;"",IF(F13&lt;&gt;"",CONCATENATE("...",D13,".",E13,".",F13,". - ",T13),IF(E13&lt;&gt;"",CONCATENATE("..",D13,".",E13,". - ",T13),CONCATENATE(D13,". - ",T13))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B13" s="2">
@@ -6106,10 +6106,10 @@
       </c>
       <c r="X13" s="2"/>
     </row>
-    <row r="14" spans="1:24" ht="51" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="str">
-        <f>IF(H14&lt;&gt;"",IF(F14&lt;&gt;"",CONCATENATE("...",D14,".",E14,".",F14,". - ",T14),IF(E14&lt;&gt;"",CONCATENATE("..",D14,".",E14,". - ",T14),CONCATENATE(D14,". - ",T14))),"")</f>
-        <v>...A.02.b. - HIV/AIDS</v>
+        <f t="shared" si="0"/>
+        <v>....A.02.b. - HIV/AIDS</v>
       </c>
       <c r="B14" s="2">
         <v>10</v>
@@ -6170,7 +6170,7 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="44" t="str">
-        <f>IF(H15&lt;&gt;"",IF(F15&lt;&gt;"",CONCATENATE("...",D15,".",E15,".",F15,". - ",T15),IF(E15&lt;&gt;"",CONCATENATE("..",D15,".",E15,". - ",T15),CONCATENATE(D15,". - ",T15))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B15" s="2">
@@ -6226,7 +6226,7 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="44" t="str">
-        <f>IF(H16&lt;&gt;"",IF(F16&lt;&gt;"",CONCATENATE("...",D16,".",E16,".",F16,". - ",T16),IF(E16&lt;&gt;"",CONCATENATE("..",D16,".",E16,". - ",T16),CONCATENATE(D16,". - ",T16))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B16" s="2">
@@ -6286,7 +6286,7 @@
     </row>
     <row r="17" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="44" t="str">
-        <f>IF(H17&lt;&gt;"",IF(F17&lt;&gt;"",CONCATENATE("...",D17,".",E17,".",F17,". - ",T17),IF(E17&lt;&gt;"",CONCATENATE("..",D17,".",E17,". - ",T17),CONCATENATE(D17,". - ",T17))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B17" s="2">
@@ -6344,7 +6344,7 @@
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="44" t="str">
-        <f>IF(H18&lt;&gt;"",IF(F18&lt;&gt;"",CONCATENATE("...",D18,".",E18,".",F18,". - ",T18),IF(E18&lt;&gt;"",CONCATENATE("..",D18,".",E18,". - ",T18),CONCATENATE(D18,". - ",T18))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B18" s="2">
@@ -6396,7 +6396,7 @@
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="44" t="str">
-        <f>IF(H19&lt;&gt;"",IF(F19&lt;&gt;"",CONCATENATE("...",D19,".",E19,".",F19,". - ",T19),IF(E19&lt;&gt;"",CONCATENATE("..",D19,".",E19,". - ",T19),CONCATENATE(D19,". - ",T19))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B19" s="2">
@@ -6413,7 +6413,7 @@
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="40" t="str">
-        <f t="shared" ref="G19:G24" si="0">CONCATENATE("c",D19,E19,F19)</f>
+        <f t="shared" ref="G19:G24" si="1">CONCATENATE("c",D19,E19,F19)</f>
         <v>cA99</v>
       </c>
       <c r="H19" s="40"/>
@@ -6454,7 +6454,7 @@
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="44" t="str">
-        <f>IF(H20&lt;&gt;"",IF(F20&lt;&gt;"",CONCATENATE("...",D20,".",E20,".",F20,". - ",T20),IF(E20&lt;&gt;"",CONCATENATE("..",D20,".",E20,". - ",T20),CONCATENATE(D20,". - ",T20))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B20" s="2">
@@ -6471,7 +6471,7 @@
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="40" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>cA99</v>
       </c>
       <c r="H20" s="40"/>
@@ -6512,7 +6512,7 @@
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="44" t="str">
-        <f>IF(H21&lt;&gt;"",IF(F21&lt;&gt;"",CONCATENATE("...",D21,".",E21,".",F21,". - ",T21),IF(E21&lt;&gt;"",CONCATENATE("..",D21,".",E21,". - ",T21),CONCATENATE(D21,". - ",T21))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B21" s="2">
@@ -6529,7 +6529,7 @@
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="40" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>cA99</v>
       </c>
       <c r="H21" s="40"/>
@@ -6570,7 +6570,7 @@
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="44" t="str">
-        <f>IF(H22&lt;&gt;"",IF(F22&lt;&gt;"",CONCATENATE("...",D22,".",E22,".",F22,". - ",T22),IF(E22&lt;&gt;"",CONCATENATE("..",D22,".",E22,". - ",T22),CONCATENATE(D22,". - ",T22))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B22" s="2">
@@ -6587,7 +6587,7 @@
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="40" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>cA99</v>
       </c>
       <c r="H22" s="40"/>
@@ -6626,10 +6626,10 @@
       </c>
       <c r="X22" s="2"/>
     </row>
-    <row r="23" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="44" t="str">
-        <f>IF(H23&lt;&gt;"",IF(F23&lt;&gt;"",CONCATENATE("...",D23,".",E23,".",F23,". - ",T23),IF(E23&lt;&gt;"",CONCATENATE("..",D23,".",E23,". - ",T23),CONCATENATE(D23,". - ",T23))),"")</f>
-        <v>..A.04. - Meningitis</v>
+        <f t="shared" si="0"/>
+        <v>...A.04. - Meningitis</v>
       </c>
       <c r="B23" s="2">
         <v>19</v>
@@ -6645,7 +6645,7 @@
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="40" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>cA04</v>
       </c>
       <c r="H23" s="40" t="str">
@@ -6687,10 +6687,10 @@
       </c>
       <c r="X23" s="2"/>
     </row>
-    <row r="24" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="44" t="str">
-        <f>IF(H24&lt;&gt;"",IF(F24&lt;&gt;"",CONCATENATE("...",D24,".",E24,".",F24,". - ",T24),IF(E24&lt;&gt;"",CONCATENATE("..",D24,".",E24,". - ",T24),CONCATENATE(D24,". - ",T24))),"")</f>
-        <v>..A.05. - Encephalitis</v>
+        <f t="shared" si="0"/>
+        <v>...A.05. - Encephalitis</v>
       </c>
       <c r="B24" s="2">
         <v>20</v>
@@ -6706,7 +6706,7 @@
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="40" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>cA05</v>
       </c>
       <c r="H24" s="40" t="str">
@@ -6748,10 +6748,10 @@
       </c>
       <c r="X24" s="2"/>
     </row>
-    <row r="25" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="44" t="str">
-        <f>IF(H25&lt;&gt;"",IF(F25&lt;&gt;"",CONCATENATE("...",D25,".",E25,".",F25,". - ",T25),IF(E25&lt;&gt;"",CONCATENATE("..",D25,".",E25,". - ",T25),CONCATENATE(D25,". - ",T25))),"")</f>
-        <v>..A.06. - Hepatitis</v>
+        <f t="shared" si="0"/>
+        <v>...A.06. - Hepatitis</v>
       </c>
       <c r="B25" s="2">
         <v>21</v>
@@ -6804,7 +6804,7 @@
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="44" t="str">
-        <f>IF(H26&lt;&gt;"",IF(F26&lt;&gt;"",CONCATENATE("...",D26,".",E26,".",F26,". - ",T26),IF(E26&lt;&gt;"",CONCATENATE("..",D26,".",E26,". - ",T26),CONCATENATE(D26,". - ",T26))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B26" s="2">
@@ -6856,10 +6856,10 @@
       </c>
       <c r="X26" s="2"/>
     </row>
-    <row r="27" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A27" s="44" t="str">
-        <f>IF(H27&lt;&gt;"",IF(F27&lt;&gt;"",CONCATENATE("...",D27,".",E27,".",F27,". - ",T27),IF(E27&lt;&gt;"",CONCATENATE("..",D27,".",E27,". - ",T27),CONCATENATE(D27,". - ",T27))),"")</f>
-        <v>...A.06.a. - Acute hepatitis B</v>
+        <f t="shared" si="0"/>
+        <v>....A.06.a. - Acute hepatitis B</v>
       </c>
       <c r="B27" s="2">
         <v>23</v>
@@ -6917,7 +6917,7 @@
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="44" t="str">
-        <f>IF(H28&lt;&gt;"",IF(F28&lt;&gt;"",CONCATENATE("...",D28,".",E28,".",F28,". - ",T28),IF(E28&lt;&gt;"",CONCATENATE("..",D28,".",E28,". - ",T28),CONCATENATE(D28,". - ",T28))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B28" s="2"/>
@@ -6943,10 +6943,10 @@
       <c r="W28" s="45"/>
       <c r="X28" s="2"/>
     </row>
-    <row r="29" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="44" t="str">
-        <f>IF(H29&lt;&gt;"",IF(F29&lt;&gt;"",CONCATENATE("...",D29,".",E29,".",F29,". - ",T29),IF(E29&lt;&gt;"",CONCATENATE("..",D29,".",E29,". - ",T29),CONCATENATE(D29,". - ",T29))),"")</f>
-        <v>...A.06.b. - Acute hepatitis C</v>
+        <f t="shared" si="0"/>
+        <v>....A.06.b. - Acute hepatitis C</v>
       </c>
       <c r="B29" s="2">
         <v>24</v>
@@ -7004,7 +7004,7 @@
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="44" t="str">
-        <f>IF(H30&lt;&gt;"",IF(F30&lt;&gt;"",CONCATENATE("...",D30,".",E30,".",F30,". - ",T30),IF(E30&lt;&gt;"",CONCATENATE("..",D30,".",E30,". - ",T30),CONCATENATE(D30,". - ",T30))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B30" s="2">
@@ -7058,7 +7058,7 @@
     </row>
     <row r="31" spans="1:24" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A31" s="44" t="str">
-        <f>IF(H31&lt;&gt;"",IF(F31&lt;&gt;"",CONCATENATE("...",D31,".",E31,".",F31,". - ",T31),IF(E31&lt;&gt;"",CONCATENATE("..",D31,".",E31,". - ",T31),CONCATENATE(D31,". - ",T31))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B31" s="2">
@@ -7109,7 +7109,7 @@
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="44" t="str">
-        <f>IF(H32&lt;&gt;"",IF(F32&lt;&gt;"",CONCATENATE("...",D32,".",E32,".",F32,". - ",T32),IF(E32&lt;&gt;"",CONCATENATE("..",D32,".",E32,". - ",T32),CONCATENATE(D32,". - ",T32))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B32" s="2">
@@ -7126,7 +7126,7 @@
       </c>
       <c r="F32" s="6"/>
       <c r="G32" s="40" t="str">
-        <f t="shared" ref="G32:G45" si="1">CONCATENATE("c",D32,E32,F32)</f>
+        <f t="shared" ref="G32:G45" si="2">CONCATENATE("c",D32,E32,F32)</f>
         <v>cA99</v>
       </c>
       <c r="H32" s="40"/>
@@ -7167,7 +7167,7 @@
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="44" t="str">
-        <f>IF(H33&lt;&gt;"",IF(F33&lt;&gt;"",CONCATENATE("...",D33,".",E33,".",F33,". - ",T33),IF(E33&lt;&gt;"",CONCATENATE("..",D33,".",E33,". - ",T33),CONCATENATE(D33,". - ",T33))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B33" s="2">
@@ -7184,7 +7184,7 @@
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>cA99</v>
       </c>
       <c r="H33" s="40"/>
@@ -7225,7 +7225,7 @@
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="44" t="str">
-        <f>IF(H34&lt;&gt;"",IF(F34&lt;&gt;"",CONCATENATE("...",D34,".",E34,".",F34,". - ",T34),IF(E34&lt;&gt;"",CONCATENATE("..",D34,".",E34,". - ",T34),CONCATENATE(D34,". - ",T34))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B34" s="2">
@@ -7242,7 +7242,7 @@
       </c>
       <c r="F34" s="6"/>
       <c r="G34" s="40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>cA99</v>
       </c>
       <c r="H34" s="40"/>
@@ -7283,7 +7283,7 @@
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="44" t="str">
-        <f>IF(H35&lt;&gt;"",IF(F35&lt;&gt;"",CONCATENATE("...",D35,".",E35,".",F35,". - ",T35),IF(E35&lt;&gt;"",CONCATENATE("..",D35,".",E35,". - ",T35),CONCATENATE(D35,". - ",T35))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B35" s="2">
@@ -7300,7 +7300,7 @@
       </c>
       <c r="F35" s="6"/>
       <c r="G35" s="40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>cA99</v>
       </c>
       <c r="H35" s="40"/>
@@ -7341,7 +7341,7 @@
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="44" t="str">
-        <f>IF(H36&lt;&gt;"",IF(F36&lt;&gt;"",CONCATENATE("...",D36,".",E36,".",F36,". - ",T36),IF(E36&lt;&gt;"",CONCATENATE("..",D36,".",E36,". - ",T36),CONCATENATE(D36,". - ",T36))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B36" s="2">
@@ -7358,7 +7358,7 @@
       </c>
       <c r="F36" s="6"/>
       <c r="G36" s="40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>cA99</v>
       </c>
       <c r="H36" s="40"/>
@@ -7399,7 +7399,7 @@
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" s="44" t="str">
-        <f>IF(H37&lt;&gt;"",IF(F37&lt;&gt;"",CONCATENATE("...",D37,".",E37,".",F37,". - ",T37),IF(E37&lt;&gt;"",CONCATENATE("..",D37,".",E37,". - ",T37),CONCATENATE(D37,". - ",T37))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B37" s="2">
@@ -7416,7 +7416,7 @@
       </c>
       <c r="F37" s="6"/>
       <c r="G37" s="40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>cA99</v>
       </c>
       <c r="H37" s="40"/>
@@ -7453,7 +7453,7 @@
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="44" t="str">
-        <f>IF(H38&lt;&gt;"",IF(F38&lt;&gt;"",CONCATENATE("...",D38,".",E38,".",F38,". - ",T38),IF(E38&lt;&gt;"",CONCATENATE("..",D38,".",E38,". - ",T38),CONCATENATE(D38,". - ",T38))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B38" s="2">
@@ -7470,7 +7470,7 @@
       </c>
       <c r="F38" s="6"/>
       <c r="G38" s="40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>cA99</v>
       </c>
       <c r="H38" s="40"/>
@@ -7507,7 +7507,7 @@
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="44" t="str">
-        <f>IF(H39&lt;&gt;"",IF(F39&lt;&gt;"",CONCATENATE("...",D39,".",E39,".",F39,". - ",T39),IF(E39&lt;&gt;"",CONCATENATE("..",D39,".",E39,". - ",T39),CONCATENATE(D39,". - ",T39))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B39" s="2">
@@ -7524,7 +7524,7 @@
       </c>
       <c r="F39" s="6"/>
       <c r="G39" s="40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>cA99</v>
       </c>
       <c r="H39" s="40"/>
@@ -7565,7 +7565,7 @@
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" s="44" t="str">
-        <f>IF(H40&lt;&gt;"",IF(F40&lt;&gt;"",CONCATENATE("...",D40,".",E40,".",F40,". - ",T40),IF(E40&lt;&gt;"",CONCATENATE("..",D40,".",E40,". - ",T40),CONCATENATE(D40,". - ",T40))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B40" s="2">
@@ -7582,7 +7582,7 @@
       </c>
       <c r="F40" s="6"/>
       <c r="G40" s="40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>cA99</v>
       </c>
       <c r="H40" s="40"/>
@@ -7623,7 +7623,7 @@
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" s="44" t="str">
-        <f>IF(H41&lt;&gt;"",IF(F41&lt;&gt;"",CONCATENATE("...",D41,".",E41,".",F41,". - ",T41),IF(E41&lt;&gt;"",CONCATENATE("..",D41,".",E41,". - ",T41),CONCATENATE(D41,". - ",T41))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B41" s="2">
@@ -7640,7 +7640,7 @@
       </c>
       <c r="F41" s="6"/>
       <c r="G41" s="40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>cA99</v>
       </c>
       <c r="H41" s="40"/>
@@ -7677,7 +7677,7 @@
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" s="44" t="str">
-        <f>IF(H42&lt;&gt;"",IF(F42&lt;&gt;"",CONCATENATE("...",D42,".",E42,".",F42,". - ",T42),IF(E42&lt;&gt;"",CONCATENATE("..",D42,".",E42,". - ",T42),CONCATENATE(D42,". - ",T42))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B42" s="2">
@@ -7694,7 +7694,7 @@
       </c>
       <c r="F42" s="6"/>
       <c r="G42" s="40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>cA99</v>
       </c>
       <c r="H42" s="40"/>
@@ -7735,7 +7735,7 @@
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="44" t="str">
-        <f>IF(H43&lt;&gt;"",IF(F43&lt;&gt;"",CONCATENATE("...",D43,".",E43,".",F43,". - ",T43),IF(E43&lt;&gt;"",CONCATENATE("..",D43,".",E43,". - ",T43),CONCATENATE(D43,". - ",T43))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B43" s="2">
@@ -7752,7 +7752,7 @@
       </c>
       <c r="F43" s="6"/>
       <c r="G43" s="40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>cA99</v>
       </c>
       <c r="H43" s="40"/>
@@ -7789,7 +7789,7 @@
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="44" t="str">
-        <f>IF(H44&lt;&gt;"",IF(F44&lt;&gt;"",CONCATENATE("...",D44,".",E44,".",F44,". - ",T44),IF(E44&lt;&gt;"",CONCATENATE("..",D44,".",E44,". - ",T44),CONCATENATE(D44,". - ",T44))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B44" s="2">
@@ -7806,7 +7806,7 @@
       </c>
       <c r="F44" s="6"/>
       <c r="G44" s="40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>cA99</v>
       </c>
       <c r="H44" s="40"/>
@@ -7847,7 +7847,7 @@
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" s="44" t="str">
-        <f>IF(H45&lt;&gt;"",IF(F45&lt;&gt;"",CONCATENATE("...",D45,".",E45,".",F45,". - ",T45),IF(E45&lt;&gt;"",CONCATENATE("..",D45,".",E45,". - ",T45),CONCATENATE(D45,". - ",T45))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B45" s="2">
@@ -7864,7 +7864,7 @@
       </c>
       <c r="F45" s="6"/>
       <c r="G45" s="40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>cA99</v>
       </c>
       <c r="H45" s="40"/>
@@ -7905,7 +7905,7 @@
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" s="44" t="str">
-        <f>IF(H46&lt;&gt;"",IF(F46&lt;&gt;"",CONCATENATE("...",D46,".",E46,".",F46,". - ",T46),IF(E46&lt;&gt;"",CONCATENATE("..",D46,".",E46,". - ",T46),CONCATENATE(D46,". - ",T46))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B46" s="2">
@@ -7960,7 +7960,7 @@
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" s="44" t="str">
-        <f>IF(H47&lt;&gt;"",IF(F47&lt;&gt;"",CONCATENATE("...",D47,".",E47,".",F47,". - ",T47),IF(E47&lt;&gt;"",CONCATENATE("..",D47,".",E47,". - ",T47),CONCATENATE(D47,". - ",T47))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B47" s="2">
@@ -8018,7 +8018,7 @@
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" s="44" t="str">
-        <f>IF(H48&lt;&gt;"",IF(F48&lt;&gt;"",CONCATENATE("...",D48,".",E48,".",F48,". - ",T48),IF(E48&lt;&gt;"",CONCATENATE("..",D48,".",E48,". - ",T48),CONCATENATE(D48,". - ",T48))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B48" s="2">
@@ -8072,7 +8072,7 @@
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" s="44" t="str">
-        <f>IF(H49&lt;&gt;"",IF(F49&lt;&gt;"",CONCATENATE("...",D49,".",E49,".",F49,". - ",T49),IF(E49&lt;&gt;"",CONCATENATE("..",D49,".",E49,". - ",T49),CONCATENATE(D49,". - ",T49))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B49" s="2">
@@ -8126,7 +8126,7 @@
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" s="44" t="str">
-        <f>IF(H50&lt;&gt;"",IF(F50&lt;&gt;"",CONCATENATE("...",D50,".",E50,".",F50,". - ",T50),IF(E50&lt;&gt;"",CONCATENATE("..",D50,".",E50,". - ",T50),CONCATENATE(D50,". - ",T50))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B50" s="2">
@@ -8180,7 +8180,7 @@
     </row>
     <row r="51" spans="1:24" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A51" s="44" t="str">
-        <f>IF(H51&lt;&gt;"",IF(F51&lt;&gt;"",CONCATENATE("...",D51,".",E51,".",F51,". - ",T51),IF(E51&lt;&gt;"",CONCATENATE("..",D51,".",E51,". - ",T51),CONCATENATE(D51,". - ",T51))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B51" s="2">
@@ -8244,10 +8244,10 @@
         <v>1314</v>
       </c>
     </row>
-    <row r="52" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A52" s="44" t="str">
-        <f>IF(H52&lt;&gt;"",IF(F52&lt;&gt;"",CONCATENATE("...",D52,".",E52,".",F52,". - ",T52),IF(E52&lt;&gt;"",CONCATENATE("..",D52,".",E52,". - ",T52),CONCATENATE(D52,". - ",T52))),"")</f>
-        <v>..A.07. - Respiratory infections</v>
+        <f t="shared" si="0"/>
+        <v>...A.07. - Respiratory infections</v>
       </c>
       <c r="B52" s="2">
         <v>47</v>
@@ -8304,10 +8304,10 @@
       </c>
       <c r="X52" s="2"/>
     </row>
-    <row r="53" spans="1:24" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53" s="44" t="str">
-        <f>IF(H53&lt;&gt;"",IF(F53&lt;&gt;"",CONCATENATE("...",D53,".",E53,".",F53,". - ",T53),IF(E53&lt;&gt;"",CONCATENATE("..",D53,".",E53,". - ",T53),CONCATENATE(D53,". - ",T53))),"")</f>
-        <v>...A.07.a. - Lower respiratory infections</v>
+        <f t="shared" si="0"/>
+        <v>....A.07.a. - Lower respiratory infections</v>
       </c>
       <c r="B53" s="2">
         <v>48</v>
@@ -8329,7 +8329,7 @@
         <v>cA07a</v>
       </c>
       <c r="H53" s="40" t="str">
-        <f t="shared" ref="H53:H54" si="2">CONCATENATE(D53,E53,F53)</f>
+        <f t="shared" ref="H53:H54" si="3">CONCATENATE(D53,E53,F53)</f>
         <v>A07a</v>
       </c>
       <c r="I53" s="5"/>
@@ -8373,10 +8373,10 @@
       </c>
       <c r="X53" s="2"/>
     </row>
-    <row r="54" spans="1:24" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54" s="44" t="str">
-        <f>IF(H54&lt;&gt;"",IF(F54&lt;&gt;"",CONCATENATE("...",D54,".",E54,".",F54,". - ",T54),IF(E54&lt;&gt;"",CONCATENATE("..",D54,".",E54,". - ",T54),CONCATENATE(D54,". - ",T54))),"")</f>
-        <v>...A.07.b. - Upper respiratory infections</v>
+        <f t="shared" si="0"/>
+        <v>....A.07.b. - Upper respiratory infections</v>
       </c>
       <c r="B54" s="2">
         <v>49</v>
@@ -8398,7 +8398,7 @@
         <v>cA07b</v>
       </c>
       <c r="H54" s="40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>A07b</v>
       </c>
       <c r="I54" s="5"/>
@@ -8444,7 +8444,7 @@
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55" s="44" t="str">
-        <f>IF(H55&lt;&gt;"",IF(F55&lt;&gt;"",CONCATENATE("...",D55,".",E55,".",F55,". - ",T55),IF(E55&lt;&gt;"",CONCATENATE("..",D55,".",E55,". - ",T55),CONCATENATE(D55,". - ",T55))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B55" s="2">
@@ -8506,10 +8506,10 @@
       </c>
       <c r="X55" s="2"/>
     </row>
-    <row r="56" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56" s="44" t="str">
-        <f>IF(H56&lt;&gt;"",IF(F56&lt;&gt;"",CONCATENATE("...",D56,".",E56,".",F56,". - ",T56),IF(E56&lt;&gt;"",CONCATENATE("..",D56,".",E56,". - ",T56),CONCATENATE(D56,". - ",T56))),"")</f>
-        <v>..A.08. - Maternal conditions</v>
+        <f t="shared" si="0"/>
+        <v>...A.08. - Maternal conditions</v>
       </c>
       <c r="B56" s="2">
         <v>51</v>
@@ -8570,7 +8570,7 @@
     </row>
     <row r="57" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A57" s="44" t="str">
-        <f>IF(H57&lt;&gt;"",IF(F57&lt;&gt;"",CONCATENATE("...",D57,".",E57,".",F57,". - ",T57),IF(E57&lt;&gt;"",CONCATENATE("..",D57,".",E57,". - ",T57),CONCATENATE(D57,". - ",T57))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B57" s="2">
@@ -8587,7 +8587,7 @@
       </c>
       <c r="F57" s="6"/>
       <c r="G57" s="40" t="str">
-        <f t="shared" ref="G57:G62" si="3">CONCATENATE("c",D57,E57,F57)</f>
+        <f t="shared" ref="G57:G62" si="4">CONCATENATE("c",D57,E57,F57)</f>
         <v>cA08</v>
       </c>
       <c r="H57" s="40"/>
@@ -8636,7 +8636,7 @@
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58" s="44" t="str">
-        <f>IF(H58&lt;&gt;"",IF(F58&lt;&gt;"",CONCATENATE("...",D58,".",E58,".",F58,". - ",T58),IF(E58&lt;&gt;"",CONCATENATE("..",D58,".",E58,". - ",T58),CONCATENATE(D58,". - ",T58))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B58" s="2">
@@ -8653,7 +8653,7 @@
       </c>
       <c r="F58" s="6"/>
       <c r="G58" s="40" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>cA08</v>
       </c>
       <c r="H58" s="40"/>
@@ -8700,7 +8700,7 @@
     </row>
     <row r="59" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A59" s="44" t="str">
-        <f>IF(H59&lt;&gt;"",IF(F59&lt;&gt;"",CONCATENATE("...",D59,".",E59,".",F59,". - ",T59),IF(E59&lt;&gt;"",CONCATENATE("..",D59,".",E59,". - ",T59),CONCATENATE(D59,". - ",T59))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B59" s="2">
@@ -8717,7 +8717,7 @@
       </c>
       <c r="F59" s="6"/>
       <c r="G59" s="40" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>cA08</v>
       </c>
       <c r="H59" s="40"/>
@@ -8766,7 +8766,7 @@
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60" s="44" t="str">
-        <f>IF(H60&lt;&gt;"",IF(F60&lt;&gt;"",CONCATENATE("...",D60,".",E60,".",F60,". - ",T60),IF(E60&lt;&gt;"",CONCATENATE("..",D60,".",E60,". - ",T60),CONCATENATE(D60,". - ",T60))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B60" s="2">
@@ -8783,7 +8783,7 @@
       </c>
       <c r="F60" s="6"/>
       <c r="G60" s="40" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>cA08</v>
       </c>
       <c r="H60" s="40"/>
@@ -8830,7 +8830,7 @@
     </row>
     <row r="61" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A61" s="44" t="str">
-        <f>IF(H61&lt;&gt;"",IF(F61&lt;&gt;"",CONCATENATE("...",D61,".",E61,".",F61,". - ",T61),IF(E61&lt;&gt;"",CONCATENATE("..",D61,".",E61,". - ",T61),CONCATENATE(D61,". - ",T61))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B61" s="2">
@@ -8847,7 +8847,7 @@
       </c>
       <c r="F61" s="6"/>
       <c r="G61" s="40" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>cA08</v>
       </c>
       <c r="H61" s="40"/>
@@ -8894,7 +8894,7 @@
     </row>
     <row r="62" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A62" s="44" t="str">
-        <f>IF(H62&lt;&gt;"",IF(F62&lt;&gt;"",CONCATENATE("...",D62,".",E62,".",F62,". - ",T62),IF(E62&lt;&gt;"",CONCATENATE("..",D62,".",E62,". - ",T62),CONCATENATE(D62,". - ",T62))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B62" s="2">
@@ -8911,7 +8911,7 @@
       </c>
       <c r="F62" s="6"/>
       <c r="G62" s="40" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>cA08</v>
       </c>
       <c r="H62" s="40"/>
@@ -8956,10 +8956,10 @@
       </c>
       <c r="X62" s="2"/>
     </row>
-    <row r="63" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A63" s="44" t="str">
-        <f>IF(H63&lt;&gt;"",IF(F63&lt;&gt;"",CONCATENATE("...",D63,".",E63,".",F63,". - ",T63),IF(E63&lt;&gt;"",CONCATENATE("..",D63,".",E63,". - ",T63),CONCATENATE(D63,". - ",T63))),"")</f>
-        <v>..A.09. - Neonatal conditions</v>
+        <f t="shared" si="0"/>
+        <v>...A.09. - Neonatal conditions</v>
       </c>
       <c r="B63" s="2">
         <v>58</v>
@@ -9020,7 +9020,7 @@
     </row>
     <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64" s="44" t="str">
-        <f>IF(H64&lt;&gt;"",IF(F64&lt;&gt;"",CONCATENATE("...",D64,".",E64,".",F64,". - ",T64),IF(E64&lt;&gt;"",CONCATENATE("..",D64,".",E64,". - ",T64),CONCATENATE(D64,". - ",T64))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B64" s="2">
@@ -9078,7 +9078,7 @@
     </row>
     <row r="65" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A65" s="44" t="str">
-        <f>IF(H65&lt;&gt;"",IF(F65&lt;&gt;"",CONCATENATE("...",D65,".",E65,".",F65,". - ",T65),IF(E65&lt;&gt;"",CONCATENATE("..",D65,".",E65,". - ",T65),CONCATENATE(D65,". - ",T65))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B65" s="2">
@@ -9136,7 +9136,7 @@
     </row>
     <row r="66" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A66" s="44" t="str">
-        <f>IF(H66&lt;&gt;"",IF(F66&lt;&gt;"",CONCATENATE("...",D66,".",E66,".",F66,". - ",T66),IF(E66&lt;&gt;"",CONCATENATE("..",D66,".",E66,". - ",T66),CONCATENATE(D66,". - ",T66))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B66" s="2">
@@ -9194,7 +9194,7 @@
     </row>
     <row r="67" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A67" s="44" t="str">
-        <f>IF(H67&lt;&gt;"",IF(F67&lt;&gt;"",CONCATENATE("...",D67,".",E67,".",F67,". - ",T67),IF(E67&lt;&gt;"",CONCATENATE("..",D67,".",E67,". - ",T67),CONCATENATE(D67,". - ",T67))),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="B67" s="2">
@@ -9258,7 +9258,7 @@
     </row>
     <row r="68" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A68" s="44" t="str">
-        <f>IF(H68&lt;&gt;"",IF(F68&lt;&gt;"",CONCATENATE("...",D68,".",E68,".",F68,". - ",T68),IF(E68&lt;&gt;"",CONCATENATE("..",D68,".",E68,". - ",T68),CONCATENATE(D68,". - ",T68))),"")</f>
+        <f t="shared" ref="A68:A131" si="5">IF(H68&lt;&gt;"",IF(F68&lt;&gt;"",CONCATENATE("....",D68,".",E68,".",F68,". - ",T68),IF(E68&lt;&gt;"",CONCATENATE("...",D68,".",E68,". - ",T68),CONCATENATE("..",D68,". - ",T68))),"")</f>
         <v/>
       </c>
       <c r="B68" s="2">
@@ -9313,7 +9313,7 @@
     </row>
     <row r="69" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A69" s="44" t="str">
-        <f>IF(H69&lt;&gt;"",IF(F69&lt;&gt;"",CONCATENATE("...",D69,".",E69,".",F69,". - ",T69),IF(E69&lt;&gt;"",CONCATENATE("..",D69,".",E69,". - ",T69),CONCATENATE(D69,". - ",T69))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B69" s="2">
@@ -9371,7 +9371,7 @@
     </row>
     <row r="70" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A70" s="44" t="str">
-        <f>IF(H70&lt;&gt;"",IF(F70&lt;&gt;"",CONCATENATE("...",D70,".",E70,".",F70,". - ",T70),IF(E70&lt;&gt;"",CONCATENATE("..",D70,".",E70,". - ",T70),CONCATENATE(D70,". - ",T70))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B70" s="2">
@@ -9429,7 +9429,7 @@
     </row>
     <row r="71" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A71" s="44" t="str">
-        <f>IF(H71&lt;&gt;"",IF(F71&lt;&gt;"",CONCATENATE("...",D71,".",E71,".",F71,". - ",T71),IF(E71&lt;&gt;"",CONCATENATE("..",D71,".",E71,". - ",T71),CONCATENATE(D71,". - ",T71))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B71" s="2">
@@ -9483,7 +9483,7 @@
     </row>
     <row r="72" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A72" s="44" t="str">
-        <f>IF(H72&lt;&gt;"",IF(F72&lt;&gt;"",CONCATENATE("...",D72,".",E72,".",F72,". - ",T72),IF(E72&lt;&gt;"",CONCATENATE("..",D72,".",E72,". - ",T72),CONCATENATE(D72,". - ",T72))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B72" s="2">
@@ -9541,7 +9541,7 @@
     </row>
     <row r="73" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A73" s="44" t="str">
-        <f>IF(H73&lt;&gt;"",IF(F73&lt;&gt;"",CONCATENATE("...",D73,".",E73,".",F73,". - ",T73),IF(E73&lt;&gt;"",CONCATENATE("..",D73,".",E73,". - ",T73),CONCATENATE(D73,". - ",T73))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B73" s="2">
@@ -9599,7 +9599,7 @@
     </row>
     <row r="74" spans="1:24" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A74" s="44" t="str">
-        <f>IF(H74&lt;&gt;"",IF(F74&lt;&gt;"",CONCATENATE("...",D74,".",E74,".",F74,". - ",T74),IF(E74&lt;&gt;"",CONCATENATE("..",D74,".",E74,". - ",T74),CONCATENATE(D74,". - ",T74))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B74" s="2">
@@ -9650,10 +9650,10 @@
       </c>
       <c r="X74" s="2"/>
     </row>
-    <row r="75" spans="1:24" ht="51" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A75" s="44" t="str">
-        <f>IF(H75&lt;&gt;"",IF(F75&lt;&gt;"",CONCATENATE("...",D75,".",E75,".",F75,". - ",T75),IF(E75&lt;&gt;"",CONCATENATE("..",D75,".",E75,". - ",T75),CONCATENATE(D75,". - ",T75))),"")</f>
-        <v>D. - Other Chronic</v>
+        <f t="shared" si="5"/>
+        <v>..D. - Other Chronic</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="35" t="s">
@@ -9688,10 +9688,10 @@
       </c>
       <c r="X75" s="2"/>
     </row>
-    <row r="76" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:24" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A76" s="44" t="str">
-        <f>IF(H76&lt;&gt;"",IF(F76&lt;&gt;"",CONCATENATE("...",D76,".",E76,".",F76,". - ",T76),IF(E76&lt;&gt;"",CONCATENATE("..",D76,".",E76,". - ",T76),CONCATENATE(D76,". - ",T76))),"")</f>
-        <v>B. - Cancer/Malignant neoplasms</v>
+        <f t="shared" si="5"/>
+        <v>..B. - Cancer/Malignant neoplasms</v>
       </c>
       <c r="B76" s="2">
         <v>70</v>
@@ -9746,10 +9746,10 @@
       </c>
       <c r="X76" s="2"/>
     </row>
-    <row r="77" spans="1:24" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A77" s="44" t="str">
-        <f>IF(H77&lt;&gt;"",IF(F77&lt;&gt;"",CONCATENATE("...",D77,".",E77,".",F77,". - ",T77),IF(E77&lt;&gt;"",CONCATENATE("..",D77,".",E77,". - ",T77),CONCATENATE(D77,". - ",T77))),"")</f>
-        <v>..B.01. - Mouth and oropharynx cancers</v>
+        <f t="shared" si="5"/>
+        <v>...B.01. - Mouth and oropharynx cancers</v>
       </c>
       <c r="B77" s="2">
         <v>71</v>
@@ -9765,7 +9765,7 @@
       </c>
       <c r="F77" s="6"/>
       <c r="G77" s="40" t="str">
-        <f t="shared" ref="G77:G86" si="4">CONCATENATE("c",D77,E77,F77)</f>
+        <f t="shared" ref="G77:G86" si="6">CONCATENATE("c",D77,E77,F77)</f>
         <v>cB01</v>
       </c>
       <c r="H77" s="40" t="str">
@@ -9807,7 +9807,7 @@
     </row>
     <row r="78" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A78" s="44" t="str">
-        <f>IF(H78&lt;&gt;"",IF(F78&lt;&gt;"",CONCATENATE("...",D78,".",E78,".",F78,". - ",T78),IF(E78&lt;&gt;"",CONCATENATE("..",D78,".",E78,". - ",T78),CONCATENATE(D78,". - ",T78))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B78" s="2">
@@ -9824,7 +9824,7 @@
       </c>
       <c r="F78" s="6"/>
       <c r="G78" s="40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>cB01</v>
       </c>
       <c r="H78" s="40"/>
@@ -9871,7 +9871,7 @@
     </row>
     <row r="79" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A79" s="44" t="str">
-        <f>IF(H79&lt;&gt;"",IF(F79&lt;&gt;"",CONCATENATE("...",D79,".",E79,".",F79,". - ",T79),IF(E79&lt;&gt;"",CONCATENATE("..",D79,".",E79,". - ",T79),CONCATENATE(D79,". - ",T79))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B79" s="2">
@@ -9888,7 +9888,7 @@
       </c>
       <c r="F79" s="6"/>
       <c r="G79" s="40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>cB01</v>
       </c>
       <c r="H79" s="40"/>
@@ -9935,7 +9935,7 @@
     </row>
     <row r="80" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A80" s="44" t="str">
-        <f>IF(H80&lt;&gt;"",IF(F80&lt;&gt;"",CONCATENATE("...",D80,".",E80,".",F80,". - ",T80),IF(E80&lt;&gt;"",CONCATENATE("..",D80,".",E80,". - ",T80),CONCATENATE(D80,". - ",T80))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B80" s="2">
@@ -9952,7 +9952,7 @@
       </c>
       <c r="F80" s="6"/>
       <c r="G80" s="40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>cB01</v>
       </c>
       <c r="H80" s="40"/>
@@ -9993,10 +9993,10 @@
       </c>
       <c r="X80" s="2"/>
     </row>
-    <row r="81" spans="1:24" ht="51" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A81" s="44" t="str">
-        <f>IF(H81&lt;&gt;"",IF(F81&lt;&gt;"",CONCATENATE("...",D81,".",E81,".",F81,". - ",T81),IF(E81&lt;&gt;"",CONCATENATE("..",D81,".",E81,". - ",T81),CONCATENATE(D81,". - ",T81))),"")</f>
-        <v>..B.02. - Oesophagus cancer</v>
+        <f t="shared" si="5"/>
+        <v>...B.02. - Oesophagus cancer</v>
       </c>
       <c r="B81" s="2">
         <v>75</v>
@@ -10012,11 +10012,11 @@
       </c>
       <c r="F81" s="6"/>
       <c r="G81" s="40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>cB02</v>
       </c>
       <c r="H81" s="40" t="str">
-        <f t="shared" ref="H81:H87" si="5">CONCATENATE(D81,E81,F81)</f>
+        <f t="shared" ref="H81:H87" si="7">CONCATENATE(D81,E81,F81)</f>
         <v>B02</v>
       </c>
       <c r="I81" s="18" t="s">
@@ -10060,10 +10060,10 @@
       </c>
       <c r="X81" s="2"/>
     </row>
-    <row r="82" spans="1:24" ht="51" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A82" s="44" t="str">
-        <f>IF(H82&lt;&gt;"",IF(F82&lt;&gt;"",CONCATENATE("...",D82,".",E82,".",F82,". - ",T82),IF(E82&lt;&gt;"",CONCATENATE("..",D82,".",E82,". - ",T82),CONCATENATE(D82,". - ",T82))),"")</f>
-        <v>..B.03. - Stomach cancer</v>
+        <f t="shared" si="5"/>
+        <v>...B.03. - Stomach cancer</v>
       </c>
       <c r="B82" s="2">
         <v>76</v>
@@ -10079,11 +10079,11 @@
       </c>
       <c r="F82" s="6"/>
       <c r="G82" s="40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>cB03</v>
       </c>
       <c r="H82" s="40" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>B03</v>
       </c>
       <c r="I82" s="18" t="s">
@@ -10129,10 +10129,10 @@
         <v>952</v>
       </c>
     </row>
-    <row r="83" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A83" s="44" t="str">
-        <f>IF(H83&lt;&gt;"",IF(F83&lt;&gt;"",CONCATENATE("...",D83,".",E83,".",F83,". - ",T83),IF(E83&lt;&gt;"",CONCATENATE("..",D83,".",E83,". - ",T83),CONCATENATE(D83,". - ",T83))),"")</f>
-        <v>..B.04. - Colon and rectum cancers</v>
+        <f t="shared" si="5"/>
+        <v>...B.04. - Colon and rectum cancers</v>
       </c>
       <c r="B83" s="2">
         <v>77</v>
@@ -10148,11 +10148,11 @@
       </c>
       <c r="F83" s="6"/>
       <c r="G83" s="40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>cB04</v>
       </c>
       <c r="H83" s="40" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>B04</v>
       </c>
       <c r="I83" s="16" t="s">
@@ -10196,10 +10196,10 @@
       </c>
       <c r="X83" s="2"/>
     </row>
-    <row r="84" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A84" s="44" t="str">
-        <f>IF(H84&lt;&gt;"",IF(F84&lt;&gt;"",CONCATENATE("...",D84,".",E84,".",F84,". - ",T84),IF(E84&lt;&gt;"",CONCATENATE("..",D84,".",E84,". - ",T84),CONCATENATE(D84,". - ",T84))),"")</f>
-        <v>..B.05. - Liver cancer</v>
+        <f t="shared" si="5"/>
+        <v>...B.05. - Liver cancer</v>
       </c>
       <c r="B84" s="2">
         <v>78</v>
@@ -10215,11 +10215,11 @@
       </c>
       <c r="F84" s="6"/>
       <c r="G84" s="40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>cB05</v>
       </c>
       <c r="H84" s="40" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>B05</v>
       </c>
       <c r="I84" s="18" t="s">
@@ -10263,10 +10263,10 @@
       </c>
       <c r="X84" s="2"/>
     </row>
-    <row r="85" spans="1:24" ht="51" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A85" s="44" t="str">
-        <f>IF(H85&lt;&gt;"",IF(F85&lt;&gt;"",CONCATENATE("...",D85,".",E85,".",F85,". - ",T85),IF(E85&lt;&gt;"",CONCATENATE("..",D85,".",E85,". - ",T85),CONCATENATE(D85,". - ",T85))),"")</f>
-        <v>..B.06. - Pancreas cancer</v>
+        <f t="shared" si="5"/>
+        <v>...B.06. - Pancreas cancer</v>
       </c>
       <c r="B85" s="2">
         <v>79</v>
@@ -10282,11 +10282,11 @@
       </c>
       <c r="F85" s="6"/>
       <c r="G85" s="40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>cB06</v>
       </c>
       <c r="H85" s="40" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>B06</v>
       </c>
       <c r="I85" s="18" t="s">
@@ -10330,10 +10330,10 @@
       </c>
       <c r="X85" s="2"/>
     </row>
-    <row r="86" spans="1:24" ht="102" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A86" s="44" t="str">
-        <f>IF(H86&lt;&gt;"",IF(F86&lt;&gt;"",CONCATENATE("...",D86,".",E86,".",F86,". - ",T86),IF(E86&lt;&gt;"",CONCATENATE("..",D86,".",E86,". - ",T86),CONCATENATE(D86,". - ",T86))),"")</f>
-        <v>..B.07. - Trachea, bronchus and lung cancers</v>
+        <f t="shared" si="5"/>
+        <v>...B.07. - Trachea, bronchus and lung cancers</v>
       </c>
       <c r="B86" s="2">
         <v>80</v>
@@ -10349,11 +10349,11 @@
       </c>
       <c r="F86" s="6"/>
       <c r="G86" s="40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>cB07</v>
       </c>
       <c r="H86" s="40" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>B07</v>
       </c>
       <c r="I86" s="18" t="s">
@@ -10397,10 +10397,10 @@
       </c>
       <c r="X86" s="2"/>
     </row>
-    <row r="87" spans="1:24" ht="102" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A87" s="44" t="str">
-        <f>IF(H87&lt;&gt;"",IF(F87&lt;&gt;"",CONCATENATE("...",D87,".",E87,".",F87,". - ",T87),IF(E87&lt;&gt;"",CONCATENATE("..",D87,".",E87,". - ",T87),CONCATENATE(D87,". - ",T87))),"")</f>
-        <v>..B.08. - Melanoma and other skin cancers</v>
+        <f t="shared" si="5"/>
+        <v>...B.08. - Melanoma and other skin cancers</v>
       </c>
       <c r="B87" s="2">
         <v>81</v>
@@ -10419,7 +10419,7 @@
         <v>952</v>
       </c>
       <c r="H87" s="40" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>B08</v>
       </c>
       <c r="J87" s="17" t="s">
@@ -10458,7 +10458,7 @@
     </row>
     <row r="88" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A88" s="44" t="str">
-        <f>IF(H88&lt;&gt;"",IF(F88&lt;&gt;"",CONCATENATE("...",D88,".",E88,".",F88,". - ",T88),IF(E88&lt;&gt;"",CONCATENATE("..",D88,".",E88,". - ",T88),CONCATENATE(D88,". - ",T88))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B88" s="2">
@@ -10475,7 +10475,7 @@
       </c>
       <c r="F88" s="6"/>
       <c r="G88" s="40" t="str">
-        <f t="shared" ref="G88:G103" si="6">CONCATENATE("c",D88,E88,F88)</f>
+        <f t="shared" ref="G88:G103" si="8">CONCATENATE("c",D88,E88,F88)</f>
         <v>cB08</v>
       </c>
       <c r="H88" s="40"/>
@@ -10522,7 +10522,7 @@
     </row>
     <row r="89" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A89" s="44" t="str">
-        <f>IF(H89&lt;&gt;"",IF(F89&lt;&gt;"",CONCATENATE("...",D89,".",E89,".",F89,". - ",T89),IF(E89&lt;&gt;"",CONCATENATE("..",D89,".",E89,". - ",T89),CONCATENATE(D89,". - ",T89))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B89" s="2">
@@ -10539,7 +10539,7 @@
       </c>
       <c r="F89" s="6"/>
       <c r="G89" s="40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>cB08</v>
       </c>
       <c r="H89" s="40"/>
@@ -10584,10 +10584,10 @@
       </c>
       <c r="X89" s="2"/>
     </row>
-    <row r="90" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A90" s="44" t="str">
-        <f>IF(H90&lt;&gt;"",IF(F90&lt;&gt;"",CONCATENATE("...",D90,".",E90,".",F90,". - ",T90),IF(E90&lt;&gt;"",CONCATENATE("..",D90,".",E90,". - ",T90),CONCATENATE(D90,". - ",T90))),"")</f>
-        <v>..B.09. - Breast cancer</v>
+        <f t="shared" si="5"/>
+        <v>...B.09. - Breast cancer</v>
       </c>
       <c r="B90" s="2">
         <v>84</v>
@@ -10603,7 +10603,7 @@
       </c>
       <c r="F90" s="6"/>
       <c r="G90" s="40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>cB09</v>
       </c>
       <c r="H90" s="40" t="str">
@@ -10651,10 +10651,10 @@
       </c>
       <c r="X90" s="2"/>
     </row>
-    <row r="91" spans="1:24" ht="51" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A91" s="44" t="str">
-        <f>IF(H91&lt;&gt;"",IF(F91&lt;&gt;"",CONCATENATE("...",D91,".",E91,".",F91,". - ",T91),IF(E91&lt;&gt;"",CONCATENATE("..",D91,".",E91,". - ",T91),CONCATENATE(D91,". - ",T91))),"")</f>
-        <v>..B.10. - Uterine cancer</v>
+        <f t="shared" si="5"/>
+        <v>...B.10. - Uterine cancer</v>
       </c>
       <c r="B91" s="2"/>
       <c r="C91" s="37" t="s">
@@ -10696,7 +10696,7 @@
     </row>
     <row r="92" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A92" s="44" t="str">
-        <f>IF(H92&lt;&gt;"",IF(F92&lt;&gt;"",CONCATENATE("...",D92,".",E92,".",F92,". - ",T92),IF(E92&lt;&gt;"",CONCATENATE("..",D92,".",E92,". - ",T92),CONCATENATE(D92,". - ",T92))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B92" s="2">
@@ -10760,7 +10760,7 @@
     </row>
     <row r="93" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A93" s="44" t="str">
-        <f>IF(H93&lt;&gt;"",IF(F93&lt;&gt;"",CONCATENATE("...",D93,".",E93,".",F93,". - ",T93),IF(E93&lt;&gt;"",CONCATENATE("..",D93,".",E93,". - ",T93),CONCATENATE(D93,". - ",T93))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B93" s="2">
@@ -10777,7 +10777,7 @@
       </c>
       <c r="F93" s="6"/>
       <c r="G93" s="40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>cB10</v>
       </c>
       <c r="H93" s="40"/>
@@ -10822,10 +10822,10 @@
       </c>
       <c r="X93" s="2"/>
     </row>
-    <row r="94" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A94" s="44" t="str">
-        <f>IF(H94&lt;&gt;"",IF(F94&lt;&gt;"",CONCATENATE("...",D94,".",E94,".",F94,". - ",T94),IF(E94&lt;&gt;"",CONCATENATE("..",D94,".",E94,". - ",T94),CONCATENATE(D94,". - ",T94))),"")</f>
-        <v>..B.11. - Ovary cancer</v>
+        <f t="shared" si="5"/>
+        <v>...B.11. - Ovary cancer</v>
       </c>
       <c r="B94" s="2">
         <v>87</v>
@@ -10841,7 +10841,7 @@
       </c>
       <c r="F94" s="6"/>
       <c r="G94" s="40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>cB11</v>
       </c>
       <c r="H94" s="40" t="str">
@@ -10889,10 +10889,10 @@
       </c>
       <c r="X94" s="2"/>
     </row>
-    <row r="95" spans="1:24" ht="51" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A95" s="44" t="str">
-        <f>IF(H95&lt;&gt;"",IF(F95&lt;&gt;"",CONCATENATE("...",D95,".",E95,".",F95,". - ",T95),IF(E95&lt;&gt;"",CONCATENATE("..",D95,".",E95,". - ",T95),CONCATENATE(D95,". - ",T95))),"")</f>
-        <v>..B.12. - Prostate cancer</v>
+        <f t="shared" si="5"/>
+        <v>...B.12. - Prostate cancer</v>
       </c>
       <c r="B95" s="2">
         <v>88</v>
@@ -10908,7 +10908,7 @@
       </c>
       <c r="F95" s="6"/>
       <c r="G95" s="40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>cB12</v>
       </c>
       <c r="H95" s="40" t="str">
@@ -10958,7 +10958,7 @@
     </row>
     <row r="96" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A96" s="44" t="str">
-        <f>IF(H96&lt;&gt;"",IF(F96&lt;&gt;"",CONCATENATE("...",D96,".",E96,".",F96,". - ",T96),IF(E96&lt;&gt;"",CONCATENATE("..",D96,".",E96,". - ",T96),CONCATENATE(D96,". - ",T96))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B96" s="2">
@@ -10975,7 +10975,7 @@
       </c>
       <c r="F96" s="6"/>
       <c r="G96" s="40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>cB99</v>
       </c>
       <c r="H96" s="40"/>
@@ -11020,10 +11020,10 @@
       </c>
       <c r="X96" s="2"/>
     </row>
-    <row r="97" spans="1:24" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A97" s="44" t="str">
-        <f>IF(H97&lt;&gt;"",IF(F97&lt;&gt;"",CONCATENATE("...",D97,".",E97,".",F97,". - ",T97),IF(E97&lt;&gt;"",CONCATENATE("..",D97,".",E97,". - ",T97),CONCATENATE(D97,". - ",T97))),"")</f>
-        <v>..B.13. - Kidney, renal pelvis and ureter cancer</v>
+        <f t="shared" si="5"/>
+        <v>...B.13. - Kidney, renal pelvis and ureter cancer</v>
       </c>
       <c r="B97" s="2">
         <v>90</v>
@@ -11039,7 +11039,7 @@
       </c>
       <c r="F97" s="6"/>
       <c r="G97" s="40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>cB13</v>
       </c>
       <c r="H97" s="40" t="str">
@@ -11087,10 +11087,10 @@
       </c>
       <c r="X97" s="2"/>
     </row>
-    <row r="98" spans="1:24" ht="51" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A98" s="44" t="str">
-        <f>IF(H98&lt;&gt;"",IF(F98&lt;&gt;"",CONCATENATE("...",D98,".",E98,".",F98,". - ",T98),IF(E98&lt;&gt;"",CONCATENATE("..",D98,".",E98,". - ",T98),CONCATENATE(D98,". - ",T98))),"")</f>
-        <v>..B.14. - Bladder cancer</v>
+        <f t="shared" si="5"/>
+        <v>...B.14. - Bladder cancer</v>
       </c>
       <c r="B98" s="2">
         <v>91</v>
@@ -11106,7 +11106,7 @@
       </c>
       <c r="F98" s="6"/>
       <c r="G98" s="40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>cB14</v>
       </c>
       <c r="H98" s="40" t="str">
@@ -11154,10 +11154,10 @@
       </c>
       <c r="X98" s="2"/>
     </row>
-    <row r="99" spans="1:24" ht="102" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A99" s="44" t="str">
-        <f>IF(H99&lt;&gt;"",IF(F99&lt;&gt;"",CONCATENATE("...",D99,".",E99,".",F99,". - ",T99),IF(E99&lt;&gt;"",CONCATENATE("..",D99,".",E99,". - ",T99),CONCATENATE(D99,". - ",T99))),"")</f>
-        <v>..B.15. - Brain and nervous system cancers</v>
+        <f t="shared" si="5"/>
+        <v>...B.15. - Brain and nervous system cancers</v>
       </c>
       <c r="B99" s="2">
         <v>92</v>
@@ -11173,7 +11173,7 @@
       </c>
       <c r="F99" s="6"/>
       <c r="G99" s="40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>cB15</v>
       </c>
       <c r="H99" s="40" t="str">
@@ -11223,7 +11223,7 @@
     </row>
     <row r="100" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A100" s="44" t="str">
-        <f>IF(H100&lt;&gt;"",IF(F100&lt;&gt;"",CONCATENATE("...",D100,".",E100,".",F100,". - ",T100),IF(E100&lt;&gt;"",CONCATENATE("..",D100,".",E100,". - ",T100),CONCATENATE(D100,". - ",T100))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B100" s="2">
@@ -11240,7 +11240,7 @@
       </c>
       <c r="F100" s="6"/>
       <c r="G100" s="40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>cB99</v>
       </c>
       <c r="H100" s="40"/>
@@ -11287,7 +11287,7 @@
     </row>
     <row r="101" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A101" s="44" t="str">
-        <f>IF(H101&lt;&gt;"",IF(F101&lt;&gt;"",CONCATENATE("...",D101,".",E101,".",F101,". - ",T101),IF(E101&lt;&gt;"",CONCATENATE("..",D101,".",E101,". - ",T101),CONCATENATE(D101,". - ",T101))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B101" s="2">
@@ -11304,7 +11304,7 @@
       </c>
       <c r="F101" s="6"/>
       <c r="G101" s="40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>cB99</v>
       </c>
       <c r="H101" s="40"/>
@@ -11351,7 +11351,7 @@
     </row>
     <row r="102" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A102" s="44" t="str">
-        <f>IF(H102&lt;&gt;"",IF(F102&lt;&gt;"",CONCATENATE("...",D102,".",E102,".",F102,". - ",T102),IF(E102&lt;&gt;"",CONCATENATE("..",D102,".",E102,". - ",T102),CONCATENATE(D102,". - ",T102))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B102" s="2">
@@ -11368,7 +11368,7 @@
       </c>
       <c r="F102" s="6"/>
       <c r="G102" s="40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>cB99</v>
       </c>
       <c r="H102" s="40"/>
@@ -11415,7 +11415,7 @@
     </row>
     <row r="103" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A103" s="44" t="str">
-        <f>IF(H103&lt;&gt;"",IF(F103&lt;&gt;"",CONCATENATE("...",D103,".",E103,".",F103,". - ",T103),IF(E103&lt;&gt;"",CONCATENATE("..",D103,".",E103,". - ",T103),CONCATENATE(D103,". - ",T103))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B103" s="2">
@@ -11432,7 +11432,7 @@
       </c>
       <c r="F103" s="6"/>
       <c r="G103" s="40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>cB99</v>
       </c>
       <c r="H103" s="40"/>
@@ -11473,10 +11473,10 @@
       </c>
       <c r="X103" s="2"/>
     </row>
-    <row r="104" spans="1:24" ht="102" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A104" s="44" t="str">
-        <f>IF(H104&lt;&gt;"",IF(F104&lt;&gt;"",CONCATENATE("...",D104,".",E104,".",F104,". - ",T104),IF(E104&lt;&gt;"",CONCATENATE("..",D104,".",E104,". - ",T104),CONCATENATE(D104,". - ",T104))),"")</f>
-        <v>..B.16. - Lymphomas and multiple myeloma</v>
+        <f t="shared" si="5"/>
+        <v>...B.16. - Lymphomas and multiple myeloma</v>
       </c>
       <c r="B104" s="2">
         <v>97</v>
@@ -11493,7 +11493,7 @@
       <c r="F104" s="6"/>
       <c r="G104" s="40"/>
       <c r="H104" s="40" t="str">
-        <f t="shared" ref="H104:H109" si="7">CONCATENATE(D104,E104,F104)</f>
+        <f t="shared" ref="H104:H109" si="9">CONCATENATE(D104,E104,F104)</f>
         <v>B16</v>
       </c>
       <c r="I104" s="5"/>
@@ -11533,10 +11533,10 @@
       </c>
       <c r="X104" s="2"/>
     </row>
-    <row r="105" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A105" s="44" t="str">
-        <f>IF(H105&lt;&gt;"",IF(F105&lt;&gt;"",CONCATENATE("...",D105,".",E105,".",F105,". - ",T105),IF(E105&lt;&gt;"",CONCATENATE("..",D105,".",E105,". - ",T105),CONCATENATE(D105,". - ",T105))),"")</f>
-        <v>...B.16.a. - Hodgkin lymphoma</v>
+        <f t="shared" si="5"/>
+        <v>....B.16.a. - Hodgkin lymphoma</v>
       </c>
       <c r="B105" s="2">
         <v>98</v>
@@ -11554,11 +11554,11 @@
         <v>1126</v>
       </c>
       <c r="G105" s="40" t="str">
-        <f t="shared" ref="G105:G111" si="8">CONCATENATE("c",D105,E105,F105)</f>
+        <f t="shared" ref="G105:G111" si="10">CONCATENATE("c",D105,E105,F105)</f>
         <v>cB16a</v>
       </c>
       <c r="H105" s="40" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>B16a</v>
       </c>
       <c r="I105" s="5"/>
@@ -11598,10 +11598,10 @@
       </c>
       <c r="X105" s="2"/>
     </row>
-    <row r="106" spans="1:24" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A106" s="44" t="str">
-        <f>IF(H106&lt;&gt;"",IF(F106&lt;&gt;"",CONCATENATE("...",D106,".",E106,".",F106,". - ",T106),IF(E106&lt;&gt;"",CONCATENATE("..",D106,".",E106,". - ",T106),CONCATENATE(D106,". - ",T106))),"")</f>
-        <v>...B.16.b. - Non-Hodgkin lymphoma</v>
+        <f t="shared" si="5"/>
+        <v>....B.16.b. - Non-Hodgkin lymphoma</v>
       </c>
       <c r="B106" s="2">
         <v>99</v>
@@ -11619,11 +11619,11 @@
         <v>1127</v>
       </c>
       <c r="G106" s="40" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>cB16b</v>
       </c>
       <c r="H106" s="40" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>B16b</v>
       </c>
       <c r="I106" s="5"/>
@@ -11663,10 +11663,10 @@
       </c>
       <c r="X106" s="2"/>
     </row>
-    <row r="107" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A107" s="44" t="str">
-        <f>IF(H107&lt;&gt;"",IF(F107&lt;&gt;"",CONCATENATE("...",D107,".",E107,".",F107,". - ",T107),IF(E107&lt;&gt;"",CONCATENATE("..",D107,".",E107,". - ",T107),CONCATENATE(D107,". - ",T107))),"")</f>
-        <v>...B.16.c. - Multiple myeloma</v>
+        <f t="shared" si="5"/>
+        <v>....B.16.c. - Multiple myeloma</v>
       </c>
       <c r="B107" s="2">
         <v>100</v>
@@ -11684,11 +11684,11 @@
         <v>1130</v>
       </c>
       <c r="G107" s="40" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>cB16c</v>
       </c>
       <c r="H107" s="40" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>B16c</v>
       </c>
       <c r="I107" s="5"/>
@@ -11728,10 +11728,10 @@
       </c>
       <c r="X107" s="2"/>
     </row>
-    <row r="108" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A108" s="44" t="str">
-        <f>IF(H108&lt;&gt;"",IF(F108&lt;&gt;"",CONCATENATE("...",D108,".",E108,".",F108,". - ",T108),IF(E108&lt;&gt;"",CONCATENATE("..",D108,".",E108,". - ",T108),CONCATENATE(D108,". - ",T108))),"")</f>
-        <v>..B.17. - Leukaemia</v>
+        <f t="shared" si="5"/>
+        <v>...B.17. - Leukaemia</v>
       </c>
       <c r="B108" s="2">
         <v>101</v>
@@ -11747,11 +11747,11 @@
       </c>
       <c r="F108" s="6"/>
       <c r="G108" s="40" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>cB17</v>
       </c>
       <c r="H108" s="40" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>B17</v>
       </c>
       <c r="I108" s="5"/>
@@ -11791,10 +11791,10 @@
       </c>
       <c r="X108" s="2"/>
     </row>
-    <row r="109" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:24" ht="51" x14ac:dyDescent="0.25">
       <c r="A109" s="44" t="str">
-        <f>IF(H109&lt;&gt;"",IF(F109&lt;&gt;"",CONCATENATE("...",D109,".",E109,".",F109,". - ",T109),IF(E109&lt;&gt;"",CONCATENATE("..",D109,".",E109,". - ",T109),CONCATENATE(D109,". - ",T109))),"")</f>
-        <v>..B.99. - Other malignant neoplasms</v>
+        <f t="shared" si="5"/>
+        <v>...B.99. - Other malignant neoplasms</v>
       </c>
       <c r="B109" s="2">
         <v>102</v>
@@ -11810,11 +11810,11 @@
       </c>
       <c r="F109" s="6"/>
       <c r="G109" s="40" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>cB99</v>
       </c>
       <c r="H109" s="40" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>B99</v>
       </c>
       <c r="I109" s="5" t="s">
@@ -11856,7 +11856,7 @@
     </row>
     <row r="110" spans="1:24" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A110" s="44" t="str">
-        <f>IF(H110&lt;&gt;"",IF(F110&lt;&gt;"",CONCATENATE("...",D110,".",E110,".",F110,". - ",T110),IF(E110&lt;&gt;"",CONCATENATE("..",D110,".",E110,". - ",T110),CONCATENATE(D110,". - ",T110))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B110" s="2">
@@ -11873,7 +11873,7 @@
       </c>
       <c r="F110" s="6"/>
       <c r="G110" s="40" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>cD99</v>
       </c>
       <c r="H110" s="40"/>
@@ -11914,8 +11914,8 @@
     </row>
     <row r="111" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A111" s="44" t="str">
-        <f>IF(H111&lt;&gt;"",IF(F111&lt;&gt;"",CONCATENATE("...",D111,".",E111,".",F111,". - ",T111),IF(E111&lt;&gt;"",CONCATENATE("..",D111,".",E111,". - ",T111),CONCATENATE(D111,". - ",T111))),"")</f>
-        <v>..D.01. - Diabetes mellitus</v>
+        <f t="shared" si="5"/>
+        <v>...D.01. - Diabetes mellitus</v>
       </c>
       <c r="B111" s="2">
         <v>104</v>
@@ -11931,7 +11931,7 @@
       </c>
       <c r="F111" s="6"/>
       <c r="G111" s="40" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>cD01</v>
       </c>
       <c r="H111" s="40" t="str">
@@ -11985,10 +11985,10 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="112" spans="1:24" ht="102" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A112" s="44" t="str">
-        <f>IF(H112&lt;&gt;"",IF(F112&lt;&gt;"",CONCATENATE("...",D112,".",E112,".",F112,". - ",T112),IF(E112&lt;&gt;"",CONCATENATE("..",D112,".",E112,". - ",T112),CONCATENATE(D112,". - ",T112))),"")</f>
-        <v>..D.02. - Endocrine, blood, immune disorders</v>
+        <f t="shared" si="5"/>
+        <v>...D.02. - Endocrine, blood, immune disorders</v>
       </c>
       <c r="B112" s="2">
         <v>105</v>
@@ -12049,7 +12049,7 @@
     </row>
     <row r="113" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A113" s="44" t="str">
-        <f>IF(H113&lt;&gt;"",IF(F113&lt;&gt;"",CONCATENATE("...",D113,".",E113,".",F113,". - ",T113),IF(E113&lt;&gt;"",CONCATENATE("..",D113,".",E113,". - ",T113),CONCATENATE(D113,". - ",T113))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B113" s="2">
@@ -12109,7 +12109,7 @@
     </row>
     <row r="114" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A114" s="44" t="str">
-        <f>IF(H114&lt;&gt;"",IF(F114&lt;&gt;"",CONCATENATE("...",D114,".",E114,".",F114,". - ",T114),IF(E114&lt;&gt;"",CONCATENATE("..",D114,".",E114,". - ",T114),CONCATENATE(D114,". - ",T114))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B114" s="2">
@@ -12169,7 +12169,7 @@
     </row>
     <row r="115" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A115" s="44" t="str">
-        <f>IF(H115&lt;&gt;"",IF(F115&lt;&gt;"",CONCATENATE("...",D115,".",E115,".",F115,". - ",T115),IF(E115&lt;&gt;"",CONCATENATE("..",D115,".",E115,". - ",T115),CONCATENATE(D115,". - ",T115))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B115" s="2">
@@ -12229,7 +12229,7 @@
     </row>
     <row r="116" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A116" s="44" t="str">
-        <f>IF(H116&lt;&gt;"",IF(F116&lt;&gt;"",CONCATENATE("...",D116,".",E116,".",F116,". - ",T116),IF(E116&lt;&gt;"",CONCATENATE("..",D116,".",E116,". - ",T116),CONCATENATE(D116,". - ",T116))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B116" s="2">
@@ -12289,7 +12289,7 @@
     </row>
     <row r="117" spans="1:24" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A117" s="44" t="str">
-        <f>IF(H117&lt;&gt;"",IF(F117&lt;&gt;"",CONCATENATE("...",D117,".",E117,".",F117,". - ",T117),IF(E117&lt;&gt;"",CONCATENATE("..",D117,".",E117,". - ",T117),CONCATENATE(D117,". - ",T117))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B117" s="2">
@@ -12346,10 +12346,10 @@
       </c>
       <c r="X117" s="2"/>
     </row>
-    <row r="118" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A118" s="44" t="str">
-        <f>IF(H118&lt;&gt;"",IF(F118&lt;&gt;"",CONCATENATE("...",D118,".",E118,".",F118,". - ",T118),IF(E118&lt;&gt;"",CONCATENATE("..",D118,".",E118,". - ",T118),CONCATENATE(D118,". - ",T118))),"")</f>
-        <v xml:space="preserve">..D.03. - Mental Health disorders </v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">...D.03. - Mental Health disorders </v>
       </c>
       <c r="B118" s="2"/>
       <c r="C118" s="32" t="s">
@@ -12390,10 +12390,10 @@
       <c r="W118" s="45"/>
       <c r="X118" s="2"/>
     </row>
-    <row r="119" spans="1:24" ht="51" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A119" s="44" t="str">
-        <f>IF(H119&lt;&gt;"",IF(F119&lt;&gt;"",CONCATENATE("...",D119,".",E119,".",F119,". - ",T119),IF(E119&lt;&gt;"",CONCATENATE("..",D119,".",E119,". - ",T119),CONCATENATE(D119,". - ",T119))),"")</f>
-        <v xml:space="preserve">..D.04. - Substance use </v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">...D.04. - Substance use </v>
       </c>
       <c r="B119" s="2"/>
       <c r="C119" s="32" t="s">
@@ -12434,7 +12434,7 @@
     </row>
     <row r="120" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A120" s="44" t="str">
-        <f>IF(H120&lt;&gt;"",IF(F120&lt;&gt;"",CONCATENATE("...",D120,".",E120,".",F120,". - ",T120),IF(E120&lt;&gt;"",CONCATENATE("..",D120,".",E120,". - ",T120),CONCATENATE(D120,". - ",T120))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B120" s="2"/>
@@ -12465,7 +12465,7 @@
     </row>
     <row r="121" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A121" s="44" t="str">
-        <f>IF(H121&lt;&gt;"",IF(F121&lt;&gt;"",CONCATENATE("...",D121,".",E121,".",F121,". - ",T121),IF(E121&lt;&gt;"",CONCATENATE("..",D121,".",E121,". - ",T121),CONCATENATE(D121,". - ",T121))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B121" s="2">
@@ -12514,7 +12514,7 @@
     </row>
     <row r="122" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A122" s="44" t="str">
-        <f>IF(H122&lt;&gt;"",IF(F122&lt;&gt;"",CONCATENATE("...",D122,".",E122,".",F122,". - ",T122),IF(E122&lt;&gt;"",CONCATENATE("..",D122,".",E122,". - ",T122),CONCATENATE(D122,". - ",T122))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B122" s="2">
@@ -12574,7 +12574,7 @@
     </row>
     <row r="123" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A123" s="44" t="str">
-        <f>IF(H123&lt;&gt;"",IF(F123&lt;&gt;"",CONCATENATE("...",D123,".",E123,".",F123,". - ",T123),IF(E123&lt;&gt;"",CONCATENATE("..",D123,".",E123,". - ",T123),CONCATENATE(D123,". - ",T123))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B123" s="2">
@@ -12634,7 +12634,7 @@
     </row>
     <row r="124" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A124" s="44" t="str">
-        <f>IF(H124&lt;&gt;"",IF(F124&lt;&gt;"",CONCATENATE("...",D124,".",E124,".",F124,". - ",T124),IF(E124&lt;&gt;"",CONCATENATE("..",D124,".",E124,". - ",T124),CONCATENATE(D124,". - ",T124))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B124" s="2">
@@ -12694,7 +12694,7 @@
     </row>
     <row r="125" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A125" s="44" t="str">
-        <f>IF(H125&lt;&gt;"",IF(F125&lt;&gt;"",CONCATENATE("...",D125,".",E125,".",F125,". - ",T125),IF(E125&lt;&gt;"",CONCATENATE("..",D125,".",E125,". - ",T125),CONCATENATE(D125,". - ",T125))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B125" s="2">
@@ -12756,10 +12756,10 @@
       </c>
       <c r="X125" s="2"/>
     </row>
-    <row r="126" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A126" s="44" t="str">
-        <f>IF(H126&lt;&gt;"",IF(F126&lt;&gt;"",CONCATENATE("...",D126,".",E126,".",F126,". - ",T126),IF(E126&lt;&gt;"",CONCATENATE("..",D126,".",E126,". - ",T126),CONCATENATE(D126,". - ",T126))),"")</f>
-        <v>...D.04.a. - Alcohol use disorders</v>
+        <f t="shared" si="5"/>
+        <v>....D.04.a. - Alcohol use disorders</v>
       </c>
       <c r="B126" s="2">
         <v>116</v>
@@ -12827,7 +12827,7 @@
     </row>
     <row r="127" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A127" s="44" t="str">
-        <f>IF(H127&lt;&gt;"",IF(F127&lt;&gt;"",CONCATENATE("...",D127,".",E127,".",F127,". - ",T127),IF(E127&lt;&gt;"",CONCATENATE("..",D127,".",E127,". - ",T127),CONCATENATE(D127,". - ",T127))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B127" s="2">
@@ -12878,10 +12878,10 @@
       </c>
       <c r="X127" s="2"/>
     </row>
-    <row r="128" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A128" s="44" t="str">
-        <f>IF(H128&lt;&gt;"",IF(F128&lt;&gt;"",CONCATENATE("...",D128,".",E128,".",F128,". - ",T128),IF(E128&lt;&gt;"",CONCATENATE("..",D128,".",E128,". - ",T128),CONCATENATE(D128,". - ",T128))),"")</f>
-        <v>...D.04.b. - Opioid use disorders</v>
+        <f t="shared" si="5"/>
+        <v>....D.04.b. - Opioid use disorders</v>
       </c>
       <c r="B128" s="2">
         <v>118</v>
@@ -12899,7 +12899,7 @@
         <v>1127</v>
       </c>
       <c r="G128" s="40" t="str">
-        <f t="shared" ref="G128:G135" si="9">CONCATENATE("c",D128,E128,F128)</f>
+        <f t="shared" ref="G128:G135" si="11">CONCATENATE("c",D128,E128,F128)</f>
         <v>cD04b</v>
       </c>
       <c r="H128" s="40" t="str">
@@ -12943,10 +12943,10 @@
       </c>
       <c r="X128" s="2"/>
     </row>
-    <row r="129" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A129" s="44" t="str">
-        <f>IF(H129&lt;&gt;"",IF(F129&lt;&gt;"",CONCATENATE("...",D129,".",E129,".",F129,". - ",T129),IF(E129&lt;&gt;"",CONCATENATE("..",D129,".",E129,". - ",T129),CONCATENATE(D129,". - ",T129))),"")</f>
-        <v>...D.04.c. - Cocaine use disorders</v>
+        <f t="shared" si="5"/>
+        <v>....D.04.c. - Cocaine use disorders</v>
       </c>
       <c r="B129" s="2">
         <v>119</v>
@@ -12964,7 +12964,7 @@
         <v>1130</v>
       </c>
       <c r="G129" s="40" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>cD04c</v>
       </c>
       <c r="H129" s="40" t="str">
@@ -13008,10 +13008,10 @@
       </c>
       <c r="X129" s="2"/>
     </row>
-    <row r="130" spans="1:24" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A130" s="44" t="str">
-        <f>IF(H130&lt;&gt;"",IF(F130&lt;&gt;"",CONCATENATE("...",D130,".",E130,".",F130,". - ",T130),IF(E130&lt;&gt;"",CONCATENATE("..",D130,".",E130,". - ",T130),CONCATENATE(D130,". - ",T130))),"")</f>
-        <v>...D.04.d. - Amphetamine use disorders</v>
+        <f t="shared" si="5"/>
+        <v>....D.04.d. - Amphetamine use disorders</v>
       </c>
       <c r="B130" s="2">
         <v>120</v>
@@ -13029,7 +13029,7 @@
         <v>1154</v>
       </c>
       <c r="G130" s="40" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>cD04d</v>
       </c>
       <c r="H130" s="40" t="str">
@@ -13075,7 +13075,7 @@
     </row>
     <row r="131" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A131" s="44" t="str">
-        <f>IF(H131&lt;&gt;"",IF(F131&lt;&gt;"",CONCATENATE("...",D131,".",E131,".",F131,". - ",T131),IF(E131&lt;&gt;"",CONCATENATE("..",D131,".",E131,". - ",T131),CONCATENATE(D131,". - ",T131))),"")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="B131" s="2">
@@ -13092,7 +13092,7 @@
       </c>
       <c r="F131" s="6"/>
       <c r="G131" s="40" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>cD04</v>
       </c>
       <c r="H131" s="40"/>
@@ -13130,7 +13130,7 @@
     </row>
     <row r="132" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A132" s="44" t="str">
-        <f>IF(H132&lt;&gt;"",IF(F132&lt;&gt;"",CONCATENATE("...",D132,".",E132,".",F132,". - ",T132),IF(E132&lt;&gt;"",CONCATENATE("..",D132,".",E132,". - ",T132),CONCATENATE(D132,". - ",T132))),"")</f>
+        <f t="shared" ref="A132:A195" si="12">IF(H132&lt;&gt;"",IF(F132&lt;&gt;"",CONCATENATE("....",D132,".",E132,".",F132,". - ",T132),IF(E132&lt;&gt;"",CONCATENATE("...",D132,".",E132,". - ",T132),CONCATENATE("..",D132,". - ",T132))),"")</f>
         <v/>
       </c>
       <c r="B132" s="2">
@@ -13147,7 +13147,7 @@
       </c>
       <c r="F132" s="6"/>
       <c r="G132" s="40" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>cD04</v>
       </c>
       <c r="H132" s="40"/>
@@ -13196,7 +13196,7 @@
     </row>
     <row r="133" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A133" s="44" t="str">
-        <f>IF(H133&lt;&gt;"",IF(F133&lt;&gt;"",CONCATENATE("...",D133,".",E133,".",F133,". - ",T133),IF(E133&lt;&gt;"",CONCATENATE("..",D133,".",E133,". - ",T133),CONCATENATE(D133,". - ",T133))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B133" s="2">
@@ -13213,7 +13213,7 @@
       </c>
       <c r="F133" s="6"/>
       <c r="G133" s="40" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>cD03</v>
       </c>
       <c r="H133" s="40"/>
@@ -13252,7 +13252,7 @@
     </row>
     <row r="134" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A134" s="44" t="str">
-        <f>IF(H134&lt;&gt;"",IF(F134&lt;&gt;"",CONCATENATE("...",D134,".",E134,".",F134,". - ",T134),IF(E134&lt;&gt;"",CONCATENATE("..",D134,".",E134,". - ",T134),CONCATENATE(D134,". - ",T134))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B134" s="2">
@@ -13269,7 +13269,7 @@
       </c>
       <c r="F134" s="6"/>
       <c r="G134" s="40" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>cD03</v>
       </c>
       <c r="H134" s="40"/>
@@ -13312,7 +13312,7 @@
     </row>
     <row r="135" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A135" s="44" t="str">
-        <f>IF(H135&lt;&gt;"",IF(F135&lt;&gt;"",CONCATENATE("...",D135,".",E135,".",F135,". - ",T135),IF(E135&lt;&gt;"",CONCATENATE("..",D135,".",E135,". - ",T135),CONCATENATE(D135,". - ",T135))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B135" s="2">
@@ -13329,7 +13329,7 @@
       </c>
       <c r="F135" s="6"/>
       <c r="G135" s="40" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>cD03</v>
       </c>
       <c r="H135" s="40"/>
@@ -13368,7 +13368,7 @@
     </row>
     <row r="136" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A136" s="44" t="str">
-        <f>IF(H136&lt;&gt;"",IF(F136&lt;&gt;"",CONCATENATE("...",D136,".",E136,".",F136,". - ",T136),IF(E136&lt;&gt;"",CONCATENATE("..",D136,".",E136,". - ",T136),CONCATENATE(D136,". - ",T136))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B136" s="2">
@@ -13417,7 +13417,7 @@
     </row>
     <row r="137" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A137" s="44" t="str">
-        <f>IF(H137&lt;&gt;"",IF(F137&lt;&gt;"",CONCATENATE("...",D137,".",E137,".",F137,". - ",T137),IF(E137&lt;&gt;"",CONCATENATE("..",D137,".",E137,". - ",T137),CONCATENATE(D137,". - ",T137))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B137" s="2">
@@ -13473,7 +13473,7 @@
     </row>
     <row r="138" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A138" s="44" t="str">
-        <f>IF(H138&lt;&gt;"",IF(F138&lt;&gt;"",CONCATENATE("...",D138,".",E138,".",F138,". - ",T138),IF(E138&lt;&gt;"",CONCATENATE("..",D138,".",E138,". - ",T138),CONCATENATE(D138,". - ",T138))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B138" s="2">
@@ -13529,7 +13529,7 @@
     </row>
     <row r="139" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A139" s="44" t="str">
-        <f>IF(H139&lt;&gt;"",IF(F139&lt;&gt;"",CONCATENATE("...",D139,".",E139,".",F139,". - ",T139),IF(E139&lt;&gt;"",CONCATENATE("..",D139,".",E139,". - ",T139),CONCATENATE(D139,". - ",T139))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B139" s="2">
@@ -13585,7 +13585,7 @@
     </row>
     <row r="140" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A140" s="44" t="str">
-        <f>IF(H140&lt;&gt;"",IF(F140&lt;&gt;"",CONCATENATE("...",D140,".",E140,".",F140,". - ",T140),IF(E140&lt;&gt;"",CONCATENATE("..",D140,".",E140,". - ",T140),CONCATENATE(D140,". - ",T140))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B140" s="2">
@@ -13641,7 +13641,7 @@
     </row>
     <row r="141" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A141" s="44" t="str">
-        <f>IF(H141&lt;&gt;"",IF(F141&lt;&gt;"",CONCATENATE("...",D141,".",E141,".",F141,". - ",T141),IF(E141&lt;&gt;"",CONCATENATE("..",D141,".",E141,". - ",T141),CONCATENATE(D141,". - ",T141))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B141" s="2">
@@ -13698,10 +13698,10 @@
         <v>607</v>
       </c>
     </row>
-    <row r="142" spans="1:24" ht="102" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A142" s="44" t="str">
-        <f>IF(H142&lt;&gt;"",IF(F142&lt;&gt;"",CONCATENATE("...",D142,".",E142,".",F142,". - ",T142),IF(E142&lt;&gt;"",CONCATENATE("..",D142,".",E142,". - ",T142),CONCATENATE(D142,". - ",T142))),"")</f>
-        <v>..D.05. - Alzheimer’s disease and other dementias</v>
+        <f t="shared" si="12"/>
+        <v>...D.05. - Alzheimer’s disease and other dementias</v>
       </c>
       <c r="B142" s="2">
         <v>132</v>
@@ -13717,7 +13717,7 @@
       </c>
       <c r="F142" s="6"/>
       <c r="G142" s="40" t="str">
-        <f t="shared" ref="G142:G148" si="10">CONCATENATE("c",D142,E142,F142)</f>
+        <f t="shared" ref="G142:G148" si="13">CONCATENATE("c",D142,E142,F142)</f>
         <v>cD05</v>
       </c>
       <c r="H142" s="40" t="str">
@@ -13763,7 +13763,7 @@
     </row>
     <row r="143" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A143" s="44" t="str">
-        <f>IF(H143&lt;&gt;"",IF(F143&lt;&gt;"",CONCATENATE("...",D143,".",E143,".",F143,". - ",T143),IF(E143&lt;&gt;"",CONCATENATE("..",D143,".",E143,". - ",T143),CONCATENATE(D143,". - ",T143))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B143" s="2">
@@ -13780,7 +13780,7 @@
       </c>
       <c r="F143" s="6"/>
       <c r="G143" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>cD06</v>
       </c>
       <c r="H143" s="40"/>
@@ -13823,7 +13823,7 @@
     </row>
     <row r="144" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A144" s="44" t="str">
-        <f>IF(H144&lt;&gt;"",IF(F144&lt;&gt;"",CONCATENATE("...",D144,".",E144,".",F144,". - ",T144),IF(E144&lt;&gt;"",CONCATENATE("..",D144,".",E144,". - ",T144),CONCATENATE(D144,". - ",T144))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B144" s="2">
@@ -13840,7 +13840,7 @@
       </c>
       <c r="F144" s="6"/>
       <c r="G144" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>cD06</v>
       </c>
       <c r="H144" s="40"/>
@@ -13883,7 +13883,7 @@
     </row>
     <row r="145" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A145" s="44" t="str">
-        <f>IF(H145&lt;&gt;"",IF(F145&lt;&gt;"",CONCATENATE("...",D145,".",E145,".",F145,". - ",T145),IF(E145&lt;&gt;"",CONCATENATE("..",D145,".",E145,". - ",T145),CONCATENATE(D145,". - ",T145))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B145" s="2">
@@ -13900,7 +13900,7 @@
       </c>
       <c r="F145" s="6"/>
       <c r="G145" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>cD06</v>
       </c>
       <c r="H145" s="40"/>
@@ -13943,7 +13943,7 @@
     </row>
     <row r="146" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A146" s="44" t="str">
-        <f>IF(H146&lt;&gt;"",IF(F146&lt;&gt;"",CONCATENATE("...",D146,".",E146,".",F146,". - ",T146),IF(E146&lt;&gt;"",CONCATENATE("..",D146,".",E146,". - ",T146),CONCATENATE(D146,". - ",T146))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B146" s="2">
@@ -13960,7 +13960,7 @@
       </c>
       <c r="F146" s="6"/>
       <c r="G146" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>cD06</v>
       </c>
       <c r="H146" s="40"/>
@@ -13999,7 +13999,7 @@
     </row>
     <row r="147" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A147" s="44" t="str">
-        <f>IF(H147&lt;&gt;"",IF(F147&lt;&gt;"",CONCATENATE("...",D147,".",E147,".",F147,". - ",T147),IF(E147&lt;&gt;"",CONCATENATE("..",D147,".",E147,". - ",T147),CONCATENATE(D147,". - ",T147))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B147" s="2">
@@ -14016,7 +14016,7 @@
       </c>
       <c r="F147" s="6"/>
       <c r="G147" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>cD06</v>
       </c>
       <c r="H147" s="40"/>
@@ -14053,10 +14053,10 @@
       </c>
       <c r="X147" s="2"/>
     </row>
-    <row r="148" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A148" s="44" t="str">
-        <f>IF(H148&lt;&gt;"",IF(F148&lt;&gt;"",CONCATENATE("...",D148,".",E148,".",F148,". - ",T148),IF(E148&lt;&gt;"",CONCATENATE("..",D148,".",E148,". - ",T148),CONCATENATE(D148,". - ",T148))),"")</f>
-        <v>..D.06. - Other neurological conditions</v>
+        <f t="shared" si="12"/>
+        <v>...D.06. - Other neurological conditions</v>
       </c>
       <c r="B148" s="2">
         <v>138</v>
@@ -14072,7 +14072,7 @@
       </c>
       <c r="F148" s="6"/>
       <c r="G148" s="40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>cD06</v>
       </c>
       <c r="H148" s="40" t="str">
@@ -14122,7 +14122,7 @@
     </row>
     <row r="149" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A149" s="44" t="str">
-        <f>IF(H149&lt;&gt;"",IF(F149&lt;&gt;"",CONCATENATE("...",D149,".",E149,".",F149,". - ",T149),IF(E149&lt;&gt;"",CONCATENATE("..",D149,".",E149,". - ",T149),CONCATENATE(D149,". - ",T149))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B149" s="2">
@@ -14177,7 +14177,7 @@
     </row>
     <row r="150" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A150" s="44" t="str">
-        <f>IF(H150&lt;&gt;"",IF(F150&lt;&gt;"",CONCATENATE("...",D150,".",E150,".",F150,". - ",T150),IF(E150&lt;&gt;"",CONCATENATE("..",D150,".",E150,". - ",T150),CONCATENATE(D150,". - ",T150))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B150" s="2">
@@ -14194,7 +14194,7 @@
       </c>
       <c r="F150" s="6"/>
       <c r="G150" s="40" t="str">
-        <f t="shared" ref="G150:G156" si="11">CONCATENATE("c",D150,E150,F150)</f>
+        <f t="shared" ref="G150:G156" si="14">CONCATENATE("c",D150,E150,F150)</f>
         <v>cD99</v>
       </c>
       <c r="H150" s="40"/>
@@ -14233,7 +14233,7 @@
     </row>
     <row r="151" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A151" s="44" t="str">
-        <f>IF(H151&lt;&gt;"",IF(F151&lt;&gt;"",CONCATENATE("...",D151,".",E151,".",F151,". - ",T151),IF(E151&lt;&gt;"",CONCATENATE("..",D151,".",E151,". - ",T151),CONCATENATE(D151,". - ",T151))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B151" s="2">
@@ -14250,7 +14250,7 @@
       </c>
       <c r="F151" s="6"/>
       <c r="G151" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>cD99</v>
       </c>
       <c r="H151" s="40"/>
@@ -14289,7 +14289,7 @@
     </row>
     <row r="152" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A152" s="44" t="str">
-        <f>IF(H152&lt;&gt;"",IF(F152&lt;&gt;"",CONCATENATE("...",D152,".",E152,".",F152,". - ",T152),IF(E152&lt;&gt;"",CONCATENATE("..",D152,".",E152,". - ",T152),CONCATENATE(D152,". - ",T152))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B152" s="2">
@@ -14306,7 +14306,7 @@
       </c>
       <c r="F152" s="6"/>
       <c r="G152" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>cD99</v>
       </c>
       <c r="H152" s="40"/>
@@ -14345,7 +14345,7 @@
     </row>
     <row r="153" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A153" s="44" t="str">
-        <f>IF(H153&lt;&gt;"",IF(F153&lt;&gt;"",CONCATENATE("...",D153,".",E153,".",F153,". - ",T153),IF(E153&lt;&gt;"",CONCATENATE("..",D153,".",E153,". - ",T153),CONCATENATE(D153,". - ",T153))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B153" s="2">
@@ -14362,7 +14362,7 @@
       </c>
       <c r="F153" s="6"/>
       <c r="G153" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>cD99</v>
       </c>
       <c r="H153" s="40"/>
@@ -14401,7 +14401,7 @@
     </row>
     <row r="154" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A154" s="44" t="str">
-        <f>IF(H154&lt;&gt;"",IF(F154&lt;&gt;"",CONCATENATE("...",D154,".",E154,".",F154,". - ",T154),IF(E154&lt;&gt;"",CONCATENATE("..",D154,".",E154,". - ",T154),CONCATENATE(D154,". - ",T154))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B154" s="2">
@@ -14418,7 +14418,7 @@
       </c>
       <c r="F154" s="6"/>
       <c r="G154" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>cD99</v>
       </c>
       <c r="H154" s="40"/>
@@ -14457,7 +14457,7 @@
     </row>
     <row r="155" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A155" s="44" t="str">
-        <f>IF(H155&lt;&gt;"",IF(F155&lt;&gt;"",CONCATENATE("...",D155,".",E155,".",F155,". - ",T155),IF(E155&lt;&gt;"",CONCATENATE("..",D155,".",E155,". - ",T155),CONCATENATE(D155,". - ",T155))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B155" s="2">
@@ -14474,7 +14474,7 @@
       </c>
       <c r="F155" s="6"/>
       <c r="G155" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>cD99</v>
       </c>
       <c r="H155" s="40"/>
@@ -14513,7 +14513,7 @@
     </row>
     <row r="156" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A156" s="44" t="str">
-        <f>IF(H156&lt;&gt;"",IF(F156&lt;&gt;"",CONCATENATE("...",D156,".",E156,".",F156,". - ",T156),IF(E156&lt;&gt;"",CONCATENATE("..",D156,".",E156,". - ",T156),CONCATENATE(D156,". - ",T156))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B156" s="2">
@@ -14530,7 +14530,7 @@
       </c>
       <c r="F156" s="6"/>
       <c r="G156" s="40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>cD99</v>
       </c>
       <c r="H156" s="40"/>
@@ -14569,10 +14569,10 @@
         <v>615</v>
       </c>
     </row>
-    <row r="157" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:24" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A157" s="44" t="str">
-        <f>IF(H157&lt;&gt;"",IF(F157&lt;&gt;"",CONCATENATE("...",D157,".",E157,".",F157,". - ",T157),IF(E157&lt;&gt;"",CONCATENATE("..",D157,".",E157,". - ",T157),CONCATENATE(D157,". - ",T157))),"")</f>
-        <v>C. - Cardiovascular diseases</v>
+        <f t="shared" si="12"/>
+        <v>..C. - Cardiovascular diseases</v>
       </c>
       <c r="B157" s="2">
         <v>147</v>
@@ -14629,7 +14629,7 @@
     </row>
     <row r="158" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A158" s="44" t="str">
-        <f>IF(H158&lt;&gt;"",IF(F158&lt;&gt;"",CONCATENATE("...",D158,".",E158,".",F158,". - ",T158),IF(E158&lt;&gt;"",CONCATENATE("..",D158,".",E158,". - ",T158),CONCATENATE(D158,". - ",T158))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B158" s="2">
@@ -14646,7 +14646,7 @@
       </c>
       <c r="F158" s="6"/>
       <c r="G158" s="40" t="str">
-        <f t="shared" ref="G158:G164" si="12">CONCATENATE("c",D158,E158,F158)</f>
+        <f t="shared" ref="G158:G164" si="15">CONCATENATE("c",D158,E158,F158)</f>
         <v>cC99</v>
       </c>
       <c r="H158" s="40"/>
@@ -14691,10 +14691,10 @@
       </c>
       <c r="X158" s="2"/>
     </row>
-    <row r="159" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A159" s="44" t="str">
-        <f>IF(H159&lt;&gt;"",IF(F159&lt;&gt;"",CONCATENATE("...",D159,".",E159,".",F159,". - ",T159),IF(E159&lt;&gt;"",CONCATENATE("..",D159,".",E159,". - ",T159),CONCATENATE(D159,". - ",T159))),"")</f>
-        <v>..C.01. - Hypertensive heart disease</v>
+        <f t="shared" si="12"/>
+        <v>...C.01. - Hypertensive heart disease</v>
       </c>
       <c r="B159" s="2">
         <v>149</v>
@@ -14710,11 +14710,11 @@
       </c>
       <c r="F159" s="6"/>
       <c r="G159" s="40" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>cC01</v>
       </c>
       <c r="H159" s="40" t="str">
-        <f t="shared" ref="H159:H164" si="13">CONCATENATE(D159,E159,F159)</f>
+        <f t="shared" ref="H159:H164" si="16">CONCATENATE(D159,E159,F159)</f>
         <v>C01</v>
       </c>
       <c r="I159" s="5"/>
@@ -14758,10 +14758,10 @@
       </c>
       <c r="X159" s="2"/>
     </row>
-    <row r="160" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A160" s="44" t="str">
-        <f>IF(H160&lt;&gt;"",IF(F160&lt;&gt;"",CONCATENATE("...",D160,".",E160,".",F160,". - ",T160),IF(E160&lt;&gt;"",CONCATENATE("..",D160,".",E160,". - ",T160),CONCATENATE(D160,". - ",T160))),"")</f>
-        <v>..C.02. - Ischaemic heart disease</v>
+        <f t="shared" si="12"/>
+        <v>...C.02. - Ischaemic heart disease</v>
       </c>
       <c r="B160" s="2">
         <v>150</v>
@@ -14777,11 +14777,11 @@
       </c>
       <c r="F160" s="6"/>
       <c r="G160" s="40" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>cC02</v>
       </c>
       <c r="H160" s="40" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>C02</v>
       </c>
       <c r="I160" s="5"/>
@@ -14827,8 +14827,8 @@
     </row>
     <row r="161" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A161" s="44" t="str">
-        <f>IF(H161&lt;&gt;"",IF(F161&lt;&gt;"",CONCATENATE("...",D161,".",E161,".",F161,". - ",T161),IF(E161&lt;&gt;"",CONCATENATE("..",D161,".",E161,". - ",T161),CONCATENATE(D161,". - ",T161))),"")</f>
-        <v>..C.03. - Stroke</v>
+        <f t="shared" si="12"/>
+        <v>...C.03. - Stroke</v>
       </c>
       <c r="B161" s="2">
         <v>151</v>
@@ -14844,11 +14844,11 @@
       </c>
       <c r="F161" s="6"/>
       <c r="G161" s="40" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>cC03</v>
       </c>
       <c r="H161" s="40" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>C03</v>
       </c>
       <c r="I161" s="5" t="s">
@@ -14896,10 +14896,10 @@
       </c>
       <c r="X161" s="2"/>
     </row>
-    <row r="162" spans="1:24" ht="102" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A162" s="44" t="str">
-        <f>IF(H162&lt;&gt;"",IF(F162&lt;&gt;"",CONCATENATE("...",D162,".",E162,".",F162,". - ",T162),IF(E162&lt;&gt;"",CONCATENATE("..",D162,".",E162,". - ",T162),CONCATENATE(D162,". - ",T162))),"")</f>
-        <v>..C.04. - Cardiomyopathy, myocarditis, endocarditis</v>
+        <f t="shared" si="12"/>
+        <v>...C.04. - Cardiomyopathy, myocarditis, endocarditis</v>
       </c>
       <c r="B162" s="2">
         <v>152</v>
@@ -14915,11 +14915,11 @@
       </c>
       <c r="F162" s="6"/>
       <c r="G162" s="40" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>cC04</v>
       </c>
       <c r="H162" s="40" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>C04</v>
       </c>
       <c r="I162" s="5"/>
@@ -14965,10 +14965,10 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="163" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A163" s="44" t="str">
-        <f>IF(H163&lt;&gt;"",IF(F163&lt;&gt;"",CONCATENATE("...",D163,".",E163,".",F163,". - ",T163),IF(E163&lt;&gt;"",CONCATENATE("..",D163,".",E163,". - ",T163),CONCATENATE(D163,". - ",T163))),"")</f>
-        <v>..C.05. -  Congestive heart failure</v>
+        <f t="shared" si="12"/>
+        <v>...C.05. -  Congestive heart failure</v>
       </c>
       <c r="B163" s="2"/>
       <c r="C163" s="36"/>
@@ -14980,11 +14980,11 @@
       </c>
       <c r="F163" s="6"/>
       <c r="G163" s="40" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>cC05</v>
       </c>
       <c r="H163" s="40" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>C05</v>
       </c>
       <c r="I163" s="5" t="s">
@@ -15018,10 +15018,10 @@
       <c r="W163" s="51"/>
       <c r="X163" s="2"/>
     </row>
-    <row r="164" spans="1:24" ht="127.5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A164" s="44" t="str">
-        <f>IF(H164&lt;&gt;"",IF(F164&lt;&gt;"",CONCATENATE("...",D164,".",E164,".",F164,". - ",T164),IF(E164&lt;&gt;"",CONCATENATE("..",D164,".",E164,". - ",T164),CONCATENATE(D164,". - ",T164))),"")</f>
-        <v>..C.99. - Other or unspecified cardiovascular diseases</v>
+        <f t="shared" si="12"/>
+        <v>...C.99. - Other or unspecified cardiovascular diseases</v>
       </c>
       <c r="B164" s="2">
         <v>153</v>
@@ -15037,11 +15037,11 @@
       </c>
       <c r="F164" s="6"/>
       <c r="G164" s="40" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>cC99</v>
       </c>
       <c r="H164" s="40" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>C99</v>
       </c>
       <c r="I164" s="5" t="s">
@@ -15093,7 +15093,7 @@
     </row>
     <row r="165" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A165" s="44" t="str">
-        <f>IF(H165&lt;&gt;"",IF(F165&lt;&gt;"",CONCATENATE("...",D165,".",E165,".",F165,". - ",T165),IF(E165&lt;&gt;"",CONCATENATE("..",D165,".",E165,". - ",T165),CONCATENATE(D165,". - ",T165))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B165" s="2">
@@ -15148,10 +15148,10 @@
       </c>
       <c r="X165" s="2"/>
     </row>
-    <row r="166" spans="1:24" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A166" s="44" t="str">
-        <f>IF(H166&lt;&gt;"",IF(F166&lt;&gt;"",CONCATENATE("...",D166,".",E166,".",F166,". - ",T166),IF(E166&lt;&gt;"",CONCATENATE("..",D166,".",E166,". - ",T166),CONCATENATE(D166,". - ",T166))),"")</f>
-        <v>..D.66. - Chronic obstructive pulmonary disease</v>
+        <f t="shared" si="12"/>
+        <v>...D.66. - Chronic obstructive pulmonary disease</v>
       </c>
       <c r="B166" s="2">
         <v>155</v>
@@ -15211,10 +15211,10 @@
       </c>
       <c r="X166" s="2"/>
     </row>
-    <row r="167" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A167" s="44" t="str">
-        <f>IF(H167&lt;&gt;"",IF(F167&lt;&gt;"",CONCATENATE("...",D167,".",E167,".",F167,". - ",T167),IF(E167&lt;&gt;"",CONCATENATE("..",D167,".",E167,". - ",T167),CONCATENATE(D167,". - ",T167))),"")</f>
-        <v>..D.67. - Asthma</v>
+        <f t="shared" si="12"/>
+        <v>...D.67. - Asthma</v>
       </c>
       <c r="B167" s="2">
         <v>156</v>
@@ -15274,10 +15274,10 @@
       </c>
       <c r="X167" s="2"/>
     </row>
-    <row r="168" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A168" s="44" t="str">
-        <f>IF(H168&lt;&gt;"",IF(F168&lt;&gt;"",CONCATENATE("...",D168,".",E168,".",F168,". - ",T168),IF(E168&lt;&gt;"",CONCATENATE("..",D168,".",E168,". - ",T168),CONCATENATE(D168,". - ",T168))),"")</f>
-        <v>..D.68. - Other respiratory diseases</v>
+        <f t="shared" si="12"/>
+        <v>...D.68. - Other respiratory diseases</v>
       </c>
       <c r="B168" s="2">
         <v>157</v>
@@ -15337,10 +15337,10 @@
       </c>
       <c r="X168" s="2"/>
     </row>
-    <row r="169" spans="1:24" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:24" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A169" s="44" t="str">
-        <f>IF(H169&lt;&gt;"",IF(F169&lt;&gt;"",CONCATENATE("...",D169,".",E169,".",F169,". - ",T169),IF(E169&lt;&gt;"",CONCATENATE("..",D169,".",E169,". - ",T169),CONCATENATE(D169,". - ",T169))),"")</f>
-        <v>..D.09. - Digestive diseases (excluding cirrhosis)</v>
+        <f t="shared" si="12"/>
+        <v>...D.09. - Digestive diseases (excluding cirrhosis)</v>
       </c>
       <c r="B169" s="2">
         <v>158</v>
@@ -15401,7 +15401,7 @@
     </row>
     <row r="170" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A170" s="44" t="str">
-        <f>IF(H170&lt;&gt;"",IF(F170&lt;&gt;"",CONCATENATE("...",D170,".",E170,".",F170,". - ",T170),IF(E170&lt;&gt;"",CONCATENATE("..",D170,".",E170,". - ",T170),CONCATENATE(D170,". - ",T170))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B170" s="2">
@@ -15418,7 +15418,7 @@
       </c>
       <c r="F170" s="6"/>
       <c r="G170" s="40" t="str">
-        <f t="shared" ref="G170:G178" si="14">CONCATENATE("c",D170,E170,F170)</f>
+        <f t="shared" ref="G170:G178" si="17">CONCATENATE("c",D170,E170,F170)</f>
         <v>cD09</v>
       </c>
       <c r="H170" s="40"/>
@@ -15459,10 +15459,10 @@
       </c>
       <c r="X170" s="2"/>
     </row>
-    <row r="171" spans="1:24" s="48" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:24" s="48" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A171" s="44" t="str">
-        <f>IF(H171&lt;&gt;"",IF(F171&lt;&gt;"",CONCATENATE("...",D171,".",E171,".",F171,". - ",T171),IF(E171&lt;&gt;"",CONCATENATE("..",D171,".",E171,". - ",T171),CONCATENATE(D171,". - ",T171))),"")</f>
-        <v>..D.11. - Cirrhosis of the liver</v>
+        <f t="shared" si="12"/>
+        <v>...D.11. - Cirrhosis of the liver</v>
       </c>
       <c r="B171" s="2">
         <v>160</v>
@@ -15478,7 +15478,7 @@
       </c>
       <c r="F171" s="6"/>
       <c r="G171" s="40" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>cD11</v>
       </c>
       <c r="H171" s="40" t="str">
@@ -15528,7 +15528,7 @@
     </row>
     <row r="172" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A172" s="44" t="str">
-        <f>IF(H172&lt;&gt;"",IF(F172&lt;&gt;"",CONCATENATE("...",D172,".",E172,".",F172,". - ",T172),IF(E172&lt;&gt;"",CONCATENATE("..",D172,".",E172,". - ",T172),CONCATENATE(D172,". - ",T172))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B172" s="2">
@@ -15545,7 +15545,7 @@
       </c>
       <c r="F172" s="6"/>
       <c r="G172" s="40" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>cD09</v>
       </c>
       <c r="H172" s="40"/>
@@ -15588,7 +15588,7 @@
     </row>
     <row r="173" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A173" s="44" t="str">
-        <f>IF(H173&lt;&gt;"",IF(F173&lt;&gt;"",CONCATENATE("...",D173,".",E173,".",F173,". - ",T173),IF(E173&lt;&gt;"",CONCATENATE("..",D173,".",E173,". - ",T173),CONCATENATE(D173,". - ",T173))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B173" s="2">
@@ -15605,7 +15605,7 @@
       </c>
       <c r="F173" s="6"/>
       <c r="G173" s="40" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>cD09</v>
       </c>
       <c r="H173" s="40"/>
@@ -15646,9 +15646,9 @@
       </c>
       <c r="X173" s="2"/>
     </row>
-    <row r="174" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A174" s="44" t="str">
-        <f>IF(H174&lt;&gt;"",IF(F174&lt;&gt;"",CONCATENATE("...",D174,".",E174,".",F174,". - ",T174),IF(E174&lt;&gt;"",CONCATENATE("..",D174,".",E174,". - ",T174),CONCATENATE(D174,". - ",T174))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B174" s="2">
@@ -15665,7 +15665,7 @@
       </c>
       <c r="F174" s="6"/>
       <c r="G174" s="40" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>cD09</v>
       </c>
       <c r="H174" s="40"/>
@@ -15708,7 +15708,7 @@
     </row>
     <row r="175" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A175" s="44" t="str">
-        <f>IF(H175&lt;&gt;"",IF(F175&lt;&gt;"",CONCATENATE("...",D175,".",E175,".",F175,". - ",T175),IF(E175&lt;&gt;"",CONCATENATE("..",D175,".",E175,". - ",T175),CONCATENATE(D175,". - ",T175))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B175" s="2">
@@ -15725,7 +15725,7 @@
       </c>
       <c r="F175" s="6"/>
       <c r="G175" s="40" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>cD09</v>
       </c>
       <c r="H175" s="40"/>
@@ -15768,7 +15768,7 @@
     </row>
     <row r="176" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A176" s="44" t="str">
-        <f>IF(H176&lt;&gt;"",IF(F176&lt;&gt;"",CONCATENATE("...",D176,".",E176,".",F176,". - ",T176),IF(E176&lt;&gt;"",CONCATENATE("..",D176,".",E176,". - ",T176),CONCATENATE(D176,". - ",T176))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B176" s="2">
@@ -15785,7 +15785,7 @@
       </c>
       <c r="F176" s="6"/>
       <c r="G176" s="40" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>cD09</v>
       </c>
       <c r="H176" s="40"/>
@@ -15828,7 +15828,7 @@
     </row>
     <row r="177" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A177" s="44" t="str">
-        <f>IF(H177&lt;&gt;"",IF(F177&lt;&gt;"",CONCATENATE("...",D177,".",E177,".",F177,". - ",T177),IF(E177&lt;&gt;"",CONCATENATE("..",D177,".",E177,". - ",T177),CONCATENATE(D177,". - ",T177))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B177" s="2">
@@ -15845,7 +15845,7 @@
       </c>
       <c r="F177" s="6"/>
       <c r="G177" s="40" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>cD09</v>
       </c>
       <c r="H177" s="40"/>
@@ -15886,9 +15886,9 @@
       </c>
       <c r="X177" s="2"/>
     </row>
-    <row r="178" spans="1:24" ht="51" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A178" s="44" t="str">
-        <f>IF(H178&lt;&gt;"",IF(F178&lt;&gt;"",CONCATENATE("...",D178,".",E178,".",F178,". - ",T178),IF(E178&lt;&gt;"",CONCATENATE("..",D178,".",E178,". - ",T178),CONCATENATE(D178,". - ",T178))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B178" s="2">
@@ -15905,7 +15905,7 @@
       </c>
       <c r="F178" s="6"/>
       <c r="G178" s="40" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>cD09</v>
       </c>
       <c r="H178" s="40"/>
@@ -15952,7 +15952,7 @@
     </row>
     <row r="179" spans="1:24" ht="33" x14ac:dyDescent="0.25">
       <c r="A179" s="44" t="str">
-        <f>IF(H179&lt;&gt;"",IF(F179&lt;&gt;"",CONCATENATE("...",D179,".",E179,".",F179,". - ",T179),IF(E179&lt;&gt;"",CONCATENATE("..",D179,".",E179,". - ",T179),CONCATENATE(D179,". - ",T179))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B179" s="2">
@@ -16005,10 +16005,10 @@
       </c>
       <c r="X179" s="2"/>
     </row>
-    <row r="180" spans="1:24" ht="51" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:24" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A180" s="44" t="str">
-        <f>IF(H180&lt;&gt;"",IF(F180&lt;&gt;"",CONCATENATE("...",D180,".",E180,".",F180,". - ",T180),IF(E180&lt;&gt;"",CONCATENATE("..",D180,".",E180,". - ",T180),CONCATENATE(D180,". - ",T180))),"")</f>
-        <v>..D.10. - Kidney diseases</v>
+        <f t="shared" si="12"/>
+        <v>...D.10. - Kidney diseases</v>
       </c>
       <c r="B180" s="2">
         <v>169</v>
@@ -16069,10 +16069,10 @@
       </c>
       <c r="X180" s="2"/>
     </row>
-    <row r="181" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A181" s="44" t="str">
-        <f>IF(H181&lt;&gt;"",IF(F181&lt;&gt;"",CONCATENATE("...",D181,".",E181,".",F181,". - ",T181),IF(E181&lt;&gt;"",CONCATENATE("..",D181,".",E181,". - ",T181),CONCATENATE(D181,". - ",T181))),"")</f>
-        <v>...D.10.a. - Acute glomerulonephritis</v>
+        <f t="shared" si="12"/>
+        <v>....D.10.a. - Acute glomerulonephritis</v>
       </c>
       <c r="B181" s="2">
         <v>170</v>
@@ -16090,7 +16090,7 @@
         <v>1126</v>
       </c>
       <c r="G181" s="40" t="str">
-        <f t="shared" ref="G181:G189" si="15">CONCATENATE("c",D181,E181,F181)</f>
+        <f t="shared" ref="G181:G189" si="18">CONCATENATE("c",D181,E181,F181)</f>
         <v>cD10a</v>
       </c>
       <c r="H181" s="40" t="str">
@@ -16136,10 +16136,10 @@
       </c>
       <c r="X181" s="2"/>
     </row>
-    <row r="182" spans="1:24" ht="127.5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A182" s="44" t="str">
-        <f>IF(H182&lt;&gt;"",IF(F182&lt;&gt;"",CONCATENATE("...",D182,".",E182,".",F182,". - ",T182),IF(E182&lt;&gt;"",CONCATENATE("..",D182,".",E182,". - ",T182),CONCATENATE(D182,". - ",T182))),"")</f>
-        <v>...D.10.b. - Chronic kidney diesease due to diabetes</v>
+        <f t="shared" si="12"/>
+        <v>....D.10.b. - Chronic kidney diesease due to diabetes</v>
       </c>
       <c r="B182" s="2">
         <v>171</v>
@@ -16157,7 +16157,7 @@
         <v>1127</v>
       </c>
       <c r="G182" s="40" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>cD10b</v>
       </c>
       <c r="H182" s="40" t="str">
@@ -16203,10 +16203,10 @@
       </c>
       <c r="X182" s="2"/>
     </row>
-    <row r="183" spans="1:24" ht="102" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A183" s="44" t="str">
-        <f>IF(H183&lt;&gt;"",IF(F183&lt;&gt;"",CONCATENATE("...",D183,".",E183,".",F183,". - ",T183),IF(E183&lt;&gt;"",CONCATENATE("..",D183,".",E183,". - ",T183),CONCATENATE(D183,". - ",T183))),"")</f>
-        <v>...D.10.c. - Other chronic kidney disease</v>
+        <f t="shared" si="12"/>
+        <v>....D.10.c. - Other chronic kidney disease</v>
       </c>
       <c r="B183" s="2">
         <v>172</v>
@@ -16224,7 +16224,7 @@
         <v>1130</v>
       </c>
       <c r="G183" s="40" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>cD10c</v>
       </c>
       <c r="H183" s="40" t="str">
@@ -16272,7 +16272,7 @@
     </row>
     <row r="184" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A184" s="44" t="str">
-        <f>IF(H184&lt;&gt;"",IF(F184&lt;&gt;"",CONCATENATE("...",D184,".",E184,".",F184,". - ",T184),IF(E184&lt;&gt;"",CONCATENATE("..",D184,".",E184,". - ",T184),CONCATENATE(D184,". - ",T184))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B184" s="2">
@@ -16289,7 +16289,7 @@
       </c>
       <c r="F184" s="6"/>
       <c r="G184" s="40" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>cD99</v>
       </c>
       <c r="H184" s="40"/>
@@ -16328,7 +16328,7 @@
     </row>
     <row r="185" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A185" s="44" t="str">
-        <f>IF(H185&lt;&gt;"",IF(F185&lt;&gt;"",CONCATENATE("...",D185,".",E185,".",F185,". - ",T185),IF(E185&lt;&gt;"",CONCATENATE("..",D185,".",E185,". - ",T185),CONCATENATE(D185,". - ",T185))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B185" s="2">
@@ -16345,7 +16345,7 @@
       </c>
       <c r="F185" s="6"/>
       <c r="G185" s="40" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>cD99</v>
       </c>
       <c r="H185" s="40"/>
@@ -16388,7 +16388,7 @@
     </row>
     <row r="186" spans="1:24" ht="33" x14ac:dyDescent="0.25">
       <c r="A186" s="44" t="str">
-        <f>IF(H186&lt;&gt;"",IF(F186&lt;&gt;"",CONCATENATE("...",D186,".",E186,".",F186,". - ",T186),IF(E186&lt;&gt;"",CONCATENATE("..",D186,".",E186,". - ",T186),CONCATENATE(D186,". - ",T186))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B186" s="2">
@@ -16405,7 +16405,7 @@
       </c>
       <c r="F186" s="6"/>
       <c r="G186" s="40" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>cD99</v>
       </c>
       <c r="H186" s="40"/>
@@ -16448,7 +16448,7 @@
     </row>
     <row r="187" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A187" s="44" t="str">
-        <f>IF(H187&lt;&gt;"",IF(F187&lt;&gt;"",CONCATENATE("...",D187,".",E187,".",F187,". - ",T187),IF(E187&lt;&gt;"",CONCATENATE("..",D187,".",E187,". - ",T187),CONCATENATE(D187,". - ",T187))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B187" s="2">
@@ -16465,7 +16465,7 @@
       </c>
       <c r="F187" s="6"/>
       <c r="G187" s="40" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>cD99</v>
       </c>
       <c r="H187" s="40"/>
@@ -16508,7 +16508,7 @@
     </row>
     <row r="188" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A188" s="44" t="str">
-        <f>IF(H188&lt;&gt;"",IF(F188&lt;&gt;"",CONCATENATE("...",D188,".",E188,".",F188,". - ",T188),IF(E188&lt;&gt;"",CONCATENATE("..",D188,".",E188,". - ",T188),CONCATENATE(D188,". - ",T188))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B188" s="2">
@@ -16525,7 +16525,7 @@
       </c>
       <c r="F188" s="6"/>
       <c r="G188" s="40" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>cD99</v>
       </c>
       <c r="H188" s="40"/>
@@ -16568,7 +16568,7 @@
     </row>
     <row r="189" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A189" s="44" t="str">
-        <f>IF(H189&lt;&gt;"",IF(F189&lt;&gt;"",CONCATENATE("...",D189,".",E189,".",F189,". - ",T189),IF(E189&lt;&gt;"",CONCATENATE("..",D189,".",E189,". - ",T189),CONCATENATE(D189,". - ",T189))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B189" s="2">
@@ -16585,7 +16585,7 @@
       </c>
       <c r="F189" s="6"/>
       <c r="G189" s="40" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>cD99</v>
       </c>
       <c r="H189" s="40"/>
@@ -16626,7 +16626,7 @@
     </row>
     <row r="190" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A190" s="44" t="str">
-        <f>IF(H190&lt;&gt;"",IF(F190&lt;&gt;"",CONCATENATE("...",D190,".",E190,".",F190,". - ",T190),IF(E190&lt;&gt;"",CONCATENATE("..",D190,".",E190,". - ",T190),CONCATENATE(D190,". - ",T190))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B190" s="2">
@@ -16685,7 +16685,7 @@
     </row>
     <row r="191" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A191" s="44" t="str">
-        <f>IF(H191&lt;&gt;"",IF(F191&lt;&gt;"",CONCATENATE("...",D191,".",E191,".",F191,". - ",T191),IF(E191&lt;&gt;"",CONCATENATE("..",D191,".",E191,". - ",T191),CONCATENATE(D191,". - ",T191))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B191" s="2">
@@ -16745,7 +16745,7 @@
     </row>
     <row r="192" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A192" s="44" t="str">
-        <f>IF(H192&lt;&gt;"",IF(F192&lt;&gt;"",CONCATENATE("...",D192,".",E192,".",F192,". - ",T192),IF(E192&lt;&gt;"",CONCATENATE("..",D192,".",E192,". - ",T192),CONCATENATE(D192,". - ",T192))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B192" s="2">
@@ -16801,7 +16801,7 @@
     </row>
     <row r="193" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A193" s="44" t="str">
-        <f>IF(H193&lt;&gt;"",IF(F193&lt;&gt;"",CONCATENATE("...",D193,".",E193,".",F193,". - ",T193),IF(E193&lt;&gt;"",CONCATENATE("..",D193,".",E193,". - ",T193),CONCATENATE(D193,". - ",T193))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B193" s="2">
@@ -16857,7 +16857,7 @@
     </row>
     <row r="194" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A194" s="44" t="str">
-        <f>IF(H194&lt;&gt;"",IF(F194&lt;&gt;"",CONCATENATE("...",D194,".",E194,".",F194,". - ",T194),IF(E194&lt;&gt;"",CONCATENATE("..",D194,".",E194,". - ",T194),CONCATENATE(D194,". - ",T194))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B194" s="2">
@@ -16913,7 +16913,7 @@
     </row>
     <row r="195" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A195" s="44" t="str">
-        <f>IF(H195&lt;&gt;"",IF(F195&lt;&gt;"",CONCATENATE("...",D195,".",E195,".",F195,". - ",T195),IF(E195&lt;&gt;"",CONCATENATE("..",D195,".",E195,". - ",T195),CONCATENATE(D195,". - ",T195))),"")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="B195" s="2">
@@ -16975,10 +16975,10 @@
       </c>
       <c r="X195" s="2"/>
     </row>
-    <row r="196" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A196" s="44" t="str">
-        <f>IF(H196&lt;&gt;"",IF(F196&lt;&gt;"",CONCATENATE("...",D196,".",E196,".",F196,". - ",T196),IF(E196&lt;&gt;"",CONCATENATE("..",D196,".",E196,". - ",T196),CONCATENATE(D196,". - ",T196))),"")</f>
-        <v>..D.12. - Congenital anomalies</v>
+        <f t="shared" ref="A196:A232" si="19">IF(H196&lt;&gt;"",IF(F196&lt;&gt;"",CONCATENATE("....",D196,".",E196,".",F196,". - ",T196),IF(E196&lt;&gt;"",CONCATENATE("...",D196,".",E196,". - ",T196),CONCATENATE("..",D196,". - ",T196))),"")</f>
+        <v>...D.12. - Congenital anomalies</v>
       </c>
       <c r="B196" s="2">
         <v>185</v>
@@ -17039,7 +17039,7 @@
     </row>
     <row r="197" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A197" s="44" t="str">
-        <f>IF(H197&lt;&gt;"",IF(F197&lt;&gt;"",CONCATENATE("...",D197,".",E197,".",F197,". - ",T197),IF(E197&lt;&gt;"",CONCATENATE("..",D197,".",E197,". - ",T197),CONCATENATE(D197,". - ",T197))),"")</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B197" s="2">
@@ -17056,7 +17056,7 @@
       </c>
       <c r="F197" s="6"/>
       <c r="G197" s="40" t="str">
-        <f t="shared" ref="G197:G202" si="16">CONCATENATE("c",D197,E197,F197)</f>
+        <f t="shared" ref="G197:G202" si="20">CONCATENATE("c",D197,E197,F197)</f>
         <v>cD12</v>
       </c>
       <c r="H197" s="40"/>
@@ -17099,7 +17099,7 @@
     </row>
     <row r="198" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A198" s="44" t="str">
-        <f>IF(H198&lt;&gt;"",IF(F198&lt;&gt;"",CONCATENATE("...",D198,".",E198,".",F198,". - ",T198),IF(E198&lt;&gt;"",CONCATENATE("..",D198,".",E198,". - ",T198),CONCATENATE(D198,". - ",T198))),"")</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B198" s="2">
@@ -17116,7 +17116,7 @@
       </c>
       <c r="F198" s="6"/>
       <c r="G198" s="40" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>cD12</v>
       </c>
       <c r="H198" s="40"/>
@@ -17159,7 +17159,7 @@
     </row>
     <row r="199" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A199" s="44" t="str">
-        <f>IF(H199&lt;&gt;"",IF(F199&lt;&gt;"",CONCATENATE("...",D199,".",E199,".",F199,". - ",T199),IF(E199&lt;&gt;"",CONCATENATE("..",D199,".",E199,". - ",T199),CONCATENATE(D199,". - ",T199))),"")</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B199" s="2">
@@ -17176,7 +17176,7 @@
       </c>
       <c r="F199" s="6"/>
       <c r="G199" s="40" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>cD12</v>
       </c>
       <c r="H199" s="40"/>
@@ -17219,7 +17219,7 @@
     </row>
     <row r="200" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A200" s="44" t="str">
-        <f>IF(H200&lt;&gt;"",IF(F200&lt;&gt;"",CONCATENATE("...",D200,".",E200,".",F200,". - ",T200),IF(E200&lt;&gt;"",CONCATENATE("..",D200,".",E200,". - ",T200),CONCATENATE(D200,". - ",T200))),"")</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B200" s="2">
@@ -17236,7 +17236,7 @@
       </c>
       <c r="F200" s="6"/>
       <c r="G200" s="40" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>cD12</v>
       </c>
       <c r="H200" s="40"/>
@@ -17279,7 +17279,7 @@
     </row>
     <row r="201" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A201" s="44" t="str">
-        <f>IF(H201&lt;&gt;"",IF(F201&lt;&gt;"",CONCATENATE("...",D201,".",E201,".",F201,". - ",T201),IF(E201&lt;&gt;"",CONCATENATE("..",D201,".",E201,". - ",T201),CONCATENATE(D201,". - ",T201))),"")</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B201" s="2">
@@ -17296,7 +17296,7 @@
       </c>
       <c r="F201" s="6"/>
       <c r="G201" s="40" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>cD12</v>
       </c>
       <c r="H201" s="40"/>
@@ -17339,7 +17339,7 @@
     </row>
     <row r="202" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A202" s="44" t="str">
-        <f>IF(H202&lt;&gt;"",IF(F202&lt;&gt;"",CONCATENATE("...",D202,".",E202,".",F202,". - ",T202),IF(E202&lt;&gt;"",CONCATENATE("..",D202,".",E202,". - ",T202),CONCATENATE(D202,". - ",T202))),"")</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B202" s="2">
@@ -17356,7 +17356,7 @@
       </c>
       <c r="F202" s="6"/>
       <c r="G202" s="40" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>cD12</v>
       </c>
       <c r="H202" s="40"/>
@@ -17399,7 +17399,7 @@
     </row>
     <row r="203" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A203" s="44" t="str">
-        <f>IF(H203&lt;&gt;"",IF(F203&lt;&gt;"",CONCATENATE("...",D203,".",E203,".",F203,". - ",T203),IF(E203&lt;&gt;"",CONCATENATE("..",D203,".",E203,". - ",T203),CONCATENATE(D203,". - ",T203))),"")</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B203" s="2">
@@ -17452,7 +17452,7 @@
     </row>
     <row r="204" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A204" s="44" t="str">
-        <f>IF(H204&lt;&gt;"",IF(F204&lt;&gt;"",CONCATENATE("...",D204,".",E204,".",F204,". - ",T204),IF(E204&lt;&gt;"",CONCATENATE("..",D204,".",E204,". - ",T204),CONCATENATE(D204,". - ",T204))),"")</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B204" s="2">
@@ -17508,7 +17508,7 @@
     </row>
     <row r="205" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A205" s="44" t="str">
-        <f>IF(H205&lt;&gt;"",IF(F205&lt;&gt;"",CONCATENATE("...",D205,".",E205,".",F205,". - ",T205),IF(E205&lt;&gt;"",CONCATENATE("..",D205,".",E205,". - ",T205),CONCATENATE(D205,". - ",T205))),"")</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B205" s="2">
@@ -17564,7 +17564,7 @@
     </row>
     <row r="206" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A206" s="44" t="str">
-        <f>IF(H206&lt;&gt;"",IF(F206&lt;&gt;"",CONCATENATE("...",D206,".",E206,".",F206,". - ",T206),IF(E206&lt;&gt;"",CONCATENATE("..",D206,".",E206,". - ",T206),CONCATENATE(D206,". - ",T206))),"")</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B206" s="2">
@@ -17620,7 +17620,7 @@
     </row>
     <row r="207" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A207" s="44" t="str">
-        <f>IF(H207&lt;&gt;"",IF(F207&lt;&gt;"",CONCATENATE("...",D207,".",E207,".",F207,". - ",T207),IF(E207&lt;&gt;"",CONCATENATE("..",D207,".",E207,". - ",T207),CONCATENATE(D207,". - ",T207))),"")</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B207" s="2">
@@ -17676,8 +17676,8 @@
     </row>
     <row r="208" spans="1:24" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A208" s="44" t="str">
-        <f>IF(H208&lt;&gt;"",IF(F208&lt;&gt;"",CONCATENATE("...",D208,".",E208,".",F208,". - ",T208),IF(E208&lt;&gt;"",CONCATENATE("..",D208,".",E208,". - ",T208),CONCATENATE(D208,". - ",T208))),"")</f>
-        <v>E. - Injuries</v>
+        <f t="shared" si="19"/>
+        <v>..E. - Injuries</v>
       </c>
       <c r="B208" s="2">
         <v>197</v>
@@ -17732,10 +17732,10 @@
       </c>
       <c r="X208" s="2"/>
     </row>
-    <row r="209" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:24" ht="41.25" x14ac:dyDescent="0.25">
       <c r="A209" s="44" t="str">
-        <f>IF(H209&lt;&gt;"",IF(F209&lt;&gt;"",CONCATENATE("...",D209,".",E209,".",F209,". - ",T209),IF(E209&lt;&gt;"",CONCATENATE("..",D209,".",E209,". - ",T209),CONCATENATE(D209,". - ",T209))),"")</f>
-        <v>..E.01. - Unintentional injuries</v>
+        <f t="shared" si="19"/>
+        <v>...E.01. - Unintentional injuries</v>
       </c>
       <c r="B209" s="2">
         <v>198</v>
@@ -17792,10 +17792,10 @@
       </c>
       <c r="X209" s="2"/>
     </row>
-    <row r="210" spans="1:24" ht="51" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:24" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A210" s="44" t="str">
-        <f>IF(H210&lt;&gt;"",IF(F210&lt;&gt;"",CONCATENATE("...",D210,".",E210,".",F210,". - ",T210),IF(E210&lt;&gt;"",CONCATENATE("..",D210,".",E210,". - ",T210),CONCATENATE(D210,". - ",T210))),"")</f>
-        <v>...E.01.a. - Road injury</v>
+        <f t="shared" si="19"/>
+        <v>....E.01.a. - Road injury</v>
       </c>
       <c r="B210" s="2">
         <v>199</v>
@@ -17813,7 +17813,7 @@
         <v>1126</v>
       </c>
       <c r="G210" s="40" t="str">
-        <f t="shared" ref="G210:G219" si="17">CONCATENATE("c",D210,E210,F210)</f>
+        <f t="shared" ref="G210:G219" si="21">CONCATENATE("c",D210,E210,F210)</f>
         <v>cE01a</v>
       </c>
       <c r="H210" s="40" t="str">
@@ -17863,7 +17863,7 @@
     </row>
     <row r="211" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A211" s="44" t="str">
-        <f>IF(H211&lt;&gt;"",IF(F211&lt;&gt;"",CONCATENATE("...",D211,".",E211,".",F211,". - ",T211),IF(E211&lt;&gt;"",CONCATENATE("..",D211,".",E211,". - ",T211),CONCATENATE(D211,". - ",T211))),"")</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B211" s="2">
@@ -17882,7 +17882,7 @@
         <v>1128</v>
       </c>
       <c r="G211" s="40" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>cE01x</v>
       </c>
       <c r="H211" s="40"/>
@@ -17923,10 +17923,10 @@
       </c>
       <c r="X211" s="2"/>
     </row>
-    <row r="212" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A212" s="44" t="str">
-        <f>IF(H212&lt;&gt;"",IF(F212&lt;&gt;"",CONCATENATE("...",D212,".",E212,".",F212,". - ",T212),IF(E212&lt;&gt;"",CONCATENATE("..",D212,".",E212,". - ",T212),CONCATENATE(D212,". - ",T212))),"")</f>
-        <v>...E.01.b. - Falls</v>
+        <f t="shared" si="19"/>
+        <v>....E.01.b. - Falls</v>
       </c>
       <c r="B212" s="2">
         <v>201</v>
@@ -17944,7 +17944,7 @@
         <v>1127</v>
       </c>
       <c r="G212" s="40" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>cE01b</v>
       </c>
       <c r="H212" s="40" t="str">
@@ -17992,7 +17992,7 @@
     </row>
     <row r="213" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A213" s="44" t="str">
-        <f>IF(H213&lt;&gt;"",IF(F213&lt;&gt;"",CONCATENATE("...",D213,".",E213,".",F213,". - ",T213),IF(E213&lt;&gt;"",CONCATENATE("..",D213,".",E213,". - ",T213),CONCATENATE(D213,". - ",T213))),"")</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B213" s="2">
@@ -18011,7 +18011,7 @@
         <v>1128</v>
       </c>
       <c r="G213" s="40" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>cE01x</v>
       </c>
       <c r="H213" s="40"/>
@@ -18052,7 +18052,7 @@
     </row>
     <row r="214" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A214" s="44" t="str">
-        <f>IF(H214&lt;&gt;"",IF(F214&lt;&gt;"",CONCATENATE("...",D214,".",E214,".",F214,". - ",T214),IF(E214&lt;&gt;"",CONCATENATE("..",D214,".",E214,". - ",T214),CONCATENATE(D214,". - ",T214))),"")</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B214" s="2">
@@ -18071,7 +18071,7 @@
         <v>1128</v>
       </c>
       <c r="G214" s="40" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>cE01x</v>
       </c>
       <c r="H214" s="40"/>
@@ -18114,7 +18114,7 @@
     </row>
     <row r="215" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A215" s="44" t="str">
-        <f>IF(H215&lt;&gt;"",IF(F215&lt;&gt;"",CONCATENATE("...",D215,".",E215,".",F215,". - ",T215),IF(E215&lt;&gt;"",CONCATENATE("..",D215,".",E215,". - ",T215),CONCATENATE(D215,". - ",T215))),"")</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B215" s="2">
@@ -18133,7 +18133,7 @@
         <v>1128</v>
       </c>
       <c r="G215" s="40" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>cE01x</v>
       </c>
       <c r="H215" s="40"/>
@@ -18174,10 +18174,10 @@
       </c>
       <c r="X215" s="2"/>
     </row>
-    <row r="216" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A216" s="44" t="str">
-        <f>IF(H216&lt;&gt;"",IF(F216&lt;&gt;"",CONCATENATE("...",D216,".",E216,".",F216,". - ",T216),IF(E216&lt;&gt;"",CONCATENATE("..",D216,".",E216,". - ",T216),CONCATENATE(D216,". - ",T216))),"")</f>
-        <v>...E.01.c. - Accidental Firearm</v>
+        <f t="shared" si="19"/>
+        <v>....E.01.c. - Accidental Firearm</v>
       </c>
       <c r="B216" s="2"/>
       <c r="C216" s="31" t="s">
@@ -18193,7 +18193,7 @@
         <v>1130</v>
       </c>
       <c r="G216" s="40" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>cE01c</v>
       </c>
       <c r="H216" s="40" t="str">
@@ -18229,7 +18229,7 @@
     </row>
     <row r="217" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A217" s="44" t="str">
-        <f>IF(H217&lt;&gt;"",IF(F217&lt;&gt;"",CONCATENATE("...",D217,".",E217,".",F217,". - ",T217),IF(E217&lt;&gt;"",CONCATENATE("..",D217,".",E217,". - ",T217),CONCATENATE(D217,". - ",T217))),"")</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B217" s="2">
@@ -18248,7 +18248,7 @@
         <v>1128</v>
       </c>
       <c r="G217" s="40" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>cE01x</v>
       </c>
       <c r="H217" s="40"/>
@@ -18291,7 +18291,7 @@
     </row>
     <row r="218" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A218" s="44" t="str">
-        <f>IF(H218&lt;&gt;"",IF(F218&lt;&gt;"",CONCATENATE("...",D218,".",E218,".",F218,". - ",T218),IF(E218&lt;&gt;"",CONCATENATE("..",D218,".",E218,". - ",T218),CONCATENATE(D218,". - ",T218))),"")</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B218" s="2"/>
@@ -18320,8 +18320,8 @@
     </row>
     <row r="219" spans="1:24" ht="102" x14ac:dyDescent="0.25">
       <c r="A219" s="44" t="str">
-        <f>IF(H219&lt;&gt;"",IF(F219&lt;&gt;"",CONCATENATE("...",D219,".",E219,".",F219,". - ",T219),IF(E219&lt;&gt;"",CONCATENATE("..",D219,".",E219,". - ",T219),CONCATENATE(D219,". - ",T219))),"")</f>
-        <v>...E.01.x. - Other unintentional injuries</v>
+        <f t="shared" si="19"/>
+        <v>....E.01.x. - Other unintentional injuries</v>
       </c>
       <c r="B219" s="2">
         <v>206</v>
@@ -18339,7 +18339,7 @@
         <v>1128</v>
       </c>
       <c r="G219" s="40" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>cE01x</v>
       </c>
       <c r="H219" s="40" t="str">
@@ -18391,7 +18391,7 @@
     </row>
     <row r="220" spans="1:24" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A220" s="44" t="str">
-        <f>IF(H220&lt;&gt;"",IF(F220&lt;&gt;"",CONCATENATE("...",D220,".",E220,".",F220,". - ",T220),IF(E220&lt;&gt;"",CONCATENATE("..",D220,".",E220,". - ",T220),CONCATENATE(D220,". - ",T220))),"")</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B220" s="2">
@@ -18442,10 +18442,10 @@
       </c>
       <c r="X220" s="2"/>
     </row>
-    <row r="221" spans="1:24" ht="51" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A221" s="44" t="str">
-        <f>IF(H221&lt;&gt;"",IF(F221&lt;&gt;"",CONCATENATE("...",D221,".",E221,".",F221,". - ",T221),IF(E221&lt;&gt;"",CONCATENATE("..",D221,".",E221,". - ",T221),CONCATENATE(D221,". - ",T221))),"")</f>
-        <v>..E.02. - Suicide/Self-harm</v>
+        <f t="shared" si="19"/>
+        <v>...E.02. - Suicide/Self-harm</v>
       </c>
       <c r="B221" s="2">
         <v>208</v>
@@ -18461,7 +18461,7 @@
       </c>
       <c r="F221" s="6"/>
       <c r="G221" s="40" t="str">
-        <f t="shared" ref="G221:G228" si="18">CONCATENATE("c",D221,E221,F221)</f>
+        <f t="shared" ref="G221:G228" si="22">CONCATENATE("c",D221,E221,F221)</f>
         <v>cE02</v>
       </c>
       <c r="H221" s="40" t="str">
@@ -18511,8 +18511,8 @@
     </row>
     <row r="222" spans="1:24" ht="255" x14ac:dyDescent="0.25">
       <c r="A222" s="44" t="str">
-        <f>IF(H222&lt;&gt;"",IF(F222&lt;&gt;"",CONCATENATE("...",D222,".",E222,".",F222,". - ",T222),IF(E222&lt;&gt;"",CONCATENATE("..",D222,".",E222,". - ",T222),CONCATENATE(D222,". - ",T222))),"")</f>
-        <v>..E.03. - Homicide/Interpersonal violence</v>
+        <f t="shared" si="19"/>
+        <v>...E.03. - Homicide/Interpersonal violence</v>
       </c>
       <c r="B222" s="2">
         <v>209</v>
@@ -18569,10 +18569,10 @@
       </c>
       <c r="X222" s="2"/>
     </row>
-    <row r="223" spans="1:24" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A223" s="44" t="str">
-        <f>IF(H223&lt;&gt;"",IF(F223&lt;&gt;"",CONCATENATE("...",D223,".",E223,".",F223,". - ",T223),IF(E223&lt;&gt;"",CONCATENATE("..",D223,".",E223,". - ",T223),CONCATENATE(D223,". - ",T223))),"")</f>
-        <v>...E.03.a. - Homicide excluding legal intervention</v>
+        <f t="shared" si="19"/>
+        <v>....E.03.a. - Homicide excluding legal intervention</v>
       </c>
       <c r="B223" s="2"/>
       <c r="C223" s="31"/>
@@ -18586,11 +18586,11 @@
         <v>1126</v>
       </c>
       <c r="G223" s="40" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>cE03a</v>
       </c>
       <c r="H223" s="40" t="str">
-        <f t="shared" ref="H223:H225" si="19">CONCATENATE(D223,E223,F223)</f>
+        <f t="shared" ref="H223:H225" si="23">CONCATENATE(D223,E223,F223)</f>
         <v>E03a</v>
       </c>
       <c r="I223" s="5"/>
@@ -18616,10 +18616,10 @@
       <c r="W223" s="45"/>
       <c r="X223" s="2"/>
     </row>
-    <row r="224" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A224" s="44" t="str">
-        <f>IF(H224&lt;&gt;"",IF(F224&lt;&gt;"",CONCATENATE("...",D224,".",E224,".",F224,". - ",T224),IF(E224&lt;&gt;"",CONCATENATE("..",D224,".",E224,". - ",T224),CONCATENATE(D224,". - ",T224))),"")</f>
-        <v>...E.03.b. - Legal intervention</v>
+        <f t="shared" si="19"/>
+        <v>....E.03.b. - Legal intervention</v>
       </c>
       <c r="B224" s="2"/>
       <c r="C224" s="31"/>
@@ -18633,11 +18633,11 @@
         <v>1127</v>
       </c>
       <c r="G224" s="40" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>cE03b</v>
       </c>
       <c r="H224" s="40" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>E03b</v>
       </c>
       <c r="I224" s="5"/>
@@ -18665,8 +18665,8 @@
     </row>
     <row r="225" spans="1:24" ht="153" x14ac:dyDescent="0.25">
       <c r="A225" s="44" t="str">
-        <f>IF(H225&lt;&gt;"",IF(F225&lt;&gt;"",CONCATENATE("...",D225,".",E225,".",F225,". - ",T225),IF(E225&lt;&gt;"",CONCATENATE("..",D225,".",E225,". - ",T225),CONCATENATE(D225,". - ",T225))),"")</f>
-        <v>...E.03.c. - Execution, War, Terroism</v>
+        <f t="shared" si="19"/>
+        <v>....E.03.c. - Execution, War, Terroism</v>
       </c>
       <c r="B225" s="2">
         <v>210</v>
@@ -18684,11 +18684,11 @@
         <v>1130</v>
       </c>
       <c r="G225" s="40" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>cE03c</v>
       </c>
       <c r="H225" s="40" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>E03c</v>
       </c>
       <c r="I225" s="5" t="s">
@@ -18732,7 +18732,7 @@
     </row>
     <row r="226" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A226" s="44" t="str">
-        <f>IF(H226&lt;&gt;"",IF(F226&lt;&gt;"",CONCATENATE("...",D226,".",E226,".",F226,". - ",T226),IF(E226&lt;&gt;"",CONCATENATE("..",D226,".",E226,". - ",T226),CONCATENATE(D226,". - ",T226))),"")</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="B226" s="82" t="s">
@@ -18748,7 +18748,7 @@
         <v>1144</v>
       </c>
       <c r="G226" s="40" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>cE01</v>
       </c>
       <c r="H226" s="40"/>
@@ -18768,10 +18768,10 @@
         <v>1221</v>
       </c>
     </row>
-    <row r="227" spans="1:24" ht="178.5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A227" s="44" t="str">
-        <f>IF(H227&lt;&gt;"",IF(F227&lt;&gt;"",CONCATENATE("...",D227,".",E227,".",F227,". - ",T227),IF(E227&lt;&gt;"",CONCATENATE("..",D227,".",E227,". - ",T227),CONCATENATE(D227,". - ",T227))),"")</f>
-        <v>..Z.01. - Symptoms, signs and ill-defined conditions, not elsewhere classified</v>
+        <f t="shared" si="19"/>
+        <v>...Z.01. - Symptoms, signs and ill-defined conditions, not elsewhere classified</v>
       </c>
       <c r="D227" s="56" t="s">
         <v>1245</v>
@@ -18780,7 +18780,7 @@
         <v>1144</v>
       </c>
       <c r="G227" s="40" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>cZ01</v>
       </c>
       <c r="H227" s="40" t="str">
@@ -18805,7 +18805,7 @@
     </row>
     <row r="228" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A228" s="44" t="str">
-        <f>IF(H228&lt;&gt;"",IF(F228&lt;&gt;"",CONCATENATE("...",D228,".",E228,".",F228,". - ",T228),IF(E228&lt;&gt;"",CONCATENATE("..",D228,".",E228,". - ",T228),CONCATENATE(D228,". - ",T228))),"")</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="D228" s="56" t="s">
@@ -18815,7 +18815,7 @@
         <v>1152</v>
       </c>
       <c r="G228" s="42" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>cA09</v>
       </c>
       <c r="H228" s="40"/>
@@ -18835,10 +18835,10 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="229" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A229" s="44" t="str">
-        <f>IF(H229&lt;&gt;"",IF(F229&lt;&gt;"",CONCATENATE("...",D229,".",E229,".",F229,". - ",T229),IF(E229&lt;&gt;"",CONCATENATE("..",D229,".",E229,". - ",T229),CONCATENATE(D229,". - ",T229))),"")</f>
-        <v>..Z.02. - Unknown/Missing Value</v>
+        <f t="shared" si="19"/>
+        <v>...Z.02. - Unknown/Missing Value</v>
       </c>
       <c r="D229" s="56" t="s">
         <v>1245</v>
@@ -18848,17 +18848,17 @@
       </c>
       <c r="G229" s="43"/>
       <c r="H229" s="40" t="str">
-        <f t="shared" ref="H229:H232" si="20">CONCATENATE(D229,E229,F229)</f>
+        <f t="shared" ref="H229:H232" si="24">CONCATENATE(D229,E229,F229)</f>
         <v>Z02</v>
       </c>
       <c r="T229" s="48" t="s">
         <v>1316</v>
       </c>
     </row>
-    <row r="230" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:24" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A230" s="44" t="str">
-        <f>IF(H230&lt;&gt;"",IF(F230&lt;&gt;"",CONCATENATE("...",D230,".",E230,".",F230,". - ",T230),IF(E230&lt;&gt;"",CONCATENATE("..",D230,".",E230,". - ",T230),CONCATENATE(D230,". - ",T230))),"")</f>
-        <v>..Z.03. - Code does not map</v>
+        <f t="shared" si="19"/>
+        <v>...Z.03. - Code does not map</v>
       </c>
       <c r="D230" s="56" t="s">
         <v>1245</v>
@@ -18868,7 +18868,7 @@
       </c>
       <c r="G230" s="43"/>
       <c r="H230" s="40" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>Z03</v>
       </c>
       <c r="I230" s="16" t="s">
@@ -18878,27 +18878,27 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="231" spans="1:24" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A231" s="44" t="str">
-        <f>IF(H231&lt;&gt;"",IF(F231&lt;&gt;"",CONCATENATE("...",D231,".",E231,".",F231,". - ",T231),IF(E231&lt;&gt;"",CONCATENATE("..",D231,".",E231,". - ",T231),CONCATENATE(D231,". - ",T231))),"")</f>
-        <v>Z. - Unknown/Missing Value</v>
+        <f t="shared" si="19"/>
+        <v>..Z. - Unknown/Missing Value</v>
       </c>
       <c r="D231" s="56" t="s">
         <v>1245</v>
       </c>
       <c r="G231" s="43"/>
       <c r="H231" s="40" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>Z</v>
       </c>
       <c r="T231" s="48" t="s">
         <v>1316</v>
       </c>
     </row>
-    <row r="232" spans="1:24" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A232" s="44" t="str">
-        <f>IF(H232&lt;&gt;"",IF(F232&lt;&gt;"",CONCATENATE("...",D232,".",E232,".",F232,". - ",T232),IF(E232&lt;&gt;"",CONCATENATE("..",D232,".",E232,". - ",T232),CONCATENATE(D232,". - ",T232))),"")</f>
-        <v>..D.99. - Other Chronic Conditions</v>
+        <f t="shared" si="19"/>
+        <v>...D.99. - Other Chronic Conditions</v>
       </c>
       <c r="D232" s="56" t="s">
         <v>1142</v>
@@ -18908,7 +18908,7 @@
       </c>
       <c r="G232" s="43"/>
       <c r="H232" s="40" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>D99</v>
       </c>
       <c r="T232" s="48" t="s">

</xml_diff>